<commit_message>
Update version info and links
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>Project Name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>compiere</t>
   </si>
   <si>
-    <t>330?</t>
-  </si>
-  <si>
     <t>http://www.compiere.com/products/download/index.php</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>2.5.5*</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>hadoop</t>
   </si>
   <si>
@@ -108,9 +102,6 @@
     <t>hibernate</t>
   </si>
   <si>
-    <t>4.2.2</t>
-  </si>
-  <si>
     <t>hsqldb</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>jboss</t>
   </si>
   <si>
-    <t>5.1.0?</t>
-  </si>
-  <si>
     <t>http://www.jboss.org/downloads/</t>
   </si>
   <si>
@@ -210,9 +198,6 @@
     <t>weka</t>
   </si>
   <si>
-    <t>3.6?</t>
-  </si>
-  <si>
     <t>xalan</t>
   </si>
   <si>
@@ -220,9 +205,6 @@
   </si>
   <si>
     <t>xerces</t>
-  </si>
-  <si>
-    <t>2.1.0.0?</t>
   </si>
   <si>
     <t>blank for unknown;subject to mistakes, please update the correct information</t>
@@ -326,6 +308,50 @@
   </si>
   <si>
     <t>I inserted -agentlib=./libagent.so into the vuze.sh, the file that runs the software</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.5*</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.11.0.0* (we will use Xerces2 Java instead)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9.0*</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>freemind.sourceforge.net/wiki/index.php/Download</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.7.13*</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.jruby.org/download</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EAP 6.2.0.GA*</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -438,7 +464,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -460,6 +486,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -743,398 +772,508 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.69921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="63" style="1"/>
-    <col min="4" max="6" width="58" style="1" customWidth="1"/>
-    <col min="7" max="17" width="22.69921875" style="1"/>
-    <col min="18" max="16384" width="8.796875" style="1"/>
+    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.69921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="63" style="1"/>
+    <col min="5" max="7" width="58" style="1" customWidth="1"/>
+    <col min="8" max="18" width="22.69921875" style="1"/>
+    <col min="19" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
+    <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A12" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A28" s="1" t="s">
+    <row r="33" spans="5:5" ht="79.2" customHeight="1">
+      <c r="E33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="1" t="s">
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" ht="79.2" customHeight="1">
-      <c r="D33" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C13" r:id="rId6"/>
-    <hyperlink ref="C14" r:id="rId7"/>
-    <hyperlink ref="C21" r:id="rId8"/>
-    <hyperlink ref="C27" r:id="rId9"/>
-    <hyperlink ref="C7" r:id="rId10"/>
-    <hyperlink ref="C8" r:id="rId11"/>
-    <hyperlink ref="C11" r:id="rId12"/>
-    <hyperlink ref="C16" r:id="rId13"/>
-    <hyperlink ref="C17" r:id="rId14"/>
-    <hyperlink ref="C18" r:id="rId15"/>
-    <hyperlink ref="C19" r:id="rId16"/>
-    <hyperlink ref="C20" r:id="rId17"/>
-    <hyperlink ref="C22" r:id="rId18"/>
-    <hyperlink ref="C23" r:id="rId19" location="quick-start"/>
-    <hyperlink ref="C24" r:id="rId20"/>
-    <hyperlink ref="C25" r:id="rId21"/>
-    <hyperlink ref="C26" r:id="rId22"/>
-    <hyperlink ref="C28" r:id="rId23"/>
-    <hyperlink ref="C29" r:id="rId24"/>
-    <hyperlink ref="C30" r:id="rId25"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D13" r:id="rId6"/>
+    <hyperlink ref="D14" r:id="rId7"/>
+    <hyperlink ref="D21" r:id="rId8"/>
+    <hyperlink ref="D27" r:id="rId9"/>
+    <hyperlink ref="D7" r:id="rId10"/>
+    <hyperlink ref="D8" r:id="rId11"/>
+    <hyperlink ref="D11" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D17" r:id="rId14"/>
+    <hyperlink ref="D18" r:id="rId15"/>
+    <hyperlink ref="D19" r:id="rId16"/>
+    <hyperlink ref="D20" r:id="rId17"/>
+    <hyperlink ref="D22" r:id="rId18"/>
+    <hyperlink ref="D23" r:id="rId19" location="quick-start"/>
+    <hyperlink ref="D24" r:id="rId20"/>
+    <hyperlink ref="D25" r:id="rId21"/>
+    <hyperlink ref="D26" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D10" r:id="rId26"/>
+    <hyperlink ref="D12" r:id="rId27"/>
+    <hyperlink ref="D15" r:id="rId28"/>
+    <hyperlink ref="C14" r:id="rId29" display="http://www.jboss.org/download-manager/file/jboss-eap-6.2.0.GA-installer.jar"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId26"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the github projects to the project list
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\2014 SUMMER\Michael\ProjectsProfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gf219d\git\ProjectsProfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,17 +14,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>Project Name</t>
-  </si>
-  <si>
-    <t>Version Analyzed</t>
   </si>
   <si>
     <t>Link</t>
@@ -315,51 +312,233 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>0.9.0*</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>freemind.sourceforge.net/wiki/index.php/Download</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.7.13*</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.jruby.org/download</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EAP 6.2.0.GA*</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>2.11.0.0* (we will use Xerces2 Java instead)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9.0*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>freemind.sourceforge.net/wiki/index.php/Download</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.2.2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.7.13*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.jruby.org/download</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EAP 6.2.0.GA*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Index</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version/Commit Analyzed</t>
+  </si>
+  <si>
+    <t>https://github.com/viqsoft/Jmin</t>
+  </si>
+  <si>
+    <t>9cec118eceb92b008f183d15cc9f991a98a88402</t>
+  </si>
+  <si>
+    <t>Jmin (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
+  </si>
+  <si>
+    <t>https://github.com/tykkidream/DemoPermissions</t>
+  </si>
+  <si>
+    <t>907dfc7610da3b0e1df76ca6b561cfbc4c60f158</t>
+  </si>
+  <si>
+    <t>https://github.com/eclipse/org.aspectj</t>
+  </si>
+  <si>
+    <t>93c58e39cf0512d0920c37a40026a6aa5f1ff26b</t>
+  </si>
+  <si>
+    <t>AspectJ</t>
+  </si>
+  <si>
+    <t>DemoPermissions (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
+  </si>
+  <si>
+    <t>MCVersion-Control (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
+  </si>
+  <si>
+    <t>74b5e6d5c055a6fd204bac8ea3300626d70bd6cb</t>
+  </si>
+  <si>
+    <t>https://github.com/kschat/MCVersion-Control</t>
+  </si>
+  <si>
+    <t>https://github.com/JSansalone/NetBeansIDE</t>
+  </si>
+  <si>
+    <t>72112e83d96b9e25d62b7230b8d436ea6cd2d7e0</t>
+  </si>
+  <si>
+    <t>02f775b196ed6eae8e0cd2a7760193c315846498</t>
+  </si>
+  <si>
+    <t>https://github.com/Almaz-KG/FileManagerFtpHttpServer</t>
+  </si>
+  <si>
+    <t>FileManagerFtpHttpServer (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
+  </si>
+  <si>
+    <t>https://github.com/zoomis/NGOMS</t>
+  </si>
+  <si>
+    <t>NGOMS</t>
+  </si>
+  <si>
+    <t>Netbeans (I think this one can be removed because we are already covering it in the qualitas corpus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35349cca1c518382d30f0267ef077a0a1bf52606 </t>
+  </si>
+  <si>
+    <t>https://github.com/vdupain/refact4j</t>
+  </si>
+  <si>
+    <t>refact4j</t>
+  </si>
+  <si>
+    <t>fe0cdc5eb70c492993dfb55c39f5a90294383fa1</t>
+  </si>
+  <si>
+    <t>https://github.com/Babast/Timelag</t>
+  </si>
+  <si>
+    <t>817075e61b8fbf02b65326e9ba4af7c118679b77</t>
+  </si>
+  <si>
+    <t>TimeLag (This one might be malicious)</t>
+  </si>
+  <si>
+    <t>https://github.com/JetBrains/intellij-community</t>
+  </si>
+  <si>
+    <t>IntelliJ IDEA Community Edition</t>
+  </si>
+  <si>
+    <t>0e8564a197eb4584a1df56670bb7ed2a47be8da2</t>
+  </si>
+  <si>
+    <t>4eeab66ebed17b91b09d4bbc9d8a302fa25bcb3e</t>
+  </si>
+  <si>
+    <t>Metasploit-framework</t>
+  </si>
+  <si>
+    <t>https://github.com/rapid7/metasploit-framework</t>
+  </si>
+  <si>
+    <t>https://github.com/aleksz/driveddoc</t>
+  </si>
+  <si>
+    <t>0b2a80d8c0f9ba2d3e8f38ff4716da7c900c1183</t>
+  </si>
+  <si>
+    <t>driveddoc</t>
+  </si>
+  <si>
+    <t>https://github.com/holisticon/tracee</t>
+  </si>
+  <si>
+    <t>TracEE</t>
+  </si>
+  <si>
+    <t>205ada0800e089131a35f5e885a627b3f79fba5b</t>
+  </si>
+  <si>
+    <t>Spring-modules</t>
+  </si>
+  <si>
+    <t>https://github.com/astubbs/spring-modules</t>
+  </si>
+  <si>
+    <t>583b9c78f663720f6a4433c488614fd8f18f82d2</t>
+  </si>
+  <si>
+    <t>Security-Manager (This is a SecuirtyManager - not a program that uses one)</t>
+  </si>
+  <si>
+    <t>f9dec14f40e0cbad54532b4dd578a9bd8bb6a11e</t>
+  </si>
+  <si>
+    <t>https://github.com/wildfly-security/security-manager</t>
+  </si>
+  <si>
+    <t>https://github.com/ngty/gjman</t>
+  </si>
+  <si>
+    <t>Gjman</t>
+  </si>
+  <si>
+    <t>79c668c24ca65c33dc9d48d2b8372cea112ad59d</t>
+  </si>
+  <si>
+    <t>visor</t>
+  </si>
+  <si>
+    <t>https://github.com/hypernet/visor</t>
+  </si>
+  <si>
+    <t>31e032ac14d0d423e1b585de7041c054ddf83b0e</t>
+  </si>
+  <si>
+    <t>https://github.com/stefanbirkner/system-rules</t>
+  </si>
+  <si>
+    <t>System Rules</t>
+  </si>
+  <si>
+    <t>baea2a647da1ab4965c9d4ad8a232786ea80ce1a</t>
+  </si>
+  <si>
+    <t>https://github.com/ch33kybutt/oxygen_libcore</t>
+  </si>
+  <si>
+    <t>79a44848bcbb39474864610cab59d0fc170ae722</t>
+  </si>
+  <si>
+    <t>oxygen-libcore</t>
+  </si>
+  <si>
+    <t>tomcat (this one can be removed because it is covered in qualitas)</t>
+  </si>
+  <si>
+    <t>https://github.com/apache/tomcat70</t>
+  </si>
+  <si>
+    <t>c94013efbbe0b07891db2a72884627b37d98b97e</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -377,7 +556,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -391,7 +570,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="宋体"/>
+      <name val="Calibri Light"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -399,7 +578,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri Light"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -408,9 +587,22 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri Light"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
       <scheme val="major"/>
     </font>
   </fonts>
@@ -464,7 +656,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -490,11 +682,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="2" builtinId="8"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -510,7 +709,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -772,17 +971,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.796875" style="1"/>
-    <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63" style="1"/>
     <col min="5" max="7" width="58" style="1" customWidth="1"/>
     <col min="8" max="18" width="22.69921875" style="1"/>
@@ -791,28 +990,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -820,13 +1019,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -834,13 +1033,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4">
         <v>1.7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -848,13 +1047,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -862,13 +1061,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -876,13 +1075,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -890,13 +1089,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -904,13 +1103,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -918,13 +1117,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -932,13 +1131,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -946,13 +1145,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -960,13 +1159,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -974,13 +1173,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -988,13 +1187,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1002,13 +1201,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1016,13 +1215,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1030,13 +1229,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1044,13 +1243,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1058,13 +1257,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1072,13 +1271,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1086,13 +1285,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D21" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1100,13 +1299,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="D22" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1114,13 +1313,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="D23" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1128,13 +1327,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D24" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1142,13 +1341,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D25" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1156,13 +1355,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="D26" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1170,22 +1369,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="E27" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1193,13 +1392,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" s="4">
         <v>3.6</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1207,13 +1406,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D29" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1221,23 +1420,307 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="43.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="43.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="43.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="43.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.8">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="28.8">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="B51" s="7"/>
+      <c r="D51" s="9"/>
+    </row>
+    <row r="53" spans="1:5" ht="79.2" customHeight="1">
+      <c r="E53" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5" ht="79.2" customHeight="1">
-      <c r="E33" s="1" t="s">
+    </row>
+    <row r="54" spans="1:5">
+      <c r="E54" s="1" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5">
-      <c r="E34" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1272,8 +1755,25 @@
     <hyperlink ref="D12" r:id="rId27"/>
     <hyperlink ref="D15" r:id="rId28"/>
     <hyperlink ref="C14" r:id="rId29" display="http://www.jboss.org/download-manager/file/jboss-eap-6.2.0.GA-installer.jar"/>
+    <hyperlink ref="D32" r:id="rId30"/>
+    <hyperlink ref="D33" r:id="rId31"/>
+    <hyperlink ref="D34" r:id="rId32"/>
+    <hyperlink ref="D35" r:id="rId33"/>
+    <hyperlink ref="D36" r:id="rId34"/>
+    <hyperlink ref="D37" r:id="rId35"/>
+    <hyperlink ref="D39" r:id="rId36"/>
+    <hyperlink ref="D40" r:id="rId37"/>
+    <hyperlink ref="D42" r:id="rId38"/>
+    <hyperlink ref="D43" r:id="rId39"/>
+    <hyperlink ref="D44" r:id="rId40"/>
+    <hyperlink ref="D45" r:id="rId41"/>
+    <hyperlink ref="D46" r:id="rId42"/>
+    <hyperlink ref="D47" r:id="rId43"/>
+    <hyperlink ref="D48" r:id="rId44"/>
+    <hyperlink ref="D49" r:id="rId45"/>
+    <hyperlink ref="D50" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId30"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding more ant information
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gf219d\git\ProjectsProfiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -38,22 +42,10 @@
     <t>Grep Results</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>Ant</t>
   </si>
   <si>
     <t>1.9.4*</t>
-  </si>
-  <si>
-    <t>http://ant.apache.org/bindownload.cgi</t>
-  </si>
-  <si>
-    <t>Tried to use my version of Ant to compile Netbeans (bad idea – took 4 hours and then the build failed because of a memory overflow error) got no useful output “Callback on VMStart.
-#################################################
-#################################################
-Agent OnUnload, agent exits.”</t>
   </si>
   <si>
     <t>At Main.java:[line 856] 
@@ -129,8 +121,7 @@
 128:        perms.setSecurityManager();
 136:            perms.restoreSecurityManager();
 143:        perms.setSecurityManager();
-154:            perms.restoreSecurityManager();
-</t>
+154:            perms.restoreSecurityManager();</t>
   </si>
   <si>
     <t>apache batik</t>
@@ -578,37 +569,32 @@
   <si>
     <t>* Denotes versions where we do not use the QC version to avoid build issues</t>
   </si>
+  <si>
+    <t>Tried to use my version of Ant to compile Netbeans (bad idea – took 4 hours and then the build failed because of a memory overflow error) got no useful output 
+“Callback on VMStart.
+#################################################
+#################################################
+Agent OnUnload, agent exits.”</t>
+  </si>
+  <si>
+    <t>binaries from: http://ant.apache.org/bindownload.cgi
+source from: http://ant.apache.org/srcdownload.cgi</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00E+00"/>
-  </numFmts>
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -632,7 +618,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
@@ -640,7 +626,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
@@ -682,120 +668,75 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="2"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -854,35 +795,311 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:AMK54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.79342723004695"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.6995305164319"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.3004694835681"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="63.0046948356808"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="58"/>
-    <col collapsed="false" hidden="false" max="18" min="8" style="1" width="22.6995305164319"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="8.79342723004695"/>
+    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="2" max="2" width="35.69921875" style="1"/>
+    <col min="3" max="3" width="37.296875" style="1"/>
+    <col min="4" max="4" width="63" style="1"/>
+    <col min="5" max="7" width="58" style="1"/>
+    <col min="8" max="18" width="22.69921875" style="1"/>
+    <col min="19" max="1025" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -905,882 +1122,877 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="C3" s="6">
+        <v>1.7</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="H27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="5" t="s">
+    </row>
+    <row r="28" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="C28" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="6" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D30" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="s">
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="43.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D32" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="s">
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" ht="15">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D33" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B33" s="10" t="s">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="43.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D34" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="43.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D35" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="43.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C37" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D37" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D38" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D39" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="15">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C40" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D40" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="s">
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="15">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C41" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C42" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D42" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C43" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D43" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D44" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" ht="28.8">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D45" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D46" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D47" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D48" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D49" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="28.8">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D50" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>158</v>
-      </c>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:5">
       <c r="B51" s="5"/>
       <c r="D51" s="9"/>
       <c r="E51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:5">
       <c r="E52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:5" ht="79.2" customHeight="1">
       <c r="E53" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="E54" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="http://ant.apache.org/bindownload.cgi"/>
-    <hyperlink ref="D3" r:id="rId2" display="http://www.apache.org/dyn/closer.cgi/xmlgraphics/batik"/>
-    <hyperlink ref="D4" r:id="rId3" display="http://c-jdbc.ow2.org/download.html"/>
-    <hyperlink ref="D5" r:id="rId4" display="http://www.compiere.com/products/download/index.php"/>
-    <hyperlink ref="D6" r:id="rId5" display="http://db.apache.org/derby/derby_downloads.html"/>
-    <hyperlink ref="D7" r:id="rId6" display="http://www.drjava.org/"/>
-    <hyperlink ref="D8" r:id="rId7" display="http://download.eclipse.org/eclipse/downloads/"/>
-    <hyperlink ref="D10" r:id="rId8" display="http://sourceforge.net/projects/galleon/files/galleon/2.5.5/"/>
-    <hyperlink ref="D11" r:id="rId9" display="http://hadoop.apache.org/releases.html"/>
-    <hyperlink ref="D12" r:id="rId10" display="http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final"/>
-    <hyperlink ref="D13" r:id="rId11" display="http://hsqldb.org/"/>
-    <hyperlink ref="C14" r:id="rId12" display="EAP 6.2.0.GA*"/>
-    <hyperlink ref="D14" r:id="rId13" display="http://www.jboss.org/downloads/"/>
-    <hyperlink ref="D15" r:id="rId14" display="http://www.jruby.org/download"/>
-    <hyperlink ref="D16" r:id="rId15" display="http://lucene.apache.org/"/>
-    <hyperlink ref="D17" r:id="rId16" display="http://myfaces.apache.org/"/>
-    <hyperlink ref="D18" r:id="rId17" display="http://nekohtml.sourceforge.net/"/>
-    <hyperlink ref="D19" r:id="rId18" display="https://netbeans.org/downloads/"/>
-    <hyperlink ref="D20" r:id="rId19" display="http://openjms.sourceforge.net/downloads.html"/>
-    <hyperlink ref="D21" r:id="rId20" display="http://quartz-scheduler.org/"/>
-    <hyperlink ref="D22" r:id="rId21" display="http://www.quickserver.org/download.html"/>
-    <hyperlink ref="D23" r:id="rId22" location="quick-start" display="http://projects.spring.io/spring-framework/#quick-start"/>
-    <hyperlink ref="D24" r:id="rId23" display="http://struts.apache.org/"/>
-    <hyperlink ref="D25" r:id="rId24" display="http://tapestry.apache.org/download.html"/>
-    <hyperlink ref="D26" r:id="rId25" display="http://tomcat.apache.org/whichversion.html"/>
-    <hyperlink ref="D27" r:id="rId26" display="http://www.vuze.com/"/>
-    <hyperlink ref="D28" r:id="rId27" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
-    <hyperlink ref="D29" r:id="rId28" display="http://xml.apache.org/xalan-j/"/>
-    <hyperlink ref="D30" r:id="rId29" display="http://xerces.apache.org/mirrors.cgi"/>
-    <hyperlink ref="D32" r:id="rId30" display="https://github.com/tykkidream/DemoPermissions"/>
-    <hyperlink ref="D33" r:id="rId31" display="https://github.com/eclipse/org.aspectj"/>
-    <hyperlink ref="D34" r:id="rId32" display="https://github.com/kschat/MCVersion-Control"/>
-    <hyperlink ref="D35" r:id="rId33" display="https://github.com/JSansalone/NetBeansIDE"/>
-    <hyperlink ref="D36" r:id="rId34" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
-    <hyperlink ref="D37" r:id="rId35" display="https://github.com/zoomis/NGOMS"/>
-    <hyperlink ref="D39" r:id="rId36" display="https://github.com/Babast/Timelag"/>
-    <hyperlink ref="D40" r:id="rId37" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="D42" r:id="rId38" display="https://github.com/aleksz/driveddoc"/>
-    <hyperlink ref="D43" r:id="rId39" display="https://github.com/holisticon/tracee"/>
-    <hyperlink ref="D44" r:id="rId40" display="https://github.com/astubbs/spring-modules"/>
-    <hyperlink ref="D45" r:id="rId41" display="https://github.com/wildfly-security/security-manager"/>
-    <hyperlink ref="D46" r:id="rId42" display="https://github.com/ngty/gjman"/>
-    <hyperlink ref="D47" r:id="rId43" display="https://github.com/hypernet/visor"/>
-    <hyperlink ref="D48" r:id="rId44" display="https://github.com/stefanbirkner/system-rules"/>
-    <hyperlink ref="D49" r:id="rId45" display="https://github.com/ch33kybutt/oxygen_libcore"/>
-    <hyperlink ref="D50" r:id="rId46" display="https://github.com/apache/tomcat70"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="C14" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22" location="quick-start"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D32" r:id="rId30"/>
+    <hyperlink ref="D33" r:id="rId31"/>
+    <hyperlink ref="D34" r:id="rId32"/>
+    <hyperlink ref="D35" r:id="rId33"/>
+    <hyperlink ref="D36" r:id="rId34"/>
+    <hyperlink ref="D37" r:id="rId35"/>
+    <hyperlink ref="D39" r:id="rId36"/>
+    <hyperlink ref="D40" r:id="rId37"/>
+    <hyperlink ref="D42" r:id="rId38"/>
+    <hyperlink ref="D43" r:id="rId39"/>
+    <hyperlink ref="D44" r:id="rId40"/>
+    <hyperlink ref="D45" r:id="rId41"/>
+    <hyperlink ref="D46" r:id="rId42"/>
+    <hyperlink ref="D47" r:id="rId43"/>
+    <hyperlink ref="D48" r:id="rId44"/>
+    <hyperlink ref="D49" r:id="rId45"/>
+    <hyperlink ref="D50" r:id="rId46"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Done Tianyuan's pilot analysis
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="168">
   <si>
     <t>Index</t>
   </si>
@@ -129,8 +129,7 @@
 128:        perms.setSecurityManager();
 136:            perms.restoreSecurityManager();
 143:        perms.setSecurityManager();
-154:            perms.restoreSecurityManager();
-</t>
+154:            perms.restoreSecurityManager();</t>
   </si>
   <si>
     <t>apache batik</t>
@@ -175,6 +174,19 @@
     <t>http://www.drjava.org/</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>./src/edu/rice/cs/drjava/model/repl/newjvm/MainJVM.java
+470://  public void enableSecurityManager() throws RemoteException {
+471://    _interpreterJVM().enableSecurityManager();
+475://  public void disableSecurityManager() throws RemoteException{
+476://    _interpreterJVM().disableSecurityManager();
+./src/edu/rice/cs/drjava/model/GlobalModel.java
+140://  public void enableSecurityManager();
+143://  public void disableSecurityManager();</t>
+  </si>
+  <si>
     <t>eclipse_SDK</t>
   </si>
   <si>
@@ -193,6 +205,135 @@
     <t>freemind.sourceforge.net/wiki/index.php/Download</t>
   </si>
   <si>
+    <t>SecurityManager Changed:
+FreeMind.java, &lt;init&gt;, 277</t>
+  </si>
+  <si>
+    <t>Location 1:
+At FreeMind.java:[line 277] 
+In method new freemind.main.FreeMind(Properties, Properties, File) 
+Value Not null: freemind.main.FreeMindSecurityManager 
+Value new 
+Value new[187](3) 14 
+Value Variable is set at:
+Location 2:
+At ApplicationSecurityEnforcer.java:[line 172] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean) 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+Location 3:
+At ApplicationSecurityEnforcer.java:[line 176] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean) 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+Location 4:
+At ApplicationSecurityEnforcer.java:[line 250] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.installSecurityManager() 
+Value Not null: org.apache.batik.util.BatikSecurityManager 
+Value new 
+Value new[187](3) 29 
+Value Variable is set at: At ApplicationSecurityEnforcer.java:[line 204]</t>
+  </si>
+  <si>
+    <t>./plugins/script/ScriptingEngine.java
+42:import freemind.main.FreeMindSecurityManager;
+229:final ScriptingSecurityManager scriptingSecurityManager = new ScriptingSecurityManager(
+231:final FreeMindSecurityManager securityManager = (FreeMindSecurityManager) System
+232:.getSecurityManager();
+255:.setFinalSecurityManager(scriptingSecurityManager);
+264:.setFinalSecurityManager(scriptingSecurityManager);
+./plugins/script/ScriptingSecurityManager.java
+22:/*$Id: ScriptingSecurityManager.java,v 1.1.2.5 2008/04/02 20:02:37 christianfoltin Exp $*/
+37:public class ScriptingSecurityManager extends SecurityManager {
+59:public ScriptingSecurityManager(boolean pWithoutFileRestriction,
+./freemind/main/FreeMindSecurityManager.java
+22:/*$Id: FreeMindSecurityManager.java,v 1.1.2.1 2008/03/14 21:15:22 christianfoltin Exp $*/
+40:public final class FreeMindSecurityManager extends SecurityManager {
+42:private SecurityManager mFinalSecurityManager = null;
+44:public FreeMindSecurityManager() {
+48: * @param pFinalSecurityManager
+52:public void setFinalSecurityManager(SecurityManager pFinalSecurityManager) {
+53:if (pFinalSecurityManager == mFinalSecurityManager) {
+54:mFinalSecurityManager = null;
+57:if (mFinalSecurityManager != null) {
+59:"There is a SecurityManager installed already.");
+61:mFinalSecurityManager = pFinalSecurityManager;
+65:if (mFinalSecurityManager == null)
+67:mFinalSecurityManager.checkAccept(pHost, pPort);
+71:if (mFinalSecurityManager == null)
+73:mFinalSecurityManager.checkAccess(pT);
+77:if (mFinalSecurityManager == null)
+79:mFinalSecurityManager.checkAccess(pG);
+83:if (mFinalSecurityManager == null)
+85:mFinalSecurityManager.checkAwtEventQueueAccess();
+89:if (mFinalSecurityManager == null)
+91:mFinalSecurityManager.checkConnect(pHost, pPort, pContext);
+95:if (mFinalSecurityManager == null)
+97:mFinalSecurityManager.checkConnect(pHost, pPort);
+101:if (mFinalSecurityManager == null)
+103:mFinalSecurityManager.checkCreateClassLoader();
+107:if (mFinalSecurityManager == null)
+109:mFinalSecurityManager.checkDelete(pFile);
+113:if (mFinalSecurityManager == null)
+115:mFinalSecurityManager.checkExec(pCmd);
+119:if (mFinalSecurityManager == null)
+121:mFinalSecurityManager.checkExit(pStatus);
+125:if (mFinalSecurityManager == null)
+127:mFinalSecurityManager.checkLink(pLib);
+131:if (mFinalSecurityManager == null)
+133:mFinalSecurityManager.checkListen(pPort);
+137:if (mFinalSecurityManager == null)
+139:mFinalSecurityManager.checkMemberAccess(arg0, arg1);
+143:if (mFinalSecurityManager == null)
+145:mFinalSecurityManager.checkMulticast(pMaddr, pTtl);
+149:if (mFinalSecurityManager == null)
+151:mFinalSecurityManager.checkMulticast(pMaddr);
+155:if (mFinalSecurityManager == null)
+157:mFinalSecurityManager.checkPackageAccess(pPkg);
+161:if (mFinalSecurityManager == null)
+163:mFinalSecurityManager.checkPackageDefinition(pPkg);
+167:if (mFinalSecurityManager == null)
+169:mFinalSecurityManager.checkPermission(pPerm, pContext);
+173:if (mFinalSecurityManager == null)
+175:mFinalSecurityManager.checkPermission(pPerm);
+179:if (mFinalSecurityManager == null)
+181:mFinalSecurityManager.checkPrintJobAccess();
+185:if (mFinalSecurityManager == null)
+187:mFinalSecurityManager.checkPropertiesAccess();
+191:if (mFinalSecurityManager == null)
+193:mFinalSecurityManager.checkPropertyAccess(pKey);
+197:if (mFinalSecurityManager == null)
+199:mFinalSecurityManager.checkRead(pFd);
+203:if (mFinalSecurityManager == null)
+205:mFinalSecurityManager.checkRead(pFile, pContext);
+209:if (mFinalSecurityManager == null)
+211:mFinalSecurityManager.checkRead(pFile);
+215:if (mFinalSecurityManager == null)
+217:mFinalSecurityManager.checkSecurityAccess(pTarget);
+221:if (mFinalSecurityManager == null)
+223:mFinalSecurityManager.checkSetFactory();
+227:if (mFinalSecurityManager == null)
+229:mFinalSecurityManager.checkSystemClipboardAccess();
+233:if (mFinalSecurityManager == null)
+235:return mFinalSecurityManager.checkTopLevelWindow(pWindow);
+239:if (mFinalSecurityManager == null)
+241:mFinalSecurityManager.checkWrite(pFd);
+245:if (mFinalSecurityManager == null)
+247:mFinalSecurityManager.checkWrite(pFile);
+251:if (mFinalSecurityManager == null)
+253:return mFinalSecurityManager.getSecurityContext();
+./freemind/main/FreeMind.java
+277:System.setSecurityManager(new FreeMindSecurityManager());
+./tests/freemind/ToolsTests.java
+35:import freemind.main.FreeMindSecurityManager;
+215:public void testUpdateWithSecurityManager() throws FileNotFoundException,
+222:System.setSecurityManager(new FreeMindSecurityManager());</t>
+  </si>
+  <si>
     <t>galleon</t>
   </si>
   <si>
@@ -232,10 +373,47 @@
     <t>jboss</t>
   </si>
   <si>
-    <t>EAP 6.2.0.GA*</t>
+    <t>5.1.0.GA</t>
   </si>
   <si>
     <t>http://www.jboss.org/downloads/</t>
+  </si>
+  <si>
+    <t>Location 1:
+At EjbModule.java:[line 627] 
+In method org.jboss.ejb.EjbModule.destroyService() 
+Value Set to null:   
+Value invokeinterface 
+Value invokeinterface[185](5) 131 
+Value Variable is set at: At EjbModule.java:[line 553]
+Location 2:
+At EjbModule.java:[line 871] 
+In method org.jboss.ejb.EjbModule.initializeContainer(Container, ConfigurationMetaData, BeanMetaData, int, DeploymentUnit) 
+Value Could be null or other value: org.jboss.security.AuthenticationManager
+Location 3:
+At SecurityPolicy.java:[line 91] 
+In method org.jboss.system.server.security.SecurityPolicy.start() 
+Value Not null: java.lang.SecurityManager 
+Value aload_0 
+Value aload_0[42](1) 
+Value Variable is set at: At SecurityPolicy.java:[line 90]
+Location 4:
+At SecurityPolicy.java:[line 97] 
+In method org.jboss.system.server.security.SecurityPolicy.stop() 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+Location 5:
+At QuartzServer.java:[line 264] 
+In method org.quartz.impl.QuartzServer.main(String[]) 
+Value Not null: java.rmi.RMISecurityManager 
+Value new 
+Value new[187](3) 37 
+Value Variable is set at:</t>
+  </si>
+  <si>
+    <t>See attached file</t>
   </si>
   <si>
     <t>jruby</t>
@@ -615,21 +793,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="3"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri Light"/>
       <family val="3"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -637,7 +815,7 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
       <family val="3"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -793,7 +971,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -862,13 +1040,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -946,6 +1123,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="4"/>
+      <c r="F3" s="0"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
@@ -963,6 +1141,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="4"/>
+      <c r="F4" s="0"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
@@ -980,6 +1159,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="4"/>
+      <c r="F5" s="0"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
@@ -997,6 +1177,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="4"/>
+      <c r="F6" s="0"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
@@ -1013,8 +1194,15 @@
       <c r="D7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1022,15 +1210,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E8" s="4"/>
+      <c r="F8" s="0"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
@@ -1039,16 +1228,23 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="G9" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1056,15 +1252,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E10" s="4"/>
+      <c r="F10" s="0"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -1073,15 +1270,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E11" s="4"/>
+      <c r="F11" s="0"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
@@ -1090,15 +1288,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E12" s="4"/>
+      <c r="F12" s="0"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
@@ -1107,15 +1306,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E13" s="4"/>
+      <c r="F13" s="0"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
@@ -1124,16 +1324,23 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="G14" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1141,13 +1348,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E15" s="4"/>
       <c r="G15" s="4"/>
@@ -1158,13 +1365,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
@@ -1175,13 +1382,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
@@ -1192,13 +1399,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E18" s="4"/>
       <c r="G18" s="4"/>
@@ -1209,13 +1416,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E19" s="4"/>
       <c r="G19" s="4"/>
@@ -1226,13 +1433,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E20" s="4"/>
       <c r="G20" s="4"/>
@@ -1243,13 +1450,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E21" s="4"/>
       <c r="G21" s="4"/>
@@ -1260,13 +1467,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E22" s="4"/>
       <c r="G22" s="4"/>
@@ -1277,13 +1484,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E23" s="4"/>
       <c r="G23" s="4"/>
@@ -1294,13 +1501,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E24" s="4"/>
       <c r="G24" s="4"/>
@@ -1311,13 +1518,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E25" s="4"/>
       <c r="G25" s="4"/>
@@ -1328,13 +1535,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E26" s="4"/>
       <c r="G26" s="4"/>
@@ -1345,22 +1552,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1368,13 +1575,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C28" s="6" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E28" s="4"/>
     </row>
@@ -1383,13 +1590,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E29" s="4"/>
     </row>
@@ -1398,13 +1605,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E30" s="4"/>
     </row>
@@ -1413,13 +1620,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E31" s="4"/>
     </row>
@@ -1428,13 +1635,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E32" s="4"/>
     </row>
@@ -1443,13 +1650,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="E33" s="4"/>
     </row>
@@ -1458,13 +1665,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E34" s="4"/>
     </row>
@@ -1473,13 +1680,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E35" s="4"/>
     </row>
@@ -1488,13 +1695,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E36" s="4"/>
     </row>
@@ -1503,13 +1710,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E37" s="4"/>
     </row>
@@ -1518,13 +1725,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="E38" s="4"/>
     </row>
@@ -1533,13 +1740,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="E39" s="4"/>
     </row>
@@ -1548,13 +1755,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E40" s="4"/>
     </row>
@@ -1563,13 +1770,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E41" s="4"/>
     </row>
@@ -1578,13 +1785,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E42" s="4"/>
     </row>
@@ -1593,13 +1800,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E43" s="4"/>
     </row>
@@ -1608,13 +1815,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E44" s="4"/>
     </row>
@@ -1623,13 +1830,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E45" s="4"/>
     </row>
@@ -1638,13 +1845,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E46" s="4"/>
     </row>
@@ -1653,13 +1860,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E47" s="4"/>
     </row>
@@ -1668,13 +1875,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E48" s="4"/>
     </row>
@@ -1683,13 +1890,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E49" s="4"/>
     </row>
@@ -1698,13 +1905,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E50" s="4"/>
     </row>
@@ -1718,12 +1925,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1739,41 +1946,40 @@
     <hyperlink ref="D11" r:id="rId9" display="http://hadoop.apache.org/releases.html"/>
     <hyperlink ref="D12" r:id="rId10" display="http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final"/>
     <hyperlink ref="D13" r:id="rId11" display="http://hsqldb.org/"/>
-    <hyperlink ref="C14" r:id="rId12" display="EAP 6.2.0.GA*"/>
-    <hyperlink ref="D14" r:id="rId13" display="http://www.jboss.org/downloads/"/>
-    <hyperlink ref="D15" r:id="rId14" display="http://www.jruby.org/download"/>
-    <hyperlink ref="D16" r:id="rId15" display="http://lucene.apache.org/"/>
-    <hyperlink ref="D17" r:id="rId16" display="http://myfaces.apache.org/"/>
-    <hyperlink ref="D18" r:id="rId17" display="http://nekohtml.sourceforge.net/"/>
-    <hyperlink ref="D19" r:id="rId18" display="https://netbeans.org/downloads/"/>
-    <hyperlink ref="D20" r:id="rId19" display="http://openjms.sourceforge.net/downloads.html"/>
-    <hyperlink ref="D21" r:id="rId20" display="http://quartz-scheduler.org/"/>
-    <hyperlink ref="D22" r:id="rId21" display="http://www.quickserver.org/download.html"/>
-    <hyperlink ref="D23" r:id="rId22" location="quick-start" display="http://projects.spring.io/spring-framework/#quick-start"/>
-    <hyperlink ref="D24" r:id="rId23" display="http://struts.apache.org/"/>
-    <hyperlink ref="D25" r:id="rId24" display="http://tapestry.apache.org/download.html"/>
-    <hyperlink ref="D26" r:id="rId25" display="http://tomcat.apache.org/whichversion.html"/>
-    <hyperlink ref="D27" r:id="rId26" display="http://www.vuze.com/"/>
-    <hyperlink ref="D28" r:id="rId27" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
-    <hyperlink ref="D29" r:id="rId28" display="http://xml.apache.org/xalan-j/"/>
-    <hyperlink ref="D30" r:id="rId29" display="http://xerces.apache.org/mirrors.cgi"/>
-    <hyperlink ref="D32" r:id="rId30" display="https://github.com/tykkidream/DemoPermissions"/>
-    <hyperlink ref="D33" r:id="rId31" display="https://github.com/eclipse/org.aspectj"/>
-    <hyperlink ref="D34" r:id="rId32" display="https://github.com/kschat/MCVersion-Control"/>
-    <hyperlink ref="D35" r:id="rId33" display="https://github.com/JSansalone/NetBeansIDE"/>
-    <hyperlink ref="D36" r:id="rId34" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
-    <hyperlink ref="D37" r:id="rId35" display="https://github.com/zoomis/NGOMS"/>
-    <hyperlink ref="D39" r:id="rId36" display="https://github.com/Babast/Timelag"/>
-    <hyperlink ref="D40" r:id="rId37" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="D42" r:id="rId38" display="https://github.com/aleksz/driveddoc"/>
-    <hyperlink ref="D43" r:id="rId39" display="https://github.com/holisticon/tracee"/>
-    <hyperlink ref="D44" r:id="rId40" display="https://github.com/astubbs/spring-modules"/>
-    <hyperlink ref="D45" r:id="rId41" display="https://github.com/wildfly-security/security-manager"/>
-    <hyperlink ref="D46" r:id="rId42" display="https://github.com/ngty/gjman"/>
-    <hyperlink ref="D47" r:id="rId43" display="https://github.com/hypernet/visor"/>
-    <hyperlink ref="D48" r:id="rId44" display="https://github.com/stefanbirkner/system-rules"/>
-    <hyperlink ref="D49" r:id="rId45" display="https://github.com/ch33kybutt/oxygen_libcore"/>
-    <hyperlink ref="D50" r:id="rId46" display="https://github.com/apache/tomcat70"/>
+    <hyperlink ref="D14" r:id="rId12" display="http://www.jboss.org/downloads/"/>
+    <hyperlink ref="D15" r:id="rId13" display="http://www.jruby.org/download"/>
+    <hyperlink ref="D16" r:id="rId14" display="http://lucene.apache.org/"/>
+    <hyperlink ref="D17" r:id="rId15" display="http://myfaces.apache.org/"/>
+    <hyperlink ref="D18" r:id="rId16" display="http://nekohtml.sourceforge.net/"/>
+    <hyperlink ref="D19" r:id="rId17" display="https://netbeans.org/downloads/"/>
+    <hyperlink ref="D20" r:id="rId18" display="http://openjms.sourceforge.net/downloads.html"/>
+    <hyperlink ref="D21" r:id="rId19" display="http://quartz-scheduler.org/"/>
+    <hyperlink ref="D22" r:id="rId20" display="http://www.quickserver.org/download.html"/>
+    <hyperlink ref="D23" r:id="rId21" location="quick-start" display="http://projects.spring.io/spring-framework/#quick-start"/>
+    <hyperlink ref="D24" r:id="rId22" display="http://struts.apache.org/"/>
+    <hyperlink ref="D25" r:id="rId23" display="http://tapestry.apache.org/download.html"/>
+    <hyperlink ref="D26" r:id="rId24" display="http://tomcat.apache.org/whichversion.html"/>
+    <hyperlink ref="D27" r:id="rId25" display="http://www.vuze.com/"/>
+    <hyperlink ref="D28" r:id="rId26" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
+    <hyperlink ref="D29" r:id="rId27" display="http://xml.apache.org/xalan-j/"/>
+    <hyperlink ref="D30" r:id="rId28" display="http://xerces.apache.org/mirrors.cgi"/>
+    <hyperlink ref="D32" r:id="rId29" display="https://github.com/tykkidream/DemoPermissions"/>
+    <hyperlink ref="D33" r:id="rId30" display="https://github.com/eclipse/org.aspectj"/>
+    <hyperlink ref="D34" r:id="rId31" display="https://github.com/kschat/MCVersion-Control"/>
+    <hyperlink ref="D35" r:id="rId32" display="https://github.com/JSansalone/NetBeansIDE"/>
+    <hyperlink ref="D36" r:id="rId33" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
+    <hyperlink ref="D37" r:id="rId34" display="https://github.com/zoomis/NGOMS"/>
+    <hyperlink ref="D39" r:id="rId35" display="https://github.com/Babast/Timelag"/>
+    <hyperlink ref="D40" r:id="rId36" display="https://github.com/JetBrains/intellij-community"/>
+    <hyperlink ref="D42" r:id="rId37" display="https://github.com/aleksz/driveddoc"/>
+    <hyperlink ref="D43" r:id="rId38" display="https://github.com/holisticon/tracee"/>
+    <hyperlink ref="D44" r:id="rId39" display="https://github.com/astubbs/spring-modules"/>
+    <hyperlink ref="D45" r:id="rId40" display="https://github.com/wildfly-security/security-manager"/>
+    <hyperlink ref="D46" r:id="rId41" display="https://github.com/ngty/gjman"/>
+    <hyperlink ref="D47" r:id="rId42" display="https://github.com/hypernet/visor"/>
+    <hyperlink ref="D48" r:id="rId43" display="https://github.com/stefanbirkner/system-rules"/>
+    <hyperlink ref="D49" r:id="rId44" display="https://github.com/ch33kybutt/oxygen_libcore"/>
+    <hyperlink ref="D50" r:id="rId45" display="https://github.com/apache/tomcat70"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Personal notes, added a little bit
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -632,11 +632,6 @@
   </si>
   <si>
     <t>* Denotes versions where we do not use the QC version to avoid build issues</t>
-  </si>
-  <si>
-    <t>From the grep result, we can see that all statements are commented out.
-DETECT_SECURITY_MANAGER_SET_LOCATION_BUG entry is not shown, which can be verified in the grep result.</t>
-    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>./plugins/script/ScriptingEngine.java
@@ -735,10 +730,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>When the program is running, the security manager is set via line 277 in FreeMind.java, which can be verified by all of the analysis. Because another SM is set in test cases, but not in the main program, the analysis tools didn't catch this case.</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>Location 1:
 At EjbModule.java:[line 627] 
 In method org.jboss.ejb.EjbModule.destroyService() 
@@ -775,6 +766,15 @@
   </si>
   <si>
     <t>Due to its complicated nature, there are multiple places where SM is set to null. However, during the running of the main program, there is no such statement happened. Our dynamic analysis showed this fact.</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>When the program is running, the security manager is set via line 277 in FreeMind.java, which can be verified by all of the analysis. Because another SM is set in test cases, but not in the main program, the analysis tools didn't catch this case. In the source code, the program defines its own SM via extending the SM class and adds more policies to it, and therefore strengens the security policy.</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>From the grep result, we can see that all statements are commented out.
+DETECT_SECURITY_MANAGER_SET_LOCATION_BUG entry is not shown, which can be verified in the grep result. Therefore I claim that the security policy is not weakened.</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -1302,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="F6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1313,7 +1313,8 @@
     <col min="3" max="3" width="37.33203125" style="1"/>
     <col min="4" max="4" width="63" style="1"/>
     <col min="5" max="7" width="58" style="1"/>
-    <col min="8" max="18" width="22.6640625" style="1"/>
+    <col min="8" max="8" width="32.5546875" style="1" customWidth="1"/>
+    <col min="9" max="18" width="22.6640625" style="1"/>
     <col min="19" max="1025" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
@@ -1462,7 +1463,7 @@
         <v>29</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1503,10 +1504,10 @@
         <v>37</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75.599999999999994" customHeight="1">
@@ -1598,13 +1599,13 @@
         <v>28</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>53</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="75.599999999999994" customHeight="1">

</xml_diff>

<commit_message>
Added the grep results and static analysis results
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="199">
   <si>
     <t>Index</t>
   </si>
@@ -248,7 +248,41 @@
     <t>http://www.apache.org/dyn/closer.cgi/xmlgraphics/batik</t>
   </si>
   <si>
-    <t>At Main.java:[line 856] </t>
+    <t> At ApplicationSecurityEnforcer.java:[line 172]
+ In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean)
+ Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+--------------------------------------------------------------
+At ApplicationSecurityEnforcer.java:[line 176] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean) 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+--------------------------------------------------------------
+At ApplicationSecurityEnforcer.java:[line 250] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.installSecurityManager() 
+Value Not null: org.apache.batik.util.BatikSecurityManager 
+Value new Value new[187](3) 29 
+Value Variable is set at: At ApplicationSecurityEnforcer.java:[line 204]</t>
+  </si>
+  <si>
+    <t>./batik-1.7/test-sources/org/apache/batik/util/ApplicationSecurityEnforcerTest.java
+89:                System.setSecurityManager(null);
+108:                System.setSecurityManager(null);
+./batik-1.7/samples/tests/resources/java/sources/com/untrusted/script/UntrustedScriptHandler.java
+103:        {"RuntimePermission setSecurityManager", new RuntimePermission("setSecurityManager")}, 
+./batik-1.7/test-resources/org/apache/batik/bridge/JarCheckPermissionsGranted.java
+98:        {"RuntimePermission setSecurityManager", new RuntimePermission("setSecurityManager")}, 
+./batik-1.7/test-resources/org/apache/batik/bridge/JarCheckPermissionsDenied.java
+98:        {"RuntimePermission setSecurityManager", new RuntimePermission("setSecurityManager")}, 
+./batik-1.7/sources/org/apache/batik/util/ApplicationSecurityEnforcer.java
+172:            System.setSecurityManager(null);
+176:                System.setSecurityManager(null);
+250:        System.setSecurityManager(securityManager);
+</t>
   </si>
   <si>
     <t>c_jdbc</t>
@@ -1190,8 +1224,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1290,10 +1324,12 @@
         <v>22</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1301,17 +1337,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1321,17 +1357,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -1341,17 +1377,17 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -1361,25 +1397,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1387,17 +1423,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1407,25 +1443,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1433,17 +1469,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1453,17 +1489,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1473,17 +1509,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -1493,17 +1529,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1513,25 +1549,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1539,17 +1575,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1559,17 +1595,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1579,17 +1615,17 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1599,17 +1635,17 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -1619,17 +1655,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1639,17 +1675,17 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1659,17 +1695,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1679,17 +1715,17 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1699,17 +1735,17 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -1719,17 +1755,17 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -1739,17 +1775,17 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -1759,13 +1795,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -1776,22 +1812,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1799,13 +1835,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -1814,13 +1850,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -1829,13 +1865,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -1844,13 +1880,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -1859,13 +1895,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -1874,13 +1910,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -1889,13 +1925,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -1904,13 +1940,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -1919,13 +1955,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -1934,13 +1970,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1949,13 +1985,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -1964,13 +2000,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -1979,13 +2015,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -1994,13 +2030,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -2009,13 +2045,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -2024,13 +2060,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -2039,13 +2075,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -2054,13 +2090,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -2069,13 +2105,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -2084,13 +2120,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -2099,13 +2135,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -2114,13 +2150,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -2129,13 +2165,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -2149,12 +2185,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Somehow I overwrote Tianyuan's static analysis restults so I manually copy and pasted them in
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gf219d\git\ProjectsProfiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="180">
   <si>
     <t>Index</t>
   </si>
@@ -248,7 +252,7 @@
     <t>http://www.apache.org/dyn/closer.cgi/xmlgraphics/batik</t>
   </si>
   <si>
-    <t> At ApplicationSecurityEnforcer.java:[line 172]
+    <t>At ApplicationSecurityEnforcer.java:[line 172]
  In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean)
  Value Set to null:   
 Value aconst_null 
@@ -281,8 +285,7 @@
 ./batik-1.7/sources/org/apache/batik/util/ApplicationSecurityEnforcer.java
 172:            System.setSecurityManager(null);
 176:                System.setSecurityManager(null);
-250:        System.setSecurityManager(securityManager);
-</t>
+250:        System.setSecurityManager(securityManager);</t>
   </si>
   <si>
     <t>c_jdbc</t>
@@ -294,9 +297,6 @@
     <t>http://c-jdbc.ow2.org/download.html</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.Main.runBuild(ClassLoader) </t>
-  </si>
-  <si>
     <t>compiere</t>
   </si>
   <si>
@@ -306,9 +306,6 @@
     <t>http://www.compiere.com/products/download/index.php</t>
   </si>
   <si>
-    <t>Value Not null: java.lang.SecurityManager </t>
-  </si>
-  <si>
     <t>derby</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t>http://db.apache.org/derby/derby_downloads.html</t>
   </si>
   <si>
-    <t>Value invokestatic </t>
-  </si>
-  <si>
     <t>drjava</t>
   </si>
   <si>
@@ -331,9 +325,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Value invokestatic[184](3) 208 </t>
   </si>
   <si>
     <t>./src/edu/rice/cs/drjava/model/repl/newjvm/MainJVM.java
@@ -359,9 +350,6 @@
     <t>http://download.eclipse.org/eclipse/downloads/</t>
   </si>
   <si>
-    <t>Value Variable is set at: At Main.java:[line 779]</t>
-  </si>
-  <si>
     <t>freemind</t>
   </si>
   <si>
@@ -373,9 +361,6 @@
   <si>
     <t>SecurityManager Changed:
 FreeMind.java, &lt;init&gt;, 277</t>
-  </si>
-  <si>
-    <t>-----------------------------------------------------------</t>
   </si>
   <si>
     <t>./plugins/script/ScriptingEngine.java
@@ -485,9 +470,6 @@
     <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
   </si>
   <si>
-    <t> At JUnitTestRunner.java:[line 347] </t>
-  </si>
-  <si>
     <t>hadoop</t>
   </si>
   <si>
@@ -497,9 +479,6 @@
     <t>http://hadoop.apache.org/releases.html</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.taskdefs.optional.junit.JUnitTestRunner.setupIOStreams(ByteArrayOutputStream, ByteArrayOutputStream) </t>
-  </si>
-  <si>
     <t>hibernate</t>
   </si>
   <si>
@@ -509,9 +488,6 @@
     <t>http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final</t>
   </si>
   <si>
-    <t>Value Not null: org.apache.tools.ant.types.Permissions </t>
-  </si>
-  <si>
     <t>hsqldb</t>
   </si>
   <si>
@@ -521,9 +497,6 @@
     <t>http://hsqldb.org/</t>
   </si>
   <si>
-    <t>Value aload_0 </t>
-  </si>
-  <si>
     <t>jboss</t>
   </si>
   <si>
@@ -533,9 +506,6 @@
     <t>http://www.jboss.org/downloads/</t>
   </si>
   <si>
-    <t>Value aload_0[42](1) </t>
-  </si>
-  <si>
     <t>See attached file</t>
   </si>
   <si>
@@ -551,9 +521,6 @@
     <t>http://www.jruby.org/download</t>
   </si>
   <si>
-    <t>Value Variable is set at: At JUnitTestRunner.java:[line 346]</t>
-  </si>
-  <si>
     <t>lucene</t>
   </si>
   <si>
@@ -572,9 +539,6 @@
     <t>http://myfaces.apache.org/</t>
   </si>
   <si>
-    <t>At Permissions.java:[line 101] </t>
-  </si>
-  <si>
     <t>nekohtml</t>
   </si>
   <si>
@@ -584,9 +548,6 @@
     <t>http://nekohtml.sourceforge.net/</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.types.Permissions.setSecurityManager() </t>
-  </si>
-  <si>
     <t>netbeans</t>
   </si>
   <si>
@@ -596,9 +557,6 @@
     <t>https://netbeans.org/downloads/</t>
   </si>
   <si>
-    <t>Value Not null: org.apache.tools.ant.types.Permissions$MySM </t>
-  </si>
-  <si>
     <t>openjms</t>
   </si>
   <si>
@@ -608,9 +566,6 @@
     <t>http://openjms.sourceforge.net/downloads.html</t>
   </si>
   <si>
-    <t>Value new Value new[187](3) 14 </t>
-  </si>
-  <si>
     <t>quartz scheduler</t>
   </si>
   <si>
@@ -620,9 +575,6 @@
     <t>http://quartz-scheduler.org/</t>
   </si>
   <si>
-    <t>Value Variable is set at:</t>
-  </si>
-  <si>
     <t>quickserver</t>
   </si>
   <si>
@@ -632,9 +584,6 @@
     <t>http://www.quickserver.org/download.html</t>
   </si>
   <si>
-    <t>---------------------------------------------------------------</t>
-  </si>
-  <si>
     <t>spring framework</t>
   </si>
   <si>
@@ -644,9 +593,6 @@
     <t>http://projects.spring.io/spring-framework/#quick-start</t>
   </si>
   <si>
-    <t> At Permissions.java:[line 171]</t>
-  </si>
-  <si>
     <t>struts</t>
   </si>
   <si>
@@ -656,9 +602,6 @@
     <t>http://struts.apache.org/</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.types.Permissions.restoreSecurityManager()</t>
-  </si>
-  <si>
     <t>tapestry</t>
   </si>
   <si>
@@ -666,9 +609,6 @@
   </si>
   <si>
     <t>http://tapestry.apache.org/download.html</t>
-  </si>
-  <si>
-    <t>Value Could be null or other value: java.lang.SecurityManager</t>
   </si>
   <si>
     <t>tomcat</t>
@@ -912,37 +852,82 @@
   <si>
     <t>* Denotes versions where we do not use the QC version to avoid build issues</t>
   </si>
+  <si>
+    <t>Location 1:
+At FreeMind.java:[line 277] 
+In method new freemind.main.FreeMind(Properties, Properties, File) 
+Value Not null: freemind.main.FreeMindSecurityManager 
+Value new 
+Value new[187](3) 14 
+Value Variable is set at:
+Location 2:
+At ApplicationSecurityEnforcer.java:[line 172] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean) 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+Location 3:
+At ApplicationSecurityEnforcer.java:[line 176] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean) 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+Location 4:
+At ApplicationSecurityEnforcer.java:[line 250] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.installSecurityManager() 
+Value Not null: org.apache.batik.util.BatikSecurityManager 
+Value new 
+Value new[187](3) 29 
+Value Variable is set at: At ApplicationSecurityEnforcer.java:[line 204]</t>
+  </si>
+  <si>
+    <t>Location 1:
+At EjbModule.java:[line 627] 
+In method org.jboss.ejb.EjbModule.destroyService() 
+Value Set to null:   
+Value invokeinterface 
+Value invokeinterface[185](5) 131 
+Value Variable is set at: At EjbModule.java:[line 553]
+Location 2:
+At EjbModule.java:[line 871] 
+In method org.jboss.ejb.EjbModule.initializeContainer(Container, ConfigurationMetaData, BeanMetaData, int, DeploymentUnit) 
+Value Could be null or other value: org.jboss.security.AuthenticationManager
+Location 3:
+At SecurityPolicy.java:[line 91] 
+In method org.jboss.system.server.security.SecurityPolicy.start() 
+Value Not null: java.lang.SecurityManager 
+Value aload_0 
+Value aload_0[42](1) 
+Value Variable is set at: At SecurityPolicy.java:[line 90]
+Location 4:
+At SecurityPolicy.java:[line 97] 
+In method org.jboss.system.server.security.SecurityPolicy.stop() 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+Location 5:
+At QuartzServer.java:[line 264] 
+In method org.quartz.impl.QuartzServer.main(String[]) 
+Value Not null: java.rmi.RMISecurityManager 
+Value new 
+Value new[187](3) 37 
+Value Variable is set at:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00E+00"/>
-  </numFmts>
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -973,7 +958,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
@@ -981,7 +966,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
@@ -989,7 +974,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
@@ -1031,128 +1016,81 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="2"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1211,36 +1149,312 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:AMK54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="E24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77934272300469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.6572769953052"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.3333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="63.0046948356808"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="58"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.5539906103286"/>
-    <col collapsed="false" hidden="false" max="18" min="9" style="1" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="8.77934272300469"/>
+    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="2" max="2" width="35.69921875" style="1"/>
+    <col min="3" max="3" width="37.296875" style="1"/>
+    <col min="4" max="4" width="63" style="1"/>
+    <col min="5" max="7" width="58" style="1"/>
+    <col min="8" max="8" width="32.5" style="1"/>
+    <col min="9" max="18" width="22.69921875" style="1"/>
+    <col min="19" max="1025" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1275,8 +1489,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="75.599999999999994" customHeight="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1310,14 +1524,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="7">
         <v>1.7</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -1332,8 +1546,8 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1346,907 +1560,845 @@
         <v>27</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="0" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="H7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="C10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="D10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="0" t="s">
-        <v>70</v>
-      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" ht="43.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" ht="15">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D33" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" ht="43.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="C34" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="D34" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" ht="43.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="7" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="D35" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" ht="43.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C36" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D36" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C37" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D37" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="10" t="s">
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C38" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D38" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" s="10" t="s">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C39" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B33" s="12" t="s">
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:5" ht="15">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C40" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" s="10" t="s">
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" ht="15">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C41" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" s="10" t="s">
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C42" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" s="10" t="s">
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C43" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" s="10" t="s">
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C44" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D44" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" s="10" t="s">
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" ht="28.8">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C45" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B39" s="10" t="s">
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C46" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D46" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" s="10" t="s">
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C47" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D47" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B41" s="10" t="s">
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C48" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D48" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" s="10" t="s">
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C49" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" s="10" t="s">
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="1:5" ht="28.8">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>196</v>
-      </c>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:5">
       <c r="B51" s="10"/>
       <c r="D51" s="11"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:5">
       <c r="E52" s="5"/>
     </row>
-    <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:5" ht="79.2" customHeight="1">
       <c r="E53" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="E54" s="1" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="binaries from: http://ant.apache.org/bindownload.cgi&#10;source from: http://ant.apache.org/srcdownload.cgi"/>
-    <hyperlink ref="D3" r:id="rId2" display="http://www.apache.org/dyn/closer.cgi/xmlgraphics/batik"/>
-    <hyperlink ref="D4" r:id="rId3" display="http://c-jdbc.ow2.org/download.html"/>
-    <hyperlink ref="D5" r:id="rId4" display="http://www.compiere.com/products/download/index.php"/>
-    <hyperlink ref="D6" r:id="rId5" display="http://db.apache.org/derby/derby_downloads.html"/>
-    <hyperlink ref="D7" r:id="rId6" display="http://www.drjava.org/"/>
-    <hyperlink ref="D8" r:id="rId7" display="http://download.eclipse.org/eclipse/downloads/"/>
-    <hyperlink ref="D10" r:id="rId8" display="http://sourceforge.net/projects/galleon/files/galleon/2.5.5/"/>
-    <hyperlink ref="D11" r:id="rId9" display="http://hadoop.apache.org/releases.html"/>
-    <hyperlink ref="D12" r:id="rId10" display="http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final"/>
-    <hyperlink ref="D13" r:id="rId11" display="http://hsqldb.org/"/>
-    <hyperlink ref="D14" r:id="rId12" display="http://www.jboss.org/downloads/"/>
-    <hyperlink ref="D15" r:id="rId13" display="http://www.jruby.org/download"/>
-    <hyperlink ref="D16" r:id="rId14" display="http://lucene.apache.org/"/>
-    <hyperlink ref="D17" r:id="rId15" display="http://myfaces.apache.org/"/>
-    <hyperlink ref="D18" r:id="rId16" display="http://nekohtml.sourceforge.net/"/>
-    <hyperlink ref="D19" r:id="rId17" display="https://netbeans.org/downloads/"/>
-    <hyperlink ref="D20" r:id="rId18" display="http://openjms.sourceforge.net/downloads.html"/>
-    <hyperlink ref="D21" r:id="rId19" display="http://quartz-scheduler.org/"/>
-    <hyperlink ref="D22" r:id="rId20" display="http://www.quickserver.org/download.html"/>
-    <hyperlink ref="D23" r:id="rId21" location="quick-start" display="http://projects.spring.io/spring-framework/#quick-start"/>
-    <hyperlink ref="D24" r:id="rId22" display="http://struts.apache.org/"/>
-    <hyperlink ref="D25" r:id="rId23" display="http://tapestry.apache.org/download.html"/>
-    <hyperlink ref="D26" r:id="rId24" display="http://tomcat.apache.org/whichversion.html"/>
-    <hyperlink ref="D27" r:id="rId25" display="http://www.vuze.com/"/>
-    <hyperlink ref="D28" r:id="rId26" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
-    <hyperlink ref="D29" r:id="rId27" display="http://xml.apache.org/xalan-j/"/>
-    <hyperlink ref="D30" r:id="rId28" display="http://xerces.apache.org/mirrors.cgi"/>
-    <hyperlink ref="D32" r:id="rId29" display="https://github.com/tykkidream/DemoPermissions"/>
-    <hyperlink ref="D33" r:id="rId30" display="https://github.com/eclipse/org.aspectj"/>
-    <hyperlink ref="D34" r:id="rId31" display="https://github.com/kschat/MCVersion-Control"/>
-    <hyperlink ref="D35" r:id="rId32" display="https://github.com/JSansalone/NetBeansIDE"/>
-    <hyperlink ref="D36" r:id="rId33" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
-    <hyperlink ref="D37" r:id="rId34" display="https://github.com/zoomis/NGOMS"/>
-    <hyperlink ref="D39" r:id="rId35" display="https://github.com/Babast/Timelag"/>
-    <hyperlink ref="D40" r:id="rId36" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="D42" r:id="rId37" display="https://github.com/aleksz/driveddoc"/>
-    <hyperlink ref="D43" r:id="rId38" display="https://github.com/holisticon/tracee"/>
-    <hyperlink ref="D44" r:id="rId39" display="https://github.com/astubbs/spring-modules"/>
-    <hyperlink ref="D45" r:id="rId40" display="https://github.com/wildfly-security/security-manager"/>
-    <hyperlink ref="D46" r:id="rId41" display="https://github.com/ngty/gjman"/>
-    <hyperlink ref="D47" r:id="rId42" display="https://github.com/hypernet/visor"/>
-    <hyperlink ref="D48" r:id="rId43" display="https://github.com/stefanbirkner/system-rules"/>
-    <hyperlink ref="D49" r:id="rId44" display="https://github.com/ch33kybutt/oxygen_libcore"/>
-    <hyperlink ref="D50" r:id="rId45" display="https://github.com/apache/tomcat70"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="D14" r:id="rId12"/>
+    <hyperlink ref="D15" r:id="rId13"/>
+    <hyperlink ref="D16" r:id="rId14"/>
+    <hyperlink ref="D17" r:id="rId15"/>
+    <hyperlink ref="D18" r:id="rId16"/>
+    <hyperlink ref="D19" r:id="rId17"/>
+    <hyperlink ref="D20" r:id="rId18"/>
+    <hyperlink ref="D21" r:id="rId19"/>
+    <hyperlink ref="D22" r:id="rId20"/>
+    <hyperlink ref="D23" r:id="rId21" location="quick-start"/>
+    <hyperlink ref="D24" r:id="rId22"/>
+    <hyperlink ref="D25" r:id="rId23"/>
+    <hyperlink ref="D26" r:id="rId24"/>
+    <hyperlink ref="D27" r:id="rId25"/>
+    <hyperlink ref="D28" r:id="rId26"/>
+    <hyperlink ref="D29" r:id="rId27"/>
+    <hyperlink ref="D30" r:id="rId28"/>
+    <hyperlink ref="D32" r:id="rId29"/>
+    <hyperlink ref="D33" r:id="rId30"/>
+    <hyperlink ref="D34" r:id="rId31"/>
+    <hyperlink ref="D35" r:id="rId32"/>
+    <hyperlink ref="D36" r:id="rId33"/>
+    <hyperlink ref="D37" r:id="rId34"/>
+    <hyperlink ref="D39" r:id="rId35"/>
+    <hyperlink ref="D40" r:id="rId36"/>
+    <hyperlink ref="D42" r:id="rId37"/>
+    <hyperlink ref="D43" r:id="rId38"/>
+    <hyperlink ref="D44" r:id="rId39"/>
+    <hyperlink ref="D45" r:id="rId40"/>
+    <hyperlink ref="D46" r:id="rId41"/>
+    <hyperlink ref="D47" r:id="rId42"/>
+    <hyperlink ref="D48" r:id="rId43"/>
+    <hyperlink ref="D49" r:id="rId44"/>
+    <hyperlink ref="D50" r:id="rId45"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committing any changes to merge
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
   <si>
     <t>Index</t>
   </si>
@@ -60,11 +60,30 @@
 source from: http://ant.apache.org/srcdownload.cgi</t>
   </si>
   <si>
-    <t>Tried to use my version of Ant to compile Netbeans (bad idea – took 4 hours and then the build failed because of a memory overflow error) got no useful output 
+    <r>
+      <t xml:space="preserve">Tried to use my version of Ant to compile Netbeans (bad idea – took 4 hours and then the build failed because of a memory overflow error) got no useful output 
+--------------------------------------------------------------------------------------
+Compile Netbeans output: 
 “Callback on VMStart.
 #################################################
 #################################################
+Agent OnUnload, agent exits.”
+--------------------------------------------------------------------------------------
+Compile JRuby otuput:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">“Callback on VMStart.
+#################################################
+#################################################
 Agent OnUnload, agent exits.”</t>
+    </r>
   </si>
   <si>
     <t>At Main.java:[line 856] 
@@ -248,7 +267,39 @@
     <t>http://www.apache.org/dyn/closer.cgi/xmlgraphics/batik</t>
   </si>
   <si>
-    <t> At ApplicationSecurityEnforcer.java:[line 172]
+    <t>Slideshow sample output:
+Callback on VMStart.
+#################################################
+#################################################
+Agent OnUnload, agent exits.
+----------------------------------------------------------------------------------------
+Squiggle Browser Sample:
+Callback on VMStart.
+#################################################
+WARNING: The SecurityManager is being disabled!!!
+SecurityManager Changed:
+ApplicationSecurityEnforcer.java, enforceSecurity, 172
+SecurityManager Changed:
+ApplicationSecurityEnforcer.java, installSecurityManager, 250
+#################################################
+Agent OnUnload, agent exits.
+----------------------------------------------------------------------------------------
+Rasterizer sample:
+Callback on VMStart.
+#################################################
+WARNING: The SecurityManager is being disabled!!!
+SecurityManager Changed:
+ApplicationSecurityEnforcer.java, enforceSecurity, 172
+SecurityManager Changed:
+ApplicationSecurityEnforcer.java, installSecurityManager, 250
+WARNING: The SecurityManager is being disabled!!!
+SecurityManager Changed:
+ApplicationSecurityEnforcer.java, enforceSecurity, 176
+#################################################
+Agent OnUnload, agent exits.</t>
+  </si>
+  <si>
+    <t>At ApplicationSecurityEnforcer.java:[line 172]
  In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean)
  Value Set to null:   
 Value aconst_null 
@@ -281,8 +332,10 @@
 ./batik-1.7/sources/org/apache/batik/util/ApplicationSecurityEnforcer.java
 172:            System.setSecurityManager(null);
 176:                System.setSecurityManager(null);
-250:        System.setSecurityManager(securityManager);
-</t>
+250:        System.setSecurityManager(securityManager);</t>
+  </si>
+  <si>
+    <t>No output.  I just ran the slideshow sample with two of the sample pictures.  I think it is possible to write an application which uses the security. </t>
   </si>
   <si>
     <t>c_jdbc</t>
@@ -294,7 +347,7 @@
     <t>http://c-jdbc.ow2.org/download.html</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.Main.runBuild(ClassLoader) </t>
+    <t>In method org.apache.tools.ant.Main.runBuild(ClassLoader)</t>
   </si>
   <si>
     <t>compiere</t>
@@ -306,7 +359,7 @@
     <t>http://www.compiere.com/products/download/index.php</t>
   </si>
   <si>
-    <t>Value Not null: java.lang.SecurityManager </t>
+    <t>Value Not null: java.lang.SecurityManager</t>
   </si>
   <si>
     <t>derby</t>
@@ -318,7 +371,7 @@
     <t>http://db.apache.org/derby/derby_downloads.html</t>
   </si>
   <si>
-    <t>Value invokestatic </t>
+    <t>Value invokestatic</t>
   </si>
   <si>
     <t>drjava</t>
@@ -333,7 +386,7 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Value invokestatic[184](3) 208 </t>
+    <t>Value invokestatic[184](3) 208</t>
   </si>
   <si>
     <t>./src/edu/rice/cs/drjava/model/repl/newjvm/MainJVM.java
@@ -485,7 +538,7 @@
     <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
   </si>
   <si>
-    <t> At JUnitTestRunner.java:[line 347] </t>
+    <t>At JUnitTestRunner.java:[line 347]</t>
   </si>
   <si>
     <t>hadoop</t>
@@ -497,7 +550,7 @@
     <t>http://hadoop.apache.org/releases.html</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.taskdefs.optional.junit.JUnitTestRunner.setupIOStreams(ByteArrayOutputStream, ByteArrayOutputStream) </t>
+    <t>In method org.apache.tools.ant.taskdefs.optional.junit.JUnitTestRunner.setupIOStreams(ByteArrayOutputStream, ByteArrayOutputStream)</t>
   </si>
   <si>
     <t>hibernate</t>
@@ -509,7 +562,7 @@
     <t>http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final</t>
   </si>
   <si>
-    <t>Value Not null: org.apache.tools.ant.types.Permissions </t>
+    <t>Value Not null: org.apache.tools.ant.types.Permissions</t>
   </si>
   <si>
     <t>hsqldb</t>
@@ -521,7 +574,7 @@
     <t>http://hsqldb.org/</t>
   </si>
   <si>
-    <t>Value aload_0 </t>
+    <t>Value aload_0</t>
   </si>
   <si>
     <t>jboss</t>
@@ -533,7 +586,7 @@
     <t>http://www.jboss.org/downloads/</t>
   </si>
   <si>
-    <t>Value aload_0[42](1) </t>
+    <t>Value aload_0[42](1)</t>
   </si>
   <si>
     <t>See attached file</t>
@@ -572,7 +625,7 @@
     <t>http://myfaces.apache.org/</t>
   </si>
   <si>
-    <t>At Permissions.java:[line 101] </t>
+    <t>At Permissions.java:[line 101]</t>
   </si>
   <si>
     <t>nekohtml</t>
@@ -584,7 +637,7 @@
     <t>http://nekohtml.sourceforge.net/</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.types.Permissions.setSecurityManager() </t>
+    <t>In method org.apache.tools.ant.types.Permissions.setSecurityManager()</t>
   </si>
   <si>
     <t>netbeans</t>
@@ -596,7 +649,7 @@
     <t>https://netbeans.org/downloads/</t>
   </si>
   <si>
-    <t>Value Not null: org.apache.tools.ant.types.Permissions$MySM </t>
+    <t>Value Not null: org.apache.tools.ant.types.Permissions$MySM</t>
   </si>
   <si>
     <t>openjms</t>
@@ -608,7 +661,7 @@
     <t>http://openjms.sourceforge.net/downloads.html</t>
   </si>
   <si>
-    <t>Value new Value new[187](3) 14 </t>
+    <t>Value new Value new[187](3) 14</t>
   </si>
   <si>
     <t>quartz scheduler</t>
@@ -644,7 +697,7 @@
     <t>http://projects.spring.io/spring-framework/#quick-start</t>
   </si>
   <si>
-    <t> At Permissions.java:[line 171]</t>
+    <t>At Permissions.java:[line 171]</t>
   </si>
   <si>
     <t>struts</t>
@@ -921,7 +974,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -946,13 +999,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="3"/>
@@ -963,6 +1009,13 @@
       <color rgb="FF006100"/>
       <name val="Calibri Light"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -987,6 +1040,12 @@
       <name val="宋体"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -1073,20 +1132,20 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1106,39 +1165,43 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1150,7 +1213,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1219,13 +1282,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1323,31 +1386,38 @@
       <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="5"/>
+      <c r="I3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="0" t="s">
-        <v>28</v>
+      <c r="F4" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1357,17 +1427,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="0" t="s">
-        <v>32</v>
+      <c r="F5" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -1377,17 +1447,17 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="0" t="s">
-        <v>36</v>
+      <c r="F6" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -1397,25 +1467,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1423,17 +1493,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="0" t="s">
-        <v>47</v>
+      <c r="F8" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1443,25 +1513,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1469,17 +1539,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="0" t="s">
-        <v>58</v>
+      <c r="F10" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1489,17 +1559,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="0" t="s">
-        <v>62</v>
+      <c r="F11" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1509,17 +1579,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="0" t="s">
-        <v>66</v>
+      <c r="F12" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -1529,17 +1599,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="0" t="s">
-        <v>70</v>
+      <c r="F13" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1549,25 +1619,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>74</v>
+        <v>42</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1575,17 +1645,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1595,17 +1665,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1615,17 +1685,17 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1635,17 +1705,17 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -1655,17 +1725,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1675,17 +1745,17 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1695,17 +1765,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1715,17 +1785,17 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1735,17 +1805,17 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -1755,17 +1825,17 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -1775,17 +1845,17 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -1795,13 +1865,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -1812,22 +1882,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1835,13 +1905,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -1850,13 +1920,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -1865,13 +1935,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -1879,14 +1949,14 @@
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>137</v>
+      <c r="B31" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -1894,14 +1964,14 @@
       <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>140</v>
+      <c r="B32" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -1909,14 +1979,14 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>143</v>
+      <c r="B33" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -1924,14 +1994,14 @@
       <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>146</v>
+      <c r="B34" s="9" t="s">
+        <v>148</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -1939,14 +2009,14 @@
       <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>149</v>
+      <c r="B35" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -1954,14 +2024,14 @@
       <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="B36" s="9" t="s">
         <v>154</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>156</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -1969,14 +2039,14 @@
       <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" s="11" t="s">
+      <c r="B37" s="9" t="s">
         <v>157</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1984,14 +2054,14 @@
       <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="D38" s="11" t="s">
+      <c r="B38" s="9" t="s">
         <v>160</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>162</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -1999,14 +2069,14 @@
       <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="D39" s="11" t="s">
+      <c r="B39" s="9" t="s">
         <v>163</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>165</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -2014,14 +2084,14 @@
       <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="B40" s="9" t="s">
         <v>166</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>168</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -2029,14 +2099,14 @@
       <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D41" s="11" t="s">
+      <c r="B41" s="9" t="s">
         <v>169</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>171</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -2044,14 +2114,14 @@
       <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="D42" s="11" t="s">
+      <c r="B42" s="9" t="s">
         <v>172</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>174</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -2059,14 +2129,14 @@
       <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>173</v>
+      <c r="B43" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -2074,14 +2144,14 @@
       <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>176</v>
+      <c r="B44" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>180</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -2089,14 +2159,14 @@
       <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>179</v>
+      <c r="B45" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -2104,14 +2174,14 @@
       <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="10" t="s">
-        <v>182</v>
+      <c r="B46" s="9" t="s">
+        <v>184</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>186</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -2119,14 +2189,14 @@
       <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>185</v>
+      <c r="B47" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>189</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -2134,14 +2204,14 @@
       <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="10" t="s">
-        <v>188</v>
+      <c r="B48" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>192</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -2149,14 +2219,14 @@
       <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="10" t="s">
-        <v>191</v>
+      <c r="B49" s="9" t="s">
+        <v>193</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -2164,20 +2234,20 @@
       <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>194</v>
+      <c r="B50" s="9" t="s">
+        <v>196</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>198</v>
       </c>
       <c r="E50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="10"/>
-      <c r="D51" s="11"/>
+      <c r="B51" s="9"/>
+      <c r="D51" s="12"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,12 +2255,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Tianyuan's static analysis agian because I forgot to pull it on the computer I was working on the last time
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gf219d\git\ProjectsProfiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="182">
   <si>
     <t>Index</t>
   </si>
@@ -79,7 +83,7 @@
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">“Callback on VMStart.
+      <t>“Callback on VMStart.
 #################################################
 #################################################
 Agent OnUnload, agent exits.”</t>
@@ -335,7 +339,7 @@
 250:        System.setSecurityManager(securityManager);</t>
   </si>
   <si>
-    <t>No output.  I just ran the slideshow sample with two of the sample pictures.  I think it is possible to write an application which uses the security. </t>
+    <t>No output.  I just ran the slideshow sample with two of the sample pictures.  I think it is possible to write an application which uses the security.</t>
   </si>
   <si>
     <t>c_jdbc</t>
@@ -347,9 +351,6 @@
     <t>http://c-jdbc.ow2.org/download.html</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.Main.runBuild(ClassLoader)</t>
-  </si>
-  <si>
     <t>compiere</t>
   </si>
   <si>
@@ -359,9 +360,6 @@
     <t>http://www.compiere.com/products/download/index.php</t>
   </si>
   <si>
-    <t>Value Not null: java.lang.SecurityManager</t>
-  </si>
-  <si>
     <t>derby</t>
   </si>
   <si>
@@ -371,9 +369,6 @@
     <t>http://db.apache.org/derby/derby_downloads.html</t>
   </si>
   <si>
-    <t>Value invokestatic</t>
-  </si>
-  <si>
     <t>drjava</t>
   </si>
   <si>
@@ -384,9 +379,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Value invokestatic[184](3) 208</t>
   </si>
   <si>
     <t>./src/edu/rice/cs/drjava/model/repl/newjvm/MainJVM.java
@@ -412,9 +404,6 @@
     <t>http://download.eclipse.org/eclipse/downloads/</t>
   </si>
   <si>
-    <t>Value Variable is set at: At Main.java:[line 779]</t>
-  </si>
-  <si>
     <t>freemind</t>
   </si>
   <si>
@@ -426,9 +415,6 @@
   <si>
     <t>SecurityManager Changed:
 FreeMind.java, &lt;init&gt;, 277</t>
-  </si>
-  <si>
-    <t>-----------------------------------------------------------</t>
   </si>
   <si>
     <t>./plugins/script/ScriptingEngine.java
@@ -538,9 +524,6 @@
     <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
   </si>
   <si>
-    <t>At JUnitTestRunner.java:[line 347]</t>
-  </si>
-  <si>
     <t>hadoop</t>
   </si>
   <si>
@@ -550,9 +533,6 @@
     <t>http://hadoop.apache.org/releases.html</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.taskdefs.optional.junit.JUnitTestRunner.setupIOStreams(ByteArrayOutputStream, ByteArrayOutputStream)</t>
-  </si>
-  <si>
     <t>hibernate</t>
   </si>
   <si>
@@ -562,9 +542,6 @@
     <t>http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final</t>
   </si>
   <si>
-    <t>Value Not null: org.apache.tools.ant.types.Permissions</t>
-  </si>
-  <si>
     <t>hsqldb</t>
   </si>
   <si>
@@ -574,9 +551,6 @@
     <t>http://hsqldb.org/</t>
   </si>
   <si>
-    <t>Value aload_0</t>
-  </si>
-  <si>
     <t>jboss</t>
   </si>
   <si>
@@ -586,9 +560,6 @@
     <t>http://www.jboss.org/downloads/</t>
   </si>
   <si>
-    <t>Value aload_0[42](1)</t>
-  </si>
-  <si>
     <t>See attached file</t>
   </si>
   <si>
@@ -604,9 +575,6 @@
     <t>http://www.jruby.org/download</t>
   </si>
   <si>
-    <t>Value Variable is set at: At JUnitTestRunner.java:[line 346]</t>
-  </si>
-  <si>
     <t>lucene</t>
   </si>
   <si>
@@ -625,9 +593,6 @@
     <t>http://myfaces.apache.org/</t>
   </si>
   <si>
-    <t>At Permissions.java:[line 101]</t>
-  </si>
-  <si>
     <t>nekohtml</t>
   </si>
   <si>
@@ -637,9 +602,6 @@
     <t>http://nekohtml.sourceforge.net/</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.types.Permissions.setSecurityManager()</t>
-  </si>
-  <si>
     <t>netbeans</t>
   </si>
   <si>
@@ -649,9 +611,6 @@
     <t>https://netbeans.org/downloads/</t>
   </si>
   <si>
-    <t>Value Not null: org.apache.tools.ant.types.Permissions$MySM</t>
-  </si>
-  <si>
     <t>openjms</t>
   </si>
   <si>
@@ -661,9 +620,6 @@
     <t>http://openjms.sourceforge.net/downloads.html</t>
   </si>
   <si>
-    <t>Value new Value new[187](3) 14</t>
-  </si>
-  <si>
     <t>quartz scheduler</t>
   </si>
   <si>
@@ -673,9 +629,6 @@
     <t>http://quartz-scheduler.org/</t>
   </si>
   <si>
-    <t>Value Variable is set at:</t>
-  </si>
-  <si>
     <t>quickserver</t>
   </si>
   <si>
@@ -685,9 +638,6 @@
     <t>http://www.quickserver.org/download.html</t>
   </si>
   <si>
-    <t>---------------------------------------------------------------</t>
-  </si>
-  <si>
     <t>spring framework</t>
   </si>
   <si>
@@ -697,9 +647,6 @@
     <t>http://projects.spring.io/spring-framework/#quick-start</t>
   </si>
   <si>
-    <t>At Permissions.java:[line 171]</t>
-  </si>
-  <si>
     <t>struts</t>
   </si>
   <si>
@@ -709,9 +656,6 @@
     <t>http://struts.apache.org/</t>
   </si>
   <si>
-    <t>In method org.apache.tools.ant.types.Permissions.restoreSecurityManager()</t>
-  </si>
-  <si>
     <t>tapestry</t>
   </si>
   <si>
@@ -719,9 +663,6 @@
   </si>
   <si>
     <t>http://tapestry.apache.org/download.html</t>
-  </si>
-  <si>
-    <t>Value Could be null or other value: java.lang.SecurityManager</t>
   </si>
   <si>
     <t>tomcat</t>
@@ -965,37 +906,82 @@
   <si>
     <t>* Denotes versions where we do not use the QC version to avoid build issues</t>
   </si>
+  <si>
+    <t>Location 1:
+At FreeMind.java:[line 277] 
+In method new freemind.main.FreeMind(Properties, Properties, File) 
+Value Not null: freemind.main.FreeMindSecurityManager 
+Value new 
+Value new[187](3) 14 
+Value Variable is set at:
+Location 2:
+At ApplicationSecurityEnforcer.java:[line 172] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean) 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+Location 3:
+At ApplicationSecurityEnforcer.java:[line 176] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean) 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+Location 4:
+At ApplicationSecurityEnforcer.java:[line 250] 
+In method org.apache.batik.util.ApplicationSecurityEnforcer.installSecurityManager() 
+Value Not null: org.apache.batik.util.BatikSecurityManager 
+Value new 
+Value new[187](3) 29 
+Value Variable is set at: At ApplicationSecurityEnforcer.java:[line 204]</t>
+  </si>
+  <si>
+    <t>Location 1:
+At EjbModule.java:[line 627] 
+In method org.jboss.ejb.EjbModule.destroyService() 
+Value Set to null:   
+Value invokeinterface 
+Value invokeinterface[185](5) 131 
+Value Variable is set at: At EjbModule.java:[line 553]
+Location 2:
+At EjbModule.java:[line 871] 
+In method org.jboss.ejb.EjbModule.initializeContainer(Container, ConfigurationMetaData, BeanMetaData, int, DeploymentUnit) 
+Value Could be null or other value: org.jboss.security.AuthenticationManager
+Location 3:
+At SecurityPolicy.java:[line 91] 
+In method org.jboss.system.server.security.SecurityPolicy.start() 
+Value Not null: java.lang.SecurityManager 
+Value aload_0 
+Value aload_0[42](1) 
+Value Variable is set at: At SecurityPolicy.java:[line 90]
+Location 4:
+At SecurityPolicy.java:[line 97] 
+In method org.jboss.system.server.security.SecurityPolicy.stop() 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+Location 5:
+At QuartzServer.java:[line 264] 
+In method org.quartz.impl.QuartzServer.main(String[]) 
+Value Not null: java.rmi.RMISecurityManager 
+Value new 
+Value new[187](3) 37 
+Value Variable is set at:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00E+00"/>
-  </numFmts>
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1026,7 +1012,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
@@ -1034,7 +1020,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
@@ -1048,7 +1034,7 @@
       <family val="2"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
@@ -1090,132 +1076,81 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="2"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1274,36 +1209,312 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:AMK54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="D11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77934272300469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.6572769953052"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.3333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="63.0046948356808"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="58"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.5539906103286"/>
-    <col collapsed="false" hidden="false" max="18" min="9" style="1" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="8.77934272300469"/>
+    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="2" max="2" width="35.69921875" style="1"/>
+    <col min="3" max="3" width="37.296875" style="1"/>
+    <col min="4" max="4" width="63" style="1"/>
+    <col min="5" max="7" width="58" style="1"/>
+    <col min="8" max="8" width="32.5" style="1"/>
+    <col min="9" max="18" width="22.69921875" style="1"/>
+    <col min="19" max="1025" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1338,8 +1549,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="75.599999999999994" customHeight="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1373,14 +1584,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="7">
         <v>1.7</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -1402,8 +1613,8 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1416,907 +1627,845 @@
         <v>29</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="H7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="C10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="D10" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>59</v>
-      </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>67</v>
+        <v>58</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>76</v>
+        <v>181</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>81</v>
+        <v>69</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:11" ht="75.599999999999994" customHeight="1">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" ht="43.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" ht="15">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D33" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" ht="43.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="C34" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="D34" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" ht="43.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C28" s="7" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="D35" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" ht="43.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C36" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D36" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C37" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D37" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="9" t="s">
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C38" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D38" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" s="9" t="s">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C39" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D39" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B33" s="13" t="s">
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:5" ht="15">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C40" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D40" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" s="9" t="s">
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" ht="15">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C41" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D41" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" s="9" t="s">
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C42" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D42" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" s="9" t="s">
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C43" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D43" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" s="9" t="s">
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C44" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D44" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" s="9" t="s">
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" ht="28.8">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C45" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D45" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B39" s="9" t="s">
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C46" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D46" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" s="9" t="s">
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C47" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D47" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B41" s="9" t="s">
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D48" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" s="9" t="s">
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C49" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D49" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" s="9" t="s">
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="1:5" ht="28.8">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D50" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" s="9" t="s">
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="B51" s="9"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="1:5" ht="79.2" customHeight="1">
+      <c r="E53" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C44" s="1" t="s">
+    </row>
+    <row r="54" spans="1:5">
+      <c r="E54" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="9"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E53" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E54" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="binaries from: http://ant.apache.org/bindownload.cgi&#10;source from: http://ant.apache.org/srcdownload.cgi"/>
-    <hyperlink ref="D3" r:id="rId2" display="http://www.apache.org/dyn/closer.cgi/xmlgraphics/batik"/>
-    <hyperlink ref="D4" r:id="rId3" display="http://c-jdbc.ow2.org/download.html"/>
-    <hyperlink ref="D5" r:id="rId4" display="http://www.compiere.com/products/download/index.php"/>
-    <hyperlink ref="D6" r:id="rId5" display="http://db.apache.org/derby/derby_downloads.html"/>
-    <hyperlink ref="D7" r:id="rId6" display="http://www.drjava.org/"/>
-    <hyperlink ref="D8" r:id="rId7" display="http://download.eclipse.org/eclipse/downloads/"/>
-    <hyperlink ref="D10" r:id="rId8" display="http://sourceforge.net/projects/galleon/files/galleon/2.5.5/"/>
-    <hyperlink ref="D11" r:id="rId9" display="http://hadoop.apache.org/releases.html"/>
-    <hyperlink ref="D12" r:id="rId10" display="http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final"/>
-    <hyperlink ref="D13" r:id="rId11" display="http://hsqldb.org/"/>
-    <hyperlink ref="D14" r:id="rId12" display="http://www.jboss.org/downloads/"/>
-    <hyperlink ref="D15" r:id="rId13" display="http://www.jruby.org/download"/>
-    <hyperlink ref="D16" r:id="rId14" display="http://lucene.apache.org/"/>
-    <hyperlink ref="D17" r:id="rId15" display="http://myfaces.apache.org/"/>
-    <hyperlink ref="D18" r:id="rId16" display="http://nekohtml.sourceforge.net/"/>
-    <hyperlink ref="D19" r:id="rId17" display="https://netbeans.org/downloads/"/>
-    <hyperlink ref="D20" r:id="rId18" display="http://openjms.sourceforge.net/downloads.html"/>
-    <hyperlink ref="D21" r:id="rId19" display="http://quartz-scheduler.org/"/>
-    <hyperlink ref="D22" r:id="rId20" display="http://www.quickserver.org/download.html"/>
-    <hyperlink ref="D23" r:id="rId21" location="quick-start" display="http://projects.spring.io/spring-framework/#quick-start"/>
-    <hyperlink ref="D24" r:id="rId22" display="http://struts.apache.org/"/>
-    <hyperlink ref="D25" r:id="rId23" display="http://tapestry.apache.org/download.html"/>
-    <hyperlink ref="D26" r:id="rId24" display="http://tomcat.apache.org/whichversion.html"/>
-    <hyperlink ref="D27" r:id="rId25" display="http://www.vuze.com/"/>
-    <hyperlink ref="D28" r:id="rId26" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
-    <hyperlink ref="D29" r:id="rId27" display="http://xml.apache.org/xalan-j/"/>
-    <hyperlink ref="D30" r:id="rId28" display="http://xerces.apache.org/mirrors.cgi"/>
-    <hyperlink ref="D32" r:id="rId29" display="https://github.com/tykkidream/DemoPermissions"/>
-    <hyperlink ref="D33" r:id="rId30" display="https://github.com/eclipse/org.aspectj"/>
-    <hyperlink ref="D34" r:id="rId31" display="https://github.com/kschat/MCVersion-Control"/>
-    <hyperlink ref="D35" r:id="rId32" display="https://github.com/JSansalone/NetBeansIDE"/>
-    <hyperlink ref="D36" r:id="rId33" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
-    <hyperlink ref="D37" r:id="rId34" display="https://github.com/zoomis/NGOMS"/>
-    <hyperlink ref="D39" r:id="rId35" display="https://github.com/Babast/Timelag"/>
-    <hyperlink ref="D40" r:id="rId36" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="D42" r:id="rId37" display="https://github.com/aleksz/driveddoc"/>
-    <hyperlink ref="D43" r:id="rId38" display="https://github.com/holisticon/tracee"/>
-    <hyperlink ref="D44" r:id="rId39" display="https://github.com/astubbs/spring-modules"/>
-    <hyperlink ref="D45" r:id="rId40" display="https://github.com/wildfly-security/security-manager"/>
-    <hyperlink ref="D46" r:id="rId41" display="https://github.com/ngty/gjman"/>
-    <hyperlink ref="D47" r:id="rId42" display="https://github.com/hypernet/visor"/>
-    <hyperlink ref="D48" r:id="rId43" display="https://github.com/stefanbirkner/system-rules"/>
-    <hyperlink ref="D49" r:id="rId44" display="https://github.com/ch33kybutt/oxygen_libcore"/>
-    <hyperlink ref="D50" r:id="rId45" display="https://github.com/apache/tomcat70"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="D14" r:id="rId12"/>
+    <hyperlink ref="D15" r:id="rId13"/>
+    <hyperlink ref="D16" r:id="rId14"/>
+    <hyperlink ref="D17" r:id="rId15"/>
+    <hyperlink ref="D18" r:id="rId16"/>
+    <hyperlink ref="D19" r:id="rId17"/>
+    <hyperlink ref="D20" r:id="rId18"/>
+    <hyperlink ref="D21" r:id="rId19"/>
+    <hyperlink ref="D22" r:id="rId20"/>
+    <hyperlink ref="D23" r:id="rId21" location="quick-start"/>
+    <hyperlink ref="D24" r:id="rId22"/>
+    <hyperlink ref="D25" r:id="rId23"/>
+    <hyperlink ref="D26" r:id="rId24"/>
+    <hyperlink ref="D27" r:id="rId25"/>
+    <hyperlink ref="D28" r:id="rId26"/>
+    <hyperlink ref="D29" r:id="rId27"/>
+    <hyperlink ref="D30" r:id="rId28"/>
+    <hyperlink ref="D32" r:id="rId29"/>
+    <hyperlink ref="D33" r:id="rId30"/>
+    <hyperlink ref="D34" r:id="rId31"/>
+    <hyperlink ref="D35" r:id="rId32"/>
+    <hyperlink ref="D36" r:id="rId33"/>
+    <hyperlink ref="D37" r:id="rId34"/>
+    <hyperlink ref="D39" r:id="rId35"/>
+    <hyperlink ref="D40" r:id="rId36"/>
+    <hyperlink ref="D42" r:id="rId37"/>
+    <hyperlink ref="D43" r:id="rId38"/>
+    <hyperlink ref="D44" r:id="rId39"/>
+    <hyperlink ref="D45" r:id="rId40"/>
+    <hyperlink ref="D46" r:id="rId41"/>
+    <hyperlink ref="D47" r:id="rId42"/>
+    <hyperlink ref="D48" r:id="rId43"/>
+    <hyperlink ref="D49" r:id="rId44"/>
+    <hyperlink ref="D50" r:id="rId45"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the grep results and the general comments for Batik, so Batik is finished.
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="185">
   <si>
     <t>Index</t>
   </si>
@@ -317,18 +317,63 @@
   </si>
   <si>
     <t>./batik-1.7/test-sources/org/apache/batik/util/ApplicationSecurityEnforcerTest.java
+37:        addTest(new CheckNoSecurityManagerOverride());
+48:    static class CheckNoSecurityManagerOverride extends AbstractTest {
+84:                SecurityManager sm = System.getSecurityManager();
+85:                if (sm == ase.lastSecurityManagerInstalled){
 89:                System.setSecurityManager(null);
+103:                SecurityManager sm = System.getSecurityManager();
+104:                if (sm == null &amp;&amp; ase.lastSecurityManagerInstalled == null) {
 108:                System.setSecurityManager(null);
 ./batik-1.7/samples/tests/resources/java/sources/com/untrusted/script/UntrustedScriptHandler.java
 103:        {"RuntimePermission setSecurityManager", new RuntimePermission("setSecurityManager")}, 
+104:        {"RuntimePermission createSecurityManager", new RuntimePermission("createSecurityManager")}, 
+235:                    SecurityManager sm = System.getSecurityManager();
 ./batik-1.7/test-resources/org/apache/batik/bridge/JarCheckPermissionsGranted.java
 98:        {"RuntimePermission setSecurityManager", new RuntimePermission("setSecurityManager")}, 
+99:        {"RuntimePermission createSecurityManager", new RuntimePermission("createSecurityManager")}, 
+178:                    SecurityManager sm = System.getSecurityManager();
 ./batik-1.7/test-resources/org/apache/batik/bridge/JarCheckPermissionsDenied.java
 98:        {"RuntimePermission setSecurityManager", new RuntimePermission("setSecurityManager")}, 
+99:        {"RuntimePermission createSecurityManager", new RuntimePermission("createSecurityManager")}, 
+196:                    SecurityManager sm = System.getSecurityManager();
 ./batik-1.7/sources/org/apache/batik/util/ApplicationSecurityEnforcer.java
+30: * This class can install a &lt;tt&gt;SecurityManager&lt;/tt&gt; for an application
+42:     * a SecurityManager installed at the time Squiggle tries
+109:     * Keeps track of the last SecurityManager installed
+111:    protected BatikSecurityManager lastSecurityManagerInstalled;
+149:     * Enforces security by installing a &lt;tt&gt;SecurityManager&lt;/tt&gt;.
+151:     * a &lt;tt&gt;SecurityManager&lt;/tt&gt; requires overriding an existing
+152:     * &lt;tt&gt;SecurityManager&lt;/tt&gt;. In other words, this method will 
+153:     * not install a new &lt;tt&gt;SecurityManager&lt;/tt&gt; if there is 
+157:        SecurityManager sm = System.getSecurityManager();
+159:        if (sm != null &amp;&amp; sm != lastSecurityManagerInstalled) {
+161:            // an 'alien' SecurityManager with either null or 
+162:            // a new SecurityManager.
 172:            System.setSecurityManager(null);
+173:            installSecurityManager();
 176:                System.setSecurityManager(null);
-250:        System.setSecurityManager(securityManager);</t>
+177:                lastSecurityManagerInstalled = null;
+200:     * Installs a SecurityManager on behalf of the application
+202:    public void installSecurityManager(){
+204:        BatikSecurityManager securityManager = new BatikSecurityManager();
+250:        System.setSecurityManager(securityManager);
+251:        lastSecurityManagerInstalled = securityManager;
+./batik-1.7/sources/org/apache/batik/util/BatikSecurityManager.java
+22: * This &lt;tt&gt;SecurityManager&lt;/tt&gt; extension exposes the &lt;tt&gt;getClassContext&lt;/tt&gt;
+27: * @version $Id: BatikSecurityManager.java 475477 2006-11-15 22:44:28Z cam $
+29:public class BatikSecurityManager extends SecurityManager {
+./batik-1.7/sources/org/apache/batik/apps/svgbrowser/WindowsAltFileSystemView.java
+44:// java.io.File.listRoots() does a SecurityManager.checkRead() which
+./batik-1.7/sources/org/apache/batik/apps/svgbrowser/JSVGViewerFrame.java
+1225:                SecurityManager sm = System.getSecurityManager();
+./batik-1.7/sources/org/apache/batik/swing/gvt/AbstractJGVTComponent.java
+1247:            SecurityManager securityManager;
+1248:            securityManager = System.getSecurityManager();
+</t>
+  </si>
+  <si>
+    <t>The code contains a possibly valid null and/or weakening of the SecurityManager.  The method enforceSecurity in the file ApplicationSecurityEnforcer.java should be investigated further.  See the Piazza post for more information.</t>
   </si>
   <si>
     <t>Slideshow sample output:
@@ -398,6 +443,72 @@
 Value new Value new[187](3) 29 
 Value Variable is set at: At ApplicationSecurityEnforcer.java:[line 204]
 This method sets the SecurityManager of the application to the application defined SecurityManager.  This line only executes after the nulling of the SecurityManager at the line 172 reference.</t>
+  </si>
+  <si>
+    <t>./batik-1.7/test-sources/org/apache/batik/util/ApplicationSecurityEnforcerTest.java
+37:        addTest(new CheckNoSecurityManagerOverride());
+48:    static class CheckNoSecurityManagerOverride extends AbstractTest {
+84:                SecurityManager sm = System.getSecurityManager();
+85:                if (sm == ase.lastSecurityManagerInstalled){
+89:                System.setSecurityManager(null);
+103:                SecurityManager sm = System.getSecurityManager();
+104:                if (sm == null &amp;&amp; ase.lastSecurityManagerInstalled == null) {
+108:                System.setSecurityManager(null);
+This class is just testing that the Application Security Enforcer will do what it is supposed to do, such as throw a SecurityExcpetion when ran after another SecurityManager is set.
+./batik-1.7/samples/tests/resources/java/sources/com/untrusted/script/UntrustedScriptHandler.java
+103:        {"RuntimePermission setSecurityManager", new RuntimePermission("setSecurityManager")}, 
+104:        {"RuntimePermission createSecurityManager", new RuntimePermission("createSecurityManager")}, 
+235:                    SecurityManager sm = System.getSecurityManager();
+A sample test to make sure that an untrusted class does not have more permissions than it should.  Multiple important permissions are checked in this file and they are supposed to throw SecurityExceptions with the current SecurityManager
+./batik-1.7/test-resources/org/apache/batik/bridge/JarCheckPermissionsGranted.java
+98:        {"RuntimePermission setSecurityManager", new RuntimePermission("setSecurityManager")}, 
+99:        {"RuntimePermission createSecurityManager", new RuntimePermission("createSecurityManager")}, 
+178:                    SecurityManager sm = System.getSecurityManager();
+Test to see if the loaded svg file has all permissions, which the test implies it should.
+./batik-1.7/test-resources/org/apache/batik/bridge/JarCheckPermissionsDenied.java
+98:        {"RuntimePermission setSecurityManager", new RuntimePermission("setSecurityManager")}, 
+99:        {"RuntimePermission createSecurityManager", new RuntimePermission("createSecurityManager")}, 
+196:                    SecurityManager sm = System.getSecurityManager();
+Tests that only the right permissions are granted in a restricted setting.
+./batik-1.7/sources/org/apache/batik/util/ApplicationSecurityEnforcer.java
+30: * This class can install a &lt;tt&gt;SecurityManager&lt;/tt&gt; for an application
+42:     * a SecurityManager installed at the time Squiggle tries
+109:     * Keeps track of the last SecurityManager installed
+111:    protected BatikSecurityManager lastSecurityManagerInstalled;
+149:     * Enforces security by installing a &lt;tt&gt;SecurityManager&lt;/tt&gt;.
+151:     * a &lt;tt&gt;SecurityManager&lt;/tt&gt; requires overriding an existing
+152:     * &lt;tt&gt;SecurityManager&lt;/tt&gt;. In other words, this method will 
+153:     * not install a new &lt;tt&gt;SecurityManager&lt;/tt&gt; if there is 
+157:        SecurityManager sm = System.getSecurityManager();
+159:        if (sm != null &amp;&amp; sm != lastSecurityManagerInstalled) {
+161:            // an 'alien' SecurityManager with either null or 
+162:            // a new SecurityManager.
+172:            System.setSecurityManager(null);
+173:            installSecurityManager();
+176:                System.setSecurityManager(null);
+177:                lastSecurityManagerInstalled = null;
+200:     * Installs a SecurityManager on behalf of the application
+202:    public void installSecurityManager(){
+204:        BatikSecurityManager securityManager = new BatikSecurityManager();
+250:        System.setSecurityManager(securityManager);
+251:        lastSecurityManagerInstalled = securityManager;
+Commented on in the static analysis
+./batik-1.7/sources/org/apache/batik/util/BatikSecurityManager.java
+22: * This &lt;tt&gt;SecurityManager&lt;/tt&gt; extension exposes the &lt;tt&gt;getClassContext&lt;/tt&gt;
+27: * @version $Id: BatikSecurityManager.java 475477 2006-11-15 22:44:28Z cam $
+29:public class BatikSecurityManager extends SecurityManager {
+This SecurityManager extension adds on the ability to return the current stack trace.
+./batik-1.7/sources/org/apache/batik/apps/svgbrowser/WindowsAltFileSystemView.java
+44:// java.io.File.listRoots() does a SecurityManager.checkRead() which
+Pretty much states that the class is a work around to a bug in the SecurityManager checkRead function at the time.
+./batik-1.7/sources/org/apache/batik/apps/svgbrowser/JSVGViewerFrame.java
+1225:                SecurityManager sm = System.getSecurityManager();
+Causes a different fileChooser to open if a SecurityManager is present
+./batik-1.7/sources/org/apache/batik/swing/gvt/AbstractJGVTComponent.java
+1247:            SecurityManager securityManager;
+1248:            securityManager = System.getSecurityManager();
+Contains a check to see if the current SecurityManager allows access to the system clipboard.
+</t>
   </si>
   <si>
     <t>c_jdbc</t>
@@ -1266,7 +1377,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1341,7 +1452,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1448,27 +1559,31 @@
       <c r="G3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="I3" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="0"/>
@@ -1480,13 +1595,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="0"/>
@@ -1498,13 +1613,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="0"/>
@@ -1516,25 +1631,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1542,13 +1657,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="0"/>
@@ -1560,25 +1675,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1586,13 +1701,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
@@ -1604,13 +1719,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
@@ -1622,13 +1737,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
@@ -1640,13 +1755,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
@@ -1658,25 +1773,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1684,13 +1799,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -1701,13 +1816,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -1718,13 +1833,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -1735,13 +1850,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -1752,13 +1867,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -1769,13 +1884,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -1786,13 +1901,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -1803,13 +1918,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -1820,13 +1935,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -1837,13 +1952,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -1854,13 +1969,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -1871,13 +1986,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -1888,22 +2003,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1911,13 +2026,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -1926,13 +2041,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -1941,13 +2056,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -1956,13 +2071,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -1971,13 +2086,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -1986,13 +2101,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -2001,13 +2116,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -2016,13 +2131,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -2031,13 +2146,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -2046,13 +2161,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -2061,13 +2176,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -2076,13 +2191,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -2091,13 +2206,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -2106,13 +2221,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -2121,13 +2236,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -2136,13 +2251,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -2151,13 +2266,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -2166,13 +2281,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -2181,13 +2296,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -2196,13 +2311,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -2211,13 +2326,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -2226,13 +2341,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -2241,13 +2356,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -2261,12 +2376,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the test output for the static analysis, grep results, and 1 dynamic analysis run for Derby
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="188">
   <si>
     <t>Index</t>
   </si>
@@ -369,8 +369,7 @@
 1225:                SecurityManager sm = System.getSecurityManager();
 ./batik-1.7/sources/org/apache/batik/swing/gvt/AbstractJGVTComponent.java
 1247:            SecurityManager securityManager;
-1248:            securityManager = System.getSecurityManager();
-</t>
+1248:            securityManager = System.getSecurityManager();</t>
   </si>
   <si>
     <t>The code contains a possibly valid null and/or weakening of the SecurityManager.  The method enforceSecurity in the file ApplicationSecurityEnforcer.java should be investigated further.  See the Piazza post for more information.</t>
@@ -507,35 +506,521 @@
 ./batik-1.7/sources/org/apache/batik/swing/gvt/AbstractJGVTComponent.java
 1247:            SecurityManager securityManager;
 1248:            securityManager = System.getSecurityManager();
-Contains a check to see if the current SecurityManager allows access to the system clipboard.
+Contains a check to see if the current SecurityManager allows access to the system clipboard.</t>
+  </si>
+  <si>
+    <t>c_jdbc</t>
+  </si>
+  <si>
+    <t>2.0.2</t>
+  </si>
+  <si>
+    <t>http://c-jdbc.ow2.org/download.html</t>
+  </si>
+  <si>
+    <t>compiere</t>
+  </si>
+  <si>
+    <t>3.5*</t>
+  </si>
+  <si>
+    <t>http://www.compiere.com/products/download/index.php</t>
+  </si>
+  <si>
+    <t>derby</t>
+  </si>
+  <si>
+    <t>10.10.2.0*</t>
+  </si>
+  <si>
+    <t>http://db.apache.org/derby/derby_downloads.html</t>
+  </si>
+  <si>
+    <t>Callback on VMStart.
+#################################################
+#################################################
+Agent OnUnload, agent exits.</t>
+  </si>
+  <si>
+    <t>In
+In method org.apache.derby.drda.NetworkServerControl.installSecurityManager(NetworkServerControlImpl) 
+Value Not null: java.lang.SecurityManager 
+Value new 
+Value new[187](3) 61 
+Value Variable is set at
+-------------------------------------------------------------
+ At RunTest.java:[line 2876] 
+In method org.apache.derbyTesting.functionTests.harness.RunTest.execTestNoProcess(Properties, String, String, String)
+Value Set to null:  
+ Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+--------------------------------------------------------------
+At RunTest.java:[line 2979] 
+In method org.apache.derbyTesting.functionTests.harness.RunTest.installSecurityManager() 
+Value Not null: java.lang.SecurityManager 
+Value new 
+Value new[187](3) 662 
+Value Variable is set at:
+---------------------------------------------------------------
+At SecurityManagerSetup.java:[line 278] 
+In method org.apache.derbyTesting.junit.SecurityManagerSetup$2.run() 
+Value Not null: java.lang.SecurityManager 
+Value new 
+Value new[187](3) 3 
+Value Variable is set at:
+-----------------------------------------------------------------
+At SecurityManagerSetup.java:[line 280]
+In method org.apache.derbyTesting.junit.SecurityManagerSetup$2.run()
+Value Not null: java.lang.SecurityManager
+Value aload_0 
+Value aload_0[42](1) 
+Value Variable is set at: 
+At SecurityManagerSetup.java:[line 277]
+------------------------------------------------------------------
+At SecurityManagerSetup.java:[line 493]
+In method org.apache.derbyTesting.junit.SecurityManagerSetup$4.run()
+Value Set to null:
+Value aconst_null
+Value aconst_null[1](1)
+Value Variable is set at:</t>
+  </si>
+  <si>
+    <t>./java/engine/org/apache/derby/jdbc/InternalDriver.java
+332:        if (System.getSecurityManager() == null) {
+./java/engine/org/apache/derby/iapi/services/info/Version.java
+62:            if (System.getSecurityManager() != null)
+./java/engine/org/apache/derby/iapi/services/cache/ClassSize.java
+266:     * Note that this method will throw a SecurityException if the SecurityManager does not
+./java/engine/org/apache/derby/iapi/security/SecurityUtil.java
+104:     * Checks that a Subject has a Permission under the SecurityManager.
+143:     * Checks that a User has a Permission under the SecurityManager.
+159:        if (System.getSecurityManager() == null) {
+./java/engine/org/apache/derby/authentication/SystemPrincipal.java
+66:     * permission checking by the SecurityManager.
+./java/engine/org/apache/derby/catalog/SystemProcedures.java
+1777:        // without a SecurityManager seems to lock in a policy with
+1779:        // when later installing a SecurityManager.
+1780:        if (System.getSecurityManager() == null)
+./java/engine/org/apache/derby/impl/jdbc/EmbedConnection.java
+2694:        if (System.getSecurityManager() == null) {
+./java/engine/org/apache/derby/impl/jdbc/EmbedConnection40.java
+285:        SecurityManager securityManager = System.getSecurityManager();
+./java/engine/org/apache/derby/impl/services/monitor/StorageFactoryService.java
+1199:                    System.getSecurityManager().checkWrite(from.getPath());
+./java/engine/org/apache/derby/impl/services/bytecode/d_BCValidate.java
+91:				// methods. Default SecurityManager behaviour is to grant access to public members
+./java/engine/org/apache/derby/impl/services/reflect/JarLoader.java
+527:     * Provide a SecurityManager with information about the class name
+./java/engine/org/apache/derby/impl/services/jmx/JMXManagementService.java
+415:            if (System.getSecurityManager() != null)
+./java/drda/org/apache/derby/drda/NetworkServerControl.java
+340:            if ( needsSecurityManager( server, command ) )
+343:                installSecurityManager( server );
+612:     * &lt;li&gt;The VM isn't already running a SecurityManager.&lt;/li&gt;
+614:     * &lt;li&gt;The customer didn't specify the -noSecurityManager flag on the startup command
+618:    private static  boolean needsSecurityManager( NetworkServerControlImpl server, int command )
+623:             (System.getSecurityManager() == null) &amp;&amp;
+645:     * Install a SecurityManager governed by the Basic startup policy. See DERBY-2196.
+647:    private static  void installSecurityManager( NetworkServerControlImpl server )
+692:        // Now install a SecurityManager, using the Basic policy file.
+698:        SecurityManager     securityManager = new SecurityManager();
+700:        System.setSecurityManager( securityManager );
+./java/drda/org/apache/derby/impl/drda/NetworkServerControlImpl.java
+116:         "noSecurityManager", "ssl"};
+402:     * default SecurityManager.
+1189:        if (System.getSecurityManager() == null) {
+./java/drda/org/apache/derby/impl/drda/NetworkServerMBeanImpl.java
+82:            if (System.getSecurityManager() != null)
+./java/client/org/apache/derby/client/net/NetConnection40.java
+401:        SecurityManager securityManager = System.getSecurityManager();
+./java/client/org/apache/derby/client/am/Version.java
+96:            java.lang.SecurityManager security = java.lang.System.getSecurityManager();
+103:            detectLocalHost(java.lang.System.getSecurityManager(), printWriter);
+137:    private static void printSystemProperty(java.lang.SecurityManager security,
+159:    private static void detectLocalHost(java.lang.SecurityManager security, java.io.PrintWriter printWriter) {
+./java/client/org/apache/derby/client/am/EncryptionManager.java
+137:    // rewritten into a DRDASecurityManager and have some of the
+./java/stubs/jdbc3/java/sql/DriverManager.java
+279:        SecurityManager securityManager = System.getSecurityManager();
+./java/testing/org/apache/derbyTesting/functionTests/util/SecurityCheck.java
+153:	 * SecurityManager.inspect(conn);
+./java/testing/org/apache/derbyTesting/functionTests/util/TestRoutines.java
+71:		s.execute("CREATE FUNCTION TESTROUTINE.HAS_SECURITY_MANAGER() RETURNS INT NO SQL EXTERNAL NAME 'org.apache.derbyTesting.functionTests.util.TestRoutines.hasSecurityManager' language java parameter style java");
+109:	public static int hasSecurityManager()
+111:		return System.getSecurityManager() == null ? 0 : 1;
+./java/testing/org/apache/derbyTesting/functionTests/harness/RunTest.java
+185:    static boolean runWithoutSecurityManager;
+1757:	        		|| "true".equalsIgnoreCase(ap.getProperty("noSecurityManager")))
+1758:	        	runWithoutSecurityManager = true;
+2365:        if (!runWithoutSecurityManager)
+2368:        	System.out.println("-- SecurityManager not installed --");
+2488:            // properties (setSecurityManager, setIO)
+2669:    	boolean installedSecurityManager = installSecurityManager();
+2874:         if (installedSecurityManager)
+2876:        	System.setSecurityManager(null);
+2941:    private static boolean installSecurityManager() throws ClassNotFoundException, IOException
+2943:    	// SecurityManager not currently work with older j9 and useProcess=false
+2948:    	boolean installedSecurityManager = false;
+2949:    	// Set up the SecurityManager in this JVM for this test.
+2950:    	boolean haveSecurityManagerAlready = System.getSecurityManager() != null;
+2951:        if (runWithoutSecurityManager)
+2953:        	// Test doesn't run with a SecurityManager,
+2955:        	if (haveSecurityManagerAlready)
+2957:        				"noSecurityManager=true,useProcess=false but SecurityManager installed by previous test");
+2959:        	    System.out.println("-- SecurityManager not installed --");
+2961:        else if (!haveSecurityManagerAlready)
+2979:		    System.setSecurityManager(new SecurityManager());
+2980:		    installedSecurityManager = true;
+2983:        return installedSecurityManager;
+./java/testing/org/apache/derbyTesting/functionTests/harness/jvm.java
+32:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+385:            SecurityManagerSetup.getPolicyFilePropertiesForOldHarness();
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/HalfCreatedDatabaseTest.java
+34:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+93:        test = SecurityManagerSetup.noSecurityManager( test );
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/Derby5652.java
+28:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+71:        test = SecurityManagerSetup.noSecurityManager( test );
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/DBInJarTest.java
+39:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+202:        return new CleanDatabaseTestSetup(SecurityManagerSetup.noSecurityManager(suite)) 
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/SecurityPolicyReloadingTest.java
+37:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+153:        test = new SecurityManagerSetup( test, undecoratedTest.makeServerPolicyName() );
+179:        test = SecurityManagerSetup.noSecurityManager(test);
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/DatabaseClassLoadingTest.java
+56:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+120:           suite.addTest(SecurityManagerSetup.noSecurityManager(
+123:           suite.addTest(SecurityManagerSetup.noSecurityManager(
+129:           suite.addTest(SecurityManagerSetup.noSecurityManager(
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/AggregateClassLoadingTest.java
+38:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+81:		return SecurityManagerSetup.noSecurityManager(
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/NativeAuthenticationServiceTest.java
+39:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+160:    private final   boolean _disableSecurityManager;
+187:         boolean    disableSecurityManager
+196:        _disableSecurityManager = disableSecurityManager;
+331:        String  securityManager = _disableSecurityManager ?
+332:            "SecurityManager OFF, " :
+333:            "SecurityManager ON, ";
+502:        if ( _disableSecurityManager ) { result = SecurityManagerSetup.noSecurityManager( result ); }
+883:            if ( _disableSecurityManager ) { vetProtocol( classpathDBName() ); }
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/SysDiagVTIMappingTest.java
+27:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+85:        return SecurityManagerSetup.noSecurityManager(
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Full.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+44:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_CleanUp.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+54:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_1.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+53:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local.java
+27:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+63:        return SecurityManagerSetup.noSecurityManager(suite);
+76:        return SecurityManagerSetup.noSecurityManager( suite );
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/Derby5937SlaveShutdownTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+79:        return new SecurityManagerSetup(
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun.java
+863:                    // + " -Djava.security.policy=\"&lt;NONE&gt;\""  // Now using noSecurityManager decorator
+1944:        ceArray.add( "-noSecurityManager" );
+1991:        sp.setProperty("noSecurityManager", 
+1992:                securityOption.equalsIgnoreCase("-noSecurityManager")?"true":"false");
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_showStateChange.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+64:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part1_3.java
+28:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+57:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part1_1.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+58:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_Encrypted_1.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+66:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/SimplePerfTest_Verify.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+71:        return SecurityManagerSetup.noSecurityManager(t);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p4.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+56:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p6.java
+33:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+65:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part2.java
+30:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+58:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part1_2.java
+28:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+65:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part1.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+66:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_1Indexing.java
+31:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+59:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p5.java
+30:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+62:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Distributed.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+59:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p2.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+63:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/SimplePerfTest.java
+36:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+76:        return SecurityManagerSetup.noSecurityManager(t);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_Derby4910.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+52:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p1.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+59:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p3.java
+28:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+61:        return SecurityManagerSetup.noSecurityManager(suite);
+./java/testing/org/apache/derbyTesting/functionTests/tests/engine/ShutdownWithoutDeregisterPermissionTest.java
+31:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+44:        return new SecurityManagerSetup(
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbcapi/InvalidLDAPServerAuthenticationTest.java
+38:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+65:        suite.addTest(SecurityManagerSetup.noSecurityManager(baseSuite(
+68:                SecurityManagerSetup.noSecurityManager(
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbcapi/AutoloadTest.java
+44:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+139:                suite.addTest(SecurityManagerSetup.noSecurityManager(
+169:        suite.addTest(SecurityManagerSetup.noSecurityManager(new AutoloadTest("testEmbeddedNotStarted")));
+197:            suite.addTest(SecurityManagerSetup.noSecurityManager(
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbcapi/LDAPAuthenticationTest.java
+43:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+149:        test = new SecurityManagerSetup(test,ldapPolicyName );
+./java/testing/org/apache/derbyTesting/functionTests/tests/upgradeTests/UpgradeRun.java
+32:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+136:        return SecurityManagerSetup.noSecurityManager(setup);
+./java/testing/org/apache/derbyTesting/functionTests/tests/upgradeTests/UpgradeTrajectoryTest.java
+45:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+255:        return SecurityManagerSetup.noSecurityManager( sfs );
+./java/testing/org/apache/derbyTesting/functionTests/tests/management/NetworkServerMBeanTest.java
+313:        // assumes noSecurityManager or that the required SocketPermission has
+./java/testing/org/apache/derbyTesting/functionTests/tests/management/MBeanTest.java
+46:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+112:         * Will run without SecurityManager for now, but could probably add a 
+120:                SecurityManagerSetup.noSecurityManager(networkServerTestSetup);
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbc4/AbortTest.java
+42:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+51: * class tests the affect of SecurityManagers on the method. A related
+68:    private boolean _hasSecurityManager;
+76:    public AbortTest(String name, boolean hasSecurityManager)
+80:        _hasSecurityManager = hasSecurityManager;
+110:    public static Test baseSuite( boolean hasSecurityManager )
+112:        AbortTest   abortTest = new AbortTest( "test_basic", hasSecurityManager );
+122:        if ( hasSecurityManager )
+124:            return new SecurityManagerSetup( test, "org/apache/derbyTesting/functionTests/tests/jdbc4/noAbortPermission.policy" );
+128:            return SecurityManagerSetup.noSecurityManager( test );
+151:        println( "AbortTest( " + _hasSecurityManager + " )" );
+152:        assertEquals( _hasSecurityManager, (System.getSecurityManager() != null) );
+229:        if ( _hasSecurityManager ) { missingPermission( wrapper1 ); }
+230:        else { noSecurityManager( wrapper1, conn2 ); }
+267:    private void    noSecurityManager(  final Wrapper41Conn wrapper1, Connection conn2  ) throws Exception
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbc4/Driver40UnbootedTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+86:        return SecurityManagerSetup.noSecurityManager( test );
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/IjConnNameTest.java
+36:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+70:        //test = SecurityManagerSetup.noSecurityManager(test);
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/SysinfoAPITest.java
+33:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/derbyrunjartest.java
+32:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+55:        return new SecurityManagerSetup(
+71:        URL result = SecurityManagerSetup.getURL(runClassName);
+146:            "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/SysinfoLocaleTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+131:        return SecurityManagerSetup.noSecurityManager(suite);
+161:        URL sysinfoURL = SecurityManagerSetup.getURL(className);
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/IjSecurityManagerTest.java
+4:   org.apache.derbyTesting.functionTests.tests.tools.IjSecurityManager
+38:public class IjSecurityManagerTest extends BaseTestCase {
+40:	public IjSecurityManagerTest(String name) {
+58:	        ij.main(new String[]{"extinout/IjSecurityManagerTest.sql"});
+73:	    Test test = TestConfiguration.embeddedSuite(IjSecurityManagerTest.class);
+78:          new String[] { "functionTests/tests/tools/IjSecurityManagerTest.sql"  },
+80:          new String[] { "IjSecurityManagerTest.sql"}
+85:		TestSuite suite = new TestSuite("IjSecurityManagerTest");
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/_Suite.java
+58:        suite.addTest(IjSecurityManagerTest.suite());
+./java/testing/org/apache/derbyTesting/functionTests/tests/compatibility/VersionedNetworkServerTestSetup.java
+45:    /** The first version to support '-noSecurityManager'. */
+97:            cmd.add("-noSecurityManager");
+179:            cmd.add("-noSecurityManager");
+./java/testing/org/apache/derbyTesting/functionTests/tests/compatibility/_Suite.java
+34:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+137:        return new SecurityManagerSetup(
+./java/testing/org/apache/derbyTesting/functionTests/tests/junitTests/compatibility/CompatibilityCombinations.java
+50: * The compatibility tests are (currently) run without a SecurityManager.
+52: * how to &lt;b&gt;not&lt;/b&gt; use a SecurityManager. --&gt; &lt;br&gt;&lt;br&gt;
+127: * test.securityOption=noSecurityManager
+172:     * The option string used to turn off running Derby server with a SecurityManager.
+173:   * Read as e.g &lt;code&gt;test.securityOption=noSecurityManager&lt;/code&gt; from the file given by
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/SysinfoTest.java
+37:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+164:     * Decorate a test with SecurityManagerSetup, clientServersuite, and
+175:                new SecurityManagerSetup(test, policyName));
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/NetworkServerControlApiTest.java
+31:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+312:        test = new SecurityManagerSetup( test,serverPolicyName );
+431:                "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+481:                "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+570:                "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+617:                "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/ProtocolTest.java
+896:        return new SecurityManagerSetup(
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/RuntimeInfoTest.java
+38:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+286:	 * Decorate a test with SecurityManagerSetup, clientServersuite, and
+304:        test = new SecurityManagerSetup(test, policyName);
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/CheckSecurityManager.java
+45:public class CheckSecurityManager extends BaseJDBCTestCase
+52:	    return TestConfiguration.defaultSuite(CheckSecurityManager.class);
+55:	public CheckSecurityManager(String name)
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/NetHarnessJavaTest.java
+30:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/GetCurrentPropertiesTest.java
+31:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+96:        test = new SecurityManagerSetup(test,serverPolicyName );
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/SSLTest.java
+34:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+101:            SecurityManagerSetup.noSecurityManager(networkServerTestSetup);
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/SecureServerTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+235:            SecurityManagerSetup.noSecurityManager(networkServerTestSetup);
+270:            list.add( "-noSecurityManager" );
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/ServerPropertiesTest.java
+41:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+209:        test = new SecurityManagerSetup(test,serverPolicyName );
+460:            "-noSecurityManager", "start"};
+473:                "-noSecurityManager", "shutdown"};
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/NetworkServerControlClientCommandTest.java
+30:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+166:        test = SecurityManagerSetup.noSecurityManager(test);
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/_Suite.java
+73:        //suite.addTest(CheckSecurityManager.suite());
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/BootLockTest.java
+39:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+102:     * Decorate test with singleUseDatabaseDecorator and noSecurityManager.
+119:        test = SecurityManagerSetup.noSecurityManager(test);
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/Derby3980DeadlockTest.java
+39:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+85:     * Decorate a test with SecurityManagerSetup, clientServersuite, and
+99:        test = new SecurityManagerSetup(test, policyName);
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/ClassLoaderBootTest.java
+46:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+106:        return SecurityManagerSetup.noSecurityManager(setup);
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/Derby5582AutomaticIndexStatisticsTest.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+34:    // private thread group. Derby5582SecurityManager will prevent other threads from 
+45:     * context of a SecurityManager that disallows modification of the parent 
+71:    	// Run just the one fixture with the custom SecurityManager
+73:        Derby5582SecurityManager sm =  new Derby5582SecurityManager();
+74:        return TestConfiguration.additionalDatabaseDecorator(new SecurityManagerSetup(t, null,
+79:     * SecurityManager which prevents modification of thread group privtg
+82:    public static class Derby5582SecurityManager  extends SecurityManager {
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/RecoveryTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+./java/testing/org/apache/derbyTesting/junit/SecurityManagerSetup.java
+3: * Derby - Class org.apache.derbyTesting.junit.SecurityManagerSetup
+56:public final class SecurityManagerSetup extends TestSetup {
+83:	private static final boolean externalSecurityManagerInstalled;
+88:		externalSecurityManagerInstalled = determineClasspath();
+116:	private SecurityManager decoratorSecurityManager = null;
+118:    public SecurityManagerSetup(Test test, String policyResource) {
+131:    public SecurityManagerSetup(Test test, String policyResource,
+146:	 * Use custom policy and SecurityManager
+150:	 * @param securityManager - Custom SecurityManager if null use the system security manager
+152:	public SecurityManagerSetup(Test test, String policyResource, SecurityManager securityManager)
+155:		this.decoratorSecurityManager = securityManager;
+173:	public static Test noSecurityManager(Test test)
+175:		if (externalSecurityManagerInstalled)
+178:        return new SecurityManagerSetup(test, NO_POLICY);
+185:	static void noSecurityManager()
+187:        installSecurityManager(NO_POLICY);
+198:        installSecurityManager(resource, decoratorSecurityManager);
+205:        else if ( !externalSecurityManagerInstalled )
+207:            uninstallSecurityManager();
+220:	 * Install a SecurityManager with the default test policy
+225:	static void installSecurityManager()
+227:		installSecurityManager( getDefaultPolicy() );
+230:	private static void installSecurityManager(String policyFile) {
+231:	   installSecurityManager(policyFile, System.getSecurityManager());
+234:	private static void installSecurityManager(String policyFile, final SecurityManager sm)
+237:		if (externalSecurityManagerInstalled)
+243:		SecurityManager currentsm = System.getSecurityManager();
+245:			// SecurityManager installed, see if it has the same settings.
+251:			SecurityManager oldSecMan = System.getSecurityManager();
+259:			uninstallSecurityManager();
+278:                        System.setSecurityManager(new SecurityManager());
+280:                        System.setSecurityManager(sm);
+342:		if (System.getSecurityManager() != null) {		
+374:		URL testing = getURL(SecurityManagerSetup.class);
+485:    private static void uninstallSecurityManager()
+493:                      System.setSecurityManager(null);
+634:        BaseTestCase.println("{SecurityManagerSetup} " + msg);
+./java/testing/org/apache/derbyTesting/junit/BaseTestCase.java
+85:     * the decorators obtained from SecurityManagerSetup.
+109:        if ( System.getSecurityManager() == null )
+111:            if (config.defaultSecurityManagerSetup())
+113:                assertSecurityManager();
+383:    public static void assertSecurityManager()
+385:    	assertNotNull("No SecurityManager installed",
+386:    			System.getSecurityManager());
+836:        return SecurityManagerSetup.jacocoEnabled;
+877:        return SecurityManagerSetup.getURL("com.vladium.emma.EMMAException");
+./java/testing/org/apache/derbyTesting/junit/TestConfiguration.java
+2007:        return SecurityManagerSetup.isJars;
+2133:     * SecurityManager related configuration.
+2141:    boolean defaultSecurityManagerSetup() {
+2147:    		SecurityManagerSetup.noSecurityManager();
+2150:            if (SecurityManagerSetup.NO_POLICY.equals(
+2156:    		SecurityManagerSetup.installSecurityManager();
+./java/testing/org/apache/derbyTesting/junit/JAXPFinder.java
+88:             *   SecurityManagerSetup.getURL(DocumentBuilderFactory.class)
+103:            URL jaxpURL = SecurityManagerSetup.getURL(
+./java/testing/org/apache/derbyTesting/junit/BaseTestSetup.java
+49:        if ( System.getSecurityManager() == null )
+51:            if (TestConfiguration.getCurrent().defaultSecurityManagerSetup())
+53:                BaseTestCase.assertSecurityManager();
+./java/testing/org/apache/derbyTesting/junit/Derby.java
+45:        if (!SecurityManagerSetup.isJars)
+62:        if (!SecurityManagerSetup.isJars)
+74:        if (!SecurityManagerSetup.isJars)
+93:        if (!SecurityManagerSetup.isJars) {
+105:        URL url = SecurityManagerSetup.getURL(className);
+./java/testing/org/apache/derbyTesting/junit/NetworkServerTestSetup.java
+161:     * the server up with no security manager using -noSecurityManager,
+336:            boolean setNoSecurityManager = true;
+341:                    setNoSecurityManager = false;
+347:                if (startupArgs[i].equals("-noSecurityManager"))
+349:                    setNoSecurityManager = false;
+353:            if (setNoSecurityManager)
+357:                newArgs[newArgs.length - 1] = "-noSecurityManager";
+./java/testing/org/apache/derbyTesting/unitTests/junit/SystemPrivilegesPermissionTest.java
+28:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+173:        suite.addTest(new SecurityManagerSetup(
+180:        if (SecurityManagerSetup.JVM_HAS_SUBJECT_AUTHORIZATION) {
+181:            suite.addTest(new SecurityManagerSetup(
+184:            suite.addTest(new SecurityManagerSetup(
+./java/testing/org/apache/derbyTesting/unitTests/junit/AssertFailureTest.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+64:            suite.addTest(new SecurityManagerSetup(new AssertFailureTest(
+68:            suite.addTest(new SecurityManagerSetup(new AssertFailureTest(
 </t>
-  </si>
-  <si>
-    <t>c_jdbc</t>
-  </si>
-  <si>
-    <t>2.0.2</t>
-  </si>
-  <si>
-    <t>http://c-jdbc.ow2.org/download.html</t>
-  </si>
-  <si>
-    <t>compiere</t>
-  </si>
-  <si>
-    <t>3.5*</t>
-  </si>
-  <si>
-    <t>http://www.compiere.com/products/download/index.php</t>
-  </si>
-  <si>
-    <t>derby</t>
-  </si>
-  <si>
-    <t>10.10.2.0*</t>
-  </si>
-  <si>
-    <t>http://db.apache.org/derby/derby_downloads.html</t>
   </si>
   <si>
     <t>drjava</t>
@@ -1377,7 +1862,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1451,8 +1936,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1621,9 +2106,15 @@
       <c r="D6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="0"/>
-      <c r="G6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1631,25 +2122,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1657,13 +2148,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="0"/>
@@ -1675,25 +2166,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1701,13 +2192,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
@@ -1719,13 +2210,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
@@ -1737,13 +2228,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
@@ -1755,13 +2246,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
@@ -1773,25 +2264,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1799,13 +2290,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -1816,13 +2307,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -1833,13 +2324,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -1850,13 +2341,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -1867,13 +2358,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -1884,13 +2375,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -1901,13 +2392,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -1918,13 +2409,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -1935,13 +2426,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -1952,13 +2443,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -1969,13 +2460,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -1986,13 +2477,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -2003,22 +2494,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2026,13 +2517,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -2041,13 +2532,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -2056,13 +2547,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -2071,13 +2562,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -2086,13 +2577,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -2101,13 +2592,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -2116,13 +2607,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -2131,13 +2622,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -2146,13 +2637,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -2161,13 +2652,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -2176,13 +2667,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -2191,13 +2682,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -2206,13 +2697,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -2221,13 +2712,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -2236,13 +2727,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -2251,13 +2742,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -2266,13 +2757,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -2281,13 +2772,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -2296,13 +2787,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -2311,13 +2802,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -2326,13 +2817,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -2341,13 +2832,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -2356,13 +2847,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -2376,12 +2867,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the static analysis notes
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="189">
   <si>
     <t>Index</t>
   </si>
@@ -536,10 +536,14 @@
     <t>http://db.apache.org/derby/derby_downloads.html</t>
   </si>
   <si>
-    <t>Callback on VMStart.
+    <t>Simple Demo Output:
+Callback on VMStart.
 #################################################
 #################################################
-Agent OnUnload, agent exits.</t>
+Agent OnUnload, agent exits.
+Coverage Result (Had an error so not 100% sure about them):
+[class, %]	[method, %]	[block, %]	[name]
+100% (1/1)	86%  (6/7)	22%  (107/494)!	all classes</t>
   </si>
   <si>
     <t>In
@@ -1019,8 +1023,58 @@
 ./java/testing/org/apache/derbyTesting/unitTests/junit/AssertFailureTest.java
 29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
 64:            suite.addTest(new SecurityManagerSetup(new AssertFailureTest(
-68:            suite.addTest(new SecurityManagerSetup(new AssertFailureTest(
-</t>
+68:            suite.addTest(new SecurityManagerSetup(new AssertFailureTest(</t>
+  </si>
+  <si>
+    <t>In
+In method org.apache.derby.drda.NetworkServerControl.installSecurityManager(NetworkServerControlImpl) 
+Value Not null: java.lang.SecurityManager 
+Value new 
+Value new[187](3) 61 
+Value Variable is set at
+Not sure why the line at the top didn't print. It should be 647.  This line is used to install a default SecurityManager if one is not already running to make sure the application always executes with some security.
+-------------------------------------------------------------
+ At RunTest.java:[line 2876] 
+In method org.apache.derbyTesting.functionTests.harness.RunTest.execTestNoProcess(Properties, String, String, String)
+Value Set to null:  
+ Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+If the test installed a SecurityManager, the test suite removes it with this line
+--------------------------------------------------------------
+At RunTest.java:[line 2979] 
+In method org.apache.derbyTesting.functionTests.harness.RunTest.installSecurityManager() 
+Value Not null: java.lang.SecurityManager 
+Value new 
+Value new[187](3) 662 
+Value Variable is set at:
+This method is called when a test needs a SecurityManager.  It sets the SecurityManager if one is not already set.
+---------------------------------------------------------------
+At SecurityManagerSetup.java:[line 278] 
+In method org.apache.derbyTesting.junit.SecurityManagerSetup$2.run() 
+Value Not null: java.lang.SecurityManager 
+Value new 
+Value new[187](3) 3 
+Value Variable is set at:
+This line sets the SecurityManager to the default SecurityManager for the system druign the tests. This only happens if no SecurityManager is defined as an argument. 
+-----------------------------------------------------------------
+At SecurityManagerSetup.java:[line 280]
+In method org.apache.derbyTesting.junit.SecurityManagerSetup$2.run()
+Value Not null: java.lang.SecurityManager
+Value aload_0 
+Value aload_0[42](1) 
+Value Variable is set at: 
+At SecurityManagerSetup.java:[line 277]
+The variable set at line is wrong for this output.  It should be line 234.  I think the fact that this is a method defined inside another method confused the results.  
+This is the way to set the SecurityManager to the specified SecurityManager sent as an argument for the test
+------------------------------------------------------------------
+At SecurityManagerSetup.java:[line 493]
+In method org.apache.derbyTesting.junit.SecurityManagerSetup$4.run()
+Value Set to null:
+Value aconst_null
+Value aconst_null[1](1)
+Value Variable is set at:
+Method to uninstall the SecurityManager for tests.  Just sets the SecurityManager to null.</t>
   </si>
   <si>
     <t>drjava</t>
@@ -1862,7 +1916,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1936,8 +1990,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="44" zoomScaleNormal="44" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2116,31 +2170,34 @@
         <v>41</v>
       </c>
       <c r="H6" s="5"/>
+      <c r="J6" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2148,13 +2205,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="0"/>
@@ -2166,25 +2223,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2192,13 +2249,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
@@ -2210,13 +2267,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
@@ -2228,13 +2285,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
@@ -2246,13 +2303,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
@@ -2264,25 +2321,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2290,13 +2347,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -2307,13 +2364,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -2324,13 +2381,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -2341,13 +2398,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -2358,13 +2415,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -2375,13 +2432,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -2392,13 +2449,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -2409,13 +2466,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -2426,13 +2483,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -2443,13 +2500,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -2460,13 +2517,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -2477,13 +2534,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -2494,22 +2551,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2517,13 +2574,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -2532,13 +2589,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -2547,13 +2604,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -2562,13 +2619,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -2577,13 +2634,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -2592,13 +2649,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -2607,13 +2664,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -2622,13 +2679,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -2637,13 +2694,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -2652,13 +2709,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -2667,13 +2724,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -2682,13 +2739,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -2697,13 +2754,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -2712,13 +2769,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -2727,13 +2784,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -2742,13 +2799,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -2757,13 +2814,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -2772,13 +2829,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -2787,13 +2844,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -2802,13 +2859,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -2817,13 +2874,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -2832,13 +2889,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -2847,13 +2904,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -2867,12 +2924,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added static analysis comments for Derby
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
   <si>
     <t>Index</t>
   </si>
@@ -1077,6 +1077,469 @@
 Method to uninstall the SecurityManager for tests.  Just sets the SecurityManager to null.</t>
   </si>
   <si>
+    <t>./java/engine/org/apache/derby/jdbc/InternalDriver.java
+332:        if (System.getSecurityManager() == null) {
+Contained in a check to see if the SecurityManager allows shutdown privaleges
+./java/engine/org/apache/derby/iapi/services/info/Version.java
+62:            if (System.getSecurityManager() != null)
+Used to check if the the program has monitor privaleges
+./java/engine/org/apache/derby/iapi/services/cache/ClassSize.java
+266:     * Note that this method will throw a SecurityException if the SecurityManager does not
+This is just a comment to say that the method could throw a SecurityException depending on the SecurityManager settings
+./java/engine/org/apache/derby/iapi/security/SecurityUtil.java
+104:     * Checks that a Subject has a Permission under the SecurityManager.
+143:     * Checks that a User has a Permission under the SecurityManager.
+159:        if (System.getSecurityManager() == null) {
+This method checks if the user has permission to run the action before doing the action.
+./java/engine/org/apache/derby/authentication/SystemPrincipal.java
+66:     * permission checking by the SecurityManager.
+This comment explains how the class interacts with the SecurityManager
+./java/engine/org/apache/derby/catalog/SystemProcedures.java
+1777:        // without a SecurityManager seems to lock in a policy with
+1779:        // when later installing a SecurityManager.
+1780:        if (System.getSecurityManager() == null)
+!!!!!!!!! This method causes the SecurityManager to update it's policy.  This seems to be only used by test cases but one of the test cases is to ensure that database administrators have the ability to update the security policy.
+./java/engine/org/apache/derby/impl/jdbc/EmbedConnection.java
+2694:        if (System.getSecurityManager() == null) {
+Used in a check to see if the program has create database privaleges
+./java/engine/org/apache/derby/impl/jdbc/EmbedConnection40.java
+285:        SecurityManager securityManager = System.getSecurityManager();
+Used to see if the program has abort permissions that this time
+./java/engine/org/apache/derby/impl/services/monitor/StorageFactoryService.java
+1199:                    System.getSecurityManager().checkWrite(from.getPath());
+Method checks to see if it has rename and write permissions
+./java/engine/org/apache/derby/impl/services/bytecode/d_BCValidate.java
+91:				// methods. Default SecurityManager behaviour is to grant access to public members
+./java/engine/org/apache/derby/impl/services/reflect/JarLoader.java
+527:     * Provide a SecurityManager with information about the class name
+Comment talking about default permissions
+./java/engine/org/apache/derby/impl/services/jmx/JMXManagementService.java
+415:            if (System.getSecurityManager() != null)
+Checks the management permissions on the SecurityManager
+./java/drda/org/apache/derby/drda/NetworkServerControl.java
+340:            if ( needsSecurityManager( server, command ) )
+343:                installSecurityManager( server );
+612:     * &lt;li&gt;The VM isn't already running a SecurityManager.&lt;/li&gt;
+614:     * &lt;li&gt;The customer didn't specify the -noSecurityManager flag on the startup command
+618:    private static  boolean needsSecurityManager( NetworkServerControlImpl server, int command )
+623:             (System.getSecurityManager() == null) &amp;&amp;
+645:     * Install a SecurityManager governed by the Basic startup policy. See DERBY-2196.
+647:    private static  void installSecurityManager( NetworkServerControlImpl server )
+692:        // Now install a SecurityManager, using the Basic policy file.
+698:        SecurityManager     securityManager = new SecurityManager();
+700:        System.setSecurityManager( securityManager );
+!!!!!!!! Sets up a SecurityManager by default if there is no other SecurityManager defined to insure there is always some security policy.
+./java/drda/org/apache/derby/impl/drda/NetworkServerControlImpl.java
+116:         "noSecurityManager", "ssl"};
+402:     * default SecurityManager.
+1189:        if (System.getSecurityManager() == null) {
+First one is just a string.  Second is a method that checks if the default SecurityManager was not started because of user input.  Third is to check if the user has Shutdown privileges
+./java/drda/org/apache/derby/impl/drda/NetworkServerMBeanImpl.java
+82:            if (System.getSecurityManager() != null)
+Just a general check permission method
+./java/client/org/apache/derby/client/net/NetConnection40.java
+401:        SecurityManager securityManager = System.getSecurityManager();
+Checks to see if the user has abort privileges
+./java/client/org/apache/derby/client/am/Version.java
+96:            java.lang.SecurityManager security = java.lang.System.getSecurityManager();
+103:            detectLocalHost(java.lang.System.getSecurityManager(), printWriter);
+137:    private static void printSystemProperty(java.lang.SecurityManager security,
+159:    private static void detectLocalHost(java.lang.SecurityManager security, java.io.PrintWriter printWriter) {
+These methods are used to print the current status of the application, including the SecurityManager settings
+./java/client/org/apache/derby/client/am/EncryptionManager.java
+137:    // rewritten into a DRDASecurityManager and have some of the
+This is a comment that these encryption capabities will later be moved to an SecurityManager
+./java/stubs/jdbc3/java/sql/DriverManager.java
+279:        SecurityManager securityManager = System.getSecurityManager();
+Checks to see if the user has logging privileges.
+./java/testing/org/apache/derbyTesting/functionTests/util/SecurityCheck.java
+153:	 * SecurityManager.inspect(conn);
+Comment to say that the method is similar to a SecurityManager check
+./java/testing/org/apache/derbyTesting/functionTests/util/TestRoutines.java
+71:		s.execute("CREATE FUNCTION TESTROUTINE.HAS_SECURITY_MANAGER() RETURNS INT NO SQL EXTERNAL NAME 'org.apache.derbyTesting.functionTests.util.TestRoutines.hasSecurityManager' language java parameter style java");
+109:	public static int hasSecurityManager()
+111:		return System.getSecurityManager() == null ? 0 : 1;
+checks to see if a SecurityManager is installed.
+./java/testing/org/apache/derbyTesting/functionTests/harness/RunTest.java
+185:    static boolean runWithoutSecurityManager;
+1757:	        		|| "true".equalsIgnoreCase(ap.getProperty("noSecurityManager")))
+1758:	        	runWithoutSecurityManager = true;
+2365:        if (!runWithoutSecurityManager)
+2368:        	System.out.println("-- SecurityManager not installed --");
+2488:            // properties (setSecurityManager, setIO)
+2669:    	boolean installedSecurityManager = installSecurityManager();
+2874:         if (installedSecurityManager)
+2876:        	System.setSecurityManager(null);
+2941:    private static boolean installSecurityManager() throws ClassNotFoundException, IOException
+2943:    	// SecurityManager not currently work with older j9 and useProcess=false
+2948:    	boolean installedSecurityManager = false;
+2949:    	// Set up the SecurityManager in this JVM for this test.
+2950:    	boolean haveSecurityManagerAlready = System.getSecurityManager() != null;
+2951:        if (runWithoutSecurityManager)
+2953:        	// Test doesn't run with a SecurityManager,
+2955:        	if (haveSecurityManagerAlready)
+2957:        				"noSecurityManager=true,useProcess=false but SecurityManager installed by previous test");
+2959:        	    System.out.println("-- SecurityManager not installed --");
+2961:        else if (!haveSecurityManagerAlready)
+2979:		    System.setSecurityManager(new SecurityManager());
+2980:		    installedSecurityManager = true;
+2983:        return installedSecurityManager;
+Handles the SecurityManager in the test cases.  It removes the SecurityManager for some tests, sets them for some, and then removes the SecurityManager after the tests finish.
+./java/testing/org/apache/derbyTesting/functionTests/harness/jvm.java
+32:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+385:            SecurityManagerSetup.getPolicyFilePropertiesForOldHarness();
+Contains a method to get the policy properties
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/HalfCreatedDatabaseTest.java
+34:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+93:        test = SecurityManagerSetup.noSecurityManager( test );
+Sets the test to have no Security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/Derby5652.java
+28:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+71:        test = SecurityManagerSetup.noSecurityManager( test );
+Sets the test to have no Security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/DBInJarTest.java
+39:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+202:        return new CleanDatabaseTestSetup(SecurityManagerSetup.noSecurityManager(suite)) 
+Sets the test suite to have no Security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/SecurityPolicyReloadingTest.java
+37:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+153:        test = new SecurityManagerSetup( test, undecoratedTest.makeServerPolicyName() );
+179:        test = SecurityManagerSetup.noSecurityManager(test);
+This method first installs a SecurityManager with the default Ploicy and then removes the policy from the SecurityManager.
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/DatabaseClassLoadingTest.java
+56:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+120:           suite.addTest(SecurityManagerSetup.noSecurityManager(
+123:           suite.addTest(SecurityManagerSetup.noSecurityManager(
+129:           suite.addTest(SecurityManagerSetup.noSecurityManager(
+Creates a couple of tests with no security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/AggregateClassLoadingTest.java
+38:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+81:		return SecurityManagerSetup.noSecurityManager(
+Sets the test to no policy and then starts a class loader for the test.
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/NativeAuthenticationServiceTest.java
+39:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+160:    private final   boolean _disableSecurityManager;
+187:         boolean    disableSecurityManager
+196:        _disableSecurityManager = disableSecurityManager;
+331:        String  securityManager = _disableSecurityManager ?
+332:            "SecurityManager OFF, " :
+333:            "SecurityManager ON, ";
+502:        if ( _disableSecurityManager ) { result = SecurityManagerSetup.noSecurityManager( result ); }
+883:            if ( _disableSecurityManager ) { vetProtocol( classpathDBName() ); }
+Intializes the test with knowledge of if a SecurityManager is set and handles the test differently if one is.
+./java/testing/org/apache/derbyTesting/functionTests/tests/lang/SysDiagVTIMappingTest.java
+27:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+85:        return SecurityManagerSetup.noSecurityManager(
+Sets up a test suite with no test file.
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Full.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+44:        return SecurityManagerSetup.noSecurityManager(suite);
+Sets up a test with no security policy.
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_CleanUp.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+54:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test with no security policy 
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_1.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+53:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test with no security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local.java
+27:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+63:        return SecurityManagerSetup.noSecurityManager(suite);
+76:        return SecurityManagerSetup.noSecurityManager( suite );
+Creates two tests with no security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/Derby5937SlaveShutdownTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+79:        return new SecurityManagerSetup(
+Installs a custom SecurityManager for this test.
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun.java
+863:                    // + " -Djava.security.policy=\"&lt;NONE&gt;\""  // Now using noSecurityManager decorator
+1944:        ceArray.add( "-noSecurityManager" );
+1991:        sp.setProperty("noSecurityManager", 
+1992:                securityOption.equalsIgnoreCase("-noSecurityManager")?"true":"false");
+Initializes a server with the no SecurityManager option for a test.
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_showStateChange.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+64:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test with no security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part1_3.java
+28:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+57:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test with no security policy.
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part1_1.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+58:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test with no security policy.
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_Encrypted_1.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+66:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test with no security policy.
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/SimplePerfTest_Verify.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+71:        return SecurityManagerSetup.noSecurityManager(t);
+Creates a test with no security policy.
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p4.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+56:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p6.java
+33:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+65:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part2.java
+30:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+58:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part1_2.java
+28:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+65:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_StateTest_part1.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+66:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_1Indexing.java
+31:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+59:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p5.java
+30:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+62:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Distributed.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+59:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p2.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+63:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/SimplePerfTest.java
+36:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+76:        return SecurityManagerSetup.noSecurityManager(t);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_Derby4910.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+52:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p1.java
+25:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+59:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/replicationTests/ReplicationRun_Local_3_p3.java
+28:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+61:        return SecurityManagerSetup.noSecurityManager(suite);
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/engine/ShutdownWithoutDeregisterPermissionTest.java
+31:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+44:        return new SecurityManagerSetup(
+Creates a test with a specific security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbcapi/InvalidLDAPServerAuthenticationTest.java
+38:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+65:        suite.addTest(SecurityManagerSetup.noSecurityManager(baseSuite(
+68:                SecurityManagerSetup.noSecurityManager(
+Creates a test without a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbcapi/AutoloadTest.java
+44:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+139:                suite.addTest(SecurityManagerSetup.noSecurityManager(
+169:        suite.addTest(SecurityManagerSetup.noSecurityManager(new AutoloadTest("testEmbeddedNotStarted")));
+197:            suite.addTest(SecurityManagerSetup.noSecurityManager(
+sets up a couple of tests with a security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbcapi/LDAPAuthenticationTest.java
+43:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+149:        test = new SecurityManagerSetup(test,ldapPolicyName );
+sets up a specific SecurityManager for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/upgradeTests/UpgradeRun.java
+32:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+136:        return SecurityManagerSetup.noSecurityManager(setup);
+sets up a test with no SecurityManager
+./java/testing/org/apache/derbyTesting/functionTests/tests/upgradeTests/UpgradeTrajectoryTest.java
+45:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+255:        return SecurityManagerSetup.noSecurityManager( sfs );
+sets up a test with no SecurityManager
+./java/testing/org/apache/derbyTesting/functionTests/tests/management/NetworkServerMBeanTest.java
+313:        // assumes noSecurityManager or that the required SocketPermission has
+Just a comment about the SecurityManager assumptions for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/management/MBeanTest.java
+46:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+112:         * Will run without SecurityManager for now, but could probably add a 
+120:                SecurityManagerSetup.noSecurityManager(networkServerTestSetup);
+Sets up a test without a SecuritManager and has a comment about it.
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbc4/AbortTest.java
+42:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+51: * class tests the affect of SecurityManagers on the method. A related
+68:    private boolean _hasSecurityManager;
+76:    public AbortTest(String name, boolean hasSecurityManager)
+80:        _hasSecurityManager = hasSecurityManager;
+110:    public static Test baseSuite( boolean hasSecurityManager )
+112:        AbortTest   abortTest = new AbortTest( "test_basic", hasSecurityManager );
+122:        if ( hasSecurityManager )
+124:            return new SecurityManagerSetup( test, "org/apache/derbyTesting/functionTests/tests/jdbc4/noAbortPermission.policy" );
+128:            return SecurityManagerSetup.noSecurityManager( test );
+151:        println( "AbortTest( " + _hasSecurityManager + " )" );
+152:        assertEquals( _hasSecurityManager, (System.getSecurityManager() != null) );
+229:        if ( _hasSecurityManager ) { missingPermission( wrapper1 ); }
+230:        else { noSecurityManager( wrapper1, conn2 ); }
+267:    private void    noSecurityManager(  final Wrapper41Conn wrapper1, Connection conn2  ) throws Exception
+Tests to see if the application has a SecurityManager and sets up some SecurityManagers for tests.
+./java/testing/org/apache/derbyTesting/functionTests/tests/jdbc4/Driver40UnbootedTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+86:        return SecurityManagerSetup.noSecurityManager( test );
+Test with SecurityManager with no policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/IjConnNameTest.java
+36:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+70:        //test = SecurityManagerSetup.noSecurityManager(test);
+Teset with SecurityManager with no policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/SysinfoAPITest.java
+33:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+Test with a custom SecurityManager
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/derbyrunjartest.java
+32:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+55:        return new SecurityManagerSetup(
+71:        URL result = SecurityManagerSetup.getURL(runClassName);
+146:            "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+Sets up a SecurityManager for a test.  Also contains the output for the start commands for the NetworkControlSerer.
+@@@@@@@@ - not really imporant but contains the command line arguements for the NetworkControlServer so they may be useful.
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/SysinfoLocaleTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+131:        return SecurityManagerSetup.noSecurityManager(suite);
+161:        URL sysinfoURL = SecurityManagerSetup.getURL(className);
+creates a test with a SecurityManager with no policy so a class loader can be used in the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/IjSecurityManagerTest.java
+4:   org.apache.derbyTesting.functionTests.tests.tools.IjSecurityManager
+38:public class IjSecurityManagerTest extends BaseTestCase {
+40:	public IjSecurityManagerTest(String name) {
+58:	        ij.main(new String[]{"extinout/IjSecurityManagerTest.sql"});
+73:	    Test test = TestConfiguration.embeddedSuite(IjSecurityManagerTest.class);
+78:          new String[] { "functionTests/tests/tools/IjSecurityManagerTest.sql"  },
+80:          new String[] { "IjSecurityManagerTest.sql"}
+85:		TestSuite suite = new TestSuite("IjSecurityManagerTest");
+Just a test name.
+./java/testing/org/apache/derbyTesting/functionTests/tests/tools/_Suite.java
+58:        suite.addTest(IjSecurityManagerTest.suite());
+Also just a test name
+./java/testing/org/apache/derbyTesting/functionTests/tests/compatibility/VersionedNetworkServerTestSetup.java
+45:    /** The first version to support '-noSecurityManager'. */
+97:            cmd.add("-noSecurityManager");
+179:            cmd.add("-noSecurityManager");
+Test to start the NetworkControlServer and allows for starting the application with no SecurityManager
+./java/testing/org/apache/derbyTesting/functionTests/tests/compatibility/_Suite.java
+34:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+137:        return new SecurityManagerSetup(
+Sets up a test with a specific SecurityManager
+./java/testing/org/apache/derbyTesting/functionTests/tests/junitTests/compatibility/CompatibilityCombinations.java
+50: * The compatibility tests are (currently) run without a SecurityManager.
+52: * how to &lt;b&gt;not&lt;/b&gt; use a SecurityManager. --&gt; &lt;br&gt;&lt;br&gt;
+127: * test.securityOption=noSecurityManager
+172:     * The option string used to turn off running Derby server with a SecurityManager.
+173:   * Read as e.g &lt;code&gt;test.securityOption=noSecurityManager&lt;/code&gt; from the file given by
+Comments that the SecurityManager is not used for this test
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/SysinfoTest.java
+37:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+164:     * Decorate a test with SecurityManagerSetup, clientServersuite, and
+175:                new SecurityManagerSetup(test, policyName));
+General method to add a security policy to tests
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/NetworkServerControlApiTest.java
+31:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+312:        test = new SecurityManagerSetup( test,serverPolicyName );
+431:                "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+481:                "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+570:                "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+617:                "start [-h &lt;host&gt;] [-p &lt;port number&gt;] [-noSecurityManager] [-ssl &lt;ssl mode&gt;]",
+Has tests for the NetworkServerControl and can disable the SecurityManager.  Also sets up a test with the default security policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/ProtocolTest.java
+896:        return new SecurityManagerSetup(
+Installs the SecurityManager for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/RuntimeInfoTest.java
+38:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+286:	 * Decorate a test with SecurityManagerSetup, clientServersuite, and
+304:        test = new SecurityManagerSetup(test, policyName);
+Installs the SecurityManager for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/CheckSecurityManager.java
+45:public class CheckSecurityManager extends BaseJDBCTestCase
+52:	    return TestConfiguration.defaultSuite(CheckSecurityManager.class);
+55:	public CheckSecurityManager(String name)
+Contains tests to see if the SecurityManager is running.
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/NetHarnessJavaTest.java
+30:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+Not really used in the file.
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/GetCurrentPropertiesTest.java
+31:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+96:        test = new SecurityManagerSetup(test,serverPolicyName );
+Sets up a specific SecurityManager policy for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/SSLTest.java
+34:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+101:            SecurityManagerSetup.noSecurityManager(networkServerTestSetup);
+Sets up a SecurityManager with no Policy
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/SecureServerTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+235:            SecurityManagerSetup.noSecurityManager(networkServerTestSetup);
+270:            list.add( "-noSecurityManager" );
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/ServerPropertiesTest.java
+41:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+209:        test = new SecurityManagerSetup(test,serverPolicyName );
+460:            "-noSecurityManager", "start"};
+473:                "-noSecurityManager", "shutdown"};
+sets up a test with a SecurityManager with no policy.  Also allows starting the NetworkServerControl client without a SecurityManager
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/NetworkServerControlClientCommandTest.java
+30:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+166:        test = SecurityManagerSetup.noSecurityManager(test);
+sets up a SecurityManager with no policy for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/derbynet/_Suite.java
+73:        //suite.addTest(CheckSecurityManager.suite());
+This line is commented out
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/BootLockTest.java
+39:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+102:     * Decorate test with singleUseDatabaseDecorator and noSecurityManager.
+119:        test = SecurityManagerSetup.noSecurityManager(test);
+Sets up a SecurityManager with no policy for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/Derby3980DeadlockTest.java
+39:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+85:     * Decorate a test with SecurityManagerSetup, clientServersuite, and
+99:        test = new SecurityManagerSetup(test, policyName);
+Sets up a SecurityManager with a specific policy for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/ClassLoaderBootTest.java
+46:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+106:        return SecurityManagerSetup.noSecurityManager(setup);
+Sets up a SecurityManager without a policy for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/Derby5582AutomaticIndexStatisticsTest.java
+29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+34:    // private thread group. Derby5582SecurityManager will prevent other threads from 
+45:     * context of a SecurityManager that disallows modification of the parent 
+71:    	// Run just the one fixture with the custom SecurityManager
+73:        Derby5582SecurityManager sm =  new Derby5582SecurityManager();
+74:        return TestConfiguration.additionalDatabaseDecorator(new SecurityManagerSetup(t, null,
+79:     * SecurityManager which prevents modification of thread group privtg
+82:    public static class Derby5582SecurityManager  extends SecurityManager {
+Sets up a specific SecurityManager for the test
+./java/testing/org/apache/derbyTesting/functionTests/tests/store/RecoveryTest.java
+35:import org.apache.derbyTesting.junit.SecurityManagerSetup;
+Not used in this file
+./java/testing/org/apache/derbyTesting/junit/SecurityManagerSetup.java
+3: * Derby - Class org.apache.derbyTesting.junit.SecurityManagerSetup
+56:public final class SecurityManagerSetup extends TestSetup {
+83:	private static final boolean externalSecurityManagerInstalled;
+88:		externalSecurityManagerInstalled = determineClasspath();
+116:	private SecurityManager decoratorSecurityManager = null;
+118:    public SecurityManagerSetup(Test test, String policyResource) {
+131:    public SecurityManagerSetup(Test test, String policyResource,
+146:	 * Use custom policy and SecurityManager
+150:	 * @param securityManager - Custom SecurityManager if null use the system security manager
+152:	public SecurityManagerSetup(Test test, String policyResource, SecurityManager securityManager)
+155:		this.decoratorSecurityManager = securityManager;
+173:	public static Test noSecurityManager(Test test)
+175:		if (externalSecurityManagerInstalled)
+178:        return new SecurityManagerSetup(test, NO_POLICY);
+185:	static void noSecurityManager()
+187:        installSecurityManager(NO_POLICY);
+198:        installSecurityManager(resource, decoratorSecurityManager);
+205:        else if ( !externalSecurityManagerInstalled )
+207:            uninstallSecurityManager();
+220:	 * Install a SecurityManager with the default test policy
+225:	static void installSecurityManager()
+227:		installSecurityManager( getDef</t>
+  </si>
+  <si>
     <t>drjava</t>
   </si>
   <si>
@@ -1916,7 +2379,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1990,8 +2453,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="44" zoomScaleNormal="44" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="44" zoomScaleNormal="44" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2128,6 +2591,7 @@
       <c r="F4" s="0"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
+      <c r="J4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -2146,6 +2610,7 @@
       <c r="F5" s="0"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
+      <c r="J5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2173,31 +2638,34 @@
       <c r="J6" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="K6" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2205,13 +2673,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="0"/>
@@ -2223,25 +2691,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2249,13 +2717,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
@@ -2267,13 +2735,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
@@ -2285,13 +2753,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
@@ -2303,13 +2771,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
@@ -2321,25 +2789,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2347,13 +2815,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -2364,13 +2832,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -2381,13 +2849,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -2398,13 +2866,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -2415,13 +2883,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -2432,13 +2900,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -2449,13 +2917,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -2466,13 +2934,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -2483,13 +2951,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -2500,13 +2968,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -2517,13 +2985,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -2534,13 +3002,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -2551,22 +3019,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2574,13 +3042,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -2589,13 +3057,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -2604,13 +3072,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -2619,13 +3087,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -2634,13 +3102,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -2649,13 +3117,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -2664,13 +3132,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -2679,13 +3147,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -2694,13 +3162,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -2709,13 +3177,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -2724,13 +3192,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -2739,13 +3207,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -2754,13 +3222,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -2769,13 +3237,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -2784,13 +3252,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -2799,13 +3267,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -2814,13 +3282,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -2829,13 +3297,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -2844,13 +3312,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -2859,13 +3327,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -2874,13 +3342,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -2889,13 +3357,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -2904,13 +3372,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -2924,12 +3392,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished the dynamic analysis notes and general notes for Derby
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="519" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="192">
   <si>
     <t>Index</t>
   </si>
@@ -543,7 +543,17 @@
 Agent OnUnload, agent exits.
 Coverage Result (Had an error so not 100% sure about them):
 [class, %]	[method, %]	[block, %]	[name]
-100% (1/1)	86%  (6/7)	22%  (107/494)!	all classes</t>
+100% (1/1)	86%  (6/7)	22%  (107/494)!	all classes
+--------------------------------------------------------------------------------------------
+Executing the NetworkServerControl in the bin folder:
+Callback on VMStart.
+#################################################
+ERROR: JVMTI: 101(JVMTI_ERROR_ABSENT_INFORMATION): Unable to get line number for SecurityManager change.
+SecurityManager Changed:
+(null), installSecurityManager, 0
+#################################################
+Agent OnUnload, agent exits.
+</t>
   </si>
   <si>
     <t>In
@@ -1024,6 +1034,12 @@
 29:import org.apache.derbyTesting.junit.SecurityManagerSetup;
 64:            suite.addTest(new SecurityManagerSetup(new AssertFailureTest(
 68:            suite.addTest(new SecurityManagerSetup(new AssertFailureTest(</t>
+  </si>
+  <si>
+    <t>Executed the only path to set the SecurityManager I saw.  I think they want the capability to update the security policy although I only saw it reachable from test cases at the moment. </t>
+  </si>
+  <si>
+    <t>From the static analysis the only path that sets a SecurityManager in the main application is when a NetworkControlServer is started.  I started a server and saw the SecurityManager was started but I got a line number error.  I think the program wants to have the capability to change the Security policy (as seen in a test comment) but I think the method is only callable by tests at the moment.</t>
   </si>
   <si>
     <t>In
@@ -2379,7 +2395,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -2453,8 +2469,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="44" zoomScaleNormal="44" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2592,6 +2608,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -2611,6 +2628,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2634,12 +2652,17 @@
       <c r="G6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="J6" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2647,25 +2670,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2673,13 +2696,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="0"/>
@@ -2691,25 +2714,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2717,13 +2740,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
@@ -2735,13 +2758,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
@@ -2753,13 +2776,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
@@ -2771,13 +2794,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
@@ -2789,25 +2812,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2815,13 +2838,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -2832,13 +2855,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -2849,13 +2872,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -2866,13 +2889,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -2883,13 +2906,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -2900,13 +2923,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -2917,13 +2940,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -2934,13 +2957,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -2951,13 +2974,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -2968,13 +2991,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -2985,13 +3008,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -3002,13 +3025,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -3019,22 +3042,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3042,13 +3065,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -3057,13 +3080,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -3072,13 +3095,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -3087,13 +3110,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -3102,13 +3125,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -3117,13 +3140,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -3132,13 +3155,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -3147,13 +3170,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -3162,13 +3185,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -3177,13 +3200,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -3192,13 +3215,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -3207,13 +3230,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -3222,13 +3245,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -3237,13 +3260,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -3252,13 +3275,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -3267,13 +3290,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -3282,13 +3305,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -3297,13 +3320,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -3312,13 +3335,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -3327,13 +3350,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -3342,13 +3365,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -3357,13 +3380,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -3372,13 +3395,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -3392,12 +3415,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add partial notes for freemind
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="195">
   <si>
     <t>Index</t>
   </si>
@@ -552,8 +552,7 @@
 SecurityManager Changed:
 (null), installSecurityManager, 0
 #################################################
-Agent OnUnload, agent exits.
-</t>
+Agent OnUnload, agent exits.</t>
   </si>
   <si>
     <t>In
@@ -1036,7 +1035,7 @@
 68:            suite.addTest(new SecurityManagerSetup(new AssertFailureTest(</t>
   </si>
   <si>
-    <t>Executed the only path to set the SecurityManager I saw.  I think they want the capability to update the security policy although I only saw it reachable from test cases at the moment. </t>
+    <t>Executed the only path to set the SecurityManager I saw.  I think they want the capability to update the security policy although I only saw it reachable from test cases at the moment.</t>
   </si>
   <si>
     <t>From the static analysis the only path that sets a SecurityManager in the main application is when a NetworkControlServer is started.  I started a server and saw the SecurityManager was started but I got a line number error.  I think the program wants to have the capability to change the Security policy (as seen in a test comment) but I think the method is only callable by tests at the moment.</t>
@@ -1732,6 +1731,15 @@
     <t>When the program is running, the security manager is set via line 277 in FreeMind.java, which can be verified by all of the analysis. Because another SM is set in test cases, but not in the main program, the analysis tools didn't catch this case. In the source code, the program defines its own SM via extending the SM class and adds more policies to it, and therefore strengens the security policy.</t>
   </si>
   <si>
+    <t>The agent correctly catches the place where Freemind changes the SM during the main program is running.</t>
+  </si>
+  <si>
+    <t>In accordance with the dynamic analysis. Batik, as its plugin, also sets SM to null. However, those behaviors aren't cought by the agent, I assume they are not loaded.</t>
+  </si>
+  <si>
+    <t>In accordance with the dynamic analysis. There is also another place where SM is changed. Since it's located in the test directory and not loaded during the run, we don't care about this.</t>
+  </si>
+  <si>
     <t>galleon</t>
   </si>
   <si>
@@ -2322,7 +2330,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2367,6 +2375,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2395,7 +2407,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -2464,13 +2476,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2607,6 +2618,7 @@
       <c r="F4" s="0"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
+      <c r="I4" s="0"/>
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
     </row>
@@ -2627,6 +2639,7 @@
       <c r="F5" s="0"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
+      <c r="I5" s="0"/>
       <c r="J5" s="0"/>
       <c r="K5" s="0"/>
     </row>
@@ -2734,19 +2747,28 @@
       <c r="H9" s="5" t="s">
         <v>61</v>
       </c>
+      <c r="I9" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
@@ -2758,13 +2780,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
@@ -2776,13 +2798,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
@@ -2794,13 +2816,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
@@ -2812,25 +2834,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2838,13 +2860,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -2855,13 +2877,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -2872,13 +2894,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -2889,13 +2911,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -2906,13 +2928,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -2923,13 +2945,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -2940,13 +2962,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -2957,13 +2979,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -2974,13 +2996,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -2991,13 +3013,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -3008,13 +3030,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -3025,13 +3047,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -3042,22 +3064,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3065,13 +3087,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -3080,13 +3102,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -3095,13 +3117,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -3110,13 +3132,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -3125,13 +3147,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -3139,14 +3161,14 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>136</v>
+      <c r="B33" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>138</v>
+        <v>140</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>141</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -3155,13 +3177,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>141</v>
+        <v>143</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -3170,13 +3192,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -3185,13 +3207,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -3200,13 +3222,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -3215,13 +3237,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>156</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -3230,13 +3252,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -3245,13 +3267,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>162</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -3260,13 +3282,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>165</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -3275,13 +3297,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>168</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -3290,13 +3312,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>168</v>
+        <v>170</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>171</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -3305,13 +3327,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>171</v>
+        <v>173</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>174</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -3320,13 +3342,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>174</v>
+        <v>176</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -3335,13 +3357,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>177</v>
+        <v>179</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>180</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -3350,13 +3372,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>180</v>
+        <v>182</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -3365,13 +3387,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>183</v>
+        <v>185</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>186</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -3380,13 +3402,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>186</v>
+        <v>188</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>189</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -3395,19 +3417,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>189</v>
+        <v>191</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>192</v>
       </c>
       <c r="E50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="9"/>
-      <c r="D51" s="11"/>
+      <c r="D51" s="12"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3415,12 +3437,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the ant general comments
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -151,7 +151,7 @@
 154:            perms.restoreSecurityManager();</t>
   </si>
   <si>
-    <t>Running the code coverage tool Emma as I was running ant shows that only 3 classes were used to build Jruby.  So I'm not sure we are getting very good code coverage with the dynamic analysis.  However, after doing the static analysis,  I expected the dynamic analysis to not output anything.  It looks like we may be able to see a SecurityManager change if we are using special compilers that need to execute Java while compiling.  Look at the Grep comments for more information.</t>
+    <t>It looks like we may be able to see a SecurityManager change if we are using special compilers that need to execute Java while compiling or write an application to use vendor specific extensions.  The only setSecurityManager I found that was valid is in the ExecuteJava.java file which is not called normally.</t>
   </si>
   <si>
     <t>No output.  Probably don't have good code coverage although any classes loaded through another classloader than the default one would not be seen with the current Emma method I used.  
@@ -2407,7 +2407,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -2476,12 +2476,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2703,6 +2704,9 @@
       <c r="H7" s="5" t="s">
         <v>51</v>
       </c>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -2721,6 +2725,9 @@
       <c r="F8" s="0"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">

</xml_diff>

<commit_message>
Commiting analysis for DrJava
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="199">
   <si>
     <t>Index</t>
   </si>
@@ -1581,6 +1581,18 @@
 DETECT_SECURITY_MANAGER_SET_LOCATION_BUG entry is not shown, which can be verified in the grep result. Therefore I claim that the security policy is not weakened.</t>
   </si>
   <si>
+    <t>Zack's Dynamic Analysis Comments – No output and shouldn't have output based on Grep results</t>
+  </si>
+  <si>
+    <t>Zack's Static Analysis Comments – No output.  This was expected from the Grep results.</t>
+  </si>
+  <si>
+    <t>Zack's Grep Comments – I got the same output as what was listed here.  I also saw that all the lines are commented out.</t>
+  </si>
+  <si>
+    <t>Zack' General Comments – All the SecurityManager lines were commented out.  This program should be removed from the dataset in my opinion.</t>
+  </si>
+  <si>
     <t>eclipse_SDK</t>
   </si>
   <si>
@@ -2174,7 +2186,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2248,6 +2260,12 @@
       <name val="Calibri Light"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2330,7 +2348,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2371,6 +2389,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2383,19 +2405,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2407,7 +2429,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -2476,13 +2498,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J4" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2707,19 +2729,31 @@
       <c r="I7" s="0"/>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
+      <c r="L7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="0"/>
@@ -2734,34 +2768,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2769,13 +2803,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
@@ -2787,13 +2821,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
@@ -2805,13 +2839,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
@@ -2823,13 +2857,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
@@ -2841,25 +2875,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2867,13 +2901,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -2884,13 +2918,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -2901,13 +2935,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -2918,13 +2952,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -2935,13 +2969,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -2952,13 +2986,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -2969,13 +3003,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -2986,13 +3020,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -3003,13 +3037,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -3020,13 +3054,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -3037,13 +3071,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -3054,13 +3088,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -3071,22 +3105,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3094,13 +3128,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -3109,13 +3143,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -3124,13 +3158,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -3139,13 +3173,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -3154,13 +3188,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -3168,14 +3202,14 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>139</v>
+      <c r="B33" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -3184,13 +3218,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -3199,13 +3233,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>147</v>
+        <v>150</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>151</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -3214,13 +3248,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>150</v>
+        <v>152</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -3229,13 +3263,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>153</v>
+        <v>155</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -3244,13 +3278,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>156</v>
+        <v>158</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>160</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -3259,13 +3293,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>159</v>
+        <v>161</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>163</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -3274,13 +3308,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>162</v>
+        <v>164</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -3289,13 +3323,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>165</v>
+        <v>167</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>169</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -3304,13 +3338,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>168</v>
+        <v>170</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>172</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -3319,13 +3353,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>171</v>
+        <v>174</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -3334,13 +3368,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>174</v>
+        <v>177</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -3349,13 +3383,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>177</v>
+        <v>180</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>181</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -3364,13 +3398,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>180</v>
+        <v>183</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -3379,13 +3413,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>183</v>
+        <v>186</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>187</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -3394,13 +3428,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>186</v>
+        <v>189</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -3409,13 +3443,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>189</v>
+        <v>192</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -3424,19 +3458,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>192</v>
+        <v>195</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>196</v>
       </c>
       <c r="E50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="9"/>
-      <c r="D51" s="12"/>
+      <c r="D51" s="13"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3444,12 +3478,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the static analysis and grep analysis for freemind
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
   <si>
     <t>Index</t>
   </si>
@@ -1752,6 +1752,140 @@
     <t>In accordance with the dynamic analysis. There is also another place where SM is changed. Since it's located in the test directory and not loaded during the run, we don't care about this.</t>
   </si>
   <si>
+    <t>Zack's Static Analysis-
+!!!!!!!! Redo this with the manually unpacked jars to see if you can get line numbers for
+ the bottom 3.
+At FreeMind.java:[line 205]
+In method new freemind.main.FreeMind(Properties, Properties, File) 
+Value Not null: freemind.main.FreeMindSecurityManager 
+Value new 
+Value new[187](3) 16 
+Value Variable is set at:
+This line sets a changable SecurityManager as the SecurityManager for the program.  The SecurityManager is later changed in the file /plugins/scripts/ScriptingEngine.java in the method executeScript.
+-------------------------------------------------------------------
+In line 172
+In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean)
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+This was analysed in the batik report - this line is used to null the SecurityManager to force a reload when updating the security policy of batik dynamically. I don't think these next 3 lines are called by Batik but I'll try to make it happen in the dynamic analysis.
+-------------------------------------------------------------------
+In line 176
+In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean)
+Value Set to null:
+Value aconst_null
+Value aconst_null[1](1)
+Value Variable is set at:
+This is the line to remove the SecurityManager.  This line only executes if batik already set the SecurityManager.
+-------------------------------------------------------------------
+In line 250
+In method org.apache.batik.util.ApplicationSecurityEnforcer.installSecurityManager()
+Value Not null: org.apache.batik.util.BatikSecurityManager
+Value new
+Value new[187](3) 29
+Value Variable is set at:
+This lines sets the application to use the batik SecurityManager
+--------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>Zack's Grep Comments - 
+./freemind/main/FreeMindSecurityManager.java
+22:/*$Id: FreeMindSecurityManager.java,v 1.1.2.1 2008/03/14 21:15:22 christianfoltin Exp $*/
+41:public final class FreeMindSecurityManager extends SecurityManager {
+43:	private SecurityManager mFinalSecurityManager=null;
+45:	public FreeMindSecurityManager() {
+48:	 * @param pFinalSecurityManager set twice the same to remove it.
+51:	public void setFinalSecurityManager(SecurityManager pFinalSecurityManager) {
+52:		if(pFinalSecurityManager == mFinalSecurityManager) {
+53:			mFinalSecurityManager = null;
+56:		if(mFinalSecurityManager != null) {
+57:			throw new SecurityException("There is a SecurityManager installed already.");
+59:		mFinalSecurityManager = pFinalSecurityManager;
+62:		if(mFinalSecurityManager == null) return;
+63:		mFinalSecurityManager.checkAccept(pHost, pPort);
+66:		if(mFinalSecurityManager == null) return;
+67:		mFinalSecurityManager.checkAccess(pT);
+70:		if(mFinalSecurityManager == null) return;
+71:		mFinalSecurityManager.checkAccess(pG);
+74:		if(mFinalSecurityManager == null) return;
+75:		mFinalSecurityManager.checkAwtEventQueueAccess();
+78:		if(mFinalSecurityManager == null) return;
+79:		mFinalSecurityManager.checkConnect(pHost, pPort, pContext);
+82:		if(mFinalSecurityManager == null) return;
+83:		mFinalSecurityManager.checkConnect(pHost, pPort);
+86:		if(mFinalSecurityManager == null) return;
+87:		mFinalSecurityManager.checkCreateClassLoader();
+90:		if(mFinalSecurityManager == null) return;
+91:		mFinalSecurityManager.checkDelete(pFile);
+94:		if(mFinalSecurityManager == null) return;
+95:		mFinalSecurityManager.checkExec(pCmd);
+98:		if(mFinalSecurityManager == null) return;
+99:		mFinalSecurityManager.checkExit(pStatus);
+102:		if(mFinalSecurityManager == null) return;
+103:		mFinalSecurityManager.checkLink(pLib);
+106:		if(mFinalSecurityManager == null) return;
+107:		mFinalSecurityManager.checkListen(pPort);
+110:		if(mFinalSecurityManager == null) return;
+111:		mFinalSecurityManager.checkMemberAccess(arg0, arg1);
+114:		if(mFinalSecurityManager == null) return;
+115:		mFinalSecurityManager.checkMulticast(pMaddr, pTtl);
+118:		if(mFinalSecurityManager == null) return;
+119:		mFinalSecurityManager.checkMulticast(pMaddr);
+122:		if(mFinalSecurityManager == null) return;
+123:		mFinalSecurityManager.checkPackageAccess(pPkg);
+126:		if(mFinalSecurityManager == null) return;
+127:		mFinalSecurityManager.checkPackageDefinition(pPkg);
+130:		if(mFinalSecurityManager == null) return;
+131:		mFinalSecurityManager.checkPermission(pPerm, pContext);
+134:		if(mFinalSecurityManager == null) return;
+135:		mFinalSecurityManager.checkPermission(pPerm);
+138:		if(mFinalSecurityManager == null) return;
+139:		mFinalSecurityManager.checkPrintJobAccess();
+142:		if(mFinalSecurityManager == null) return;
+143:		mFinalSecurityManager.checkPropertiesAccess();
+146:		if(mFinalSecurityManager == null) return;
+147:		mFinalSecurityManager.checkPropertyAccess(pKey);
+150:		if(mFinalSecurityManager == null) return;
+151:		mFinalSecurityManager.checkRead(pFd);
+154:		if(mFinalSecurityManager == null) return;
+155:		mFinalSecurityManager.checkRead(pFile, pContext);
+158:		if(mFinalSecurityManager == null) return;
+159:		mFinalSecurityManager.checkRead(pFile);
+162:		if(mFinalSecurityManager == null) return;
+163:		mFinalSecurityManager.checkSecurityAccess(pTarget);
+166:		if(mFinalSecurityManager == null) return;
+167:		mFinalSecurityManager.checkSetFactory();
+170:		if(mFinalSecurityManager == null) return;
+171:		mFinalSecurityManager.checkSystemClipboardAccess();
+174:		if(mFinalSecurityManager == null) return true;
+175:		return mFinalSecurityManager.checkTopLevelWindow(pWindow);
+178:		if(mFinalSecurityManager == null) return;
+179:		mFinalSecurityManager.checkWrite(pFd);
+182:		if(mFinalSecurityManager == null) return;
+183:		mFinalSecurityManager.checkWrite(pFile);
+186:		if(mFinalSecurityManager == null) return super.getSecurityContext();
+187:		return mFinalSecurityManager.getSecurityContext();
+This is the greneral FreeMindSecurityManager class.  It is set at the beginnning of FreeMind and implements the policy of the SecurityManager in mFinalSecurityManager.  It can be set and then nulled but it can't change from one SecurityManager's policies to another SecurityManager's policies directly.
+./freemind/main/FreeMind.java
+205:		System.setSecurityManager(new FreeMindSecurityManager());
+This is set at the beginning of the program.  It creates a FreeMindSecurityManager which intially has a null policy.
+./plugins/script/ScriptingSecurityManager.java
+22:/*$Id: ScriptingSecurityManager.java,v 1.1.2.5 2008/04/02 20:02:37 christianfoltin Exp $*/
+37:public class ScriptingSecurityManager extends SecurityManager {
+59:	public ScriptingSecurityManager(boolean pWithoutFileRestriction, boolean pWithoutNetworkRestriction,
+This SecurityManager allows the configuration of specific SecurityManager for different instances based on the parameters in the constructor.  This SecurityManager is set as the policy of the FreeMindSecurityManager when executing Groovy scripts in the file ScriptingEngine and then immediately removed as the policy of the FreeMindSecurityManager.
+./plugins/script/ScriptingEngine.java
+42:import freemind.main.FreeMindSecurityManager;
+226:		final ScriptingSecurityManager scriptingSecurityManager = new ScriptingSecurityManager(
+228:		final FreeMindSecurityManager securityManager = (FreeMindSecurityManager) System
+229:				.getSecurityManager();
+244:						securityManager.setFinalSecurityManager(scriptingSecurityManager);
+252:							securityManager.setFinalSecurityManager(scriptingSecurityManager);
+This file instantiaates a scriptingSecurityManager with the policy dependent on how trusted the script is (for example, if the script is signed the policy allows more permissions. )  Then it sets the scriptingSecurityManager as the policy to implement in the FreeMindSecurityManager.  Once the script is executed, it removes the securityManager by calling the setFinalSecurityManger with the same arguments.  This means that the SecurityManager only has a policy when untrusted code is running (minimizing policy enforcment to the location it is needed), and thus changing dynamically.
+</t>
+  </si>
+  <si>
     <t>galleon</t>
   </si>
   <si>
@@ -2419,7 +2553,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -2488,12 +2622,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H5" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2802,19 +2937,25 @@
       <c r="K9" s="11" t="s">
         <v>68</v>
       </c>
+      <c r="M9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
@@ -2826,13 +2967,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
@@ -2844,13 +2985,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
@@ -2862,13 +3003,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
@@ -2880,25 +3021,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2906,13 +3047,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -2923,13 +3064,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -2940,13 +3081,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -2957,13 +3098,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -2974,13 +3115,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -2991,13 +3132,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -3008,13 +3149,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -3025,13 +3166,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -3042,13 +3183,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -3059,13 +3200,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -3076,13 +3217,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -3093,13 +3234,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -3110,22 +3251,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3133,13 +3274,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -3148,13 +3289,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -3163,13 +3304,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -3178,13 +3319,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -3193,13 +3334,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -3208,13 +3349,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -3223,13 +3364,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -3238,13 +3379,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -3253,13 +3394,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -3268,13 +3409,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -3283,13 +3424,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -3298,13 +3439,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -3313,13 +3454,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -3328,13 +3469,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -3343,13 +3484,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -3358,13 +3499,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -3373,13 +3514,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -3388,13 +3529,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -3403,13 +3544,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -3418,13 +3559,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -3433,13 +3574,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -3448,13 +3589,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -3463,13 +3604,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -3483,12 +3624,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing all of the Freemind notes
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="211">
   <si>
     <t>Index</t>
   </si>
@@ -1602,6 +1602,9 @@
     <t>http://download.eclipse.org/eclipse/downloads/</t>
   </si>
   <si>
+    <t>s if batik already set the SecurityManager.</t>
+  </si>
+  <si>
     <t>freemind</t>
   </si>
   <si>
@@ -1752,9 +1755,36 @@
     <t>In accordance with the dynamic analysis. There is also another place where SM is changed. Since it's located in the test directory and not loaded during the run, we don't care about this.</t>
   </si>
   <si>
+    <t>Zack's Dynamic Analysis Comments -
+Starting and then exiting Freemind:
+Callback on VMStart.
+#################################################
+SecurityManager Changed:
+FreeMind.java, &lt;init&gt;, 205
+#################################################
+Agent OnUnload, agent exits.
+This is the result I expected. The FreemindSecurityManager is set at the beginning of the application. 
+-------------------------------------------------------------------
+Saving the default picture as an SVG file (Using File &gt; Export &gt; As SVG)
+Callback on VMStart.
+#################################################
+SecurityManager Changed:
+FreeMind.java, &lt;init&gt;, 205
+#################################################
+Agent OnUnload, agent exits.
+This test was done to confirm that the SVG saving plugin which used Batik, did not interact with the SecurityManager sets in Batik.  The test showed there was no interaction.
+-------------------------------------------------------------------
+Running a groovy script to print "Hello World" and then exitting (Tools &gt; Script Editor &gt; Actions &gt; New Script)
+Callback on VMStart.
+#################################################
+SecurityManager Changed:
+FreeMind.java, &lt;init&gt;, 205
+#################################################
+Agent OnUnload, agent exits.
+This path doesn't directly change the SecurityManager but it changes one of its fields which effects the permissions of the currently executing code.  I think this this is an execution where the SecurityManager was weakened although I don't think we are testing for this type of weakening at the moment.</t>
+  </si>
+  <si>
     <t>Zack's Static Analysis-
-!!!!!!!! Redo this with the manually unpacked jars to see if you can get line numbers for
- the bottom 3.
 At FreeMind.java:[line 205]
 In method new freemind.main.FreeMind(Properties, Properties, File) 
 Value Not null: freemind.main.FreeMindSecurityManager 
@@ -1882,8 +1912,10 @@
 229:				.getSecurityManager();
 244:						securityManager.setFinalSecurityManager(scriptingSecurityManager);
 252:							securityManager.setFinalSecurityManager(scriptingSecurityManager);
-This file instantiaates a scriptingSecurityManager with the policy dependent on how trusted the script is (for example, if the script is signed the policy allows more permissions. )  Then it sets the scriptingSecurityManager as the policy to implement in the FreeMindSecurityManager.  Once the script is executed, it removes the securityManager by calling the setFinalSecurityManger with the same arguments.  This means that the SecurityManager only has a policy when untrusted code is running (minimizing policy enforcment to the location it is needed), and thus changing dynamically.
-</t>
+This file instantiaates a scriptingSecurityManager with the policy dependent on how trusted the script is (for example, if the script is signed the policy allows more permissions. )  Then it sets the scriptingSecurityManager as the policy to implement in the FreeMindSecurityManager.  Once the script is executed, it removes the securityManager by calling the setFinalSecurityManger with the same arguments.  This means that the SecurityManager only has a policy when untrusted code is running (minimizing policy enforcment to the location it is needed), and thus changing dynamically.</t>
+  </si>
+  <si>
+    <t>Zack' General Comments – In the main program there is a SecurityManager set at the beginning which allows all permissions.  In a plugin, the current SecurityManager's policy is strengthened at then set back to allowing all permissions.</t>
   </si>
   <si>
     <t>galleon</t>
@@ -1895,6 +1927,9 @@
     <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
   </si>
   <si>
+    <t>In line 176</t>
+  </si>
+  <si>
     <t>hadoop</t>
   </si>
   <si>
@@ -1904,6 +1939,9 @@
     <t>http://hadoop.apache.org/releases.html</t>
   </si>
   <si>
+    <t>In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean)</t>
+  </si>
+  <si>
     <t>hibernate</t>
   </si>
   <si>
@@ -1913,6 +1951,9 @@
     <t>http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final</t>
   </si>
   <si>
+    <t>Value Set to null:</t>
+  </si>
+  <si>
     <t>hsqldb</t>
   </si>
   <si>
@@ -1920,6 +1961,9 @@
   </si>
   <si>
     <t>http://hsqldb.org/</t>
+  </si>
+  <si>
+    <t>Value aconst_null</t>
   </si>
   <si>
     <t>jboss</t>
@@ -1971,6 +2015,9 @@
     <t>Due to its complicated nature, there are multiple places where SM is set to null. However, during the running of the main program, there is no such statement happened. Our dynamic analysis showed this fact.</t>
   </si>
   <si>
+    <t>Value aconst_null[1](1)</t>
+  </si>
+  <si>
     <t>jruby</t>
   </si>
   <si>
@@ -1980,6 +2027,9 @@
     <t>http://www.jruby.org/download</t>
   </si>
   <si>
+    <t>Value Variable is set at:</t>
+  </si>
+  <si>
     <t>lucene</t>
   </si>
   <si>
@@ -1996,6 +2046,9 @@
   </si>
   <si>
     <t>http://myfaces.apache.org/</t>
+  </si>
+  <si>
+    <t>This is the line to remove the SecurityManager.  This line only e</t>
   </si>
   <si>
     <t>nekohtml</t>
@@ -2553,7 +2606,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -2622,13 +2675,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H5" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J6" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N10" activeCellId="0" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2902,46 +2955,56 @@
       <c r="I8" s="0"/>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
+      <c r="M8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2949,97 +3012,112 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
+      <c r="M10" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
+      <c r="M11" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
+      <c r="M12" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
+      <c r="M13" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>88</v>
+        <v>95</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3047,30 +3125,33 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
+      <c r="M15" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -3081,30 +3162,33 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
+      <c r="M17" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -3115,13 +3199,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -3132,13 +3216,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -3149,13 +3233,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -3166,13 +3250,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -3183,13 +3267,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -3200,13 +3284,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -3217,13 +3301,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -3234,13 +3318,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -3251,22 +3335,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3274,13 +3358,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -3289,13 +3373,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -3304,13 +3388,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -3319,13 +3403,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -3334,13 +3418,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -3349,13 +3433,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -3364,13 +3448,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -3379,13 +3463,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -3394,13 +3478,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -3409,13 +3493,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -3424,13 +3508,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -3439,13 +3523,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -3454,13 +3538,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -3469,13 +3553,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -3484,13 +3568,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -3499,13 +3583,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -3514,13 +3598,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -3529,13 +3613,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -3544,13 +3628,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -3559,13 +3643,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -3574,13 +3658,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -3589,13 +3673,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -3604,13 +3688,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -3624,12 +3708,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the static analysis comments to JBoss
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="204">
   <si>
     <t>Index</t>
   </si>
@@ -1602,9 +1602,6 @@
     <t>http://download.eclipse.org/eclipse/downloads/</t>
   </si>
   <si>
-    <t>s if batik already set the SecurityManager.</t>
-  </si>
-  <si>
     <t>freemind</t>
   </si>
   <si>
@@ -1927,9 +1924,6 @@
     <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
   </si>
   <si>
-    <t>In line 176</t>
-  </si>
-  <si>
     <t>hadoop</t>
   </si>
   <si>
@@ -1939,9 +1933,6 @@
     <t>http://hadoop.apache.org/releases.html</t>
   </si>
   <si>
-    <t>In method org.apache.batik.util.ApplicationSecurityEnforcer.enforceSecurity(boolean)</t>
-  </si>
-  <si>
     <t>hibernate</t>
   </si>
   <si>
@@ -1951,9 +1942,6 @@
     <t>http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final</t>
   </si>
   <si>
-    <t>Value Set to null:</t>
-  </si>
-  <si>
     <t>hsqldb</t>
   </si>
   <si>
@@ -1961,9 +1949,6 @@
   </si>
   <si>
     <t>http://hsqldb.org/</t>
-  </si>
-  <si>
-    <t>Value aconst_null</t>
   </si>
   <si>
     <t>jboss</t>
@@ -2015,7 +2000,46 @@
     <t>Due to its complicated nature, there are multiple places where SM is set to null. However, during the running of the main program, there is no such statement happened. Our dynamic analysis showed this fact.</t>
   </si>
   <si>
-    <t>Value aconst_null[1](1)</t>
+    <t>Zack's Static Analysis Comments - 
+At EjbModule.java:[line 627] 
+In method org.jboss.ejb.EjbModule.destroyService() 
+Value Set to null:   
+Value invokeinterface 
+Value invokeinterface[185](5) 131 
+Value Variable is set at: 
+At EjbModule.java:[line 553]
+This is a false positive.
+-------------------------------------------------
+ At EjbModule.java:[line 871] 
+In method org.jboss.ejb.EjbModule.initializeContainer(Container, ConfigurationMetaData, BeanMetaData, int, DeploymentUnit) 
+Value Could be null or other value: org.jboss.security.AuthenticationManager
+This is also a false positive
+-------------------------------------------------
+At SecurityPolicy.java:[line 91] 
+In method org.jboss.system.server.security.SecurityPolicy.start() 
+Value Not null: java.lang.SecurityManager 
+Value aload_0 
+Value aload_0[42](1) 
+Value Variable is set at: 
+At SecurityPolicy.java:[line 90]
+Sets the SecurityManager if the SecurityManager field of the class is set.
+I've only seen this class even used in a test case and the line was commented out.  I don't think the program ever reaches this statement.
+--------------------------------------------------
+At SecurityPolicy.java:[line 97] 
+In method org.jboss.system.server.security.SecurityPolicy.stop() 
+Value Set to null:   
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:
+This nulls the SecurityManager. I've only seen this class even used in a test case and the line was commented out.  I don't think the program ever reaches this statement.
+--------------------------------------------------
+At QuartzServer.java:[line 264]
+In method org.quartz.impl.QuartzServer.main(String[]) 
+Value Not null: java.rmi.RMISecurityManager 
+Value new 
+Value new[187](3) 37 
+Value Variable is set at:
+@@@@@ Haven't found this file yet.  Lets see if the grep results turn up anything.</t>
   </si>
   <si>
     <t>jruby</t>
@@ -2027,9 +2051,6 @@
     <t>http://www.jruby.org/download</t>
   </si>
   <si>
-    <t>Value Variable is set at:</t>
-  </si>
-  <si>
     <t>lucene</t>
   </si>
   <si>
@@ -2046,9 +2067,6 @@
   </si>
   <si>
     <t>http://myfaces.apache.org/</t>
-  </si>
-  <si>
-    <t>This is the line to remove the SecurityManager.  This line only e</t>
   </si>
   <si>
     <t>nekohtml</t>
@@ -2606,7 +2624,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -2680,8 +2698,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J6" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N10" activeCellId="0" sqref="N10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H11" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2955,56 +2973,56 @@
       <c r="I8" s="0"/>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
-      <c r="M8" s="0" t="s">
-        <v>59</v>
-      </c>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
       <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="J9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="L9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="M9" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="N9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="O9" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3012,112 +3030,100 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="0"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="M10" s="1" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="0"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="M11" s="1" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="0"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="M12" s="1" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="0"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="M13" s="1" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3125,70 +3131,65 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="M15" s="1" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
+      <c r="M16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="M17" s="1" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -3199,13 +3200,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -3216,13 +3217,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -3233,13 +3234,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -3250,13 +3251,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -3267,13 +3268,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -3284,13 +3285,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -3301,13 +3302,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -3318,13 +3319,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -3335,22 +3336,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3358,13 +3359,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -3373,13 +3374,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -3388,13 +3389,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -3403,13 +3404,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -3418,13 +3419,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -3433,13 +3434,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -3448,13 +3449,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -3463,13 +3464,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -3478,13 +3479,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -3493,13 +3494,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -3508,13 +3509,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -3523,13 +3524,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -3538,13 +3539,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -3553,13 +3554,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -3568,13 +3569,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -3583,13 +3584,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -3598,13 +3599,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -3613,13 +3614,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -3628,13 +3629,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -3643,13 +3644,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -3658,13 +3659,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -3673,13 +3674,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -3688,13 +3689,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -3708,12 +3709,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the download website for JBoss
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -1957,7 +1957,7 @@
     <t>5.1.0.GA</t>
   </si>
   <si>
-    <t>http://www.jboss.org/downloads/</t>
+    <t>http://sourceforge.net/projects/jboss/files/JBoss/JBoss-5.1.0.GA/</t>
   </si>
   <si>
     <t>Location 1:
@@ -2624,7 +2624,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -2698,8 +2698,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H11" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B11" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3042,6 +3042,7 @@
       <c r="F10" s="0"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
+      <c r="M10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -3060,6 +3061,7 @@
       <c r="F11" s="0"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
+      <c r="M11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -3078,6 +3080,7 @@
       <c r="F12" s="0"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
+      <c r="M12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -3096,6 +3099,7 @@
       <c r="F13" s="0"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
+      <c r="M13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -3142,6 +3146,7 @@
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
+      <c r="M15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -3730,7 +3735,7 @@
     <hyperlink ref="D11" r:id="rId9" display="http://hadoop.apache.org/releases.html"/>
     <hyperlink ref="D12" r:id="rId10" display="http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final"/>
     <hyperlink ref="D13" r:id="rId11" display="http://hsqldb.org/"/>
-    <hyperlink ref="D14" r:id="rId12" display="http://www.jboss.org/downloads/"/>
+    <hyperlink ref="D14" r:id="rId12" display="http://sourceforge.net/projects/jboss/files/JBoss/JBoss-5.1.0.GA/"/>
     <hyperlink ref="D15" r:id="rId13" display="http://www.jruby.org/download"/>
     <hyperlink ref="D16" r:id="rId14" display="http://lucene.apache.org/"/>
     <hyperlink ref="D17" r:id="rId15" display="http://myfaces.apache.org/"/>

</xml_diff>

<commit_message>
Added the analysis for JBoss
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="207">
   <si>
     <t>Index</t>
   </si>
@@ -1912,7 +1912,7 @@
 This file instantiaates a scriptingSecurityManager with the policy dependent on how trusted the script is (for example, if the script is signed the policy allows more permissions. )  Then it sets the scriptingSecurityManager as the policy to implement in the FreeMindSecurityManager.  Once the script is executed, it removes the securityManager by calling the setFinalSecurityManger with the same arguments.  This means that the SecurityManager only has a policy when untrusted code is running (minimizing policy enforcment to the location it is needed), and thus changing dynamically.</t>
   </si>
   <si>
-    <t>Zack' General Comments – In the main program there is a SecurityManager set at the beginning which allows all permissions.  In a plugin, the current SecurityManager's policy is strengthened at then set back to allowing all permissions.</t>
+    <t>Zack' General Comments – In the main program there is a SecurityManager set at the beginning which allows all permissions.  In a plugin, the current SecurityManager's policy is strengthened at then set back to allowing all permissions. This application will not run if a SecurityManager is set before the program that requires pervents the SecurityManager from being changed.</t>
   </si>
   <si>
     <t>galleon</t>
@@ -1998,6 +1998,10 @@
   </si>
   <si>
     <t>Due to its complicated nature, there are multiple places where SM is set to null. However, during the running of the main program, there is no such statement happened. Our dynamic analysis showed this fact.</t>
+  </si>
+  <si>
+    <t>Zack's Dynamic Analysis Comments - 
+No output when running run.sh in the bin folder but that is what I expected from the static analysis</t>
   </si>
   <si>
     <t>Zack's Static Analysis Comments - 
@@ -2040,6 +2044,482 @@
 Value new[187](3) 37 
 Value Variable is set at:
 @@@@@ Haven't found this file yet.  Lets see if the grep results turn up anything.</t>
+  </si>
+  <si>
+    <t>Zack's Grep Comments - 
+./aspects/src/main/org/jboss/aspects/library/SecurityActions.java
+115:      if (System.getSecurityManager() == null)
+127:      if (System.getSecurityManager() == null)
+139:      if (System.getSecurityManager() == null)
+This class performs security restricted actions and so it checks to see if a SecurityManager is set before doing them and adjusts accordingly. 
+./testsuite/src/main/org/jboss/test/deployment/test/DeploymentServiceUnitTestCase.java
+572:    * the SecurityManager mbean for the messaging service. The mbean property
+595:      String name = "jboss.mq:service=SecurityManager";
+Updates an mbean of the messaging SecurityManager during a test case.
+./testsuite/src/main/org/jboss/test/web/test/WebIntegrationUnitTestCase.java
+217:      hdr = request.getResponseHeader("X-SubjectFilter-SubjectSecurityManager");
+218:      log.info("X-SubjectFilter-SubjectSecurityManager: "+hdr);
+219:      assertTrue("X-SubjectFilter-SubjectSecurityManager("+hdr+") is NOT null", hdr != null);
+This test seems to mke sure it can read the SecurityManager sent by html when working with another web application.
+./testsuite/src/main/org/jboss/test/web/test/CustomErrorsUnitTestCase.java
+42:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+This is just an import statment that wasn't used.
+./testsuite/src/main/org/jboss/test/web/test/FormAuthUnitTestCase.java
+39:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+235:      ObjectName name = new ObjectName("jboss.security:service=JaasSecurityManager");
+236:      JaasSecurityManagerServiceMBean secMgrService = (JaasSecurityManagerServiceMBean)
+237:         MBeanServerInvocationHandler.newProxyInstance(conn, name, JaasSecurityManagerServiceMBean.class, false);
+This is a test to insure that the security restrictions placed by the 
+./testsuite/src/main/org/jboss/test/web/servlets/SubjectFilter.java
+36:import org.jboss.security.SubjectSecurityManager;
+75:      SubjectSecurityManager mgr = (SubjectSecurityManager) ctx.lookup("java:comp/env/security/securityMgr");
+77:      httpResponse.addHeader("X-SubjectFilter-SubjectSecurityManager", s0.toString());
+test for transmitting the current SecurityManager which is really an authenticator and not the same thing as a System.lang.SecurityManager
+./testsuite/src/main/org/jboss/test/web/security/JASPISecurityFilter.java
+113:         //with the JASPISecurityManager Service
+115:         ObjectName oname = new ObjectName("jboss.security:service=JASPISecurityManager");
+Creates an authentication manager for the test
+./testsuite/src/main/org/jboss/test/securitymgr/ejb/IOStatelessSessionBean.java
+26:import java.lang.SecurityManager;
+131:      SecurityManager secmgr = new SecurityManager()
+137:      System.setSecurityManager(secmgr);
+Tests for running JBoss with an outside set SecurityManager
+./testsuite/src/main/org/jboss/test/txtimer/test/EntityBeanTestCase.java
+113:      String defaultPrincipal = (String) server.getAttribute(new ObjectName("jboss.security:service=JaasSecurityManager"), "DefaultUnauthenticatedPrincipal");
+test that gets an atribute from the authentication manager
+./testsuite/src/main/org/jboss/test/classloader/leak/clstore/ClassLoaderTracker.java
+28:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+35:   private JaasSecurityManagerServiceMBean securityManagerService;
+67:   public JaasSecurityManagerServiceMBean getSecurityManagerService()
+72:   public void setSecurityManagerService(JaasSecurityManagerServiceMBean securityManagerService)
+Used in a test to check the current Authentication manager and the current class loader.
+./testsuite/src/main/org/jboss/test/classloader/leak/clstore/ClassLoaderTrackerMBean.java
+26:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+41:   public JaasSecurityManagerServiceMBean getSecurityManagerService();
+43:   public void setSecurityManagerService(JaasSecurityManagerServiceMBean svc);
+./testsuite/src/main/org/jboss/test/bankiiop/test/BankStressTestCase.java
+489:      if (System.getSecurityManager() == null) 
+490:         System.setSecurityManager(new java.rmi.RMISecurityManager());
+Sets a securitymanager for the test
+./testsuite/src/main/org/jboss/test/security/test/DeepCopySubjectUnitTestCase.java
+179:    * Test the Deep Copy of Subjects by the JaasSecurityManager
+197:    * Turn the deep copy of subjects on the JaasSecurityManagerService
+205:      this.getServer().invoke(new ObjectName("jboss.security:service=JaasSecurityManager"),
+test deep copies of the authentication manager
+./testsuite/src/main/org/jboss/test/security/test/EJBSpecUnitTestCase.java
+47:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+101:      ObjectName secMgrName = new ObjectName("jboss.security:service=JaasSecurityManager");
+102:      JaasSecurityManagerServiceMBean secMgr = (JaasSecurityManagerServiceMBean) MBeanServerInvocationHandler
+103:            .newProxyInstance(conn, secMgrName, JaasSecurityManagerServiceMBean.class, false);
+874:      ObjectName secMgrName = new ObjectName("jboss.security:service=JaasSecurityManager");
+875:      JaasSecurityManagerServiceMBean secMgr = (JaasSecurityManagerServiceMBean) MBeanServerInvocationHandler
+876:            .newProxyInstance(conn, secMgrName, JaasSecurityManagerServiceMBean.class, false);
+tests using the authentication manager
+./testsuite/src/main/org/jboss/test/security/test/SecurityMgrStressTestCase.java
+48:import org.jboss.security.plugins.JaasSecurityManager;
+51:/** Stress testing of the JaasSecurityManager
+85:      JaasSecurityManager secMgr = new JaasSecurityManager("testIdentity", new SecurityAssociationHandler());
+177:      JaasSecurityManager secMgr;
+186:      AuthTester(JaasSecurityManager secMgr, AuthorizationManager am, int iterations, int id)
+tests using the authentication manager
+./testsuite/src/main/org/jboss/test/security/test/JaasSecurityManagerUnitTestCase.java
+31:import org.jboss.security.plugins.JaasSecurityManager;
+39:/** Tests of the JaasSecurityManager implementation.
+44:public class JaasSecurityManagerUnitTestCase
+47:   static Logger log = Logger.getLogger(JaasSecurityManagerUnitTestCase.class);
+49:   public JaasSecurityManagerUnitTestCase(String name)
+72:      JaasSecurityManager sm = new JaasSecurityManager("testStringCharArrayCredential", handler);
+93:      JaasSecurityManager sm = new JaasSecurityManager("testStringCharArrayCredential", handler);
+tests using the authenticaion manager
+./testsuite/src/main/org/jboss/test/security/servlets/DeepCopySubjectServlet.java
+48:import org.jboss.security.SubjectSecurityManager;
+88:         SubjectSecurityManager manager = (SubjectSecurityManager)context.lookup("java:comp/env/security/securityMgr");M
+108:   private Subject getAuthenticatedSubject(SubjectSecurityManager mgr) 
+199:      ObjectName on = new ObjectName("jboss.security:service=JaasSecurityManager");
+test using the authentiation manager
+./testsuite/src/main/org/jboss/test/security/ejb/EntityBeanImpl.java
+109:           log.debug("Found SecurityManager: "+securityMgr);
+test that looks up the current security domain
+./testsuite/src/main/org/jboss/test/security/ejb/Cmp2Bean.java
+100:         log.debug("Found SecurityManager: " + securityMgr);
+test that looks up the current security domain
+./testsuite/src/main/org/jboss/test/jmx/test/DeployXMBeanUnitTestCase.java
+201:         ObjectName defaultSecMgr = new ObjectName("jboss.security:service=JaasSecurityManager");
+204:         assertTrue("SecMgr == jboss.security:service=JaasSecurityManager", secMgr.equals(defaultSecMgr));
+298:         ObjectName defaultSecMgr = new ObjectName("jboss.security:service=JaasSecurityManager");
+301:         assertTrue("SecMgr == jboss.security:service=JaasSecurityManager", secMgr.equals(defaultSecMgr));
+test using the authentiation manager
+./testsuite/src/main/org/jboss/test/jmx/interceptors/JNDISecurity.java
+36:import org.jboss.security.SubjectSecurityManager;
+56:   private SubjectSecurityManager authMgr;
+69:      this.authMgr = (SubjectSecurityManager) ctx.lookup(securityDomain);
+test using the authentiation manager
+./tomcat/src/main/org/jboss/web/tomcat/service/DeployerConfig.java
+26:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+128:   private JaasSecurityManagerServiceMBean secMgrService;  
+335:   public JaasSecurityManagerServiceMBean getSecurityManagerService()
+339:   public void setSecurityManagerService(JaasSecurityManagerServiceMBean mgr)
+test using the authentiation manager
+./tomcat/src/main/org/jboss/web/tomcat/service/deployers/DeployerConfig.java
+27:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+118:   private JaasSecurityManagerServiceMBean secMgrService;
+275:   public JaasSecurityManagerServiceMBean getSecurityManagerService()
+280:   public void setSecurityManagerService(JaasSecurityManagerServiceMBean mgr)
+test using the authentiation manager
+./tomcat/src/main/org/jboss/web/tomcat/service/deployers/TomcatDeployerMBean.java
+24:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+129:    * Set the SecurityManagerService binding. This is used to flush any associated authentication cache on session
+132:    * @param mgr the JaasSecurityManagerServiceMBean
+134:   public void setSecurityManagerService(JaasSecurityManagerServiceMBean mgr);
+test using the authentiation manager
+./tomcat/src/main/org/jboss/web/tomcat/service/deployers/TomcatDeployer.java
+38:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+132:   private JaasSecurityManagerServiceMBean secMgrService;
+310:   public void setSecurityManagerService(JaasSecurityManagerServiceMBean mgr)
+439:      config.setSecurityManagerService(secMgrService);
+test using the authentiation manager
+./tomcat/src/main/org/jboss/web/tomcat/service/deployers/TomcatDeployment.java
+374:      SecurityAssociationValve valve = new SecurityAssociationValve(metaData, config.getSecurityManagerService());
+Gets a value from the authentication manager
+./tomcat/src/main/org/jboss/web/tomcat/service/deployers/TomcatService.java
+52:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+584:   public void setSecurityManagerService(JaasSecurityManagerServiceMBean mgr)
+587:         tomcatDeployer.setSecurityManagerService(mgr);
+Sets an authentication manager
+./tomcat/src/main/org/jboss/web/tomcat/security/JBossSecurityMgrRealm.java
+43: * @see org.jboss.security.SubjectSecurityManager
+comment for extra information. This class is blank
+./tomcat/src/main/org/jboss/web/tomcat/security/SecurityAssociationValve.java
+44:import org.jboss.security.plugins.JaasSecurityManagerServiceMBean;
+72:   private JaasSecurityManagerServiceMBean secMgrService;
+76:      JaasSecurityManagerServiceMBean secMgrService)
+uses an authentication manager
+./tomcat/src/main/org/jboss/web/tomcat/security/JBossWebRealm.java
+62:import org.jboss.security.SubjectSecurityManager;
+198:         SubjectSecurityManager securityMgr = getSubjectSecurityManager("authenticate(X509Certificate[] certs)");
+289:         SubjectSecurityManager securityMgr = getSubjectSecurityManager("authenticate( digest related)");
+378:         SubjectSecurityManager securityMgr = getSubjectSecurityManager("authenticate(username,cred)");
+838:    * Get the JBoss SubjectSecurityManager (AuthenticationManager)
+842:   private SubjectSecurityManager getSubjectSecurityManager(String wherefrom)
+844:      SubjectSecurityManager subjectSecurityManager = null;
+856:           subjectSecurityManager = (SubjectSecurityManager) securityCtx.lookup("securityMgr");
+861:      if(subjectSecurityManager == null &amp;&amp; securityManagerFallback)
+867:            subjectSecurityManager = (SubjectSecurityManager)ic.lookup(str);
+873:      return subjectSecurityManager;
+Uses an authentication manager
+./tomcat/src/main/org/jboss/web/tomcat/security/JBossExtendedSecurityMgrRealm.java
+78:         this.authenticationManagerService = new ObjectName("jboss.security:service=JASPISecurityManager");
+270:            "getSecurityManager", 
+uses an authentication manager
+./tomcat/src/main/org/jboss/web/tomcat/security/SecurityFlushSessionListener.java
+41:import org.jboss.security.SubjectSecurityManager;
+103:      ObjectName on = new ObjectName("jboss.security:service=JaasSecurityManager");
+157:      SubjectSecurityManager mgr = null;
+160:         mgr = getSecurityManagerService(); 
+163:         log.debug("Obtaining SecurityManagerService failed::",e);
+189:   private SubjectSecurityManager getSecurityManagerService() throws Exception
+191:      //Get the SecurityManagerService from JNDI
+193:      return (SubjectSecurityManager) ctx.lookup("java:comp/env/security/securityMgr");
+200:    * @param on ObjectName of the JaasSecurityManagerService
+uses an authentication manager
+./varia/src/main/org/jboss/services/binding/SystemPropertyBinder.java
+58:         if (System.getSecurityManager() == null)
+84:         if (System.getSecurityManager() == null)
+written to work if a securitymanager is set, uses the permissions of this class and not the caller
+./varia/src/main/org/jboss/security/srp/SRPClientSession.java
+281:      SecurityManager sm = System.getSecurityManager();
+performs a permission check if a SecurityManager is set
+./varia/src/main/org/jboss/security/srp/SRPServerSession.java
+233:      SecurityManager sm = System.getSecurityManager();
+performs a permission check if a SecurityManager is set
+./system-jmx/src/main/org/jboss/system/SecurityActions.java
+46:      if (System.getSecurityManager() == null)
+64:      if (System.getSecurityManager() == null)
+Uses the current classes permissions instead of a caller if a SecurityManager is set
+./system-jmx/src/main/org/jboss/system/metadata/ServiceMetaDataParser.java
+757:         SecurityManager manager = System.getSecurityManager();
+Uses the current classes permissions instead of a caller if a SecurityManager is set
+./system-jmx/src/main/org/jboss/system/deployers/managed/SecurityActions.java
+41:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+checks if a SecurityManager is set and returns the result.
+./system-jmx/src/tests/org/jboss/test/system/deployers/test/ServiceUnitNameTestCase.java
+80:      SecurityManager sm = suspendSecurity();
+I don't completely understand what is going on here.  Based on the method names it looks like the test was written to remove the SecurityManager for the test and then reset it at the end.  However, the suspendSecurity method is not definned in the file so I'm not sure where it is and thus what is happening exactly.
+./server/src/main/org/jboss/web/deployers/AbstractWarDeployment.java
+806:    * NullSecurityManager instance which simply allows all access.
+used in reference to an authentication manager
+./server/src/main/org/jboss/invocation/jrmp/server/JRMPInvoker.java
+711:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+850:         SecurityManager sm = System.getSecurityManager();
+First line just returns if a SecurityManager is set.  The second one uses the priviledges of the class instead of the caller if a SecurityManager is defined.
+./server/src/main/org/jboss/invocation/pooled/server/PooledInvoker.java
+891:         SecurityManager sm = System.getSecurityManager();
+uses the priviledges of the class instead of the caller if a SecurityManager is defined.
+./server/src/main/org/jboss/invocation/SecurityActions.java
+41:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+returns if a SecurityManager is set
+./server/src/main/org/jboss/invocation/MarshalledInvocation.java
+137:      if( System.getSecurityManager() != null )
+192:      if( System.getSecurityManager() != null )
+241:      if( System.getSecurityManager() != null )
+uses the priviledges of the class instead of the caller if a SecurityManager is defined.
+./server/src/main/org/jboss/invocation/local/LocalInvoker.java
+164:         SecurityManager sm = System.getSecurityManager();
+195:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+first one uses the priviledges of the class instead of the caller if a SecurityManager is defined.  Second just returns if a SecurityManager is currently defined for the system.
+./server/src/main/org/jboss/logging/SysPropertyActions.java
+85:      if( System.getSecurityManager() == null )
+95:      if( System.getSecurityManager() == null )
+uses the priviledges of the class instead of the caller if a SecurityManager is defined.
+./server/src/main/org/jboss/proxy/SecurityActions.java
+46:         return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+returns if a SecurityManager is currently set.
+./server/src/main/org/jboss/proxy/ejb/handle/StatefulHandleImpl.java
+274:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+returns if a SecurityManager is currently set.
+./server/src/main/org/jboss/proxy/ejb/ProxyFactory.java
+393:         if(container.getSecurityManager() != null)
+395:            String secDomain = container.getSecurityManager().getSecurityDomain();
+437:            if(container.getSecurityManager() != null)
+439:               String secDomain = container.getSecurityManager().getSecurityDomain();
+579:      if(container.getSecurityManager() != null)
+581:         String secDomain = container.getSecurityManager().getSecurityDomain();
+637:         if(container.getSecurityManager() != null)
+639:            String secDomain = container.getSecurityManager().getSecurityDomain();
+uses the authentication manager
+./server/src/main/org/jboss/ejb/Container.java
+197:   /** This is the SecurityManager */
+325:   public void setSecurityManager(AuthenticationManager sm)
+330:   public AuthenticationManager getSecurityManager()
+1621:         SecurityManager sm = System.getSecurityManager();
+Top three lines reference the authentication manager.  The bottom one uses different priviledges if a SecurityManager is set.
+./server/src/main/org/jboss/ejb/txtimer/SecurityActions.java
+200:      if(System.getSecurityManager() == null)
+212:      if(System.getSecurityManager() == null)
+228:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+Top two use different priviledges if a SecurityManager is set.  Bottom one checks if a SecurityManager is set.
+./server/src/main/org/jboss/ejb/plugins/SecurityProxyInterceptor.java
+80:         securityManager = container.getSecurityManager();
+refers to authentication manager
+./server/src/main/org/jboss/ejb/plugins/SecurityInterceptor.java
+160:         securityManager = container.getSecurityManager();
+193:         securityManager = container.getSecurityManager();
+refers to authentication manager
+./server/src/main/org/jboss/ejb/plugins/SecurityActions.java
+218:      if(System.getSecurityManager() == null)
+230:      if(System.getSecurityManager() == null)
+242:      if(System.getSecurityManager() == null)
+256:      if(System.getSecurityManager() == null)
+272:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+Runs with different permissions if a SecurityManager is set.  Last one is check if SecurityManager is set
+./server/src/main/org/jboss/ejb/plugins/local/BaseLocalProxyFactory.java
+485:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+527:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+614:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+Checks if SecurityManager is set.
+./server/src/main/org/jboss/ejb/plugins/StatefulSessionInstanceInterceptor.java
+237:            AuthenticationManager am = container.getSecurityManager();
+reference to authentication manager.
+./server/src/main/org/jboss/ejb/plugins/cmp/jdbc/bridge/JDBCCMRFieldBridge.java
+2338:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+Check if SecurityManager is set.
+./server/src/main/org/jboss/ejb/plugins/cmp/jdbc/bridge/SecurityActions.java
+210:      if(System.getSecurityManager() == null)
+222:      if(System.getSecurityManager() == null)
+234:      if(System.getSecurityManager() == null)
+248:      if(System.getSecurityManager() == null)
+264:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+Runs with different permissions if a SecurityManager is set.  Last one is check if SecurityManager is set
+./server/src/main/org/jboss/ejb/plugins/cmp/jdbc/JDBCAbstractCreateCommand.java
+79:      securityManager = manager.getContainer().getSecurityManager();
+reference to authentication manager
+./server/src/main/org/jboss/ejb/plugins/cmp/jdbc/CascadeDeleteStrategy.java
+351:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+checks if securityManager is set
+./server/src/main/org/jboss/ejb/plugins/cmp/jdbc/TCLAction.java
+37:         return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+checks if securityManager is set
+./server/src/main/org/jboss/ejb/plugins/cmp/jdbc2/bridge/JDBCCMRFieldBridge2.java
+1736:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+checks if securityManager is set
+./server/src/main/org/jboss/ejb/plugins/RunAsSecurityInterceptor.java
+84:         securityManager = container.getSecurityManager();
+reference to authenticatton manager
+./server/src/main/org/jboss/ejb/plugins/security/PreSecurityInterceptor.java
+60:         AuthenticationManager am = container.getSecurityManager();
+reference to authenticaiton manager
+./server/src/main/org/jboss/ejb/EjbModule.java
+627:         con.setSecurityManager(null);
+866:            Object securityMgr = sdc.getSecurityManager();
+871:            container.setSecurityManager(ejbS);
+1051:      boolean hasSecurityDomain = con.getSecurityManager() != null;
+references to authentication manager
+./server/src/main/org/jboss/ejb/SecurityActions.java
+134:      if( System.getSecurityManager() == null )
+183:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+233:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+391:      if(System.getSecurityManager() == null) 
+handles permissions differently if SecurityManager is set.  Also checks if one is set.
+./server/src/main/org/jboss/ejb/EnterpriseContext.java
+213:      if( con.getSecurityManager() != null )
+reference to authentication manager
+./server/src/main/org/jboss/jmx/connector/invoker/SecurityActions.java
+173:      if(System.getSecurityManager() == null)
+184:      if(System.getSecurityManager() == null)
+handles permissions differently if SecurityManager is set.
+./server/src/main/org/jboss/jmx/connector/invoker/AuthenticationInterceptor.java
+34:import org.jboss.security.SubjectSecurityManager;
+49:   private SubjectSecurityManager securityMgr;
+119:         securityMgr = (SubjectSecurityManager) ctx.lookup(securityDomain);
+reference to authentication manager
+./mbeans/src/main/org/jboss/mx/server/TCLAction.java
+37:         return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+checks if SecurityManager is set
+./connector/src/main/org/jboss/resource/connectionmanager/ConnectionValidator.java
+122:      SecurityManager sm = System.getSecurityManager();
+handles permissions differently if SecurityManager is set.
+./connector/src/main/org/jboss/resource/connectionmanager/IdleRemover.java
+138:      SecurityManager sm = System.getSecurityManager();
+handles permissions differently if SecurityManager is set.
+./connector/src/main/org/jboss/resource/connectionmanager/BaseConnectionManager2.java
+93:    * JaasSecurityManagerService.
+109:   protected ObjectName jaasSecurityManagerService;
+222:   public ObjectName getJaasSecurityManagerService()
+224:      return this.jaasSecurityManagerService; 
+230:   public void setJaasSecurityManagerService(final ObjectName jaasSecurityManagerService)
+232:      this.jaasSecurityManagerService = jaasSecurityManagerService;
+360:       * if (jaasSecurityManagerService != null &amp;&amp; securityDomainJndiName != null)
+361:         server.invoke(jaasSecurityManagerService, "flushAuthenticationCache", new Object[] { securityDomainJndiName }, new String[] { String.class.getName() });
+reference to authentication manager
+./connector/src/main/org/jboss/resource/connectionmanager/BaseConnectionManager2MBean.java
+99:    * Get the JaasSecurityManagerService value.
+101:    * @return the JaasSecurityManagerService value.
+104:   ObjectName getJaasSecurityManagerService();
+107:    * Set the JaasSecurityManagerService value.
+109:    * @param jaasSecurityManagerService The new JaasSecurityManagerService value.
+112:   void setJaasSecurityManagerService(ObjectName jaasSecurityManagerService); 
+reference to authentication manager
+./connector/src/main/org/jboss/resource/deployers/builder/ConnectionManagerBuilder.java
+48:   private static final String JAAS_JMX = "jboss.security:service=JaasSecurityManager";
+152:      attribute = buildDependencyAttribute("JaasSecurityManagerService", jaasJMXName);
+reference to authentication manager
+./system/src/main/org/jboss/system/server/profileservice/persistence/ManagedObjectRecreationHelper.java
+114:         if (System.getSecurityManager() == null)
+handles permissions differently if a SecurityManager is set
+./system/src/main/org/jboss/system/server/profileservice/repository/AbstractProfileLifeCycleAction.java
+82:      SecurityManager sm = System.getSecurityManager();
+handles permissions differently if a SecurityManager is set
+./system/src/main/org/jboss/system/server/security/SecurityPolicy.java
+38:   private SecurityManager securityManager;
+48:   public SecurityManager getSecurityManager()
+58:   public void setSecurityManager(SecurityManager securityManager)
+91:         System.setSecurityManager(securityManager);
+97:         System.setSecurityManager(null);
+This class interacts with the system SecurityManager but I only see it called with test cases
+./system/src/main/org/jboss/deployers/plugins/managed/SecurityActions.java
+41:            return System.getSecurityManager() == null ? NON_PRIVILEGED : PRIVILEGED;
+checks if securityManager set
+./messaging/src/main/org/jboss/jms/server/jbosssx/JBossASSecurityMetadataStore.java
+47: * authorization to a JaasSecurityManager.
+93:   // SecurityManager implementation --------------------------------
+reference to authenticaiton manager
+./messaging/src/main/org/jboss/jms/server/jbosssx/SecurityActions.java
+115:     if(System.getSecurityManager() == null)
+handles permissions differently if a securityManager is set.
+./messaging/src/main/org/jboss/mq/server/jmx/Topic.java
+248:    * @see org.jboss.mq.server.jmx.TopicMBean#setSecurityManager(javax.management.ObjectName)
+250:   public void setSecurityManager(ObjectName arg0)
+method is empty
+./messaging/src/main/org/jboss/mq/server/jmx/TopicMBean.java
+82:   public abstract void setSecurityManager(ObjectName arg0);
+this is an interface definition
+./messaging/src/main/org/jboss/mq/server/jmx/Queue.java
+278:	public void setSecurityManager(ObjectName arg0) {
+method is empty
+./messaging/src/main/org/jboss/mq/server/jmx/QueueMBean.java
+67:   public void setSecurityManager(ObjectName arg0);
+interface definition
+./cluster/src/main/org/jboss/ha/jndi/DetachedHANamingService.java
+672:            if (System.getSecurityManager() == null)
+handles permissions differently if securitymanager is set
+./security/src/main/org/jboss/security/plugins/SecurityDomainContext.java
+31:import org.jboss.security.SubjectSecurityManager;
+101:      if( securityMgr instanceof SubjectSecurityManager )
+103:         subject = ((SubjectSecurityManager)securityMgr).getActiveSubject();
+107:   public AuthenticationManager getSecurityManager()
+reference to authentication manager
+./security/src/main/org/jboss/security/plugins/SecurityManagerMBean.java
+35:public interface SecurityManagerMBean
+Name of interface - used with the authentication manager
+./security/src/main/org/jboss/security/plugins/JaasSecurityManager.java
+36:import org.jboss.security.SubjectSecurityManager;
+38:import org.jboss.security.plugins.auth.JaasSecurityManagerBase;
+42:/** The JaasSecurityManager is responsible both for authenticating credentials
+57:public class JaasSecurityManager extends ServiceMBeanSupport
+58:   implements SubjectSecurityManager, RealmMapping
+60:   private JaasSecurityManagerBase delegate = null;
+62:   /** Creates a default JaasSecurityManager for with a securityDomain
+65:   public JaasSecurityManager()
+69:   /** Creates a JaasSecurityManager for with a securityDomain
+76:   public JaasSecurityManager(String securityDomain, CallbackHandler handler)
+78:      delegate = new JaasSecurityManagerBase(securityDomain,handler); 
+119:    property shared across all JaasSecurityManager instances.
+references to the authentication manager
+./security/src/main/org/jboss/security/plugins/JaasSecurityManagerService.java
+73: * This is a JMX service which manages JAAS based SecurityManagers.
+74: * JAAS SecurityManagers are responsible for validating credentials
+76: * org.jboss.security.plugins.JaasSecurityManager implementation but
+79: * @see JaasSecurityManager
+80: * @see org.jboss.security.SubjectSecurityManager
+88:public class JaasSecurityManagerService
+90:   implements JaasSecurityManagerServiceMBean
+97:   private static String securityMgrClassName = "org.jboss.security.plugins.JaasSecurityManager";
+99:   private static Class securityMgrClass = JaasSecurityManager.class;
+131:      log = Logger.getLogger(JaasSecurityManagerService.class);
+139:   public JaasSecurityManagerService()
+152:   public String getSecurityManagerClassName()
+156:   public void setSecurityManagerClassName(String className)
+183:      return JaasSecurityManagerService.callbackHandlerClassName;
+241:    * @see JaasSecurityManagerServiceMBean#getDeepCopySubjectMode()
+249:    * @see JaasSecurityManagerServiceMBean#getDeepCopySubjectMode() 
+353:// Begin SecurityManagerMBean interface methods
+360:         isValid = sdc.getSecurityManager().isValid(principal, credential, null);
+393:          boolean isValid = sdc.getSecurityManager().isValid(principal, credential, subject);
+398:                   sdc.getSecurityManager().getSecurityDomain());
+418:          boolean isValid = sdc.getSecurityManager().isValid(principal, credential, subject);
+423:                  sdc.getSecurityManager().getSecurityDomain() );
+434:// End SecurityManagerMBean interface methods
+484:      log.debug("SecurityMgrClass="+JaasSecurityManagerService.securityMgrClass);
+485:      log.debug("CallbackHandlerClass="+JaasSecurityManagerService.callbackHandlerClass);
+661:    * @see JaasSecurityManagerServiceMBean#getJCAInformation()
+references to the authentication manager
+./security/src/main/org/jboss/security/plugins/JaasSecurityManagerServiceMBean.java
+33: * The management interface for the JaasSecurityManagerService mbean.
+38:public interface JaasSecurityManagerServiceMBean
+39:   extends ServiceMBean, SecurityManagerMBean
+41:   ObjectName OBJECT_NAME = ObjectNameFactory.create("jboss.security:service=JaasSecurityManager");
+71:   String getSecurityManagerClassName();
+81:   void setSecurityManagerClassName(String className)
+references to authentication manager
+./security/src/main/org/jboss/security/plugins/JaasSecurityDomain.java
+63: * The JaasSecurityDomain is an extension of JaasSecurityManager that addes the notion of a KeyStore, and JSSE
+109:public class JaasSecurityDomain extends JaasSecurityManager implements SecurityDomain, JaasSecurityDomainMBean
+149:   private ObjectName managerServiceName = JaasSecurityManagerServiceMBean.OBJECT_NAME;
+491:      SecurityManager sm = System.getSecurityManager();
+515:      SecurityManager sm = System.getSecurityManager();
+581:      // Only register with the JaasSecurityManagerService if its defined
+585:          * Register with the JaasSecurityManagerServiceMBean. This allows this JaasSecurityDomain to function as the
+Does 2 extra permission checks if SecurityManagers are in use.  Rest is references to authentication manager.
+./security/src/main/org/jboss/security/integration/JNDIContextEstablishment.java
+37: *  to provide the SubjectSecurityManager implementation
+comment about authetication manager
+./security/src/main/org/jboss/security/integration/JNDIBasedSecurityManagement.java
+75:   protected String authenticationMgrClass = "org.jboss.security.plugins.JaasSecurityManager";
+413:      SecurityManager sm = System.getSecurityManager();
+first is authentication manager. second is an extra permisson check if a SecurityManager is set.</t>
+  </si>
+  <si>
+    <t>Zack' General Comments – JBoss mainly interacts with the authentication manager (which it calls a security manager) and not the system security manager.  The only place I saw that could set the securitymanager in the code was only referenced by a test case.  This means that the main application never references it.  I get the feeling that JBoss was written to allow the user to set a SecurityManager before running.  However, program doesn't work with the a default SecurityManager set so it would require policy tweaking.</t>
   </si>
   <si>
     <t>jruby</t>
@@ -2696,10 +3176,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B11" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M5" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3024,6 +3504,7 @@
       <c r="O9" s="9" t="s">
         <v>72</v>
       </c>
+      <c r="P9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -3126,8 +3607,17 @@
       <c r="H14" s="5" t="s">
         <v>90</v>
       </c>
+      <c r="L14" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="M14" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3135,13 +3625,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -3153,13 +3643,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -3171,13 +3661,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -3188,13 +3678,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -3205,13 +3695,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
@@ -3222,13 +3712,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -3239,13 +3729,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -3256,13 +3746,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -3273,13 +3763,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -3290,13 +3780,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24" s="5"/>
@@ -3307,13 +3797,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25" s="5"/>
@@ -3324,13 +3814,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -3341,22 +3831,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3364,13 +3854,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -3379,13 +3869,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -3394,13 +3884,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -3409,13 +3899,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -3424,13 +3914,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -3439,13 +3929,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -3454,13 +3944,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -3469,13 +3959,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -3484,13 +3974,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -3499,13 +3989,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -3514,13 +4004,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -3529,13 +4019,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -3544,13 +4034,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -3559,13 +4049,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -3574,13 +4064,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -3589,13 +4079,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -3604,13 +4094,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -3619,13 +4109,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -3634,13 +4124,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -3649,13 +4139,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -3664,13 +4154,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -3679,13 +4169,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -3694,13 +4184,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -3714,12 +4204,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Distribute projects into categories
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\2014 SUMMER\Michael\ProjectsProfiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="519" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="519"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -2866,11 +2870,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00E+00"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -2878,21 +2878,6 @@
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2923,7 +2908,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
@@ -2931,7 +2916,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
@@ -2939,7 +2924,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
@@ -2959,8 +2944,30 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2979,134 +2986,110 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="5">
+    <cellStyle name="TableStyleLight1" xfId="4"/>
+    <cellStyle name="差" xfId="1" builtinId="27"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8"/>
+    <cellStyle name="好" xfId="2" builtinId="26"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -3165,36 +3148,312 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:AMK54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M5" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" activeCellId="10" sqref="B4 B9 B10 B20 B21 B22 B23 B24 B25 B28 B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.79342723004695"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.6995305164319"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.3004694835681"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="63.0046948356808"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="58"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.5023474178404"/>
-    <col collapsed="false" hidden="false" max="18" min="9" style="1" width="22.6995305164319"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="8.79342723004695"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="35.6640625" style="1"/>
+    <col min="3" max="3" width="37.33203125" style="1"/>
+    <col min="4" max="4" width="63" style="1"/>
+    <col min="5" max="7" width="58" style="1"/>
+    <col min="8" max="8" width="32.44140625" style="1"/>
+    <col min="9" max="18" width="22.6640625" style="1"/>
+    <col min="19" max="1025" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:16" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3229,11 +3488,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:16" s="3" customFormat="1" ht="75.599999999999994" customHeight="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -3264,14 +3523,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="7">
         <v>1.7</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -3298,16 +3557,16 @@
       <c r="K3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="0"/>
-      <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
-      <c r="O3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -3317,19 +3576,19 @@
         <v>32</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="0"/>
+      <c r="F4"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="0"/>
-      <c r="J4" s="0"/>
-      <c r="K4" s="0"/>
-      <c r="L4" s="0"/>
-      <c r="M4" s="0"/>
-      <c r="N4" s="0"/>
-      <c r="O4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3342,22 +3601,22 @@
         <v>35</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="0"/>
+      <c r="F5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="0"/>
-      <c r="J5" s="0"/>
-      <c r="K5" s="0"/>
-      <c r="L5" s="0"/>
-      <c r="M5" s="0"/>
-      <c r="N5" s="0"/>
-      <c r="O5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="17" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -3387,13 +3646,13 @@
       <c r="K6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="0"/>
-      <c r="M6" s="0"/>
-      <c r="N6" s="0"/>
-      <c r="O6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -3417,9 +3676,9 @@
       <c r="H7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
-      <c r="K7" s="0"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
       <c r="L7" s="9" t="s">
         <v>52</v>
       </c>
@@ -3433,11 +3692,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="17" t="s">
         <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -3447,22 +3706,22 @@
         <v>58</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="0"/>
+      <c r="F8"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="0"/>
-      <c r="J8" s="0"/>
-      <c r="K8" s="0"/>
-      <c r="L8" s="0"/>
-      <c r="M8" s="0"/>
-      <c r="N8" s="0"/>
-      <c r="O8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="18" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3504,13 +3763,13 @@
       <c r="O9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="P9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="18" t="s">
         <v>73</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -3520,13 +3779,13 @@
         <v>75</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="0"/>
+      <c r="F10"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="M10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -3539,13 +3798,13 @@
         <v>78</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="0"/>
+      <c r="F11"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="M11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -3558,13 +3817,13 @@
         <v>81</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="0"/>
+      <c r="F12"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="M12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3577,16 +3836,16 @@
         <v>84</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="0"/>
+      <c r="F13"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="M13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="17" t="s">
         <v>85</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -3620,8 +3879,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -3636,10 +3895,10 @@
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="M15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:16" ht="75.599999999999994" customHeight="1">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -3654,10 +3913,10 @@
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="M16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3673,8 +3932,8 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -3690,11 +3949,11 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="17" t="s">
         <v>107</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -3707,11 +3966,11 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="18" t="s">
         <v>110</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -3724,11 +3983,11 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="18" t="s">
         <v>113</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -3741,11 +4000,11 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="18" t="s">
         <v>116</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -3758,11 +4017,11 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="18" t="s">
         <v>119</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -3775,11 +4034,11 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="18" t="s">
         <v>122</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -3792,11 +4051,11 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="18" t="s">
         <v>125</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -3809,8 +4068,8 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -3826,11 +4085,11 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="17" t="s">
         <v>131</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -3849,14 +4108,14 @@
         <v>136</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="7">
         <v>3.6</v>
       </c>
       <c r="D28" s="8" t="s">
@@ -3864,8 +4123,8 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -3879,11 +4138,11 @@
       </c>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="18" t="s">
         <v>142</v>
       </c>
       <c r="C30" s="9" t="s">
@@ -3894,8 +4153,8 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:8" ht="75.599999999999994" customHeight="1">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -3909,8 +4168,8 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:8" ht="43.2">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -3924,8 +4183,8 @@
       </c>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+    <row r="33" spans="1:5" ht="15">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
@@ -3939,8 +4198,8 @@
       </c>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+    <row r="34" spans="1:5" ht="43.2">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
@@ -3954,8 +4213,8 @@
       </c>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+    <row r="35" spans="1:5" ht="43.2">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
@@ -3969,8 +4228,8 @@
       </c>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+    <row r="36" spans="1:5" ht="57.6">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -3984,8 +4243,8 @@
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+    <row r="37" spans="1:5">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -3999,8 +4258,8 @@
       </c>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+    <row r="38" spans="1:5">
+      <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
@@ -4014,8 +4273,8 @@
       </c>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+    <row r="39" spans="1:5">
+      <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -4029,8 +4288,8 @@
       </c>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+    <row r="40" spans="1:5" ht="15">
+      <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
@@ -4044,8 +4303,8 @@
       </c>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+    <row r="41" spans="1:5" ht="15">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
@@ -4059,8 +4318,8 @@
       </c>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+    <row r="42" spans="1:5">
+      <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -4074,8 +4333,8 @@
       </c>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
+    <row r="43" spans="1:5">
+      <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
@@ -4089,8 +4348,8 @@
       </c>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+    <row r="44" spans="1:5">
+      <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
@@ -4104,8 +4363,8 @@
       </c>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+    <row r="45" spans="1:5" ht="43.2">
+      <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
@@ -4119,8 +4378,8 @@
       </c>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+    <row r="46" spans="1:5">
+      <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
@@ -4134,8 +4393,8 @@
       </c>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+    <row r="47" spans="1:5">
+      <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
@@ -4149,8 +4408,8 @@
       </c>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+    <row r="48" spans="1:5">
+      <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
@@ -4164,8 +4423,8 @@
       </c>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+    <row r="49" spans="1:5">
+      <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
@@ -4179,8 +4438,8 @@
       </c>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+    <row r="50" spans="1:5" ht="28.8">
+      <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
@@ -4194,78 +4453,74 @@
       </c>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:5">
       <c r="B51" s="9"/>
       <c r="D51" s="12"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:5">
       <c r="E52" s="5"/>
     </row>
-    <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:5" ht="79.2" customHeight="1">
       <c r="E53" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:5">
       <c r="E54" s="1" t="s">
         <v>206</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="binaries from: http://ant.apache.org/bindownload.cgi&#10;source from: http://ant.apache.org/srcdownload.cgi"/>
-    <hyperlink ref="D3" r:id="rId2" display="http://www.apache.org/dyn/closer.cgi/xmlgraphics/batik"/>
-    <hyperlink ref="D4" r:id="rId3" display="http://c-jdbc.ow2.org/download.html"/>
-    <hyperlink ref="D5" r:id="rId4" display="http://www.compiere.com/products/download/index.php"/>
-    <hyperlink ref="D6" r:id="rId5" display="http://db.apache.org/derby/derby_downloads.html"/>
-    <hyperlink ref="D7" r:id="rId6" display="http://www.drjava.org/"/>
-    <hyperlink ref="D8" r:id="rId7" display="http://download.eclipse.org/eclipse/downloads/"/>
-    <hyperlink ref="D10" r:id="rId8" display="http://sourceforge.net/projects/galleon/files/galleon/2.5.5/"/>
-    <hyperlink ref="D11" r:id="rId9" display="http://hadoop.apache.org/releases.html"/>
-    <hyperlink ref="D12" r:id="rId10" display="http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final"/>
-    <hyperlink ref="D13" r:id="rId11" display="http://hsqldb.org/"/>
-    <hyperlink ref="D14" r:id="rId12" display="http://sourceforge.net/projects/jboss/files/JBoss/JBoss-5.1.0.GA/"/>
-    <hyperlink ref="D15" r:id="rId13" display="http://www.jruby.org/download"/>
-    <hyperlink ref="D16" r:id="rId14" display="http://lucene.apache.org/"/>
-    <hyperlink ref="D17" r:id="rId15" display="http://myfaces.apache.org/"/>
-    <hyperlink ref="D18" r:id="rId16" display="http://nekohtml.sourceforge.net/"/>
-    <hyperlink ref="D19" r:id="rId17" display="https://netbeans.org/downloads/"/>
-    <hyperlink ref="D20" r:id="rId18" display="http://openjms.sourceforge.net/downloads.html"/>
-    <hyperlink ref="D21" r:id="rId19" display="http://quartz-scheduler.org/"/>
-    <hyperlink ref="D22" r:id="rId20" display="http://www.quickserver.org/download.html"/>
-    <hyperlink ref="D23" r:id="rId21" location="quick-start" display="http://projects.spring.io/spring-framework/#quick-start"/>
-    <hyperlink ref="D24" r:id="rId22" display="http://struts.apache.org/"/>
-    <hyperlink ref="D25" r:id="rId23" display="http://tapestry.apache.org/download.html"/>
-    <hyperlink ref="D26" r:id="rId24" display="http://tomcat.apache.org/whichversion.html"/>
-    <hyperlink ref="D27" r:id="rId25" display="http://www.vuze.com/"/>
-    <hyperlink ref="D28" r:id="rId26" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
-    <hyperlink ref="D29" r:id="rId27" display="http://xml.apache.org/xalan-j/"/>
-    <hyperlink ref="D30" r:id="rId28" display="http://xerces.apache.org/mirrors.cgi"/>
-    <hyperlink ref="D32" r:id="rId29" display="https://github.com/tykkidream/DemoPermissions"/>
-    <hyperlink ref="D33" r:id="rId30" display="https://github.com/eclipse/org.aspectj"/>
-    <hyperlink ref="D34" r:id="rId31" display="https://github.com/kschat/MCVersion-Control"/>
-    <hyperlink ref="D35" r:id="rId32" display="https://github.com/JSansalone/NetBeansIDE"/>
-    <hyperlink ref="D36" r:id="rId33" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
-    <hyperlink ref="D37" r:id="rId34" display="https://github.com/zoomis/NGOMS"/>
-    <hyperlink ref="D39" r:id="rId35" display="https://github.com/Babast/Timelag"/>
-    <hyperlink ref="D40" r:id="rId36" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="D42" r:id="rId37" display="https://github.com/aleksz/driveddoc"/>
-    <hyperlink ref="D43" r:id="rId38" display="https://github.com/holisticon/tracee"/>
-    <hyperlink ref="D44" r:id="rId39" display="https://github.com/astubbs/spring-modules"/>
-    <hyperlink ref="D45" r:id="rId40" display="https://github.com/wildfly-security/security-manager"/>
-    <hyperlink ref="D46" r:id="rId41" display="https://github.com/ngty/gjman"/>
-    <hyperlink ref="D47" r:id="rId42" display="https://github.com/hypernet/visor"/>
-    <hyperlink ref="D48" r:id="rId43" display="https://github.com/stefanbirkner/system-rules"/>
-    <hyperlink ref="D49" r:id="rId44" display="https://github.com/ch33kybutt/oxygen_libcore"/>
-    <hyperlink ref="D50" r:id="rId45" display="https://github.com/apache/tomcat70"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="D14" r:id="rId12"/>
+    <hyperlink ref="D15" r:id="rId13"/>
+    <hyperlink ref="D16" r:id="rId14"/>
+    <hyperlink ref="D17" r:id="rId15"/>
+    <hyperlink ref="D18" r:id="rId16"/>
+    <hyperlink ref="D19" r:id="rId17"/>
+    <hyperlink ref="D20" r:id="rId18"/>
+    <hyperlink ref="D21" r:id="rId19"/>
+    <hyperlink ref="D22" r:id="rId20"/>
+    <hyperlink ref="D23" r:id="rId21" location="quick-start"/>
+    <hyperlink ref="D24" r:id="rId22"/>
+    <hyperlink ref="D25" r:id="rId23"/>
+    <hyperlink ref="D26" r:id="rId24"/>
+    <hyperlink ref="D27" r:id="rId25"/>
+    <hyperlink ref="D28" r:id="rId26"/>
+    <hyperlink ref="D29" r:id="rId27"/>
+    <hyperlink ref="D30" r:id="rId28"/>
+    <hyperlink ref="D32" r:id="rId29"/>
+    <hyperlink ref="D33" r:id="rId30"/>
+    <hyperlink ref="D34" r:id="rId31"/>
+    <hyperlink ref="D35" r:id="rId32"/>
+    <hyperlink ref="D36" r:id="rId33"/>
+    <hyperlink ref="D37" r:id="rId34"/>
+    <hyperlink ref="D39" r:id="rId35"/>
+    <hyperlink ref="D40" r:id="rId36"/>
+    <hyperlink ref="D42" r:id="rId37"/>
+    <hyperlink ref="D43" r:id="rId38"/>
+    <hyperlink ref="D44" r:id="rId39"/>
+    <hyperlink ref="D45" r:id="rId40"/>
+    <hyperlink ref="D46" r:id="rId41"/>
+    <hyperlink ref="D47" r:id="rId42"/>
+    <hyperlink ref="D48" r:id="rId43"/>
+    <hyperlink ref="D49" r:id="rId44"/>
+    <hyperlink ref="D50" r:id="rId45"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Marked two projects in github as duplicate
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -2871,7 +2871,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2966,8 +2966,17 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2996,8 +3005,13 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -3020,8 +3034,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -3031,8 +3060,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3080,13 +3112,21 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="5" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="5" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="5" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="TableStyleLight1" xfId="4"/>
     <cellStyle name="差" xfId="1" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="3" builtinId="8"/>
     <cellStyle name="好" xfId="2" builtinId="26"/>
+    <cellStyle name="检查单元格" xfId="5" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3437,8 +3477,8 @@
   </sheetPr>
   <dimension ref="A1:AMK54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" activeCellId="10" sqref="B4 B9 B10 B20 B21 B22 B23 B24 B25 B28 B30"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4198,7 +4238,7 @@
       </c>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="43.2">
+    <row r="34" spans="1:5" ht="43.8" thickBot="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -4213,22 +4253,22 @@
       </c>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="43.2">
-      <c r="A35" s="1">
+    <row r="35" spans="1:5" ht="58.8" thickTop="1" thickBot="1">
+      <c r="A35" s="19">
         <v>34</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="21" t="s">
         <v>159</v>
       </c>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" ht="57.6">
+    <row r="36" spans="1:5" ht="58.2" thickTop="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -4423,7 +4463,7 @@
       </c>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" ht="15" thickBot="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -4438,22 +4478,22 @@
       </c>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" ht="28.8">
-      <c r="A50" s="1">
+    <row r="50" spans="1:5" ht="44.4" thickTop="1" thickBot="1">
+      <c r="A50" s="19">
         <v>49</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="21" t="s">
         <v>204</v>
       </c>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" ht="15" thickTop="1">
       <c r="B51" s="9"/>
       <c r="D51" s="12"/>
       <c r="E51" s="5"/>

</xml_diff>

<commit_message>
added the analysis of c-jdbc
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\2014 SUMMER\Michael\ProjectsProfiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="519"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="519" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="214">
   <si>
     <t>Index</t>
   </si>
@@ -519,7 +515,63 @@
     <t>2.0.2</t>
   </si>
   <si>
-    <t>http://c-jdbc.ow2.org/download.html</t>
+    <t>http://c-jdbc.ow2.org/download.html
+Specifically downloaded from: http://forge.ow2.org/project/showfiles.php?group_id=42</t>
+  </si>
+  <si>
+    <t>Didn't run – static analysis showed the program didn't touch the system security manager in any way.</t>
+  </si>
+  <si>
+    <t>No output – There were no setSecurityManager calls in the program</t>
+  </si>
+  <si>
+    <t>./src/org/objectweb/cjdbc/controller/core/ControllerFactory.java
+49:import org.objectweb.cjdbc.controller.core.security.ControllerSecurityManager;
+389:  public void setUpSecurity(ControllerSecurityManager security)
+./src/org/objectweb/cjdbc/controller/core/Controller.java
+67:import org.objectweb.cjdbc.controller.core.security.ControllerSecurityManager;
+119:  private ControllerSecurityManager security;
+880:  public ControllerSecurityManager getSecurity()
+888:  public void setSecurity(ControllerSecurityManager security)
+./src/org/objectweb/cjdbc/controller/core/security/ControllerSecurityManager.java
+41:public class ControllerSecurityManager implements XmlComponent
+58:  public ControllerSecurityManager()
+./src/org/objectweb/cjdbc/controller/xml/ControllerParser.java
+50:import org.objectweb.cjdbc.controller.core.security.ControllerSecurityManager;
+79:  private ControllerSecurityManager security;
+324:      security = new ControllerSecurityManager();
+</t>
+  </si>
+  <si>
+    <t>This application should be removed from the dataset.  It doesn't effect the system security manager in any way.</t>
+  </si>
+  <si>
+    <t>No comments – didn't run</t>
+  </si>
+  <si>
+    <t>no comments – no output</t>
+  </si>
+  <si>
+    <t>./src/org/objectweb/cjdbc/controller/core/ControllerFactory.java
+49:import org.objectweb.cjdbc.controller.core.security.ControllerSecurityManager;
+389:  public void setUpSecurity(ControllerSecurityManager security)
+indirectly set up a connection permission manager.  This method is uninteresting by itself.
+./src/org/objectweb/cjdbc/controller/core/Controller.java
+67:import org.objectweb.cjdbc.controller.core.security.ControllerSecurityManager;
+119:  private ControllerSecurityManager security;
+880:  public ControllerSecurityManager getSecurity()
+888:  public void setSecurity(ControllerSecurityManager security)
+Allows setting the connection permission manager
+./src/org/objectweb/cjdbc/controller/core/security/ControllerSecurityManager.java
+41:public class ControllerSecurityManager implements XmlComponent
+58:  public ControllerSecurityManager()
+Class to manage what permissions different connections have.  This class does not extend the system.lang.SecurityManager.
+./src/org/objectweb/cjdbc/controller/xml/ControllerParser.java
+50:import org.objectweb.cjdbc.controller.core.security.ControllerSecurityManager;
+79:  private ControllerSecurityManager security;
+324:      security = new ControllerSecurityManager();
+sets up a connection permission manager for the program.
+</t>
   </si>
   <si>
     <t>compiere</t>
@@ -2870,12 +2922,38 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
+  </numFmts>
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -2895,20 +2973,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
@@ -2916,7 +2994,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
@@ -2924,7 +3002,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri Light"/>
@@ -2933,9 +3011,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2944,39 +3043,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2991,50 +3059,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="3">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3049,87 +3099,165 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+  <cellStyleXfs count="25">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+  <cellXfs count="24">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="5" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="5" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="5" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="1" xfId="24" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="TableStyleLight1" xfId="4"/>
-    <cellStyle name="差" xfId="1" builtinId="27"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8"/>
-    <cellStyle name="好" xfId="2" builtinId="26"/>
-    <cellStyle name="检查单元格" xfId="5" builtinId="23"/>
+  <cellStyles count="11">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Check Cell" xfId="24" builtinId="54" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -3140,7 +3268,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF9C0006"/>
       <rgbColor rgb="FF006100"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -3171,7 +3299,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFC7CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -3179,7 +3307,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFA5A5A5"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -3187,313 +3315,37 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="FF3F3F3F"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMK54"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="1"/>
-    <col min="2" max="2" width="35.6640625" style="1"/>
-    <col min="3" max="3" width="37.33203125" style="1"/>
-    <col min="4" max="4" width="63" style="1"/>
-    <col min="5" max="7" width="58" style="1"/>
-    <col min="8" max="8" width="32.44140625" style="1"/>
-    <col min="9" max="18" width="22.6640625" style="1"/>
-    <col min="19" max="1025" width="8.77734375" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77934272300469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.6572769953052"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.3333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="63.0046948356808"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="58"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.4366197183099"/>
+    <col collapsed="false" hidden="false" max="18" min="9" style="1" width="22.6666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="8.77934272300469"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1">
+    <row r="1" s="2" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3528,1039 +3380,1065 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="3" customFormat="1" ht="75.599999999999994" customHeight="1">
-      <c r="A2" s="3">
+    <row r="2" s="3" customFormat="true" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A3" s="1">
+    <row r="3" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8" t="n">
         <v>1.7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-    </row>
-    <row r="4" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A4" s="1">
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-    </row>
-    <row r="5" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A5" s="1">
+      <c r="E4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="O6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="N10" s="0"/>
+      <c r="O10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+      <c r="O11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
+      <c r="N12" s="0"/>
+      <c r="O12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
+      <c r="O13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="8" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" customFormat="false" ht="43.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B34" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="18" t="n">
         <v>34</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="B35" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-    </row>
-    <row r="6" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="17" t="s">
+      <c r="B36" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B37" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="B38" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="B39" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="B40" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="B41" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="B42" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="B43" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="B44" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="B45" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-    </row>
-    <row r="7" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B46" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B47" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="B48" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="B49" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" customFormat="false" ht="44.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="18" t="n">
         <v>49</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-    </row>
-    <row r="9" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="P9"/>
-    </row>
-    <row r="10" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="M15"/>
-    </row>
-    <row r="16" spans="1:16" ht="75.599999999999994" customHeight="1">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="M16"/>
-    </row>
-    <row r="17" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" ht="75.599999999999994" customHeight="1">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" ht="43.2">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" ht="15">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" ht="43.8" thickBot="1">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" ht="58.8" thickTop="1" thickBot="1">
-      <c r="A35" s="19">
-        <v>34</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" ht="58.2" thickTop="1">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" ht="15">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" ht="15">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" ht="43.2">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" ht="15" thickBot="1">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" ht="44.4" thickTop="1" thickBot="1">
-      <c r="A50" s="19">
-        <v>49</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="D50" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" ht="15" thickTop="1">
-      <c r="B51" s="9"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:5" ht="79.2" customHeight="1">
+      <c r="B50" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="10"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D10" r:id="rId8"/>
-    <hyperlink ref="D11" r:id="rId9"/>
-    <hyperlink ref="D12" r:id="rId10"/>
-    <hyperlink ref="D13" r:id="rId11"/>
-    <hyperlink ref="D14" r:id="rId12"/>
-    <hyperlink ref="D15" r:id="rId13"/>
-    <hyperlink ref="D16" r:id="rId14"/>
-    <hyperlink ref="D17" r:id="rId15"/>
-    <hyperlink ref="D18" r:id="rId16"/>
-    <hyperlink ref="D19" r:id="rId17"/>
-    <hyperlink ref="D20" r:id="rId18"/>
-    <hyperlink ref="D21" r:id="rId19"/>
-    <hyperlink ref="D22" r:id="rId20"/>
-    <hyperlink ref="D23" r:id="rId21" location="quick-start"/>
-    <hyperlink ref="D24" r:id="rId22"/>
-    <hyperlink ref="D25" r:id="rId23"/>
-    <hyperlink ref="D26" r:id="rId24"/>
-    <hyperlink ref="D27" r:id="rId25"/>
-    <hyperlink ref="D28" r:id="rId26"/>
-    <hyperlink ref="D29" r:id="rId27"/>
-    <hyperlink ref="D30" r:id="rId28"/>
-    <hyperlink ref="D32" r:id="rId29"/>
-    <hyperlink ref="D33" r:id="rId30"/>
-    <hyperlink ref="D34" r:id="rId31"/>
-    <hyperlink ref="D35" r:id="rId32"/>
-    <hyperlink ref="D36" r:id="rId33"/>
-    <hyperlink ref="D37" r:id="rId34"/>
-    <hyperlink ref="D39" r:id="rId35"/>
-    <hyperlink ref="D40" r:id="rId36"/>
-    <hyperlink ref="D42" r:id="rId37"/>
-    <hyperlink ref="D43" r:id="rId38"/>
-    <hyperlink ref="D44" r:id="rId39"/>
-    <hyperlink ref="D45" r:id="rId40"/>
-    <hyperlink ref="D46" r:id="rId41"/>
-    <hyperlink ref="D47" r:id="rId42"/>
-    <hyperlink ref="D48" r:id="rId43"/>
-    <hyperlink ref="D49" r:id="rId44"/>
-    <hyperlink ref="D50" r:id="rId45"/>
+    <hyperlink ref="D2" r:id="rId1" display="binaries from: http://ant.apache.org/bindownload.cgi&#10;source from: http://ant.apache.org/srcdownload.cgi"/>
+    <hyperlink ref="D3" r:id="rId2" display="http://www.apache.org/dyn/closer.cgi/xmlgraphics/batik"/>
+    <hyperlink ref="D5" r:id="rId3" display="http://www.compiere.com/products/download/index.php"/>
+    <hyperlink ref="D6" r:id="rId4" display="http://db.apache.org/derby/derby_downloads.html"/>
+    <hyperlink ref="D7" r:id="rId5" display="http://www.drjava.org/"/>
+    <hyperlink ref="D8" r:id="rId6" display="http://download.eclipse.org/eclipse/downloads/"/>
+    <hyperlink ref="D10" r:id="rId7" display="http://sourceforge.net/projects/galleon/files/galleon/2.5.5/"/>
+    <hyperlink ref="D11" r:id="rId8" display="http://hadoop.apache.org/releases.html"/>
+    <hyperlink ref="D12" r:id="rId9" display="http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final"/>
+    <hyperlink ref="D13" r:id="rId10" display="http://hsqldb.org/"/>
+    <hyperlink ref="D14" r:id="rId11" display="http://sourceforge.net/projects/jboss/files/JBoss/JBoss-5.1.0.GA/"/>
+    <hyperlink ref="D15" r:id="rId12" display="http://www.jruby.org/download"/>
+    <hyperlink ref="D16" r:id="rId13" display="http://lucene.apache.org/"/>
+    <hyperlink ref="D17" r:id="rId14" display="http://myfaces.apache.org/"/>
+    <hyperlink ref="D18" r:id="rId15" display="http://nekohtml.sourceforge.net/"/>
+    <hyperlink ref="D19" r:id="rId16" display="https://netbeans.org/downloads/"/>
+    <hyperlink ref="D20" r:id="rId17" display="http://openjms.sourceforge.net/downloads.html"/>
+    <hyperlink ref="D21" r:id="rId18" display="http://quartz-scheduler.org/"/>
+    <hyperlink ref="D22" r:id="rId19" display="http://www.quickserver.org/download.html"/>
+    <hyperlink ref="D23" r:id="rId20" location="quick-start" display="http://projects.spring.io/spring-framework/#quick-start"/>
+    <hyperlink ref="D24" r:id="rId21" display="http://struts.apache.org/"/>
+    <hyperlink ref="D25" r:id="rId22" display="http://tapestry.apache.org/download.html"/>
+    <hyperlink ref="D26" r:id="rId23" display="http://tomcat.apache.org/whichversion.html"/>
+    <hyperlink ref="D27" r:id="rId24" display="http://www.vuze.com/"/>
+    <hyperlink ref="D28" r:id="rId25" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
+    <hyperlink ref="D29" r:id="rId26" display="http://xml.apache.org/xalan-j/"/>
+    <hyperlink ref="D30" r:id="rId27" display="http://xerces.apache.org/mirrors.cgi"/>
+    <hyperlink ref="D32" r:id="rId28" display="https://github.com/tykkidream/DemoPermissions"/>
+    <hyperlink ref="D33" r:id="rId29" display="https://github.com/eclipse/org.aspectj"/>
+    <hyperlink ref="D34" r:id="rId30" display="https://github.com/kschat/MCVersion-Control"/>
+    <hyperlink ref="D35" r:id="rId31" display="https://github.com/JSansalone/NetBeansIDE"/>
+    <hyperlink ref="D36" r:id="rId32" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
+    <hyperlink ref="D37" r:id="rId33" display="https://github.com/zoomis/NGOMS"/>
+    <hyperlink ref="D39" r:id="rId34" display="https://github.com/Babast/Timelag"/>
+    <hyperlink ref="D40" r:id="rId35" display="https://github.com/JetBrains/intellij-community"/>
+    <hyperlink ref="D42" r:id="rId36" display="https://github.com/aleksz/driveddoc"/>
+    <hyperlink ref="D43" r:id="rId37" display="https://github.com/holisticon/tracee"/>
+    <hyperlink ref="D44" r:id="rId38" display="https://github.com/astubbs/spring-modules"/>
+    <hyperlink ref="D45" r:id="rId39" display="https://github.com/wildfly-security/security-manager"/>
+    <hyperlink ref="D46" r:id="rId40" display="https://github.com/ngty/gjman"/>
+    <hyperlink ref="D47" r:id="rId41" display="https://github.com/hypernet/visor"/>
+    <hyperlink ref="D48" r:id="rId42" display="https://github.com/stefanbirkner/system-rules"/>
+    <hyperlink ref="D49" r:id="rId43" display="https://github.com/ch33kybutt/oxygen_libcore"/>
+    <hyperlink ref="D50" r:id="rId44" display="https://github.com/apache/tomcat70"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId46"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed c_jdbc from green to white category because it was determined the program should be in the white category after manual inspection
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -539,8 +539,7 @@
 ./src/org/objectweb/cjdbc/controller/xml/ControllerParser.java
 50:import org.objectweb.cjdbc.controller.core.security.ControllerSecurityManager;
 79:  private ControllerSecurityManager security;
-324:      security = new ControllerSecurityManager();
-</t>
+324:      security = new ControllerSecurityManager();</t>
   </si>
   <si>
     <t>This application should be removed from the dataset.  It doesn't effect the system security manager in any way.</t>
@@ -570,8 +569,7 @@
 50:import org.objectweb.cjdbc.controller.core.security.ControllerSecurityManager;
 79:  private ControllerSecurityManager security;
 324:      security = new ControllerSecurityManager();
-sets up a connection permission manager for the program.
-</t>
+sets up a connection permission manager for the program.</t>
   </si>
   <si>
     <t>compiere</t>
@@ -2952,13 +2950,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="3"/>
@@ -2969,6 +2960,13 @@
       <color rgb="FF006100"/>
       <name val="Calibri Light"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -3011,16 +3009,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Droid Sans Fallback"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3134,13 +3133,13 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3152,11 +3151,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3180,7 +3179,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3188,11 +3187,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3200,15 +3199,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3252,11 +3251,11 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Check Cell" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Check Cell" xfId="24" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3329,8 +3328,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3467,7 +3466,7 @@
       <c r="D4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -3485,7 +3484,7 @@
       <c r="J4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="L4" s="0"/>
@@ -3627,7 +3626,7 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3674,7 +3673,7 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -3885,7 +3884,7 @@
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="13" t="s">
         <v>117</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -3902,7 +3901,7 @@
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="13" t="s">
         <v>120</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -3919,7 +3918,7 @@
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="13" t="s">
         <v>123</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -3936,7 +3935,7 @@
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="13" t="s">
         <v>126</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -3953,7 +3952,7 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="13" t="s">
         <v>129</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -3970,7 +3969,7 @@
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="13" t="s">
         <v>132</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -4027,7 +4026,7 @@
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="13" t="s">
         <v>144</v>
       </c>
       <c r="C28" s="8" t="n">
@@ -4057,7 +4056,7 @@
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="13" t="s">
         <v>149</v>
       </c>
       <c r="C30" s="10" t="s">

</xml_diff>

<commit_message>
Added the analysis for galleon
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="221">
   <si>
     <t>Index</t>
   </si>
@@ -1976,6 +1976,77 @@
   </si>
   <si>
     <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
+  </si>
+  <si>
+    <t>Callback on VMStart.
+#################################################
+SecurityManager Changed:
+Server.java, setup, 211
+#################################################
+Agent OnUnload, agent exits.</t>
+  </si>
+  <si>
+    <t>At RMIProvider.java:[line 59]
+In method org.apache.axis.providers.java.RMIProvider.makeNewServiceObject(MessageContext, String)
+Value Not null: java.rmi.RMISecurityManager 
+Value new 
+Value new[187](3) 11 
+Value Variable is set at:
+---------------------------------------------------------------------------------
+At Server.java:[line 208]
+In method org.lnicholls.galleon.server.Server.setup(ArrayList)
+Value Not null: org.lnicholls.galleon.server.Server$1
+ Value new
+ Value new[187](3) 89 
+Value Variable is set at:
+</t>
+  </si>
+  <si>
+    <t>./src/org/lnicholls/galleon/util/CustomSecurityManager.java
+23:public class CustomSecurityManager extends SecurityManager {
+25:	public CustomSecurityManager()
+45:		     * SecurityManager.checkMemeberAccess [0]
+./src/org/lnicholls/galleon/server/Server.java
+42:import java.rmi.RMISecurityManager;
+88:		//System.setSecurityManager(new CustomSecurityManager());
+208:				System.setSecurityManager (new RMISecurityManager() {
+800:		if (true || System.getSecurityManager() instanceof CustomSecurityManager)</t>
+  </si>
+  <si>
+    <t>This program only sets a SecurityManager if the server has a remote host.  No nulling or weaking is happening.</t>
+  </si>
+  <si>
+    <t>Location where SM is set is covered in the static analysis.  The program only sets a SecurityManager.</t>
+  </si>
+  <si>
+    <t>At RMIProvider.java:[line 59]
+In method org.apache.axis.providers.java.RMIProvider.makeNewServiceObject(MessageContext, String)
+Value Not null: java.rmi.RMISecurityManager 
+Value new 
+Value new[187](3) 11 
+Value Variable is set at:
+This is not included in the source code so it must be included in one of the jar files.  Looking at this code online, if this method is called without a SecurityManager set for the system, the program sets an RMISecurityManager as the system security manager.  I'm not sure if this method is ever called.  It is never called directly by the galleon code although it may be called indirectly through another call in apache axis.
+----------------------------------------------------------
+At Server.java:[line 208]
+In method org.lnicholls.galleon.server.Server.setup(ArrayList)
+Value Not null: org.lnicholls.galleon.server.Server$1
+ Value new
+ Value new[187](3) 89 
+Value Variable is set at:
+An RMI SecurityManager is set if the system property remoteHost is not empty. which implies that the server is interacting with a different machine as the controller.</t>
+  </si>
+  <si>
+    <t>./src/org/lnicholls/galleon/util/CustomSecurityManager.java
+23:public class CustomSecurityManager extends SecurityManager {
+25:	public CustomSecurityManager()
+45:		     * SecurityManager.checkMemeberAccess [0]
+Adds a new method to the SecurityManager extension.  However, the line to call this function is commented out in Server.java so this class is never instantiated.
+./src/org/lnicholls/galleon/server/Server.java
+42:import java.rmi.RMISecurityManager;
+88:		//System.setSecurityManager(new CustomSecurityManager());
+208:				System.setSecurityManager (new RMISecurityManager() {
+800:		if (true || System.getSecurityManager() instanceof CustomSecurityManager)
+This was covered in the static analysis.  This is confusing because a CustomSecurityManager can never be set since it is commented out at line 88 but they check for it in line 800.</t>
   </si>
   <si>
     <t>hadoop</t>
@@ -3251,11 +3322,11 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Check Cell" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="24" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3328,8 +3399,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3682,10 +3753,27 @@
       <c r="D10" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="L10" s="0"/>
       <c r="M10" s="0"/>
       <c r="N10" s="0"/>
@@ -3696,13 +3784,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="0"/>
@@ -3718,13 +3806,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="0"/>
@@ -3740,13 +3828,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="0"/>
@@ -3762,37 +3850,37 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>56</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3800,13 +3888,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E15" s="6"/>
       <c r="G15" s="6"/>
@@ -3817,13 +3905,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="E16" s="6"/>
       <c r="G16" s="6"/>
@@ -3834,13 +3922,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E17" s="6"/>
       <c r="G17" s="6"/>
@@ -3851,13 +3939,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E18" s="6"/>
       <c r="G18" s="6"/>
@@ -3868,13 +3956,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E19" s="6"/>
       <c r="G19" s="6"/>
@@ -3885,13 +3973,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E20" s="6"/>
       <c r="G20" s="6"/>
@@ -3902,13 +3990,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="E21" s="6"/>
       <c r="G21" s="6"/>
@@ -3919,13 +4007,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="E22" s="6"/>
       <c r="G22" s="6"/>
@@ -3936,13 +4024,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E23" s="6"/>
       <c r="G23" s="6"/>
@@ -3953,13 +4041,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E24" s="6"/>
       <c r="G24" s="6"/>
@@ -3970,13 +4058,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E25" s="6"/>
       <c r="G25" s="6"/>
@@ -3987,13 +4075,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="6"/>
@@ -4004,22 +4092,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4027,13 +4115,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E28" s="6"/>
     </row>
@@ -4042,13 +4130,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E29" s="6"/>
     </row>
@@ -4057,13 +4145,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E30" s="6"/>
     </row>
@@ -4072,13 +4160,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -4087,13 +4175,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -4102,13 +4190,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -4117,13 +4205,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E34" s="6"/>
     </row>
@@ -4132,13 +4220,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -4147,13 +4235,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -4162,13 +4250,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -4177,13 +4265,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -4192,13 +4280,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -4207,13 +4295,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -4222,13 +4310,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -4237,13 +4325,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E42" s="6"/>
     </row>
@@ -4252,13 +4340,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -4267,13 +4355,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -4282,13 +4370,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="E45" s="6"/>
     </row>
@@ -4297,13 +4385,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -4312,13 +4400,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E47" s="6"/>
     </row>
@@ -4327,13 +4415,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E48" s="6"/>
     </row>
@@ -4342,13 +4430,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="E49" s="6"/>
     </row>
@@ -4357,13 +4445,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E50" s="6"/>
     </row>
@@ -4377,12 +4465,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the analysis of openjms
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="228">
   <si>
     <t>Index</t>
   </si>
@@ -2046,8 +2046,7 @@
 88:		//System.setSecurityManager(new CustomSecurityManager());
 208:				System.setSecurityManager (new RMISecurityManager() {
 800:		if (true || System.getSecurityManager() instanceof CustomSecurityManager)
-This was covered in the static analysis.  This is confusing because a CustomSecurityManager can never be set since it is commented out at line 88 but they check for it in line 800.
-</t>
+This was covered in the static analysis.  This is confusing because a CustomSecurityManager can never be set since it is commented out at line 88 but they check for it in line 800.</t>
   </si>
   <si>
     <t>hadoop</t>
@@ -2731,6 +2730,31 @@
     <t>http://openjms.sourceforge.net/downloads.html</t>
   </si>
   <si>
+    <t>Didn't run.  There is no code to effect the SecurityManager in the main program</t>
+  </si>
+  <si>
+    <t>No output – There were no setSecurityManager calls in the main program.  Only in a test case.</t>
+  </si>
+  <si>
+    <t>./modules/net/src/test/java/org/exolab/jms/net/socket/SocketManagedConnectionFactoryTestCase.java
+126:        SecurityManager manager = new SecurityManager() {
+135:        SecurityManager original = System.getSecurityManager();
+136:        System.setSecurityManager(manager);
+140:            System.setSecurityManager(original);</t>
+  </si>
+  <si>
+    <t>This program only tests if the code still works when a SecurityManager is set in a test case.  So no weakening or nulling occurs or even interacting with the SecurityManager in the main program.</t>
+  </si>
+  <si>
+    <t>./modules/net/src/test/java/org/exolab/jms/net/socket/SocketManagedConnectionFactoryTestCase.java
+126:        SecurityManager manager = new SecurityManager() {
+135:        SecurityManager original = System.getSecurityManager();
+136:        System.setSecurityManager(manager);
+140:            System.setSecurityManager(original);
+A test to see if the connection can occur with a SecurityManager default SecurityManager set.  The test saves the current SecurityManager at the time of starting the test and restores it at the end.
+</t>
+  </si>
+  <si>
     <t>quartz scheduler</t>
   </si>
   <si>
@@ -3257,7 +3281,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3326,6 +3350,10 @@
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3366,12 +3394,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="25" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3439,13 +3467,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4023,7 +4051,7 @@
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="17" t="s">
         <v>126</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -4032,22 +4060,40 @@
       <c r="D20" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E21" s="6"/>
       <c r="G21" s="6"/>
@@ -4058,13 +4104,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E22" s="6"/>
       <c r="G22" s="6"/>
@@ -4075,13 +4121,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E23" s="6"/>
       <c r="G23" s="6"/>
@@ -4092,13 +4138,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E24" s="6"/>
       <c r="G24" s="6"/>
@@ -4109,13 +4155,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E25" s="6"/>
       <c r="G25" s="6"/>
@@ -4126,13 +4172,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="6"/>
@@ -4143,22 +4189,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4166,13 +4212,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E28" s="6"/>
     </row>
@@ -4181,13 +4227,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="E29" s="6"/>
     </row>
@@ -4196,13 +4242,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E30" s="6"/>
     </row>
@@ -4211,13 +4257,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -4226,13 +4272,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>166</v>
+        <v>170</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>171</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -4240,14 +4286,14 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="18" t="s">
-        <v>167</v>
+      <c r="B33" s="19" t="s">
+        <v>172</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>169</v>
+        <v>173</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -4256,28 +4302,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>172</v>
+        <v>176</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>177</v>
       </c>
       <c r="E34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="19" t="n">
+      <c r="A35" s="20" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>175</v>
+      <c r="B35" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -4286,13 +4332,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>178</v>
+        <v>181</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>183</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -4301,13 +4347,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>181</v>
+        <v>184</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>186</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -4316,13 +4362,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>184</v>
+        <v>187</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>189</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -4331,13 +4377,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>187</v>
+        <v>190</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>192</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -4346,13 +4392,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>190</v>
+        <v>193</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>195</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -4361,13 +4407,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>193</v>
+        <v>196</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>198</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -4376,13 +4422,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>196</v>
+        <v>199</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>201</v>
       </c>
       <c r="E42" s="6"/>
     </row>
@@ -4391,13 +4437,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>199</v>
+        <v>203</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>204</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -4406,13 +4452,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>202</v>
+        <v>206</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>207</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -4421,13 +4467,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>205</v>
+        <v>209</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>210</v>
       </c>
       <c r="E45" s="6"/>
     </row>
@@ -4436,13 +4482,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>208</v>
+        <v>212</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>213</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -4451,13 +4497,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>211</v>
+        <v>215</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="E47" s="6"/>
     </row>
@@ -4466,13 +4512,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>214</v>
+        <v>218</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>219</v>
       </c>
       <c r="E48" s="6"/>
     </row>
@@ -4481,34 +4527,34 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>217</v>
+        <v>221</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="E49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="44.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="19" t="n">
+      <c r="A50" s="20" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="D50" s="21" t="s">
-        <v>220</v>
+      <c r="B50" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>225</v>
       </c>
       <c r="E50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="10"/>
-      <c r="D51" s="17"/>
+      <c r="D51" s="18"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4516,12 +4562,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added analysis for quartz
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="235">
   <si>
     <t>Index</t>
   </si>
@@ -2751,17 +2751,59 @@
 135:        SecurityManager original = System.getSecurityManager();
 136:        System.setSecurityManager(manager);
 140:            System.setSecurityManager(original);
-A test to see if the connection can occur with a SecurityManager default SecurityManager set.  The test saves the current SecurityManager at the time of starting the test and restores it at the end.
+A test to see if the connection can occur with a SecurityManager default SecurityManager set.  The test saves the current SecurityManager at the time of starting the test and restores it at the end.</t>
+  </si>
+  <si>
+    <t>quartz scheduler</t>
+  </si>
+  <si>
+    <t>2.2.1*</t>
+  </si>
+  <si>
+    <t>http://quartz-scheduler.org/downloads</t>
+  </si>
+  <si>
+    <t>Callback on VMStart.
+#################################################
+SecurityManager Changed:
+QuartzServer.java, main, 178
+#################################################
+Agent OnUnload, agent exits.</t>
+  </si>
+  <si>
+    <t>At QuartzServer.java:[line 178]
+In method org.quartz.impl.QuartzServer.main(String[])
+Value Not null: java.rmi.RMISecurityManager
+Value new 
+Value new[187](3) 37 
+Value Variable is set at:</t>
+  </si>
+  <si>
+    <t>./src/org/quartz/impl/QuartzServer.java
+177:        if (System.getSecurityManager() == null) {
+178:            System.setSecurityManager(new java.rmi.RMISecurityManager());</t>
+  </si>
+  <si>
+    <t>The program sets an RMISecurityManager if no SecurityManager is set when running the main program in QuartzServer.java.  Other than that no interaction with the SecurityManager occurs (so no nulling or weakening happening).</t>
+  </si>
+  <si>
+    <t>Sets SecurityManager at start of program as expected from Grep results</t>
+  </si>
+  <si>
+    <t>At QuartzServer.java:[line 178]
+In method org.quartz.impl.QuartzServer.main(String[])
+Value Not null: java.rmi.RMISecurityManager
+Value new 
+Value new[187](3) 37 
+Value Variable is set at:
+Sets the SecurityManager at the beginning of the QuartzServer startup if the program is not started with a SecurityManager already running.</t>
+  </si>
+  <si>
+    <t>./src/org/quartz/impl/QuartzServer.java
+177:        if (System.getSecurityManager() == null) {
+178:            System.setSecurityManager(new java.rmi.RMISecurityManager());
+First two lines of the main function.  If the program is ran without a SecurityManager, set the SecurityManager to the RMISecurityManager.
 </t>
-  </si>
-  <si>
-    <t>quartz scheduler</t>
-  </si>
-  <si>
-    <t>2.2.1*</t>
-  </si>
-  <si>
-    <t>http://quartz-scheduler.org/</t>
   </si>
   <si>
     <t>quickserver</t>
@@ -3394,12 +3436,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="25" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3473,7 +3515,7 @@
   <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3873,6 +3915,9 @@
         <v>93</v>
       </c>
       <c r="H11" s="6"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
       <c r="N11" s="0"/>
@@ -3897,6 +3942,9 @@
         <v>97</v>
       </c>
       <c r="H12" s="6"/>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
       <c r="L12" s="0"/>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
@@ -3919,6 +3967,9 @@
       <c r="F13" s="0"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
@@ -3949,6 +4000,9 @@
       <c r="H14" s="6" t="s">
         <v>106</v>
       </c>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
       <c r="L14" s="10" t="s">
         <v>107</v>
       </c>
@@ -3976,8 +4030,12 @@
         <v>113</v>
       </c>
       <c r="E15" s="6"/>
+      <c r="F15" s="0"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -3993,8 +4051,12 @@
         <v>116</v>
       </c>
       <c r="E16" s="6"/>
+      <c r="F16" s="0"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -4010,8 +4072,12 @@
         <v>119</v>
       </c>
       <c r="E17" s="6"/>
+      <c r="F17" s="0"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -4027,8 +4093,12 @@
         <v>122</v>
       </c>
       <c r="E18" s="6"/>
+      <c r="F18" s="0"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -4044,8 +4114,12 @@
         <v>125</v>
       </c>
       <c r="E19" s="6"/>
+      <c r="F19" s="0"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -4095,22 +4169,40 @@
       <c r="D21" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="E22" s="6"/>
       <c r="G22" s="6"/>
@@ -4121,13 +4213,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E23" s="6"/>
       <c r="G23" s="6"/>
@@ -4138,13 +4230,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E24" s="6"/>
       <c r="G24" s="6"/>
@@ -4155,13 +4247,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E25" s="6"/>
       <c r="G25" s="6"/>
@@ -4172,13 +4264,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="6"/>
@@ -4189,22 +4281,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4212,13 +4304,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E28" s="6"/>
     </row>
@@ -4227,13 +4319,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="E29" s="6"/>
     </row>
@@ -4242,13 +4334,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E30" s="6"/>
     </row>
@@ -4257,13 +4349,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -4272,13 +4364,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -4287,13 +4379,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -4302,13 +4394,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E34" s="6"/>
     </row>
@@ -4317,13 +4409,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -4332,13 +4424,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -4347,13 +4439,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -4362,13 +4454,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -4377,13 +4469,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -4392,13 +4484,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -4407,13 +4499,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -4422,13 +4514,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="E42" s="6"/>
     </row>
@@ -4437,13 +4529,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -4452,13 +4544,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -4467,13 +4559,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="E45" s="6"/>
     </row>
@@ -4482,13 +4574,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -4497,13 +4589,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="E47" s="6"/>
     </row>
@@ -4512,13 +4604,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E48" s="6"/>
     </row>
@@ -4527,13 +4619,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="E49" s="6"/>
     </row>
@@ -4542,13 +4634,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E50" s="6"/>
     </row>
@@ -4562,12 +4654,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the quickserver analysis
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="253">
   <si>
     <t>Index</t>
   </si>
@@ -2938,6 +2938,98 @@
     <t>http://www.quickserver.org/download.html</t>
   </si>
   <si>
+    <t>Callback on VMStart.
+#################################################
+SecurityManager Changed:
+QuickServer.java, startServer, 453
+#################################################
+Agent OnUnload, agent exits.</t>
+  </si>
+  <si>
+    <t>At QuickServer.java:[line 453]
+In method org.quickserver.net.server.QuickServer.startServer()
+Value Could be null or other value: java.lang.SecurityManager 
+Value invokevirtual
+Value invokevirtual[182](3) 129 
+Value Variable is set at:</t>
+  </si>
+  <si>
+    <t>./src/main/org/quickserver/util/xmlreader/QuickServerConfig.java
+94:	 * Sets the SecurityManager class
+97:	 * class that extends {@link java.lang.SecurityManager}.
+98:	 * @see #getSecurityManagerClass
+101:	public void setSecurityManagerClass(String securityManagerClass) {
+106:	 * Returns the SecurityManager class
+107:	 * @see #setSecurityManagerClass
+110:	public String getSecurityManagerClass() {
+240:		if(getSecurityManagerClass()!=null) {
+241:			sb.append(pad+"\t&lt;security-manager-class&gt;"+getSecurityManagerClass()+"&lt;/security-manager-class&gt;\n");
+./src/main/org/quickserver/net/server/QuickServer.java
+452:		if(getSecurityManagerClass()!=null) {
+453:			System.setSecurityManager(getSecurityManager());
+1548:		qs.setSecurityManagerClass(config.getSecurityManagerClass());
+2100:	 * Sets the SecurityManager class
+2102:	 * that extends {@link java.lang.SecurityManager}.
+2103:	 * @see #getSecurityManagerClass
+2106:	public void setSecurityManagerClass(String securityManagerClass) {
+2111:	 * Returns the SecurityManager class
+2112:	 * @see #setSecurityManagerClass
+2115:	public String getSecurityManagerClass() {
+2119:	public SecurityManager getSecurityManager() throws AppException {
+2120:		if(getSecurityManagerClass()==null)
+2122:		SecurityManager sm = null;
+2124:			sm = (SecurityManager) 
+2125:				getClass(getSecurityManagerClass(), true).newInstance();
+./src/main/org/quickserver/security/AccessManager.java
+22: * This is a simple SecurityManager template.
+25:public class AccessManager extends SecurityManager {
+</t>
+  </si>
+  <si>
+    <t>This program sets a SecurityManager if one is specified in the configuration file when starting the server.  No weakening or nulling occurred.  This would conflict if another SecurityManager was set before running but it wouldn't make sense to if you specified to initialize one in the configuration file.</t>
+  </si>
+  <si>
+    <t>Initializes the SecurityManager specified in the configuration file using reflection.  This is  also covered in the static analysis and the grep results.</t>
+  </si>
+  <si>
+    <t>Initializes the SecurityManager specified in the configuration file using reflection.  This is  also covered in the dynamic analysis and the grep results.</t>
+  </si>
+  <si>
+    <t>./src/main/org/quickserver/util/xmlreader/QuickServerConfig.java
+94:	 * Sets the SecurityManager class
+97:	 * class that extends {@link java.lang.SecurityManager}.
+98:	 * @see #getSecurityManagerClass
+101:	public void setSecurityManagerClass(String securityManagerClass) {
+106:	 * Returns the SecurityManager class
+107:	 * @see #setSecurityManagerClass
+110:	public String getSecurityManagerClass() {
+240:		if(getSecurityManagerClass()!=null) {
+241:			sb.append(pad+"\t&lt;security-manager-class&gt;"+getSecurityManagerClass()+"&lt;/security-manager-class&gt;\n");
+This class is used to configure the server start-up.  It contains a field that stores the class to initalize the SecurityManager of the server to.
+./src/main/org/quickserver/net/server/QuickServer.java
+452:		if(getSecurityManagerClass()!=null) {
+453:			System.setSecurityManager(getSecurityManager());
+1548:		qs.setSecurityManagerClass(config.getSecurityManagerClass());
+2100:	 * Sets the SecurityManager class
+2102:	 * that extends {@link java.lang.SecurityManager}.
+2103:	 * @see #getSecurityManagerClass
+2106:	public void setSecurityManagerClass(String securityManagerClass) {
+2111:	 * Returns the SecurityManager class
+2112:	 * @see #setSecurityManagerClass
+2115:	public String getSecurityManagerClass() {
+2119:	public SecurityManager getSecurityManager() throws AppException {
+2120:		if(getSecurityManagerClass()==null)
+2122:		SecurityManager sm = null;
+2124:			sm = (SecurityManager) 
+2125:				getClass(getSecurityManagerClass(), true).newInstance();
+This class initializes a SecurityManager for the server and for the system if the SecurityManager class is defined as a valid extender of the SecurityManager.
+./src/main/org/quickserver/security/AccessManager.java
+22: * This is a simple SecurityManager template.
+25:public class AccessManager extends SecurityManager {
+This class in an example SecurityManager that allows everything.  Equivalent to all permissions.
+</t>
+  </si>
+  <si>
     <t>spring framework</t>
   </si>
   <si>
@@ -3215,7 +3307,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3317,6 +3409,12 @@
       <name val="Calibri Light"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3445,11 +3543,11 @@
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3530,35 +3628,39 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3570,13 +3672,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3644,12 +3746,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4098,6 +4201,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="0"/>
       <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
       <c r="L12" s="0"/>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
@@ -4128,6 +4232,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
@@ -4160,6 +4265,7 @@
       </c>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
       <c r="L14" s="10" t="s">
         <v>114</v>
       </c>
@@ -4204,6 +4310,7 @@
       <c r="J15" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="K15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -4219,8 +4326,12 @@
         <v>127</v>
       </c>
       <c r="E16" s="6"/>
+      <c r="F16" s="0"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -4236,8 +4347,12 @@
         <v>130</v>
       </c>
       <c r="E17" s="6"/>
+      <c r="F17" s="0"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -4253,8 +4368,12 @@
         <v>133</v>
       </c>
       <c r="E18" s="6"/>
+      <c r="F18" s="0"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -4270,8 +4389,12 @@
         <v>136</v>
       </c>
       <c r="E19" s="6"/>
+      <c r="F19" s="0"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -4356,22 +4479,40 @@
       <c r="D22" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E23" s="6"/>
       <c r="G23" s="6"/>
@@ -4382,13 +4523,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E24" s="6"/>
       <c r="G24" s="6"/>
@@ -4399,13 +4540,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E25" s="6"/>
       <c r="G25" s="6"/>
@@ -4416,13 +4557,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="6"/>
@@ -4433,22 +4574,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4456,13 +4597,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E28" s="6"/>
     </row>
@@ -4471,13 +4612,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E29" s="6"/>
     </row>
@@ -4486,13 +4627,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="E30" s="6"/>
     </row>
@@ -4501,13 +4642,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -4516,13 +4657,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>189</v>
+        <v>195</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>196</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -4530,14 +4671,14 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>190</v>
+      <c r="B33" s="22" t="s">
+        <v>197</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>192</v>
+        <v>198</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>199</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -4546,28 +4687,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>195</v>
+        <v>201</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>202</v>
       </c>
       <c r="E34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="22" t="n">
+      <c r="A35" s="23" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>198</v>
+      <c r="B35" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -4576,13 +4717,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>201</v>
+        <v>206</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -4591,13 +4732,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>204</v>
+        <v>209</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>211</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -4606,13 +4747,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>207</v>
+        <v>212</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>214</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -4621,13 +4762,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>217</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -4636,13 +4777,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>220</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -4651,13 +4792,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>216</v>
+        <v>221</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>223</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -4666,13 +4807,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>219</v>
+        <v>224</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>226</v>
       </c>
       <c r="E42" s="6"/>
     </row>
@@ -4681,13 +4822,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>222</v>
+        <v>228</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>229</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -4696,13 +4837,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>225</v>
+        <v>231</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>232</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -4711,13 +4852,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>228</v>
+        <v>234</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>235</v>
       </c>
       <c r="E45" s="6"/>
     </row>
@@ -4726,13 +4867,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>231</v>
+        <v>237</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>238</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -4741,13 +4882,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>234</v>
+        <v>240</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>241</v>
       </c>
       <c r="E47" s="6"/>
     </row>
@@ -4756,13 +4897,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>237</v>
+        <v>243</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>244</v>
       </c>
       <c r="E48" s="6"/>
     </row>
@@ -4771,34 +4912,34 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>240</v>
+        <v>246</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>247</v>
       </c>
       <c r="E49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="44.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="22" t="n">
+      <c r="A50" s="23" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="D50" s="24" t="s">
-        <v>243</v>
+      <c r="B50" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>250</v>
       </c>
       <c r="E50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="10"/>
-      <c r="D51" s="20"/>
+      <c r="D51" s="21"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4806,12 +4947,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added where the Eclipse source was downloaded from
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -1701,7 +1701,8 @@
     <t>4.4*</t>
   </si>
   <si>
-    <t>http://download.eclipse.org/eclipse/downloads/</t>
+    <t>http://download.eclipse.org/eclipse/downloads/
+http://download.eclipse.org/eclipse/downloads/drops4/R-4.4-201406061215/</t>
   </si>
   <si>
     <t>freemind</t>
@@ -2982,8 +2983,7 @@
 2125:				getClass(getSecurityManagerClass(), true).newInstance();
 ./src/main/org/quickserver/security/AccessManager.java
 22: * This is a simple SecurityManager template.
-25:public class AccessManager extends SecurityManager {
-</t>
+25:public class AccessManager extends SecurityManager {</t>
   </si>
   <si>
     <t>This program sets a SecurityManager if one is specified in the configuration file when starting the server.  No weakening or nulling occurred.  This would conflict if another SecurityManager was set before running but it wouldn't make sense to if you specified to initialize one in the configuration file.</t>
@@ -3026,8 +3026,7 @@
 ./src/main/org/quickserver/security/AccessManager.java
 22: * This is a simple SecurityManager template.
 25:public class AccessManager extends SecurityManager {
-This class in an example SecurityManager that allows everything.  Equivalent to all permissions.
-</t>
+This class in an example SecurityManager that allows everything.  Equivalent to all permissions.</t>
   </si>
   <si>
     <t>spring framework</t>
@@ -3307,7 +3306,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3409,12 +3408,6 @@
       <name val="Calibri Light"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri Light"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3543,11 +3536,11 @@
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3628,39 +3621,35 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3672,13 +3661,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3746,13 +3735,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4044,7 +4033,7 @@
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="12" t="s">
         <v>69</v>
       </c>
       <c r="E8" s="6"/>
@@ -4494,7 +4483,7 @@
       <c r="I22" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="10" t="s">
         <v>163</v>
       </c>
       <c r="K22" s="10" t="s">
@@ -4662,7 +4651,7 @@
       <c r="C32" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="20" t="s">
         <v>196</v>
       </c>
       <c r="E32" s="6"/>
@@ -4671,13 +4660,13 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>197</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="20" t="s">
         <v>199</v>
       </c>
       <c r="E33" s="6"/>
@@ -4692,22 +4681,22 @@
       <c r="C34" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="20" t="s">
         <v>202</v>
       </c>
       <c r="E34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="n">
+      <c r="A35" s="22" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="24" t="s">
         <v>205</v>
       </c>
       <c r="E35" s="6"/>
@@ -4719,10 +4708,10 @@
       <c r="B36" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="20" t="s">
         <v>208</v>
       </c>
       <c r="E36" s="6"/>
@@ -4734,10 +4723,10 @@
       <c r="B37" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="20" t="s">
         <v>211</v>
       </c>
       <c r="E37" s="6"/>
@@ -4749,10 +4738,10 @@
       <c r="B38" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="20" t="s">
         <v>214</v>
       </c>
       <c r="E38" s="6"/>
@@ -4764,10 +4753,10 @@
       <c r="B39" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="20" t="s">
         <v>217</v>
       </c>
       <c r="E39" s="6"/>
@@ -4779,10 +4768,10 @@
       <c r="B40" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="20" t="s">
         <v>220</v>
       </c>
       <c r="E40" s="6"/>
@@ -4794,10 +4783,10 @@
       <c r="B41" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="20" t="s">
         <v>223</v>
       </c>
       <c r="E41" s="6"/>
@@ -4809,10 +4798,10 @@
       <c r="B42" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="20" t="s">
         <v>226</v>
       </c>
       <c r="E42" s="6"/>
@@ -4827,7 +4816,7 @@
       <c r="C43" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="20" t="s">
         <v>229</v>
       </c>
       <c r="E43" s="6"/>
@@ -4842,7 +4831,7 @@
       <c r="C44" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="20" t="s">
         <v>232</v>
       </c>
       <c r="E44" s="6"/>
@@ -4857,7 +4846,7 @@
       <c r="C45" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D45" s="20" t="s">
         <v>235</v>
       </c>
       <c r="E45" s="6"/>
@@ -4872,7 +4861,7 @@
       <c r="C46" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D46" s="21" t="s">
+      <c r="D46" s="20" t="s">
         <v>238</v>
       </c>
       <c r="E46" s="6"/>
@@ -4887,7 +4876,7 @@
       <c r="C47" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D47" s="20" t="s">
         <v>241</v>
       </c>
       <c r="E47" s="6"/>
@@ -4902,7 +4891,7 @@
       <c r="C48" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="D48" s="20" t="s">
         <v>244</v>
       </c>
       <c r="E48" s="6"/>
@@ -4917,29 +4906,29 @@
       <c r="C49" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D49" s="21" t="s">
+      <c r="D49" s="20" t="s">
         <v>247</v>
       </c>
       <c r="E49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="44.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="23" t="n">
+      <c r="A50" s="22" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="D50" s="25" t="s">
+      <c r="D50" s="24" t="s">
         <v>250</v>
       </c>
       <c r="E50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="10"/>
-      <c r="D51" s="21"/>
+      <c r="D51" s="20"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4962,45 +4951,44 @@
     <hyperlink ref="D5" r:id="rId3" display="http://www.compiere.com/products/download/index.php"/>
     <hyperlink ref="D6" r:id="rId4" display="http://db.apache.org/derby/derby_downloads.html"/>
     <hyperlink ref="D7" r:id="rId5" display="http://www.drjava.org/"/>
-    <hyperlink ref="D8" r:id="rId6" display="http://download.eclipse.org/eclipse/downloads/"/>
-    <hyperlink ref="D10" r:id="rId7" display="http://sourceforge.net/projects/galleon/files/galleon/2.5.5/"/>
-    <hyperlink ref="D11" r:id="rId8" display="http://hadoop.apache.org/releases.html"/>
-    <hyperlink ref="D12" r:id="rId9" display="http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final"/>
-    <hyperlink ref="D13" r:id="rId10" display="http://hsqldb.org/"/>
-    <hyperlink ref="D14" r:id="rId11" display="http://sourceforge.net/projects/jboss/files/JBoss/JBoss-5.1.0.GA/"/>
-    <hyperlink ref="D15" r:id="rId12" display="http://www.jruby.org/download"/>
-    <hyperlink ref="D16" r:id="rId13" display="http://lucene.apache.org/"/>
-    <hyperlink ref="D17" r:id="rId14" display="http://myfaces.apache.org/"/>
-    <hyperlink ref="D18" r:id="rId15" display="http://nekohtml.sourceforge.net/"/>
-    <hyperlink ref="D19" r:id="rId16" display="https://netbeans.org/downloads/"/>
-    <hyperlink ref="D20" r:id="rId17" display="http://openjms.sourceforge.net/downloads.html"/>
-    <hyperlink ref="D21" r:id="rId18" display="http://quartz-scheduler.org/downloads"/>
-    <hyperlink ref="D22" r:id="rId19" display="http://www.quickserver.org/download.html"/>
-    <hyperlink ref="D23" r:id="rId20" location="quick-start" display="http://projects.spring.io/spring-framework/#quick-start"/>
-    <hyperlink ref="D24" r:id="rId21" display="http://struts.apache.org/"/>
-    <hyperlink ref="D25" r:id="rId22" display="http://tapestry.apache.org/download.html"/>
-    <hyperlink ref="D26" r:id="rId23" display="http://tomcat.apache.org/whichversion.html"/>
-    <hyperlink ref="D27" r:id="rId24" display="http://www.vuze.com/"/>
-    <hyperlink ref="D28" r:id="rId25" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
-    <hyperlink ref="D29" r:id="rId26" display="http://xml.apache.org/xalan-j/"/>
-    <hyperlink ref="D30" r:id="rId27" display="http://xerces.apache.org/mirrors.cgi"/>
-    <hyperlink ref="D32" r:id="rId28" display="https://github.com/tykkidream/DemoPermissions"/>
-    <hyperlink ref="D33" r:id="rId29" display="https://github.com/eclipse/org.aspectj"/>
-    <hyperlink ref="D34" r:id="rId30" display="https://github.com/kschat/MCVersion-Control"/>
-    <hyperlink ref="D35" r:id="rId31" display="https://github.com/JSansalone/NetBeansIDE"/>
-    <hyperlink ref="D36" r:id="rId32" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
-    <hyperlink ref="D37" r:id="rId33" display="https://github.com/zoomis/NGOMS"/>
-    <hyperlink ref="D39" r:id="rId34" display="https://github.com/Babast/Timelag"/>
-    <hyperlink ref="D40" r:id="rId35" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="D42" r:id="rId36" display="https://github.com/aleksz/driveddoc"/>
-    <hyperlink ref="D43" r:id="rId37" display="https://github.com/holisticon/tracee"/>
-    <hyperlink ref="D44" r:id="rId38" display="https://github.com/astubbs/spring-modules"/>
-    <hyperlink ref="D45" r:id="rId39" display="https://github.com/wildfly-security/security-manager"/>
-    <hyperlink ref="D46" r:id="rId40" display="https://github.com/ngty/gjman"/>
-    <hyperlink ref="D47" r:id="rId41" display="https://github.com/hypernet/visor"/>
-    <hyperlink ref="D48" r:id="rId42" display="https://github.com/stefanbirkner/system-rules"/>
-    <hyperlink ref="D49" r:id="rId43" display="https://github.com/ch33kybutt/oxygen_libcore"/>
-    <hyperlink ref="D50" r:id="rId44" display="https://github.com/apache/tomcat70"/>
+    <hyperlink ref="D10" r:id="rId6" display="http://sourceforge.net/projects/galleon/files/galleon/2.5.5/"/>
+    <hyperlink ref="D11" r:id="rId7" display="http://hadoop.apache.org/releases.html"/>
+    <hyperlink ref="D12" r:id="rId8" display="http://mvnrepository.com/artifact/org.hibernate/hibernate-core/4.2.2.Final"/>
+    <hyperlink ref="D13" r:id="rId9" display="http://hsqldb.org/"/>
+    <hyperlink ref="D14" r:id="rId10" display="http://sourceforge.net/projects/jboss/files/JBoss/JBoss-5.1.0.GA/"/>
+    <hyperlink ref="D15" r:id="rId11" display="http://www.jruby.org/download"/>
+    <hyperlink ref="D16" r:id="rId12" display="http://lucene.apache.org/"/>
+    <hyperlink ref="D17" r:id="rId13" display="http://myfaces.apache.org/"/>
+    <hyperlink ref="D18" r:id="rId14" display="http://nekohtml.sourceforge.net/"/>
+    <hyperlink ref="D19" r:id="rId15" display="https://netbeans.org/downloads/"/>
+    <hyperlink ref="D20" r:id="rId16" display="http://openjms.sourceforge.net/downloads.html"/>
+    <hyperlink ref="D21" r:id="rId17" display="http://quartz-scheduler.org/downloads"/>
+    <hyperlink ref="D22" r:id="rId18" display="http://www.quickserver.org/download.html"/>
+    <hyperlink ref="D23" r:id="rId19" location="quick-start" display="http://projects.spring.io/spring-framework/#quick-start"/>
+    <hyperlink ref="D24" r:id="rId20" display="http://struts.apache.org/"/>
+    <hyperlink ref="D25" r:id="rId21" display="http://tapestry.apache.org/download.html"/>
+    <hyperlink ref="D26" r:id="rId22" display="http://tomcat.apache.org/whichversion.html"/>
+    <hyperlink ref="D27" r:id="rId23" display="http://www.vuze.com/"/>
+    <hyperlink ref="D28" r:id="rId24" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
+    <hyperlink ref="D29" r:id="rId25" display="http://xml.apache.org/xalan-j/"/>
+    <hyperlink ref="D30" r:id="rId26" display="http://xerces.apache.org/mirrors.cgi"/>
+    <hyperlink ref="D32" r:id="rId27" display="https://github.com/tykkidream/DemoPermissions"/>
+    <hyperlink ref="D33" r:id="rId28" display="https://github.com/eclipse/org.aspectj"/>
+    <hyperlink ref="D34" r:id="rId29" display="https://github.com/kschat/MCVersion-Control"/>
+    <hyperlink ref="D35" r:id="rId30" display="https://github.com/JSansalone/NetBeansIDE"/>
+    <hyperlink ref="D36" r:id="rId31" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
+    <hyperlink ref="D37" r:id="rId32" display="https://github.com/zoomis/NGOMS"/>
+    <hyperlink ref="D39" r:id="rId33" display="https://github.com/Babast/Timelag"/>
+    <hyperlink ref="D40" r:id="rId34" display="https://github.com/JetBrains/intellij-community"/>
+    <hyperlink ref="D42" r:id="rId35" display="https://github.com/aleksz/driveddoc"/>
+    <hyperlink ref="D43" r:id="rId36" display="https://github.com/holisticon/tracee"/>
+    <hyperlink ref="D44" r:id="rId37" display="https://github.com/astubbs/spring-modules"/>
+    <hyperlink ref="D45" r:id="rId38" display="https://github.com/wildfly-security/security-manager"/>
+    <hyperlink ref="D46" r:id="rId39" display="https://github.com/ngty/gjman"/>
+    <hyperlink ref="D47" r:id="rId40" display="https://github.com/hypernet/visor"/>
+    <hyperlink ref="D48" r:id="rId41" display="https://github.com/stefanbirkner/system-rules"/>
+    <hyperlink ref="D49" r:id="rId42" display="https://github.com/ch33kybutt/oxygen_libcore"/>
+    <hyperlink ref="D50" r:id="rId43" display="https://github.com/apache/tomcat70"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
changed Eclipse source download comments
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -1702,7 +1702,8 @@
   </si>
   <si>
     <t>http://download.eclipse.org/eclipse/downloads/
-http://download.eclipse.org/eclipse/downloads/drops4/R-4.4-201406061215/</t>
+Source downloaded with the command : git clone -b master --recursive git://git.eclipse.org/gitroot/platform/eclipse.platform.releng.aggregator.git 
+As seen on the website http://www.vogella.com/tutorials/EclipsePlatformDevelopment/article.html step 11.3</t>
   </si>
   <si>
     <t>freemind</t>
@@ -3740,8 +3741,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
added the update step for the eclipse source download
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -1703,7 +1703,7 @@
   <si>
     <t>http://download.eclipse.org/eclipse/downloads/
 Source downloaded with the command : git clone -b master --recursive git://git.eclipse.org/gitroot/platform/eclipse.platform.releng.aggregator.git 
-As seen on the website http://www.vogella.com/tutorials/EclipsePlatformDevelopment/article.html step 11.3</t>
+As seen on the website http://www.vogella.com/tutorials/EclipsePlatformDevelopment/article.html step 11.3;  can then change to correct version using step 12.2</t>
   </si>
   <si>
     <t>freemind</t>
@@ -3742,7 +3742,7 @@
   <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Add some stuff on White
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="262">
   <si>
     <t>Index</t>
   </si>
@@ -2028,12 +2028,8 @@
     <t>http://sourceforge.net/projects/galleon/files/galleon/2.5.5/</t>
   </si>
   <si>
-    <t>Callback on VMStart.
-#################################################
-SecurityManager Changed:
-Server.java, setup, 211
-#################################################
-Agent OnUnload, agent exits.</t>
+    <t>SecurityManager Changed:
+Server.java, setup, 211</t>
   </si>
   <si>
     <t>At RMIProvider.java:[line 59]
@@ -2856,6 +2852,12 @@
 39:  public TestSecurityManager() {</t>
   </si>
   <si>
+    <t>A third-party library – apache ant that could potentially changes SM, while this behavior isn't cached</t>
+  </si>
+  <si>
+    <t>According to the comments made in  TestSecurityManager.java, there is a defined TestSecurityManager that is set during the JVM starts that prevents test code from calling the System.exit(0) method.</t>
+  </si>
+  <si>
     <t>myfaces_core</t>
   </si>
   <si>
@@ -2898,7 +2900,7 @@
 ./myfaces_core-2.0.2/src/myfaces-core-2.0.2-src/src/javax/faces/component/_ClassUtils.java
 373:        if (System.getSecurityManager() != null) {
 ./myfaces_core-2.0.2/src/myfaces-core-2.0.2-src/src/javax/faces/FactoryFinder.java
-363:            if (System.getSecurityManager() != null) {   </t>
+363:            if (System.getSecurityManager() != null) {</t>
   </si>
   <si>
     <t>nekohtml</t>
@@ -2917,10 +2919,14 @@
     <t>netbeans</t>
   </si>
   <si>
-    <t>6.9.1</t>
+    <t>8.0*</t>
   </si>
   <si>
     <t>https://netbeans.org/downloads/</t>
+  </si>
+  <si>
+    <t>SecurityManager Changed:
+TopSecurityManager.java, install, 542</t>
   </si>
   <si>
     <t>openjms</t>
@@ -2965,12 +2971,8 @@
     <t>http://quartz-scheduler.org/downloads</t>
   </si>
   <si>
-    <t>Callback on VMStart.
-#################################################
-SecurityManager Changed:
-QuartzServer.java, main, 178
-#################################################
-Agent OnUnload, agent exits.</t>
+    <t>SecurityManager Changed:
+QuartzServer.java, main, 178</t>
   </si>
   <si>
     <t>At QuartzServer.java:[line 178]
@@ -3016,12 +3018,8 @@
     <t>http://www.quickserver.org/download.html</t>
   </si>
   <si>
-    <t>Callback on VMStart.
-#################################################
-SecurityManager Changed:
-QuickServer.java, startServer, 453
-#################################################
-Agent OnUnload, agent exits.</t>
+    <t>SecurityManager Changed:
+QuickServer.java, startServer, 453</t>
   </si>
   <si>
     <t>At QuickServer.java:[line 453]
@@ -3236,18 +3234,20 @@
     <t>http://www.vuze.com/</t>
   </si>
   <si>
-    <t>Callback on VMStart.
-#################################################
-SecurityManager Changed:
-SESecurityManagerImpl.java, installSecurityManager, 373
-#################################################
-Agent OnUnload, agent exits.</t>
-  </si>
-  <si>
-    <t>I inserted -agentlib=./libagent.so into the vuze.sh, the file that runs the software</t>
-  </si>
-  <si>
-    <t>Vuze defines it's own Security Manager, thus strengthes its security policy</t>
+    <t>SecurityManager Changed:
+SESecurityManagerImpl.java, installSecurityManager, 373</t>
+  </si>
+  <si>
+    <t>At SESecurityManagerImpl.java:[line 373] 
+In method org.gudy.azureus2.core3.security.impl.SESecurityManagerImpl.installSecurityManager() 
+Value Not null: org.gudy.azureus2.core3.security.impl.SESecurityManagerImpl$AzureusSecurityManager 
+Value new 
+Value new[187](3) 424 
+Value Variable is set at:
+At SESecurityManagerImpl.java:[line 371]</t>
+  </si>
+  <si>
+    <t>We can see that Vuze defines it's own Security Manager called AzureusSecurityManager and changes it via installSecurityManager method in SESecurityManagerImpl.java line 373. </t>
   </si>
   <si>
     <t>weka</t>
@@ -3500,7 +3500,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3602,6 +3602,12 @@
       <name val="Calibri Light"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3730,11 +3736,11 @@
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3815,35 +3821,39 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3855,13 +3865,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3933,8 +3943,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3949,7 +3959,7 @@
     <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="8.77934272300469"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4516,28 +4526,36 @@
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="0"/>
-      <c r="J16" s="0"/>
-      <c r="K16" s="0"/>
+      <c r="J16" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="0"/>
+      <c r="F17" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="G17" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="H17" s="6"/>
+        <v>135</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
@@ -4547,22 +4565,24 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="0" t="s">
         <v>60</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="H18" s="6"/>
+        <v>139</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="I18" s="0"/>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
@@ -4572,15 +4592,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="E19" s="6"/>
+        <v>142</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="F19" s="0"/>
       <c r="G19" s="6" t="s">
         <v>112</v>
@@ -4595,25 +4617,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>37</v>
@@ -4622,7 +4644,7 @@
         <v>38</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4630,34 +4652,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4665,34 +4687,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4700,15 +4722,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E23" s="6"/>
+      <c r="F23" s="0"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
@@ -4717,15 +4740,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E24" s="6"/>
+      <c r="F24" s="0"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
@@ -4734,15 +4758,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E25" s="6"/>
+      <c r="F25" s="0"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
@@ -4751,13 +4776,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>60</v>
@@ -4766,67 +4791,78 @@
         <v>60</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="H26" s="6"/>
+        <v>184</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>185</v>
+        <v>188</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>187</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E28" s="6"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>193</v>
+        <v>196</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4834,13 +4870,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E30" s="6"/>
     </row>
@@ -4849,13 +4885,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -4864,13 +4900,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>202</v>
+        <v>204</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>205</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -4878,14 +4914,14 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>203</v>
+      <c r="B33" s="22" t="s">
+        <v>206</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>205</v>
+        <v>207</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -4894,28 +4930,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>208</v>
+        <v>210</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>211</v>
       </c>
       <c r="E34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="22" t="n">
+      <c r="A35" s="23" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>211</v>
+      <c r="B35" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>214</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -4924,13 +4960,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>217</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -4939,13 +4975,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>217</v>
+        <v>218</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>220</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -4954,13 +4990,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>223</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -4969,13 +5005,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>223</v>
+        <v>224</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>226</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -4984,13 +5020,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>229</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -4999,13 +5035,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>232</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -5014,13 +5050,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>235</v>
       </c>
       <c r="E42" s="6"/>
     </row>
@@ -5029,13 +5065,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>235</v>
+        <v>237</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>238</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -5044,13 +5080,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>238</v>
+        <v>240</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>241</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -5059,13 +5095,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>241</v>
+        <v>243</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>244</v>
       </c>
       <c r="E45" s="6"/>
     </row>
@@ -5074,13 +5110,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>244</v>
+        <v>246</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>247</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -5089,13 +5125,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>247</v>
+        <v>249</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>250</v>
       </c>
       <c r="E47" s="6"/>
     </row>
@@ -5104,13 +5140,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>250</v>
+        <v>252</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>253</v>
       </c>
       <c r="E48" s="6"/>
     </row>
@@ -5119,34 +5155,34 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>253</v>
+        <v>255</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>256</v>
       </c>
       <c r="E49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="44.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="22" t="n">
+      <c r="A50" s="23" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="23" t="s">
-        <v>254</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="D50" s="24" t="s">
-        <v>256</v>
+      <c r="B50" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>259</v>
       </c>
       <c r="E50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="10"/>
-      <c r="D51" s="20"/>
+      <c r="D51" s="21"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5154,12 +5190,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add netbeans's findbugs output, and xerces grep results
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="271">
   <si>
     <t>Index</t>
   </si>
@@ -2938,6 +2938,9 @@
 TopSecurityManager.java, install, 542</t>
   </si>
   <si>
+    <t>see attached file</t>
+  </si>
+  <si>
     <t>openjms</t>
   </si>
   <si>
@@ -3957,13 +3960,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -4035,8 +4038,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4703,7 +4706,9 @@
       <c r="E19" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="F19" s="0"/>
+      <c r="F19" s="0" t="s">
+        <v>147</v>
+      </c>
       <c r="G19" s="6" t="s">
         <v>113</v>
       </c>
@@ -4717,25 +4722,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>37</v>
@@ -4744,7 +4749,7 @@
         <v>38</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4752,34 +4757,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4787,34 +4792,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4822,16 +4827,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F23" s="0"/>
       <c r="G23" s="6"/>
@@ -4844,22 +4849,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>178</v>
-      </c>
       <c r="F24" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="0"/>
@@ -4870,25 +4875,25 @@
         <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>60</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I25" s="0"/>
       <c r="K25" s="0"/>
@@ -4898,13 +4903,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>60</v>
@@ -4913,7 +4918,7 @@
         <v>60</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>100</v>
@@ -4926,26 +4931,26 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>113</v>
       </c>
       <c r="H27" s="0"/>
       <c r="I27" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4953,13 +4958,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="0"/>
@@ -4971,20 +4976,20 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>100</v>
@@ -4995,13 +5000,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1" t="s">
@@ -5016,13 +5021,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -5031,13 +5036,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -5046,13 +5051,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -5061,13 +5066,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E34" s="6"/>
     </row>
@@ -5076,13 +5081,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -5091,13 +5096,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -5106,13 +5111,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -5121,13 +5126,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -5136,13 +5141,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -5151,13 +5156,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -5166,13 +5171,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -5181,13 +5186,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E42" s="6"/>
     </row>
@@ -5196,13 +5201,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -5211,13 +5216,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -5226,13 +5231,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E45" s="6"/>
     </row>
@@ -5241,13 +5246,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -5256,13 +5261,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E47" s="6"/>
     </row>
@@ -5271,13 +5276,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E48" s="6"/>
     </row>
@@ -5286,13 +5291,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E49" s="6"/>
     </row>
@@ -5301,13 +5306,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E50" s="6"/>
     </row>
@@ -5321,12 +5326,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the vuze source code location
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -2256,7 +2256,7 @@
 447:	 * @see java.lang.Secur</t>
   </si>
   <si>
-    <t>Nulling and weakening both happen in this application.  The weakening is running Ant because it restores the original SecurityManager while nulling occurs for running Eclipse in WebStart and in OSGi mode.  Eclipse doesn't call the SecurityManager functions of Batik.  </t>
+    <t>Nulling and weakening both happen in this application.  The weakening is running Ant because it restores the original SecurityManager while nulling occurs for running Eclipse in WebStart and in OSGi mode.  Eclipse doesn't call the SecurityManager functions of Batik.</t>
   </si>
   <si>
     <t>From running Eclipse with Web Start Main 
@@ -2386,7 +2386,7 @@
 Value aconst_null 
 Value aconst_null[1](1) 
 Value Variable is set at:
-!!!!!! This allows the SecurityManager set by the SystemBundleActivator to be removed </t>
+!!!!!! This allows the SecurityManager set by the SystemBundleActivator to be removed</t>
   </si>
   <si>
     <t>./eclipse.platform.swt/bundles/org.eclipse.swt/Eclipse SWT Browser/win32/org/eclipse/swt/browser/WebSite.java
@@ -4417,10 +4417,12 @@
     <t>Vuze (originally Azureus)</t>
   </si>
   <si>
-    <t>5.3*</t>
-  </si>
-  <si>
-    <t>http://www.vuze.com/</t>
+    <t>5.3*
+</t>
+  </si>
+  <si>
+    <t>http://www.vuze.com/
+Source: http://dev.vuze.com/</t>
   </si>
   <si>
     <t>SecurityManager Changed:
@@ -4689,7 +4691,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4791,12 +4793,6 @@
       <name val="Calibri Light"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Droid Sans Fallback"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4925,11 +4921,11 @@
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4990,10 +4986,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5022,31 +5014,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5058,13 +5050,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -5132,13 +5124,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5436,7 +5428,7 @@
       <c r="E8" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -5445,7 +5437,7 @@
       <c r="H8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="6" t="s">
         <v>74</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -5463,13 +5455,13 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>79</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -5484,13 +5476,13 @@
       <c r="H9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="17" t="s">
         <v>86</v>
       </c>
       <c r="L9" s="10" t="s">
@@ -5510,13 +5502,13 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>91</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -5592,7 +5584,7 @@
       <c r="C12" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>111</v>
       </c>
       <c r="E12" s="6"/>
@@ -5691,7 +5683,7 @@
       <c r="C15" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>128</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -5834,7 +5826,7 @@
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>155</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -5869,7 +5861,7 @@
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>163</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -5904,7 +5896,7 @@
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>173</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -5939,7 +5931,7 @@
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>183</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -5961,7 +5953,7 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>187</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -5987,7 +5979,7 @@
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>192</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -6046,10 +6038,10 @@
       <c r="B27" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="12" t="s">
         <v>203</v>
       </c>
       <c r="E27" s="10" t="s">
@@ -6070,7 +6062,7 @@
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>207</v>
       </c>
       <c r="C28" s="8" t="n">
@@ -6112,7 +6104,7 @@
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>213</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -6154,7 +6146,7 @@
       <c r="C32" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="21" t="s">
         <v>221</v>
       </c>
       <c r="E32" s="6"/>
@@ -6163,13 +6155,13 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="22" t="s">
         <v>222</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="21" t="s">
         <v>224</v>
       </c>
       <c r="E33" s="6"/>
@@ -6184,22 +6176,22 @@
       <c r="C34" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="21" t="s">
         <v>227</v>
       </c>
       <c r="E34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="24" t="n">
+      <c r="A35" s="23" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D35" s="25" t="s">
         <v>230</v>
       </c>
       <c r="E35" s="6"/>
@@ -6211,10 +6203,10 @@
       <c r="B36" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="21" t="s">
         <v>233</v>
       </c>
       <c r="E36" s="6"/>
@@ -6226,10 +6218,10 @@
       <c r="B37" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="21" t="s">
         <v>236</v>
       </c>
       <c r="E37" s="6"/>
@@ -6241,10 +6233,10 @@
       <c r="B38" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="21" t="s">
         <v>239</v>
       </c>
       <c r="E38" s="6"/>
@@ -6256,10 +6248,10 @@
       <c r="B39" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="21" t="s">
         <v>242</v>
       </c>
       <c r="E39" s="6"/>
@@ -6271,10 +6263,10 @@
       <c r="B40" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="21" t="s">
         <v>245</v>
       </c>
       <c r="E40" s="6"/>
@@ -6286,10 +6278,10 @@
       <c r="B41" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="21" t="s">
         <v>248</v>
       </c>
       <c r="E41" s="6"/>
@@ -6301,10 +6293,10 @@
       <c r="B42" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="21" t="s">
         <v>251</v>
       </c>
       <c r="E42" s="6"/>
@@ -6319,7 +6311,7 @@
       <c r="C43" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="21" t="s">
         <v>254</v>
       </c>
       <c r="E43" s="6"/>
@@ -6334,7 +6326,7 @@
       <c r="C44" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="21" t="s">
         <v>257</v>
       </c>
       <c r="E44" s="6"/>
@@ -6349,7 +6341,7 @@
       <c r="C45" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="21" t="s">
         <v>260</v>
       </c>
       <c r="E45" s="6"/>
@@ -6364,7 +6356,7 @@
       <c r="C46" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="21" t="s">
         <v>263</v>
       </c>
       <c r="E46" s="6"/>
@@ -6379,7 +6371,7 @@
       <c r="C47" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="21" t="s">
         <v>266</v>
       </c>
       <c r="E47" s="6"/>
@@ -6394,7 +6386,7 @@
       <c r="C48" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="21" t="s">
         <v>269</v>
       </c>
       <c r="E48" s="6"/>
@@ -6409,29 +6401,29 @@
       <c r="C49" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D49" s="22" t="s">
+      <c r="D49" s="21" t="s">
         <v>272</v>
       </c>
       <c r="E49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="44.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="24" t="n">
+      <c r="A50" s="23" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="25" t="s">
+      <c r="B50" s="24" t="s">
         <v>273</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="D50" s="26" t="s">
+      <c r="D50" s="25" t="s">
         <v>275</v>
       </c>
       <c r="E50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="10"/>
-      <c r="D51" s="22"/>
+      <c r="D51" s="21"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6471,27 +6463,26 @@
     <hyperlink ref="D24" r:id="rId20" display="http://struts.apache.org/"/>
     <hyperlink ref="D25" r:id="rId21" display="http://tapestry.apache.org/download.html"/>
     <hyperlink ref="D26" r:id="rId22" display="http://tomcat.apache.org/whichversion.html"/>
-    <hyperlink ref="D27" r:id="rId23" display="http://www.vuze.com/"/>
-    <hyperlink ref="D28" r:id="rId24" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
-    <hyperlink ref="D29" r:id="rId25" display="http://xml.apache.org/xalan-j/"/>
-    <hyperlink ref="D30" r:id="rId26" display="http://xerces.apache.org/mirrors.cgi"/>
-    <hyperlink ref="D32" r:id="rId27" display="https://github.com/tykkidream/DemoPermissions"/>
-    <hyperlink ref="D33" r:id="rId28" display="https://github.com/eclipse/org.aspectj"/>
-    <hyperlink ref="D34" r:id="rId29" display="https://github.com/kschat/MCVersion-Control"/>
-    <hyperlink ref="D35" r:id="rId30" display="https://github.com/JSansalone/NetBeansIDE"/>
-    <hyperlink ref="D36" r:id="rId31" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
-    <hyperlink ref="D37" r:id="rId32" display="https://github.com/zoomis/NGOMS"/>
-    <hyperlink ref="D39" r:id="rId33" display="https://github.com/Babast/Timelag"/>
-    <hyperlink ref="D40" r:id="rId34" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="D42" r:id="rId35" display="https://github.com/aleksz/driveddoc"/>
-    <hyperlink ref="D43" r:id="rId36" display="https://github.com/holisticon/tracee"/>
-    <hyperlink ref="D44" r:id="rId37" display="https://github.com/astubbs/spring-modules"/>
-    <hyperlink ref="D45" r:id="rId38" display="https://github.com/wildfly-security/security-manager"/>
-    <hyperlink ref="D46" r:id="rId39" display="https://github.com/ngty/gjman"/>
-    <hyperlink ref="D47" r:id="rId40" display="https://github.com/hypernet/visor"/>
-    <hyperlink ref="D48" r:id="rId41" display="https://github.com/stefanbirkner/system-rules"/>
-    <hyperlink ref="D49" r:id="rId42" display="https://github.com/ch33kybutt/oxygen_libcore"/>
-    <hyperlink ref="D50" r:id="rId43" display="https://github.com/apache/tomcat70"/>
+    <hyperlink ref="D28" r:id="rId23" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
+    <hyperlink ref="D29" r:id="rId24" display="http://xml.apache.org/xalan-j/"/>
+    <hyperlink ref="D30" r:id="rId25" display="http://xerces.apache.org/mirrors.cgi"/>
+    <hyperlink ref="D32" r:id="rId26" display="https://github.com/tykkidream/DemoPermissions"/>
+    <hyperlink ref="D33" r:id="rId27" display="https://github.com/eclipse/org.aspectj"/>
+    <hyperlink ref="D34" r:id="rId28" display="https://github.com/kschat/MCVersion-Control"/>
+    <hyperlink ref="D35" r:id="rId29" display="https://github.com/JSansalone/NetBeansIDE"/>
+    <hyperlink ref="D36" r:id="rId30" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
+    <hyperlink ref="D37" r:id="rId31" display="https://github.com/zoomis/NGOMS"/>
+    <hyperlink ref="D39" r:id="rId32" display="https://github.com/Babast/Timelag"/>
+    <hyperlink ref="D40" r:id="rId33" display="https://github.com/JetBrains/intellij-community"/>
+    <hyperlink ref="D42" r:id="rId34" display="https://github.com/aleksz/driveddoc"/>
+    <hyperlink ref="D43" r:id="rId35" display="https://github.com/holisticon/tracee"/>
+    <hyperlink ref="D44" r:id="rId36" display="https://github.com/astubbs/spring-modules"/>
+    <hyperlink ref="D45" r:id="rId37" display="https://github.com/wildfly-security/security-manager"/>
+    <hyperlink ref="D46" r:id="rId38" display="https://github.com/ngty/gjman"/>
+    <hyperlink ref="D47" r:id="rId39" display="https://github.com/hypernet/visor"/>
+    <hyperlink ref="D48" r:id="rId40" display="https://github.com/stefanbirkner/system-rules"/>
+    <hyperlink ref="D49" r:id="rId41" display="https://github.com/ch33kybutt/oxygen_libcore"/>
+    <hyperlink ref="D50" r:id="rId42" display="https://github.com/apache/tomcat70"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added comments for Vuze
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="282">
   <si>
     <t>Index</t>
   </si>
@@ -4425,8 +4425,12 @@
 Source: http://dev.vuze.com/</t>
   </si>
   <si>
-    <t>SecurityManager Changed:
-SESecurityManagerImpl.java, installSecurityManager, 373</t>
+    <t>Callback on VMStart.
+#################################################
+SecurityManager Changed:
+SESecurityManagerImpl.java, installSecurityManager, 373
+#################################################
+Agent OnUnload, agent exits.</t>
   </si>
   <si>
     <t>At SESecurityManagerImpl.java:[line 373] 
@@ -4434,11 +4438,495 @@
 Value Not null: org.gudy.azureus2.core3.security.impl.SESecurityManagerImpl$AzureusSecurityManager 
 Value new 
 Value new[187](3) 424 
-Value Variable is set at:
-At SESecurityManagerImpl.java:[line 371]</t>
-  </si>
-  <si>
-    <t>We can see that Vuze defines it's own Security Manager called AzureusSecurityManager and changes it via installSecurityManager method in SESecurityManagerImpl.java line 373.</t>
+Value Variable is set at: At 
+SESecurityManagerImpl.java:[line 371]</t>
+  </si>
+  <si>
+    <t>./org/gudy/azureus2/pluginsimpl/local/utils/resourcedownloader/ResourceDownloaderURLImpl.java
+286:						SESecurityManager.setPasswordHandler( url, this );
+354:								if ( SESecurityManager.installServerCertificates( url ) != null ){
+388:						SESecurityManager.setPasswordHandler( url, null );
+582:						SESecurityManager.setPasswordHandler( outer_url, this );
+1073:										if ( SESecurityManager.installServerCertificates( current_url ) != null ){
+1144:						SESecurityManager.setPasswordHandler( outer_url, null );
+./org/gudy/azureus2/pluginsimpl/local/utils/resourceuploader/ResourceUploaderURLImpl.java
+35:import org.gudy.azureus2.core3.security.SESecurityManager;
+144:						SESecurityManager.setPasswordHandler( url, this );
+224:								if ( SESecurityManager.installServerCertificates( url ) != null ){
+258:						SESecurityManager.setPasswordHandler( url, null );
+./org/gudy/azureus2/pluginsimpl/local/utils/UtilitiesImpl.java
+51:import org.gudy.azureus2.plugins.utils.security.SESecurityManager;
+525:	public SESecurityManager
+526:	getSecurityManager()
+528:		return( new SESecurityManagerImpl( core ));
+./org/gudy/azureus2/pluginsimpl/local/utils/security/SESecurityManagerImpl.java
+55:SESecurityManagerImpl 
+56:	implements org.gudy.azureus2.plugins.utils.security.SESecurityManager
+64:	SESecurityManagerImpl(
+96:			SESecurityManager.installAuthenticator();
+132:		SESecurityManager.addPasswordListener( sepl );
+143:			SESecurityManager.removePasswordListener( sepl );
+165:		SESecurityManager.addCertificateListener( sepl );
+176:			SESecurityManager.removeCertificateListener( sepl );
+184:		return( SESecurityManager.installServerCertificates( url ));
+192:		return( SESecurityManager.getKeyStore());
+200:		return( SESecurityManager.getTrustStore());
+212:		return( SESecurityManager.createSelfSignedCertificate(alias, cert_dn, strength ));		
+./org/gudy/azureus2/pluginsimpl/local/utils/security/SESTSConnectionImpl.java
+55:import org.gudy.azureus2.plugins.utils.security.SESecurityManager;
+629:			if ( block_crypto == SESecurityManager.BLOCK_ENCRYPTION_NONE ){
+781:			if ( block_crypto != SESecurityManager.BLOCK_ENCRYPTION_NONE ){
+820:			}else if ( block_crypto != SESecurityManager.BLOCK_ENCRYPTION_NONE ){
+./org/gudy/azureus2/pluginsimpl/local/PluginInitializer.java
+39:import org.gudy.azureus2.core3.security.SESecurityManager;
+2427:		Class&lt;?&gt;[] stack = SESecurityManager.getClassContext();
+2490:			Class[] context = SESecurityManager.getClassContext();
+./org/gudy/azureus2/plugins/utils/Utilities.java
+203:	public SESecurityManager
+204:	getSecurityManager();
+./org/gudy/azureus2/plugins/utils/security/SEPublicKey.java
+36:		 * import via SESecurityManager.decodePublicKey
+./org/gudy/azureus2/plugins/utils/security/SESecurityManager.java
+40:SESecurityManager 
+./org/gudy/azureus2/ui/swt/views/configsections/ConfigSectionSecurity.java
+40:import org.gudy.azureus2.core3.security.SESecurityManager;
+163:										if ( SESecurityManager.resetTrustStore( false )){
+195:	    reset_certs_button.setEnabled( SESecurityManager.resetTrustStore( true ));
+272:			        	SESecurityManager.clearPasswords();
+./org/gudy/azureus2/ui/swt/UIExitUtilsSWT.java
+34:import org.gudy.azureus2.core3.security.SESecurityManager;
+136:					SESecurityManager.exitVM(1);
+./org/gudy/azureus2/ui/swt/auth/CertificateTrustWindow.java
+38:import org.gudy.azureus2.core3.security.SESecurityManager;
+56:		SESecurityManager.addCertificateListener( this );
+./org/gudy/azureus2/ui/swt/auth/AuthenticatorWindow.java
+64:		SESecurityManager.addPasswordListener( this );
+./org/gudy/azureus2/ui/swt/auth/CertificateCreatorWindow.java
+38:import org.gudy.azureus2.core3.security.SESecurityManager;
+127:			alias_field.setText( SESecurityManager.DEFAULT_ALIAS );
+233:						SESecurityManager.createSelfSignedCertificate( alias, dn, strength );
+./org/gudy/azureus2/ui/webplugin/WebPlugin.java
+1412:									hash = plugin_interface.getUtilities().getSecurityManager().calculateSHA1( 
+./org/gudy/azureus2/core3/torrentdownloader/impl/TorrentDownloaderImpl.java
+50:import org.gudy.azureus2.core3.security.SESecurityManager;
+418:	    				if ( SESecurityManager.installServerCertificates( url ) != null ){
+./org/gudy/azureus2/core3/util/jar/AEJarBuilder.java
+36:import org.gudy.azureus2.core3.security.SESecurityManager;
+111:				SEKeyDetails	kd = SESecurityManager.getKeyDetails( sign_alias );
+126:							SESecurityManager.getKeystoreName(),
+127:							SESecurityManager.getKeystorePassword());
+./org/gudy/azureus2/core3/util/ED2KHasher.java
+138:		SESecurityManager.initialise();
+./org/gudy/azureus2/core3/util/TimeLimitedTask.java
+24:import org.gudy.azureus2.core3.security.SESecurityManager;
+89:							SESecurityManager.stopThread( thread );
+./org/gudy/azureus2/core3/tracker/client/impl/bt/TRTrackerBTAnnouncerImpl.java
+45:import org.gudy.azureus2.core3.security.SESecurityManager;
+1257:						if ( SESecurityManager.installServerCertificates( reqUrl ) != null ){
+1573: 				 auth = SESecurityManager.getPasswordAuthentication( UDP_REALM, reqUrl );
+1715:			 						SESecurityManager.setPasswordAuthenticationOutcome( UDP_REALM, reqUrl, true );
+1810:			SESecurityManager.setPasswordAuthenticationOutcome( UDP_REALM, reqUrl, false );
+./org/gudy/azureus2/core3/tracker/client/impl/bt/TrackerStatus.java
+43:import org.gudy.azureus2.core3.security.SESecurityManager;
+1202:					if ( SESecurityManager.installServerCertificates( reqUrl ) != null ){
+1273:			auth = SESecurityManager.getPasswordAuthentication( "UDP Tracker", reqUrl );
+1431:			SESecurityManager.setPasswordAuthenticationOutcome( TRTrackerBTAnnouncerImpl.UDP_REALM, reqUrl, auth_ok );
+./org/gudy/azureus2/core3/tracker/server/impl/tcp/blocking/TRBlockingServer.java
+34:import org.gudy.azureus2.core3.security.SESecurityManager;
+99:					SSLServerSocketFactory factory = SESecurityManager.getSSLServerSocketFactory();
+./org/gudy/azureus2/core3/config/impl/ConfigurationChecker.java
+246:	  	SESecurityManager.initialise();
+./org/gudy/azureus2/core3/security/impl/SESecurityManagerImpl.java
+52:import org.gudy.azureus2.core3.security.SESecurityManager;
+62:SESecurityManagerImpl 
+66:	protected static SESecurityManagerImpl	singleton = new SESecurityManagerImpl();
+133:	private	AzureusSecurityManager	my_sec_man;
+135:	protected AEMonitor	this_mon	= new AEMonitor( "SESecurityManager" );
+137:	public static SESecurityManagerImpl
+165:		keystore_name 		= FileUtil.getUserFile(SESecurityManager.SSL_KEYS).getAbsolutePath();
+166:		truststore_name 	= FileUtil.getUserFile(SESecurityManager.SSL_CERTS).getAbsolutePath();
+170:		System.setProperty( "javax.net.ssl.trustStorePassword", SESecurityManager.SSL_PASSWORD );
+202:			SESecurityManagerBC.initialise();
+212:		installSecurityManager();
+347:		return(	SESecurityManager.SSL_PASSWORD );	
+351:	installSecurityManager()
+369:				final SecurityManager	old_sec_man	= System.getSecurityManager();
+371:				my_sec_man = new AzureusSecurityManager( old_sec_man );
+373:				System.setSecurityManager( my_sec_man );
+430:					protected AEMonitor	auth_mon = new AEMonitor( "SESecurityManager:auth");
+568:					keystore.store(out, SESecurityManager.SSL_PASSWORD.toCharArray());
+622:				keystore.load(in, SESecurityManager.SSL_PASSWORD.toCharArray());
+665:				key_store.load(kis, SESecurityManager.SSL_PASSWORD.toCharArray());
+676:		keyManagerFactory.init(key_store, SESecurityManager.SSL_PASSWORD.toCharArray());
+721:		final Key key = key_store.getKey( alias, SESecurityManager.SSL_PASSWORD.toCharArray());
+766:		return( SESecurityManagerBC.createSelfSignedCertificate( this, alias, cert_dn, strength ));
+1072:			key_store.setKeyEntry( alias, public_key, SESecurityManager.SSL_PASSWORD.toCharArray(), certChain );
+1079:				key_store.store(out, SESecurityManager.SSL_PASSWORD.toCharArray());
+1125:					keystore.store(out, SESecurityManager.SSL_PASSWORD.toCharArray());
+1369:	AzureusSecurityManager
+1370:		extends SecurityManager
+1372:		private SecurityManager	old_sec_man;
+1375:		AzureusSecurityManager(
+1376:			SecurityManager		_old_sec_man )
+1443:				}else if ( name.equals( "setSecurityManager" )){
+1485:		SESecurityManagerImpl man = SESecurityManagerImpl.getSingleton();
+./org/gudy/azureus2/core3/security/impl/SESecurityManagerBC.java
+48:SESecurityManagerBC 
+93:		SESecurityManagerImpl	manager,
+./org/gudy/azureus2/core3/security/SESecurityManager.java
+2: * File    : SESecurityManager.java
+39:SESecurityManager
+52:		SESecurityManagerImpl.getSingleton().initialise();
+59:		SESecurityManagerImpl.getSingleton().exitVM(status);
+66:		SESecurityManagerImpl.getSingleton().stopThread(t);
+71:		SESecurityManagerImpl.getSingleton().installAuthenticator();
+78:		return( SESecurityManagerImpl.getSingleton().resetTrustStore( test_only ));
+84:		return(	SESecurityManagerImpl.getSingleton().getKeystoreName());
+90:		return(	SESecurityManagerImpl.getSingleton().getKeystorePassword());
+98:		return( SESecurityManagerImpl.getSingleton().getSSLServerSocketFactory());
+104:		return( SESecurityManagerImpl.getSingleton().getSSLSocketFactory());
+111:		return( SESecurityManagerImpl.getSingleton().installServerCertificates(https_url));
+120:		return( SESecurityManagerImpl.getSingleton().installServerCertificates( alias, ip, port ));
+131:		return( SESecurityManagerImpl.getSingleton().createSelfSignedCertificate( alias, cert_dn, strength ));
+140:		return( SESecurityManagerImpl.getSingleton().getKeyDetails( alias ));
+148:		return( SESecurityManagerImpl.getSingleton().getKeyStore());
+156:		return( SESecurityManagerImpl.getSingleton().getTrustStore());
+164:		return( SESecurityManagerImpl.getSingleton().getPasswordAuthentication(realm, tracker));	
+173:		SESecurityManagerImpl.getSingleton().setPasswordAuthenticationOutcome(realm, tracker, success);	
+180:		SESecurityManagerImpl.getSingleton().addPasswordListener(l);	
+187:		SESecurityManagerImpl.getSingleton().removePasswordListener(l);	
+193:		SESecurityManagerImpl.getSingleton().clearPasswords();
+200:		SESecurityManagerImpl.getSingleton().setThreadPasswordHandler(l);
+206:		SESecurityManagerImpl.getSingleton().unsetThreadPasswordHandler();
+215:		SESecurityManagerImpl.getSingleton().setPasswordHandler( url, l );
+222:		SESecurityManagerImpl.getSingleton().addCertificateListener(l);
+230:		SESecurityManagerImpl.getSingleton().setCertificateHandler(url,l);
+237:		SESecurityManagerImpl.getSingleton().removeCertificateListener(l);
+243:		return( SESecurityManagerImpl.getSingleton().getClassContext());
+./com/aelitis/azureus/core/networkmanager/admin/impl/NetworkAdminSpeedTesterBTImpl.java
+40:import org.gudy.azureus2.core3.security.SESecurityManager;
+204:            	SESecurityManager.setCertificateHandler( 
+./com/aelitis/azureus/core/download/DiskManagerFileInfoURL.java
+36:import org.gudy.azureus2.core3.security.SESecurityManager;
+569:						SESecurityManager.setThreadPasswordHandler( DiskManagerFileInfoURL.this );
+670:										if ( SESecurityManager.installServerCertificates( target ) != null ){
+733:						SESecurityManager.unsetThreadPasswordHandler();
+./com/aelitis/azureus/core/util/http/HTTPAuthHelper.java
+37:import org.gudy.azureus2.core3.security.SESecurityManager;
+507:						factory = SESecurityManager.installServerCertificates( "AZ-sniffer:" + delegate_to_host + ":" + port, delegate_to_host, delegate_to_port );
+./com/aelitis/azureus/core/impl/AzureusCoreImpl.java
+46:import org.gudy.azureus2.core3.security.SESecurityManager;
+1460:						SESecurityManager.exitVM(0);
+1682:								SESecurityManager.exitVM(0);
+./com/aelitis/azureus/core/security/CryptoManagerPasswordHandler.java
+46:		 * @param handler_type	from AESecurityManager.HANDLER_x enum
+./com/aelitis/azureus/core/security/impl/CryptoManagerImpl.java
+40:import org.gudy.azureus2.core3.security.SESecurityManager;
+91:		SESecurityManager.initialise();
+./com/aelitis/azureus/plugins/extseed/util/ExternalSeedHTTPDownloaderRange.java
+44:import org.gudy.azureus2.core3.security.SESecurityManager;
+124:			SESecurityManager.setThreadPasswordHandler( this );
+245:							if ( SESecurityManager.installServerCertificates( target ) != null ){
+428:			SESecurityManager.unsetThreadPasswordHandler();
+./com/aelitis/azureus/plugins/extseed/util/ExternalSeedHTTPDownloaderLinear.java
+35:import org.gudy.azureus2.core3.security.SESecurityManager;
+213:					SESecurityManager.setThreadPasswordHandler( this );
+402:					SESecurityManager.unsetThreadPasswordHandler();
+./com/aelitis/azureus/plugins/net/buddy/BuddyPluginBuddy.java
+51:import org.gudy.azureus2.plugins.utils.security.SESecurityManager;
+2268:			SESecurityManager sec_man = plugin.getSecurityManager();
+./com/aelitis/azureus/plugins/net/buddy/BuddyPlugin.java
+65:import org.gudy.azureus2.plugins.utils.security.SESecurityManager;
+161:	public static final int BLOCK_CRYPTO	= SESecurityManager.BLOCK_ENCRYPTION_AES;
+164:	//public static final int BLOCK_CRYPTO	= SESecurityManager.BLOCK_ENCRYPTION_NONE;
+199:	private SESecurityManager	sec_man;
+260:		sec_man = plugin_interface.getUtilities().getSecurityManager();
+3087:	protected SESecurityManager
+3088:	getSecurityManager()
+./com/aelitis/azureus/plugins/upnp/UPnPPlugin.java
+610:										plugin_interface.getUtilities().getSecurityManager().calculateSHA1(
+./com/aelitis/azureus/ui/swt/shells/main/MainWindowImpl.java
+1558:		//SESecurityManagerImpl.getSingleton().exitVM(0);
+./com/aelitis/azureus/ui/console/MakeTorrent.java
+129:      SESecurityManager.exitVM(0);
+134:      if(!ok) SESecurityManager.exitVM(-1);
+139:      SESecurityManager.exitVM(-1);
+146:      SESecurityManager.exitVM(-1);
+</t>
+  </si>
+  <si>
+    <t>This program sets a SecurityManager during normal execution.  It allows weakening if a SecurityManager is set before running which allows for changing the SecurityManager and it contains code to save the old SecurityManager and use it in general permission checks.  It seems that the SecurityManager can only be set once (the that does it is a singleton), however there is one file which seems to call it with a parameter.  However, I don't see a constuctor with a parameter so I think that is dead code, if that is not the case, the SecurityManager may be set twice on some executions.  However, it is only set once on a normal Execution.  Also, that constructor with a parameter is used to return a different type so I think this section is buggy at best (in file UtilitiesImpl.java)</t>
+  </si>
+  <si>
+    <t>Callback on VMStart.
+#################################################
+SecurityManager Changed:
+SESecurityManagerImpl.java, installSecurityManager, 373
+#################################################
+Agent OnUnload, agent exits.
+Vuze intializes a singleton that starts a SecurityManager.  This SecurityManager uses the old SecurityManager for general permission checks and prevents system exits in certain configurations.  It also allows all file writes and reads.</t>
+  </si>
+  <si>
+    <t>At SESecurityManagerImpl.java:[line 373] 
+In method org.gudy.azureus2.core3.security.impl.SESecurityManagerImpl.installSecurityManager() 
+Value Not null: org.gudy.azureus2.core3.security.impl.SESecurityManagerImpl$AzureusSecurityManager 
+Value new 
+Value new[187](3) 424 
+Value Variable is set at: At 
+SESecurityManagerImpl.java:[line 371]
+This line is covered in the dynamic analysis.  The program sets a AzureusSecurityManager and saves the old one inside of the new SecurityManager for general permission checks.  However, specific permission checks (such as system exit and file write) are handled by the AzureusSecurityManager.</t>
+  </si>
+  <si>
+    <t>./org/gudy/azureus2/pluginsimpl/local/utils/resourcedownloader/ResourceDownloaderURLImpl.java
+286:						SESecurityManager.setPasswordHandler( url, this );
+354:								if ( SESecurityManager.installServerCertificates( url ) != null ){
+388:						SESecurityManager.setPasswordHandler( url, null );
+582:						SESecurityManager.setPasswordHandler( outer_url, this );
+1073:										if ( SESecurityManager.installServerCertificates( current_url ) != null ){
+1144:						SESecurityManager.setPasswordHandler( outer_url, null );
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/pluginsimpl/local/utils/resourceuploader/ResourceUploaderURLImpl.java
+35:import org.gudy.azureus2.core3.security.SESecurityManager;
+144:						SESecurityManager.setPasswordHandler( url, this );
+224:								if ( SESecurityManager.installServerCertificates( url ) != null ){
+258:						SESecurityManager.setPasswordHandler( url, null );
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/pluginsimpl/local/utils/UtilitiesImpl.java
+51:import org.gudy.azureus2.plugins.utils.security.SESecurityManager;
+525:	public SESecurityManager
+526:	getSecurityManager()
+528:		return( new SESecurityManagerImpl( core ));
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager.  getSecurityMnager returns an SESecurityManager
+./org/gudy/azureus2/pluginsimpl/local/utils/security/SESecurityManagerImpl.java
+55:SESecurityManagerImpl 
+56:	implements org.gudy.azureus2.plugins.utils.security.SESecurityManager
+64:	SESecurityManagerImpl(
+96:			SESecurityManager.installAuthenticator();
+132:		SESecurityManager.addPasswordListener( sepl );
+143:			SESecurityManager.removePasswordListener( sepl );
+165:		SESecurityManager.addCertificateListener( sepl );
+176:			SESecurityManager.removeCertificateListener( sepl );
+184:		return( SESecurityManager.installServerCertificates( url ));
+192:		return( SESecurityManager.getKeyStore());
+200:		return( SESecurityManager.getTrustStore());
+212:		return( SESecurityManager.createSelfSignedCertificate(alias, cert_dn, strength ));		
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/pluginsimpl/local/utils/security/SESTSConnectionImpl.java
+55:import org.gudy.azureus2.plugins.utils.security.SESecurityManager;
+629:			if ( block_crypto == SESecurityManager.BLOCK_ENCRYPTION_NONE ){
+781:			if ( block_crypto != SESecurityManager.BLOCK_ENCRYPTION_NONE ){
+820:			}else if ( block_crypto != SESecurityManager.BLOCK_ENCRYPTION_NONE ){
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/pluginsimpl/local/PluginInitializer.java
+39:import org.gudy.azureus2.core3.security.SESecurityManager;
+2427:		Class&lt;?&gt;[] stack = SESecurityManager.getClassContext();
+2490:			Class[] context = SESecurityManager.getClassContext();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/plugins/utils/Utilities.java
+203:	public SESecurityManager
+204:	getSecurityManager();
+Method declaration for interface
+./org/gudy/azureus2/plugins/utils/security/SEPublicKey.java
+36:		 * import via SESecurityManager.decodePublicKey
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/plugins/utils/security/SESecurityManager.java
+40:SESecurityManager 
+This is an interface
+./org/gudy/azureus2/ui/swt/views/configsections/ConfigSectionSecurity.java
+40:import org.gudy.azureus2.core3.security.SESecurityManager;
+163:										if ( SESecurityManager.resetTrustStore( false )){
+195:	    reset_certs_button.setEnabled( SESecurityManager.resetTrustStore( true ));
+272:			        	SESecurityManager.clearPasswords();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/ui/swt/UIExitUtilsSWT.java
+34:import org.gudy.azureus2.core3.security.SESecurityManager;
+136:					SESecurityManager.exitVM(1);
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/ui/swt/auth/CertificateTrustWindow.java
+38:import org.gudy.azureus2.core3.security.SESecurityManager;
+56:		SESecurityManager.addCertificateListener( this );
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/ui/swt/auth/AuthenticatorWindow.java
+64:		SESecurityManager.addPasswordListener( this );
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/ui/swt/auth/CertificateCreatorWindow.java
+38:import org.gudy.azureus2.core3.security.SESecurityManager;
+127:			alias_field.setText( SESecurityManager.DEFAULT_ALIAS );
+233:						SESecurityManager.createSelfSignedCertificate( alias, dn, strength );
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/ui/webplugin/WebPlugin.java
+1412:									hash = plugin_interface.getUtilities().getSecurityManager().calculateSHA1( 
+The getSecurityManager returns the authetication manager SESecurityManager.  SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/core3/torrentdownloader/impl/TorrentDownloaderImpl.java
+50:import org.gudy.azureus2.core3.security.SESecurityManager;
+418:	    				if ( SESecurityManager.installServerCertificates( url ) != null ){
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/core3/util/jar/AEJarBuilder.java
+36:import org.gudy.azureus2.core3.security.SESecurityManager;
+111:				SEKeyDetails	kd = SESecurityManager.getKeyDetails( sign_alias );
+126:							SESecurityManager.getKeystoreName(),
+127:							SESecurityManager.getKeystorePassword());
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/core3/util/ED2KHasher.java
+138:		SESecurityManager.initialise();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/core3/util/TimeLimitedTask.java
+24:import org.gudy.azureus2.core3.security.SESecurityManager;
+89:							SESecurityManager.stopThread( thread );
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/core3/tracker/client/impl/bt/TRTrackerBTAnnouncerImpl.java
+45:import org.gudy.azureus2.core3.security.SESecurityManager;
+1257:						if ( SESecurityManager.installServerCertificates( reqUrl ) != null ){
+1573: 				 auth = SESecurityManager.getPasswordAuthentication( UDP_REALM, reqUrl );
+1715:			 						SESecurityManager.setPasswordAuthenticationOutcome( UDP_REALM, reqUrl, true );
+1810:			SESecurityManager.setPasswordAuthenticationOutcome( UDP_REALM, reqUrl, false );
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/core3/tracker/client/impl/bt/TrackerStatus.java
+43:import org.gudy.azureus2.core3.security.SESecurityManager;
+1202:					if ( SESecurityManager.installServerCertificates( reqUrl ) != null ){
+1273:			auth = SESecurityManager.getPasswordAuthentication( "UDP Tracker", reqUrl );
+1431:			SESecurityManager.setPasswordAuthenticationOutcome( TRTrackerBTAnnouncerImpl.UDP_REALM, reqUrl, auth_ok );
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/core3/tracker/server/impl/tcp/blocking/TRBlockingServer.java
+34:import org.gudy.azureus2.core3.security.SESecurityManager;
+99:					SSLServerSocketFactory factory = SESecurityManager.getSSLServerSocketFactory();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/core3/config/impl/ConfigurationChecker.java
+246:	  	SESecurityManager.initialise();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./org/gudy/azureus2/core3/security/impl/SESecurityManagerImpl.java
+52:import org.gudy.azureus2.core3.security.SESecurityManager;
+62:SESecurityManagerImpl 
+66:	protected static SESecurityManagerImpl	singleton = new SESecurityManagerImpl();
+133:	private	AzureusSecurityManager	my_sec_man;
+135:	protected AEMonitor	this_mon	= new AEMonitor( "SESecurityManager" );
+137:	public static SESecurityManagerImpl
+165:		keystore_name 		= FileUtil.getUserFile(SESecurityManager.SSL_KEYS).getAbsolutePath();
+166:		truststore_name 	= FileUtil.getUserFile(SESecurityManager.SSL_CERTS).getAbsolutePath();
+170:		System.setProperty( "javax.net.ssl.trustStorePassword", SESecurityManager.SSL_PASSWORD );
+202:			SESecurityManagerBC.initialise();
+212:		installSecurityManager();
+347:		return(	SESecurityManager.SSL_PASSWORD );	
+351:	installSecurityManager()
+369:				final SecurityManager	old_sec_man	= System.getSecurityManager();
+371:				my_sec_man = new AzureusSecurityManager( old_sec_man );
+373:				System.setSecurityManager( my_sec_man );
+430:					protected AEMonitor	auth_mon = new AEMonitor( "SESecurityManager:auth");
+568:					keystore.store(out, SESecurityManager.SSL_PASSWORD.toCharArray());
+622:				keystore.load(in, SESecurityManager.SSL_PASSWORD.toCharArray());
+665:				key_store.load(kis, SESecurityManager.SSL_PASSWORD.toCharArray());
+676:		keyManagerFactory.init(key_store, SESecurityManager.SSL_PASSWORD.toCharArray());
+721:		final Key key = key_store.getKey( alias, SESecurityManager.SSL_PASSWORD.toCharArray());
+766:		return( SESecurityManagerBC.createSelfSignedCertificate( this, alias, cert_dn, strength ));
+1072:			key_store.setKeyEntry( alias, public_key, SESecurityManager.SSL_PASSWORD.toCharArray(), certChain );
+1079:				key_store.store(out, SESecurityManager.SSL_PASSWORD.toCharArray());
+1125:					keystore.store(out, SESecurityManager.SSL_PASSWORD.toCharArray());
+1369:	AzureusSecurityManager
+1370:		extends SecurityManager
+1372:		private SecurityManager	old_sec_man;
+1375:		AzureusSecurityManager(
+1376:			SecurityManager		_old_sec_man )
+1443:				}else if ( name.equals( "setSecurityManager" )){
+1485:		SESecurityManagerImpl man = SESecurityManagerImpl.getSingleton();
+This class sets and defines an AzureusSecurityManager.  This SecurityManager does extend System.lang.SecurityManager.  This SecurityManager is set on normal execuation and will allow weakening if the program has permissions to set a SecurityManager.
+./org/gudy/azureus2/core3/security/impl/SESecurityManagerBC.java
+48:SESecurityManagerBC 
+93:		SESecurityManagerImpl	manager,
+uses the program that class a system securityManager to communicate with the authentication manager
+./org/gudy/azureus2/core3/security/SESecurityManager.java
+2: * File    : SESecurityManager.java
+39:SESecurityManager
+52:		SESecurityManagerImpl.getSingleton().initialise();
+59:		SESecurityManagerImpl.getSingleton().exitVM(status);
+66:		SESecurityManagerImpl.getSingleton().stopThread(t);
+71:		SESecurityManagerImpl.getSingleton().installAuthenticator();
+78:		return( SESecurityManagerImpl.getSingleton().resetTrustStore( test_only ));
+84:		return(	SESecurityManagerImpl.getSingleton().getKeystoreName());
+90:		return(	SESecurityManagerImpl.getSingleton().getKeystorePassword());
+98:		return( SESecurityManagerImpl.getSingleton().getSSLServerSocketFactory());
+104:		return( SESecurityManagerImpl.getSingleton().getSSLSocketFactory());
+111:		return( SESecurityManagerImpl.getSingleton().installServerCertificates(https_url));
+120:		return( SESecurityManagerImpl.getSingleton().installServerCertificates( alias, ip, port ));
+131:		return( SESecurityManagerImpl.getSingleton().createSelfSignedCertificate( alias, cert_dn, strength ));
+140:		return( SESecurityManagerImpl.getSingleton().getKeyDetails( alias ));
+148:		return( SESecurityManagerImpl.getSingleton().getKeyStore());
+156:		return( SESecurityManagerImpl.getSingleton().getTrustStore());
+164:		return( SESecurityManagerImpl.getSingleton().getPasswordAuthentication(realm, tracker));	
+173:		SESecurityManagerImpl.getSingleton().setPasswordAuthenticationOutcome(realm, tracker, success);	
+180:		SESecurityManagerImpl.getSingleton().addPasswordListener(l);	
+187:		SESecurityManagerImpl.getSingleton().removePasswordListener(l);	
+193:		SESecurityManagerImpl.getSingleton().clearPasswords();
+200:		SESecurityManagerImpl.getSingleton().setThreadPasswordHandler(l);
+206:		SESecurityManagerImpl.getSingleton().unsetThreadPasswordHandler();
+215:		SESecurityManagerImpl.getSingleton().setPasswordHandler( url, l );
+222:		SESecurityManagerImpl.getSingleton().addCertificateListener(l);
+230:		SESecurityManagerImpl.getSingleton().setCertificateHandler(url,l);
+237:		SESecurityManagerImpl.getSingleton().removeCertificateListener(l);
+243:		return( SESecurityManagerImpl.getSingleton().getClassContext());
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/core/networkmanager/admin/impl/NetworkAdminSpeedTesterBTImpl.java
+40:import org.gudy.azureus2.core3.security.SESecurityManager;
+204:            	SESecurityManager.setCertificateHandler( 
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/core/download/DiskManagerFileInfoURL.java
+36:import org.gudy.azureus2.core3.security.SESecurityManager;
+569:						SESecurityManager.setThreadPasswordHandler( DiskManagerFileInfoURL.this );
+670:										if ( SESecurityManager.installServerCertificates( target ) != null ){
+733:						SESecurityManager.unsetThreadPasswordHandler();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/core/util/http/HTTPAuthHelper.java
+37:import org.gudy.azureus2.core3.security.SESecurityManager;
+507:						factory = SESecurityManager.installServerCertificates( "AZ-sniffer:" + delegate_to_host + ":" + port, delegate_to_host, delegate_to_port );
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/core/impl/AzureusCoreImpl.java
+46:import org.gudy.azureus2.core3.security.SESecurityManager;
+1460:						SESecurityManager.exitVM(0);
+1682:								SESecurityManager.exitVM(0);
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/core/security/CryptoManagerPasswordHandler.java
+46:		 * @param handler_type	from AESecurityManager.HANDLER_x enum
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/core/security/impl/CryptoManagerImpl.java
+40:import org.gudy.azureus2.core3.security.SESecurityManager;
+91:		SESecurityManager.initialise();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/plugins/extseed/util/ExternalSeedHTTPDownloaderRange.java
+44:import org.gudy.azureus2.core3.security.SESecurityManager;
+124:			SESecurityManager.setThreadPasswordHandler( this );
+245:							if ( SESecurityManager.installServerCertificates( target ) != null ){
+428:			SESecurityManager.unsetThreadPasswordHandler();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/plugins/extseed/util/ExternalSeedHTTPDownloaderLinear.java
+35:import org.gudy.azureus2.core3.security.SESecurityManager;
+213:					SESecurityManager.setThreadPasswordHandler( this );
+402:					SESecurityManager.unsetThreadPasswordHandler();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/plugins/net/buddy/BuddyPluginBuddy.java
+51:import org.gudy.azureus2.plugins.utils.security.SESecurityManager;
+2268:			SESecurityManager sec_man = plugin.getSecurityManager();
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/plugins/net/buddy/BuddyPlugin.java
+65:import org.gudy.azureus2.plugins.utils.security.SESecurityManager;
+161:	public static final int BLOCK_CRYPTO	= SESecurityManager.BLOCK_ENCRYPTION_AES;
+164:	//public static final int BLOCK_CRYPTO	= SESecurityManager.BLOCK_ENCRYPTION_NONE;
+199:	private SESecurityManager	sec_man;
+260:		sec_man = plugin_interface.getUtilities().getSecurityManager();
+3087:	protected SESecurityManager
+3088:	getSecurityManager()
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/plugins/upnp/UPnPPlugin.java
+610:										plugin_interface.getUtilities().getSecurityManager().calculateSHA1(
+This getSecurityManager returns an SESecurityManager.  SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+./com/aelitis/azureus/ui/swt/shells/main/MainWindowImpl.java
+1558:		//SESecurityManagerImpl.getSingleton().exitVM(0);
+This is commented out
+./com/aelitis/azureus/ui/console/MakeTorrent.java
+129:      SESecurityManager.exitVM(0);
+134:      if(!ok) SESecurityManager.exitVM(-1);
+139:      SESecurityManager.exitVM(-1);
+146:      SESecurityManager.exitVM(-1);
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+</t>
   </si>
   <si>
     <t>weka</t>
@@ -5129,8 +5617,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6050,12 +6538,20 @@
       <c r="F27" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H27" s="0"/>
-      <c r="I27" s="1" t="s">
+      <c r="G27" s="10" t="s">
         <v>206</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6063,13 +6559,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="0"/>
@@ -6081,20 +6577,20 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>107</v>
@@ -6105,13 +6601,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1" t="s">
@@ -6126,13 +6622,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -6141,13 +6637,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -6156,13 +6652,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -6171,13 +6667,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E34" s="6"/>
     </row>
@@ -6186,13 +6682,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -6201,13 +6697,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -6216,13 +6712,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -6231,13 +6727,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -6246,13 +6742,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -6261,13 +6757,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -6276,13 +6772,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -6291,13 +6787,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="E42" s="6"/>
     </row>
@@ -6306,13 +6802,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -6321,13 +6817,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -6336,13 +6832,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="E45" s="6"/>
     </row>
@@ -6351,13 +6847,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -6366,13 +6862,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E47" s="6"/>
     </row>
@@ -6381,13 +6877,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="E48" s="6"/>
     </row>
@@ -6396,13 +6892,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E49" s="6"/>
     </row>
@@ -6411,13 +6907,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E50" s="6"/>
     </row>
@@ -6431,12 +6927,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the comments for Weka
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="289">
   <si>
     <t>Index</t>
   </si>
@@ -4417,8 +4417,7 @@
     <t>Vuze (originally Azureus)</t>
   </si>
   <si>
-    <t>5.3*
-</t>
+    <t>5.3*</t>
   </si>
   <si>
     <t>http://www.vuze.com/
@@ -4651,8 +4650,7 @@
 129:      SESecurityManager.exitVM(0);
 134:      if(!ok) SESecurityManager.exitVM(-1);
 139:      SESecurityManager.exitVM(-1);
-146:      SESecurityManager.exitVM(-1);
-</t>
+146:      SESecurityManager.exitVM(-1);</t>
   </si>
   <si>
     <t>This program sets a SecurityManager during normal execution.  It allows weakening if a SecurityManager is set before running which allows for changing the SecurityManager and it contains code to save the old SecurityManager and use it in general permission checks.  It seems that the SecurityManager can only be set once (the that does it is a singleton), however there is one file which seems to call it with a parameter.  However, I don't see a constuctor with a parameter so I think that is dead code, if that is not the case, the SecurityManager may be set twice on some executions.  However, it is only set once on a normal Execution.  Also, that constructor with a parameter is used to return a different type so I think this section is buggy at best (in file UtilitiesImpl.java)</t>
@@ -4925,14 +4923,63 @@
 134:      if(!ok) SESecurityManager.exitVM(-1);
 139:      SESecurityManager.exitVM(-1);
 146:      SESecurityManager.exitVM(-1);
-SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager
+SESecurityManager is an authentication manger that does not extend System.lang.SecurityManager</t>
+  </si>
+  <si>
+    <t>weka</t>
+  </si>
+  <si>
+    <t>http://www.cs.waikato.ac.nz/ml/weka/downloading.html</t>
+  </si>
+  <si>
+    <t>Callback on VMStart.
+#################################################
+SecurityManager Changed:
+RemoteEngine.java, main, 323
+#################################################
+Agent OnUnload, agent exits.</t>
+  </si>
+  <si>
+    <t>At RemoteEngine.java:[line 323]
+In method weka.experiment.RemoteEngine.main(String[])
+Value Not null: java.rmi.RMISecurityManager 
+Value new Value new[187](3) 88 
+Value Variable is set at</t>
+  </si>
+  <si>
+    <t>./src/main/java/weka/experiment/RemoteEngine.java
+35:import java.rmi.RMISecurityManager;
+322:    if (System.getSecurityManager() == null) {
+323:      System.setSecurityManager(new RMISecurityManager());
 </t>
   </si>
   <si>
-    <t>weka</t>
-  </si>
-  <si>
-    <t>http://www.cs.waikato.ac.nz/ml/weka/downloading.html</t>
+    <t>No weaking or nulling occurs.  There are multiple mains for this jar and only the RemoteEngine.java file sets a SecurityManager if the program is started without running one.  It sets the SecurityManager as the first thing in the main function.</t>
+  </si>
+  <si>
+    <t>Callback on VMStart.
+#################################################
+SecurityManager Changed:
+RemoteEngine.java, main, 323
+#################################################
+Agent OnUnload, agent exits.
+When running the remote engine main, a SecurityManager is set if one is not already set as the first part of the main.</t>
+  </si>
+  <si>
+    <t>At RemoteEngine.java:[line 323]
+In method weka.experiment.RemoteEngine.main(String[])
+Value Not null: java.rmi.RMISecurityManager 
+Value new Value new[187](3) 88 
+Value Variable is set at
+This is covered in the dynamic analysis.  When a the main for the Remote Engine is called, the program sets a security manager if one is not already set.</t>
+  </si>
+  <si>
+    <t>./src/main/java/weka/experiment/RemoteEngine.java
+35:import java.rmi.RMISecurityManager;
+322:    if (System.getSecurityManager() == null) {
+323:      System.setSecurityManager(new RMISecurityManager());
+This is covered in the static and dynamic analysis.  If a SecurityManager is not set when starting the main in RemoteEngine.java, a new SecurityManager is set.
+</t>
   </si>
   <si>
     <t>xalan</t>
@@ -5538,13 +5585,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -5617,8 +5664,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6435,6 +6482,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="0"/>
+      <c r="J23" s="0"/>
       <c r="K23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6461,6 +6509,7 @@
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="0"/>
+      <c r="J24" s="0"/>
       <c r="K24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6489,6 +6538,7 @@
         <v>196</v>
       </c>
       <c r="I25" s="0"/>
+      <c r="J25" s="0"/>
       <c r="K25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6517,6 +6567,7 @@
         <v>107</v>
       </c>
       <c r="I26" s="0"/>
+      <c r="J26" s="0"/>
       <c r="K26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6567,30 +6618,47 @@
       <c r="D28" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="0"/>
-      <c r="G28" s="0"/>
-      <c r="H28" s="0"/>
+      <c r="E28" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>107</v>
@@ -6601,13 +6669,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1" t="s">
@@ -6622,13 +6690,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -6637,13 +6705,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -6652,13 +6720,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -6667,13 +6735,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="E34" s="6"/>
     </row>
@@ -6682,13 +6750,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -6697,13 +6765,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -6712,13 +6780,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -6727,13 +6795,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -6742,13 +6810,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -6757,13 +6825,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -6772,13 +6840,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -6787,13 +6855,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="E42" s="6"/>
     </row>
@@ -6802,13 +6870,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -6817,13 +6885,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -6832,13 +6900,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="E45" s="6"/>
     </row>
@@ -6847,13 +6915,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -6862,13 +6930,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="E47" s="6"/>
     </row>
@@ -6877,13 +6945,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="E48" s="6"/>
     </row>
@@ -6892,13 +6960,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="E49" s="6"/>
     </row>
@@ -6907,13 +6975,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="E50" s="6"/>
     </row>
@@ -6927,12 +6995,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the color of Vuze - I realize it is not the right shade but I don't seem to have the background color of the other green ones as an option in LibreOffice
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -4950,8 +4950,7 @@
     <t>./src/main/java/weka/experiment/RemoteEngine.java
 35:import java.rmi.RMISecurityManager;
 322:    if (System.getSecurityManager() == null) {
-323:      System.setSecurityManager(new RMISecurityManager());
-</t>
+323:      System.setSecurityManager(new RMISecurityManager());</t>
   </si>
   <si>
     <t>No weaking or nulling occurs.  There are multiple mains for this jar and only the RemoteEngine.java file sets a SecurityManager if the program is started without running one.  It sets the SecurityManager as the first thing in the main function.</t>
@@ -4978,8 +4977,7 @@
 35:import java.rmi.RMISecurityManager;
 322:    if (System.getSecurityManager() == null) {
 323:      System.setSecurityManager(new RMISecurityManager());
-This is covered in the static and dynamic analysis.  If a SecurityManager is not set when starting the main in RemoteEngine.java, a new SecurityManager is set.
-</t>
+This is covered in the static and dynamic analysis.  If a SecurityManager is not set when starting the main in RemoteEngine.java, a new SecurityManager is set.</t>
   </si>
   <si>
     <t>xalan</t>
@@ -5226,7 +5224,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5331,6 +5329,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF00AE00"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="1"/>
@@ -5351,7 +5356,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5380,6 +5385,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3DEB3D"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -5456,11 +5467,11 @@
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5545,35 +5556,39 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5585,20 +5600,20 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFC5000B"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF3DEB3D"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -5644,7 +5659,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFA5A5A5"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00AE00"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -5664,8 +5679,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6574,7 +6589,7 @@
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="21" t="s">
         <v>201</v>
       </c>
       <c r="C27" s="10" t="s">
@@ -6710,7 +6725,7 @@
       <c r="C32" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="22" t="s">
         <v>232</v>
       </c>
       <c r="E32" s="6"/>
@@ -6719,13 +6734,13 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="23" t="s">
         <v>233</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="22" t="s">
         <v>235</v>
       </c>
       <c r="E33" s="6"/>
@@ -6740,22 +6755,22 @@
       <c r="C34" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="22" t="s">
         <v>238</v>
       </c>
       <c r="E34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="n">
+      <c r="A35" s="24" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="26" t="s">
         <v>241</v>
       </c>
       <c r="E35" s="6"/>
@@ -6767,10 +6782,10 @@
       <c r="B36" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="22" t="s">
         <v>244</v>
       </c>
       <c r="E36" s="6"/>
@@ -6782,10 +6797,10 @@
       <c r="B37" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="22" t="s">
         <v>247</v>
       </c>
       <c r="E37" s="6"/>
@@ -6797,10 +6812,10 @@
       <c r="B38" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="22" t="s">
         <v>250</v>
       </c>
       <c r="E38" s="6"/>
@@ -6812,10 +6827,10 @@
       <c r="B39" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="27" t="s">
         <v>252</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="22" t="s">
         <v>253</v>
       </c>
       <c r="E39" s="6"/>
@@ -6827,10 +6842,10 @@
       <c r="B40" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="22" t="s">
         <v>256</v>
       </c>
       <c r="E40" s="6"/>
@@ -6842,10 +6857,10 @@
       <c r="B41" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="29" t="s">
         <v>258</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="22" t="s">
         <v>259</v>
       </c>
       <c r="E41" s="6"/>
@@ -6857,10 +6872,10 @@
       <c r="B42" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="22" t="s">
         <v>262</v>
       </c>
       <c r="E42" s="6"/>
@@ -6875,7 +6890,7 @@
       <c r="C43" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="22" t="s">
         <v>265</v>
       </c>
       <c r="E43" s="6"/>
@@ -6890,7 +6905,7 @@
       <c r="C44" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="22" t="s">
         <v>268</v>
       </c>
       <c r="E44" s="6"/>
@@ -6905,7 +6920,7 @@
       <c r="C45" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D45" s="22" t="s">
         <v>271</v>
       </c>
       <c r="E45" s="6"/>
@@ -6920,7 +6935,7 @@
       <c r="C46" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D46" s="21" t="s">
+      <c r="D46" s="22" t="s">
         <v>274</v>
       </c>
       <c r="E46" s="6"/>
@@ -6935,7 +6950,7 @@
       <c r="C47" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D47" s="22" t="s">
         <v>277</v>
       </c>
       <c r="E47" s="6"/>
@@ -6950,7 +6965,7 @@
       <c r="C48" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="D48" s="22" t="s">
         <v>280</v>
       </c>
       <c r="E48" s="6"/>
@@ -6965,29 +6980,29 @@
       <c r="C49" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D49" s="21" t="s">
+      <c r="D49" s="22" t="s">
         <v>283</v>
       </c>
       <c r="E49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="44.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="23" t="n">
+      <c r="A50" s="24" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="D50" s="25" t="s">
+      <c r="D50" s="26" t="s">
         <v>286</v>
       </c>
       <c r="E50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="10"/>
-      <c r="D51" s="21"/>
+      <c r="D51" s="22"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add comments for Netbeans and springframework
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="295">
   <si>
     <t>Index</t>
   </si>
@@ -4029,6 +4029,18 @@
     <t>see attached file</t>
   </si>
   <si>
+    <t>Only one place detected. When the program is run, the GuiRunlevel.java runs the GUI and then installs the SM to advance the policy. SM is defined in TopSecurityManager.java</t>
+  </si>
+  <si>
+    <t> see left, there is also a place that sets TopSM to null, in Activatior.java line 105. However, this behavior is not detected</t>
+  </si>
+  <si>
+    <t>There is one called TopSM which is loaded when app is run. TopSM is the core SM that NB basic uses. It checks various behaviors like read or write. Besides this, there is another SM called CountingSecurityManager used in testing, and does basically the same.</t>
+  </si>
+  <si>
+    <t>There are other place where SM is changed found by FindBugs. However, those behaviors are done by third-party library code. Findbugs catches the TopSM installation, which proves that it's the only place where SM is changed for Netbeans.</t>
+  </si>
+  <si>
     <t>openjms</t>
   </si>
   <si>
@@ -4214,6 +4226,148 @@
   </si>
   <si>
     <t>A library framework</t>
+  </si>
+  <si>
+    <t>./spring-core/src/test/java/org/springframework/core/env/StandardEnvironmentTests.java
+376:	public void getSystemProperties_withAndWithoutSecurityManager() {
+394:		SecurityManager oldSecurityManager = System.getSecurityManager();
+395:		SecurityManager securityManager = new SecurityManager() {
+414:		System.setSecurityManager(securityManager);
+432:			// SecurityManager that disallows access to system properties), they
+443:		System.setSecurityManager(oldSecurityManager);
+451:	public void getSystemEnvironment_withAndWithoutSecurityManager() {
+461:		SecurityManager oldSecurityManager = System.getSecurityManager();
+462:		SecurityManager securityManager = new SecurityManager() {
+476:		System.setSecurityManager(securityManager);
+486:		System.setSecurityManager(oldSecurityManager);
+./spring-beans/src/test/java/org/springframework/beans/factory/support/security/CallbacksSecurityTests.java
+285:		if (System.getSecurityManager() == null) {
+294:			System.setSecurityManager(new SecurityManager());
+./spring-beans/src/main/java/org/springframework/beans/factory/support/FactoryBeanRegistrySupport.java
+57:			if (System.getSecurityManager() != null) {
+153:			if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/AbstractBeanFactory.java
+156:	/** Security context used when running with a SecurityManager */
+460:				if (System.getSecurityManager() != null) {
+1308:			if (System.getSecurityManager() != null) {
+1555:		AccessControlContext acc = (System.getSecurityManager() != null ? getAccessControlContext() : null);
+./spring-beans/src/main/java/org/springframework/beans/factory/support/DefaultListableBeanFactory.java
+238:			if (System.getSecurityManager() != null) {
+689:					if (System.getSecurityManager() != null &amp;&amp; factory instanceof SmartFactoryBean) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/AbstractAutowireCapableBeanFactory.java
+355:			if (System.getSecurityManager() != null) {
+1061:			if (System.getSecurityManager() != null) {
+1416:		if (System.getSecurityManager() != null) {
+1531:		if (System.getSecurityManager() != null) {
+1598:			if (System.getSecurityManager() != null) {
+1657:		if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/DisposableBeanAdapter.java
+248:				if (System.getSecurityManager() != null) {
+286:			if (System.getSecurityManager() != null) {
+327:			if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/SimpleInstantiationStrategy.java
+71:						if (System.getSecurityManager() != null) {
+115:			if (System.getSecurityManager() != null) {
+150:			if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/ConstructorResolver.java
+258:			if (System.getSecurityManager() != null) {
+324:		if (System.getSecurityManager() != null) {
+573:			if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/BeanWrapperImpl.java
+731:				if (System.getSecurityManager() != null) {
+746:			if (System.getSecurityManager() != null) {
+1084:								if (System.getSecurityManager()!= null) {
+1098:								if (System.getSecurityManager() != null) {
+1129:					if (System.getSecurityManager()!= null) {
+1143:				if (System.getSecurityManager() != null) {
+./spring-context/src/test/java/org/springframework/context/support/EnvironmentSecurityManagerIntegrationTests.java
+39: * Tests integration between Environment and SecurityManagers. See SPR-9970.
+43:public class EnvironmentSecurityManagerIntegrationTests {
+45:	private SecurityManager originalSecurityManager;
+50:		originalSecurityManager = System.getSecurityManager();
+58:		System.setSecurityManager(originalSecurityManager);
+63:		SecurityManager securityManager = new SecurityManager() {
+74:		System.setSecurityManager(securityManager);
+84:		SecurityManager securityManager = new SecurityManager() {
+105:		System.setSecurityManager(securityManager);
+./spring-context/src/test/java/org/springframework/context/expression/ApplicationContextExpressionTests.java
+263:	public void systemPropertiesSecurityManager() {
+272:		SecurityManager oldSecurityManager = System.getSecurityManager();
+276:			SecurityManager securityManager = new SecurityManager() {
+286:			System.setSecurityManager(securityManager);
+294:			System.setSecurityManager(oldSecurityManager);
+./spring-core/src/test/java/org/springframework/core/env/StandardEnvironmentTests.java
+376:	public void getSystemProperties_withAndWithoutSecurityManager() {
+394:		SecurityManager oldSecurityManager = System.getSecurityManager();
+395:		SecurityManager securityManager = new SecurityManager() {
+414:		System.setSecurityManager(securityManager);
+432:			// SecurityManager that disallows access to system properties), they
+443:		System.setSecurityManager(oldSecurityManager);
+451:	public void getSystemEnvironment_withAndWithoutSecurityManager() {
+461:		SecurityManager oldSecurityManager = System.getSecurityManager();
+462:		SecurityManager securityManager = new SecurityManager() {
+476:		System.setSecurityManager(securityManager);
+486:		System.setSecurityManager(oldSecurityManager);
+./spring-beans/src/test/java/org/springframework/beans/factory/support/security/CallbacksSecurityTests.java
+285:		if (System.getSecurityManager() == null) {
+294:			System.setSecurityManager(new SecurityManager());
+./spring-beans/src/main/java/org/springframework/beans/factory/support/FactoryBeanRegistrySupport.java
+57:			if (System.getSecurityManager() != null) {
+153:			if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/AbstractBeanFactory.java
+156:	/** Security context used when running with a SecurityManager */
+460:				if (System.getSecurityManager() != null) {
+1308:			if (System.getSecurityManager() != null) {
+1555:		AccessControlContext acc = (System.getSecurityManager() != null ? getAccessControlContext() : null);
+./spring-beans/src/main/java/org/springframework/beans/factory/support/DefaultListableBeanFactory.java
+238:			if (System.getSecurityManager() != null) {
+689:					if (System.getSecurityManager() != null &amp;&amp; factory instanceof SmartFactoryBean) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/AbstractAutowireCapableBeanFactory.java
+355:			if (System.getSecurityManager() != null) {
+1061:			if (System.getSecurityManager() != null) {
+1416:		if (System.getSecurityManager() != null) {
+1531:		if (System.getSecurityManager() != null) {
+1598:			if (System.getSecurityManager() != null) {
+1657:		if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/DisposableBeanAdapter.java
+248:				if (System.getSecurityManager() != null) {
+286:			if (System.getSecurityManager() != null) {
+327:			if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/SimpleInstantiationStrategy.java
+71:						if (System.getSecurityManager() != null) {
+115:			if (System.getSecurityManager() != null) {
+150:			if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/factory/support/ConstructorResolver.java
+258:			if (System.getSecurityManager() != null) {
+324:		if (System.getSecurityManager() != null) {
+573:			if (System.getSecurityManager() != null) {
+./spring-beans/src/main/java/org/springframework/beans/BeanWrapperImpl.java
+731:				if (System.getSecurityManager() != null) {
+746:			if (System.getSecurityManager() != null) {
+1084:								if (System.getSecurityManager()!= null) {
+1098:								if (System.getSecurityManager() != null) {
+1129:					if (System.getSecurityManager()!= null) {
+1143:				if (System.getSecurityManager() != null) {
+./spring-context/src/test/java/org/springframework/context/support/EnvironmentSecurityManagerIntegrationTests.java
+39: * Tests integration between Environment and SecurityManagers. See SPR-9970.
+43:public class EnvironmentSecurityManagerIntegrationTests {
+45:	private SecurityManager originalSecurityManager;
+50:		originalSecurityManager = System.getSecurityManager();
+58:		System.setSecurityManager(originalSecurityManager);
+63:		SecurityManager securityManager = new SecurityManager() {
+74:		System.setSecurityManager(securityManager);
+84:		SecurityManager securityManager = new SecurityManager() {
+105:		System.setSecurityManager(securityManager);
+./spring-context/src/test/java/org/springframework/context/expression/ApplicationContextExpressionTests.java
+263:	public void systemPropertiesSecurityManager() {
+272:		SecurityManager oldSecurityManager = System.getSecurityManager();
+276:			SecurityManager securityManager = new SecurityManager() {
+286:			System.setSecurityManager(securityManager);
+294:			System.setSecurityManager(oldSecurityManager);
+</t>
+  </si>
+  <si>
+    <t>The code basically does System.setSecurityManager(System.getSecurityManager()); Policy is maintained.</t>
   </si>
   <si>
     <t>struts</t>
@@ -5471,7 +5625,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5544,6 +5698,10 @@
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="5" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5600,13 +5758,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -5674,13 +5832,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6137,8 +6294,12 @@
       <c r="D12" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="0"/>
+      <c r="E12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="G12" s="6" t="s">
         <v>112</v>
       </c>
@@ -6197,7 +6358,9 @@
       <c r="D14" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="F14" s="10" t="s">
         <v>119</v>
       </c>
@@ -6304,7 +6467,9 @@
       <c r="D17" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="F17" s="0" t="s">
         <v>60</v>
       </c>
@@ -6331,7 +6496,9 @@
       <c r="D18" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="F18" s="0" t="s">
         <v>60</v>
       </c>
@@ -6367,35 +6534,43 @@
       <c r="G19" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="0"/>
-      <c r="J19" s="0"/>
-      <c r="K19" s="0"/>
+      <c r="H19" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>155</v>
+      <c r="B20" s="19" t="s">
+        <v>159</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>37</v>
@@ -6404,42 +6579,42 @@
         <v>38</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>163</v>
+      <c r="B21" s="20" t="s">
+        <v>167</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6447,55 +6622,61 @@
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="20" t="s">
-        <v>183</v>
+      <c r="B23" s="21" t="s">
+        <v>187</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F23" s="0"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+        <v>190</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>192</v>
+      </c>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
@@ -6504,25 +6685,27 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="20" t="s">
-        <v>187</v>
+      <c r="B24" s="21" t="s">
+        <v>193</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="H24" s="6"/>
+        <v>197</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
       <c r="K24" s="0"/>
@@ -6531,26 +6714,26 @@
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="20" t="s">
-        <v>192</v>
+      <c r="B25" s="21" t="s">
+        <v>198</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>60</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
@@ -6561,13 +6744,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>60</v>
@@ -6576,7 +6759,7 @@
         <v>60</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>107</v>
@@ -6589,35 +6772,35 @@
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>201</v>
+      <c r="B27" s="22" t="s">
+        <v>207</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6625,34 +6808,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6660,20 +6843,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="E29" s="6"/>
+        <v>228</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="F29" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>107</v>
@@ -6684,20 +6869,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="E30" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="F30" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>120</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6705,13 +6895,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -6720,13 +6910,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>232</v>
+        <v>237</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>238</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -6734,14 +6924,14 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="23" t="s">
-        <v>233</v>
+      <c r="B33" s="24" t="s">
+        <v>239</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>235</v>
+        <v>240</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>241</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -6750,28 +6940,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>238</v>
+        <v>243</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>244</v>
       </c>
       <c r="E34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="24" t="n">
+      <c r="A35" s="25" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>241</v>
+      <c r="B35" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>247</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -6780,13 +6970,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>244</v>
+        <v>248</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>250</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -6795,13 +6985,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>247</v>
+        <v>251</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>253</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -6810,13 +7000,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>250</v>
+        <v>254</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>256</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -6825,13 +7015,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>253</v>
+        <v>257</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>259</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -6840,13 +7030,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>256</v>
+        <v>260</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>261</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>262</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -6855,13 +7045,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>259</v>
+        <v>263</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>265</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -6870,13 +7060,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>262</v>
+        <v>266</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>268</v>
       </c>
       <c r="E42" s="6"/>
     </row>
@@ -6885,13 +7075,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>265</v>
+        <v>270</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>271</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -6900,13 +7090,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>268</v>
+        <v>273</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>274</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -6915,13 +7105,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>271</v>
+        <v>276</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>277</v>
       </c>
       <c r="E45" s="6"/>
     </row>
@@ -6930,13 +7120,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>274</v>
+        <v>279</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>280</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -6945,13 +7135,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>277</v>
+        <v>282</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>283</v>
       </c>
       <c r="E47" s="6"/>
     </row>
@@ -6960,13 +7150,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>286</v>
       </c>
       <c r="E48" s="6"/>
     </row>
@@ -6975,34 +7165,34 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>283</v>
+        <v>288</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>289</v>
       </c>
       <c r="E49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="44.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="24" t="n">
+      <c r="A50" s="25" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>285</v>
-      </c>
-      <c r="D50" s="26" t="s">
-        <v>286</v>
+      <c r="B50" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>292</v>
       </c>
       <c r="E50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="10"/>
-      <c r="D51" s="22"/>
+      <c r="D51" s="23"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7010,12 +7200,12 @@
     </row>
     <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done only grep till Timelag
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="304">
   <si>
     <t>Index</t>
   </si>
@@ -4032,7 +4032,7 @@
     <t>Only one place detected. When the program is run, the GuiRunlevel.java runs the GUI and then installs the SM to advance the policy. SM is defined in TopSecurityManager.java</t>
   </si>
   <si>
-    <t> see left, there is also a place that sets TopSM to null, in Activatior.java line 105. However, this behavior is not detected</t>
+    <t>see left, there is also a place that sets TopSM to null, in Activatior.java line 105. However, this behavior is not detected</t>
   </si>
   <si>
     <t>There is one called TopSM which is loaded when app is run. TopSM is the core SM that NB basic uses. It checks various behaviors like read or write. Besides this, there is another SM called CountingSecurityManager used in testing, and does basically the same.</t>
@@ -4363,8 +4363,7 @@
 272:		SecurityManager oldSecurityManager = System.getSecurityManager();
 276:			SecurityManager securityManager = new SecurityManager() {
 286:			System.setSecurityManager(securityManager);
-294:			System.setSecurityManager(oldSecurityManager);
-</t>
+294:			System.setSecurityManager(oldSecurityManager);</t>
   </si>
   <si>
     <t>The code basically does System.setSecurityManager(System.getSecurityManager()); Policy is maintained.</t>
@@ -5193,6 +5192,49 @@
     <t>https://github.com/viqsoft/Jmin</t>
   </si>
   <si>
+    <t>./src/org/jmin/gui/GuiDefinition.java
+24:import org.jmin.gui.security.SecurityManager;
+432:			return SecurityManager.getInstance().implies(permissionArray);
+./src/org/jmin/gui/security/LogoutHook.java
+5:  private SecurityManager securityManager;
+7:  public LogoutHook(SecurityManager securityManager) {
+./src/org/jmin/gui/security/SecurityLauncher.java
+21:    SecurityManager.getInstance().initSecurityContext(getSecurityContext());
+22:    SecurityManager.getInstance().login();
+31:    SecurityManager.getInstance().initSecurityContext(getSecurityContext());
+32:    SecurityManager.getInstance().login();
+42:    SecurityManager.getInstance().initSecurityContext(getSecurityContext());
+43:    SecurityManager.getInstance().login();
+./src/org/jmin/gui/security/SecurityView.java
+65:      return SecurityManager.getInstance().implies(permissionArray);
+./src/org/jmin/gui/security/SecurityManager.java
+10:public class SecurityManager {
+15:  private static SecurityManager securityManager;
+20:  public synchronized static SecurityManager getInstance() {
+22:      securityManager = new SecurityManager();
+./src/org/jmin/gui/GuiDefinition.java
+24:import org.jmin.gui.security.SecurityManager;
+432:			return SecurityManager.getInstance().implies(permissionArray);
+./src/org/jmin/gui/security/LogoutHook.java
+5:  private SecurityManager securityManager;
+7:  public LogoutHook(SecurityManager securityManager) {
+./src/org/jmin/gui/security/SecurityLauncher.java
+21:    SecurityManager.getInstance().initSecurityContext(getSecurityContext());
+22:    SecurityManager.getInstance().login();
+31:    SecurityManager.getInstance().initSecurityContext(getSecurityContext());
+32:    SecurityManager.getInstance().login();
+42:    SecurityManager.getInstance().initSecurityContext(getSecurityContext());
+43:    SecurityManager.getInstance().login();
+./src/org/jmin/gui/security/SecurityView.java
+65:      return SecurityManager.getInstance().implies(permissionArray);
+./src/org/jmin/gui/security/SecurityManager.java
+10:public class SecurityManager {
+15:  private static SecurityManager securityManager;
+20:  public synchronized static SecurityManager getInstance() {
+22:      securityManager = new SecurityManager();
+</t>
+  </si>
+  <si>
     <t>DemoPermissions (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
   </si>
   <si>
@@ -5202,6 +5244,19 @@
     <t>https://github.com/tykkidream/DemoPermissions</t>
   </si>
   <si>
+    <t>./src/main/java/demo/permissions/security/manager/SecurityBus.java
+18:			SecurityManager securityManager = SecurityManager.getManager();
+./src/main/java/demo/permissions/security/manager/SecurityManager.java
+6:public class SecurityManager {
+9:	private static SecurityManager securityManager = new SecurityManager();
+11:	public static SecurityManager getManager() {
+15:	private SecurityManager() {
+</t>
+  </si>
+  <si>
+    <t>Simply from grep result we know that it doesn't change SM anyways.</t>
+  </si>
+  <si>
     <t>AspectJ</t>
   </si>
   <si>
@@ -5211,6 +5266,23 @@
     <t>https://github.com/eclipse/org.aspectj</t>
   </si>
   <si>
+    <t>./testing/src/org/aspectj/testing/harness/bridge/JavaRun.java
+183:            RunSecurityManager.ME.setJavaRunThread(this);
+202:            if (thrown instanceof RunSecurityManager.ExitCalledException) {
+203:                int i = ((RunSecurityManager.ExitCalledException) thrown).exitCode;
+205:            } else if (thrown instanceof RunSecurityManager.AwtUsedException) {
+207:                throw (RunSecurityManager.AwtUsedException) thrown;
+218:        } catch (RunSecurityManager.ExitCalledException e) {
+232:            RunSecurityManager.ME.releaseJavaRunThread(this);
+595:                System.setSecurityManager(RunSecurityManager.ME);
+795:    public static class RunSecurityManager extends SecurityManager {
+796:        public static RunSecurityManager ME = new RunSecurityManager();
+798:        private RunSecurityManager(){}
+./tests/ltw/NullSecurityManager.java
+2:public class NullSecurityManager extends SecurityManager {
+</t>
+  </si>
+  <si>
     <t>MCVersion-Control (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
   </si>
   <si>
@@ -5220,6 +5292,9 @@
     <t>https://github.com/kschat/MCVersion-Control</t>
   </si>
   <si>
+    <t>A trivial one</t>
+  </si>
+  <si>
     <t>Netbeans (I think this one can be removed because we are already covering it in the qualitas corpus)</t>
   </si>
   <si>
@@ -5256,6 +5331,22 @@
     <t>https://github.com/vdupain/refact4j</t>
   </si>
   <si>
+    <t>./src/test/java/org/refact4j/util/CheckExitSecurityManager.java
+3:public class CheckExitSecurityManager extends SecurityManagerDecorator {
+5:    public CheckExitSecurityManager(SecurityManager securityManager) {
+10:        throw new SecurityManagerSecurityException(status);
+./src/test/java/org/refact4j/util/SecurityManagerSecurityException.java
+3:public class SecurityManagerSecurityException extends SecurityException {
+6:    public SecurityManagerSecurityException(int status) {
+./src/test/java/org/refact4j/util/SecurityManagerDecorator.java
+7:public class SecurityManagerDecorator extends SecurityManager {
+9:    private SecurityManager securityManager;
+11:    public SecurityManagerDecorator(SecurityManager securityManager) {</t>
+  </si>
+  <si>
+    <t>Defines SM in the test code but never set it explicitly.</t>
+  </si>
+  <si>
     <t>TimeLag (This one might be malicious)</t>
   </si>
   <si>
@@ -5263,6 +5354,14 @@
   </si>
   <si>
     <t>https://github.com/Babast/Timelag</t>
+  </si>
+  <si>
+    <t>./src/jtimelag/JTimelag.java
+6:        System.setSecurityManager(null); 
+</t>
+  </si>
+  <si>
+    <t>It's setting SM to null in Jtimelag.java and set a frame visible.</t>
   </si>
   <si>
     <t>IntelliJ IDEA Community Edition</t>
@@ -5510,7 +5609,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5526,13 +5625,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFE6E6FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF99CC99"/>
       </patternFill>
     </fill>
     <fill>
@@ -5545,6 +5644,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF3DEB3D"/>
         <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6E6FF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CC99"/>
+        <bgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
   </fills>
@@ -5625,7 +5736,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5718,11 +5829,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5758,13 +5877,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -5782,12 +5901,12 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF99CC99"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFE6E6FF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -5834,10 +5953,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6890,322 +7009,387 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+    <row r="31" s="23" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B32" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D32" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="G32" s="10" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+    <row r="33" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B33" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="C33" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E32" s="6"/>
+      <c r="D33" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="G33" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>241</v>
+      </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+    <row r="34" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" customFormat="false" ht="43.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="26" t="s">
         <v>242</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="25" t="s">
         <v>244</v>
       </c>
       <c r="E34" s="6"/>
+      <c r="G34" s="10" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="35" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25" t="n">
+    <row r="35" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="H35" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="27" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>246</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>249</v>
-      </c>
-      <c r="D36" s="23" t="s">
+      <c r="B36" s="28" t="s">
         <v>250</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>252</v>
       </c>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="H37" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="C37" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>253</v>
-      </c>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>37</v>
-      </c>
       <c r="B38" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="D38" s="23" t="s">
         <v>256</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>258</v>
       </c>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="G39" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C39" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>259</v>
-      </c>
-      <c r="E39" s="6"/>
+      <c r="B40" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="G40" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+    <row r="41" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>261</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>40</v>
-      </c>
       <c r="B41" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C41" s="30" t="s">
-        <v>264</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>265</v>
+        <v>269</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>271</v>
       </c>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>267</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>268</v>
+        <v>272</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>274</v>
       </c>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>271</v>
+        <v>275</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>277</v>
       </c>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D44" s="23" t="s">
-        <v>274</v>
+        <v>279</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>280</v>
       </c>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>277</v>
+        <v>282</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>283</v>
       </c>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D46" s="23" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>286</v>
       </c>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>283</v>
+        <v>288</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>289</v>
       </c>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>286</v>
+        <v>291</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>292</v>
       </c>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D49" s="23" t="s">
-        <v>289</v>
+        <v>294</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>295</v>
       </c>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" customFormat="false" ht="44.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="25" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="C50" s="25" t="s">
-        <v>291</v>
-      </c>
-      <c r="D50" s="27" t="s">
-        <v>292</v>
+    <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>298</v>
       </c>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="10"/>
-      <c r="D51" s="23"/>
+    <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="27" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>301</v>
+      </c>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="10"/>
+      <c r="D52" s="25"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E53" s="1" t="s">
-        <v>293</v>
-      </c>
+    <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="6"/>
     </row>
-    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>294</v>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -7235,23 +7419,24 @@
     <hyperlink ref="D28" r:id="rId23" display="http://www.cs.waikato.ac.nz/ml/weka/downloading.html"/>
     <hyperlink ref="D29" r:id="rId24" display="http://xml.apache.org/xalan-j/"/>
     <hyperlink ref="D30" r:id="rId25" display="http://xerces.apache.org/mirrors.cgi"/>
-    <hyperlink ref="D32" r:id="rId26" display="https://github.com/tykkidream/DemoPermissions"/>
-    <hyperlink ref="D33" r:id="rId27" display="https://github.com/eclipse/org.aspectj"/>
-    <hyperlink ref="D34" r:id="rId28" display="https://github.com/kschat/MCVersion-Control"/>
-    <hyperlink ref="D35" r:id="rId29" display="https://github.com/JSansalone/NetBeansIDE"/>
-    <hyperlink ref="D36" r:id="rId30" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
-    <hyperlink ref="D37" r:id="rId31" display="https://github.com/zoomis/NGOMS"/>
-    <hyperlink ref="D39" r:id="rId32" display="https://github.com/Babast/Timelag"/>
-    <hyperlink ref="D40" r:id="rId33" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="D42" r:id="rId34" display="https://github.com/aleksz/driveddoc"/>
-    <hyperlink ref="D43" r:id="rId35" display="https://github.com/holisticon/tracee"/>
-    <hyperlink ref="D44" r:id="rId36" display="https://github.com/astubbs/spring-modules"/>
-    <hyperlink ref="D45" r:id="rId37" display="https://github.com/wildfly-security/security-manager"/>
-    <hyperlink ref="D46" r:id="rId38" display="https://github.com/ngty/gjman"/>
-    <hyperlink ref="D47" r:id="rId39" display="https://github.com/hypernet/visor"/>
-    <hyperlink ref="D48" r:id="rId40" display="https://github.com/stefanbirkner/system-rules"/>
-    <hyperlink ref="D49" r:id="rId41" display="https://github.com/ch33kybutt/oxygen_libcore"/>
-    <hyperlink ref="D50" r:id="rId42" display="https://github.com/apache/tomcat70"/>
+    <hyperlink ref="D32" r:id="rId26" display="https://github.com/viqsoft/Jmin"/>
+    <hyperlink ref="D33" r:id="rId27" display="https://github.com/tykkidream/DemoPermissions"/>
+    <hyperlink ref="D34" r:id="rId28" display="https://github.com/eclipse/org.aspectj"/>
+    <hyperlink ref="D35" r:id="rId29" display="https://github.com/kschat/MCVersion-Control"/>
+    <hyperlink ref="D36" r:id="rId30" display="https://github.com/JSansalone/NetBeansIDE"/>
+    <hyperlink ref="D37" r:id="rId31" display="https://github.com/Almaz-KG/FileManagerFtpHttpServer"/>
+    <hyperlink ref="D38" r:id="rId32" display="https://github.com/zoomis/NGOMS"/>
+    <hyperlink ref="D40" r:id="rId33" display="https://github.com/Babast/Timelag"/>
+    <hyperlink ref="D41" r:id="rId34" display="https://github.com/JetBrains/intellij-community"/>
+    <hyperlink ref="D43" r:id="rId35" display="https://github.com/aleksz/driveddoc"/>
+    <hyperlink ref="D44" r:id="rId36" display="https://github.com/holisticon/tracee"/>
+    <hyperlink ref="D45" r:id="rId37" display="https://github.com/astubbs/spring-modules"/>
+    <hyperlink ref="D46" r:id="rId38" display="https://github.com/wildfly-security/security-manager"/>
+    <hyperlink ref="D47" r:id="rId39" display="https://github.com/ngty/gjman"/>
+    <hyperlink ref="D48" r:id="rId40" display="https://github.com/hypernet/visor"/>
+    <hyperlink ref="D49" r:id="rId41" display="https://github.com/stefanbirkner/system-rules"/>
+    <hyperlink ref="D50" r:id="rId42" display="https://github.com/ch33kybutt/oxygen_libcore"/>
+    <hyperlink ref="D51" r:id="rId43" display="https://github.com/apache/tomcat70"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add more grep results
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="316">
   <si>
     <t>Index</t>
   </si>
@@ -5291,8 +5291,7 @@
   <si>
     <t>./src/com/mcvs/core/SecurityManager.java
 3:public class SecurityManager {
-}
-</t>
+}</t>
   </si>
   <si>
     <t>A trivial one</t>
@@ -5391,6 +5390,61 @@
     <t>https://github.com/rapid7/metasploit-framework</t>
   </si>
   <si>
+    <t>./external/source/exploits/cve-2012-5076/MyPayload.java
+22:        System.setSecurityManager(null);
+./external/source/exploits/cve-2012-5076/Exploit.java
+58:            //System.out.println("SecurityManager:" + System.getSecurityManager());
+./external/source/exploits/jre17u17/Exploit.java
+32:	static void disableSecurityManager() throws Throwable {
+48:		if (u2.field2.f29 == System.getSecurityManager()) {
+50:		} else if (u2.field2.f30 == System.getSecurityManager()) {
+61:			//System.out.println(System.getSecurityManager());
+62:			disableSecurityManager();
+63:			//System.out.println(System.getSecurityManager());
+./external/source/exploits/cve-2013-2460/DisableSecurityManagerAction.java
+6: * Class for disabling the SecurityManager.
+11:public class DisableSecurityManagerAction implements PrivilegedExceptionAction {
+13:	public DisableSecurityManagerAction() {
+24:		System.setSecurityManager(null);
+./external/source/exploits/cve-2013-2460/Exploit.java
+37:					"DisableSecurityManagerAction.class");
+75:					"DisableSecurityManagerAction", classBuffer);
+./external/source/exploits/CVE-2013-2465/Exploit.java
+15:			for(int i=1; i &lt;= 5 &amp;&amp; System.getSecurityManager() != null; i++){
+21:			if (System.getSecurityManager() == null) {
+76:            String name = "setSecurityManager";
+177:                // call System.setSecurityManager(null)
+180:                // show results: SecurityManager should be null
+185:            //System.out.println(System.getSecurityManager() == null ? "Ok.":"Fail.");
+./external/source/exploits/CVE-2011-3544/Exploit.java
+10:* attacker to disable Java SecurityManager, and then run abitrary code.
+28:			// Disable SecurityManager, and then run the payload
+33:				"	java.lang.System.setSecurityManager(null);" +
+./external/source/exploits/CVE-2012-4681/Exploit.java
+28:        Statement localStatement = new Statement(System.class, "setSecurityManager", new Object[1]);
+./external/source/exploits/cve-2012-5088/B.java
+16:    System.setSecurityManager(null);
+./external/source/exploits/CVE-2012-1723/src/cve1723/Attacker.java
+60:		final String tool = System.getSecurityManager() == null ? "null" : System.getSecurityManager().toString();
+./external/source/exploits/CVE-2010-0840/vuln/Exploit.java
+27:		String methodName = "setSecurityManager";
+./external/source/exploits/CVE-2010-0094/Payloader.java
+33:		System.setSecurityManager(null);
+./external/source/exploits/cve-2013-1488/FakeDriver2.java
+24:				"	java.lang.System.setSecurityManager(null);" +
+./external/source/exploits/cve-2013-0431/B.java
+16:    System.setSecurityManager(null);
+./external/source/exploits/cve-2013-1493/Init.java
+174:            if (System.getSecurityManager() == null) {
+212:            long sm = getAddress(System.getSecurityManager());
+219:                    if (System.getSecurityManager() == null) {
+./external/source/exploits/cve-2013-0422/B.java
+16:    System.setSecurityManager(null);
+./external/source/exploits/cve-2012-5076_2/B.java
+16:    System.setSecurityManager(null);
+</t>
+  </si>
+  <si>
     <t>driveddoc</t>
   </si>
   <si>
@@ -5398,6 +5452,14 @@
   </si>
   <si>
     <t>https://github.com/aleksz/driveddoc</t>
+  </si>
+  <si>
+    <t>./src/test/java/com/gmail/at/zhuikov/aleksandr/driveddoc/RestrictedFileWritingRule.java
+12:		System.setSecurityManager(new SecurityManager() {
+28:		System.setSecurityManager(null); // or save and restore original</t>
+  </si>
+  <si>
+    <t>Although it sets SM to null via after() method inRestrictedFileWritingRule.java, this method is called nowhere.</t>
   </si>
   <si>
     <t>TracEE</t>
@@ -5409,6 +5471,21 @@
     <t>https://github.com/holisticon/tracee</t>
   </si>
   <si>
+    <t>./api/src/test/java/io/tracee/BackendProviderResolverGetClassLoaderTest.java
+16:	public void shouldFetchContextClassloaderWithoutSecurityManager() {
+17:		System.setSecurityManager(null);
+23:	public void shouldReturnClassloaderOfClassWithoutSecurityManager() {
+24:		System.setSecurityManager(null);
+30:	public void shouldFetchContextClassloaderWithSecurityManager() {
+31:		System.setSecurityManager(new TestSecurityManager());
+37:	public void shouldReturnClassloaderOfClassWithSecurityManager() {
+38:		System.setSecurityManager(new TestSecurityManager());
+50:		System.setSecurityManager(null);
+53:	private class TestSecurityManager extends SecurityManager {
+./api/src/main/java/io/tracee/BackendProviderResolver.java
+139:			if (System.getSecurityManager() != null) {</t>
+  </si>
+  <si>
     <t>Spring-modules</t>
   </si>
   <si>
@@ -5416,6 +5493,22 @@
   </si>
   <si>
     <t>https://github.com/astubbs/spring-modules</t>
+  </si>
+  <si>
+    <t>./projects/javaspaces/src/test/org/springmodules/javaspaces/SecurityTests.java
+9:import java.rmi.RMISecurityManager;
+22:	public void testRMISecurityManager() throws Exception {
+23:		SecurityManager securityManager = System.getSecurityManager();
+29:			System.setSecurityManager(new RMISecurityManager());
+30:			System.setSecurityManager(null);
+33:			System.setSecurityManager(securityManager);
+./projects/javaspaces/src/java/org/springmodules/jini/JiniSecuritySetter.java
+28:	private SecurityManager securityManager, oldSecurityManager;
+51:		System.setSecurityManager(oldSecurityManager);
+56:		oldSecurityManager = System.getSecurityManager();
+59:		System.setSecurityManager(securityManager);
+79:	public SecurityManager getSecurityManager() {
+86:	public void setSecurityManager(SecurityManager securityManager) {</t>
   </si>
   <si>
     <t>Security-Manager (This is a SecuirtyManager - not a program that uses one)</t>
@@ -5436,6 +5529,35 @@
     <t>https://github.com/ngty/gjman</t>
   </si>
   <si>
+    <t>./lib/gjman/java_hacks/ForbidSystemExit.java
+10:    final SecurityManager securityManager = new SecurityManager() {
+17:    System.setSecurityManager( securityManager ) ;
+21:    System.setSecurityManager( null ) ;
+</t>
+  </si>
+  <si>
+    <t>Related code:class ForbidSystemExit
+{
+  public static class Exception extends SecurityException { }
+  public static void apply() {
+    final SecurityManager securityManager = new SecurityManager() {
+      public void checkPermission( Permission permission ) {
+        if( permission.getName().startsWith("exitVM") ) {
+          throw new Exception() ;
+        }
+      }
+    } ;
+    System.setSecurityManager( securityManager ) ;
+  }
+  public static void unapply() {
+    System.setSecurityManager( null ) ;
+  }
+}</t>
+  </si>
+  <si>
+    <t>← don't think it's doing something harmful. In contrast, it fortfies the policy by preventing exiting.</t>
+  </si>
+  <si>
     <t>visor</t>
   </si>
   <si>
@@ -5452,6 +5574,169 @@
   </si>
   <si>
     <t>https://github.com/stefanbirkner/system-rules</t>
+  </si>
+  <si>
+    <t>./src/test/java/org/junit/contrib/java/lang/system/ExpectedSystemExitTest.java
+3:import static java.lang.System.getSecurityManager;
+4:import static java.lang.System.setSecurityManager;
+113:	public void restoreOldSecurityManager() throws Throwable {
+114:		SecurityManager manager = new ArbitrarySecurityManager();
+115:		setSecurityManager(manager);
+117:		assertThat(getSecurityManager(), sameInstance(manager));
+121:	public void delegateToOldSecurityManager() throws Throwable {
+122:		SecurityManager manager = new ArbitrarySecurityManager();
+123:		setSecurityManager(manager);
+155:			assertEquals(ARBITRARY_CONTEXT, getSecurityManager()
+174:	private static class ArbitrarySecurityManager extends SecurityManager {
+./src/test/java/org/junit/contrib/java/lang/system/ProvideSecurityManagerTest.java
+3:import static java.lang.System.getSecurityManager;
+12:public class ProvideSecurityManagerTest {
+13:	private static final SecurityManager MANAGER = new SecurityManager() {
+22:			assertThat(getSecurityManager(), is(MANAGER));
+26:	public ProvideSecurityManager rule = new ProvideSecurityManager(MANAGER);
+34:	public void restoreOriginalSecurityManager() throws Throwable {
+35:		SecurityManager originalManager = getSecurityManager();
+37:		assertThat(getSecurityManager(), is(originalManager));
+./src/test/java/org/junit/contrib/java/lang/system/internal/NoExitSecurityManagerTest.java
+22:public class NoExitSecurityManagerTest {
+31:	private final SecurityManager originalSecurityManager = mock(SecurityManager.class);
+32:	private final NoExitSecurityManager managerWithOriginal = new NoExitSecurityManager(
+33:			originalSecurityManager);
+34:	private final NoExitSecurityManager managerWithoutOriginal = new NoExitSecurityManager(
+46:		when(originalSecurityManager.getInCheck()).thenReturn(true);
+56:	public void provideSecurityContextOfOriginalSecurityManager() {
+58:		when(originalSecurityManager.getSecurityContext()).thenReturn(context);
+71:		verify(originalSecurityManager).checkPermission(permission);
+85:		verify(originalSecurityManager).checkPermission(permission, context);
+98:		verify(originalSecurityManager).checkCreateClassLoader();
+110:		verify(originalSecurityManager).checkAccess(thread);
+123:		verify(originalSecurityManager).checkAccess(threadGroup);
+135:		verify(originalSecurityManager).checkExec("arbitrary cmd");
+146:		verify(originalSecurityManager).checkLink("arbitrary lib");
+158:		verify(originalSecurityManager).checkRead(fileDescriptor);
+170:		verify(originalSecurityManager).checkRead("arbitrary file");
+182:		verify(originalSecurityManager).checkRead("arbitrary file", context);
+195:		verify(originalSecurityManager).checkWrite(fileDescriptor);
+207:		verify(originalSecurityManager).checkWrite("arbitrary file");
+218:		verify(originalSecurityManager).checkDelete("arbitrary file");
+230:		verify(originalSecurityManager).checkConnect("host", port);
+244:		verify(originalSecurityManager).checkConnect("host", port, context);
+258:		verify(originalSecurityManager).checkListen(port);
+271:		verify(originalSecurityManager).checkAccept("host", port);
+284:		verify(originalSecurityManager).checkMulticast(inetAddress);
+298:		verify(originalSecurityManager).checkMulticast(inetAddress, ttl);
+311:		verify(originalSecurityManager).checkPropertiesAccess();
+322:		verify(originalSecurityManager).checkPropertyAccess("arbitrary key");
+333:		when(originalSecurityManager.checkTopLevelWindow(window)).thenReturn(
+347:		verify(originalSecurityManager).checkPrintJobAccess();
+358:		verify(originalSecurityManager).checkSystemClipboardAccess();
+369:		verify(originalSecurityManager).checkAwtEventQueueAccess();
+380:		verify(originalSecurityManager).checkPackageAccess("arbitrary package");
+391:		verify(originalSecurityManager).checkPackageDefinition(
+403:		verify(originalSecurityManager).checkSetFactory();
+416:		verify(originalSecurityManager)
+430:		verify(originalSecurityManager).checkSecurityAccess("arbitrary target");
+439:	public void provideThreadGroupOfOriginalSecurityManager() {
+441:		when(originalSecurityManager.getThreadGroup()).thenReturn(threadGroup);
+./src/main/java/org/junit/contrib/java/lang/system/ExpectedSystemExit.java
+3:import static java.lang.System.getSecurityManager;
+11:import org.junit.contrib.java.lang.system.internal.NoExitSecurityManager;
+113:		ProvideSecurityManager noExitSecurityManagerRule = createNoExitSecurityManagerRule();
+115:		return noExitSecurityManagerRule.apply(statement, description);
+118:	private ProvideSecurityManager createNoExitSecurityManagerRule() {
+119:		NoExitSecurityManager noExitSecurityManager = new NoExitSecurityManager(
+120:				getSecurityManager());
+121:		return new ProvideSecurityManager(noExitSecurityManager);
+139:		NoExitSecurityManager securityManager = (NoExitSecurityManager) getSecurityManager();
+./src/main/java/org/junit/contrib/java/lang/system/ProvideSecurityManager.java
+3:import static java.lang.System.getSecurityManager;
+4:import static java.lang.System.setSecurityManager;
+9: * The {@code ProvideSecurityManager} rule provides an arbitrary security
+14: *     private final MySecurityManager securityManager
+15: *       = new MySecurityManager();
+18: *     public final ProvideSecurityManager provideSecurityManager
+19: *       = new ProvideSecurityManager(securityManager);
+23: *       assertEquals(securityManager, System.getSecurityManager());
+28:public class ProvideSecurityManager extends ExternalResource {
+29:	private final SecurityManager manager;
+30:	private SecurityManager originalManager;
+32:	public ProvideSecurityManager(SecurityManager manager) {
+38:		originalManager = getSecurityManager();
+39:		setSecurityManager(manager);
+44:		setSecurityManager(originalManager);
+./src/main/java/org/junit/contrib/java/lang/system/internal/NoExitSecurityManager.java
+8: * A {@code NoExitSecurityManager} throws a {@link CheckExitCalled} exception
+12:public class NoExitSecurityManager extends SecurityManager {
+13:	private final SecurityManager originalSecurityManager;
+16:	public NoExitSecurityManager(SecurityManager originalSecurityManager) {
+17:		this.originalSecurityManager = originalSecurityManager;
+41:		return (originalSecurityManager != null)
+42:				&amp;&amp; originalSecurityManager.getInCheck();
+47:		return (originalSecurityManager == null) ? super.getSecurityContext()
+48:				: originalSecurityManager.getSecurityContext();
+53:		if (originalSecurityManager != null)
+54:			originalSecurityManager.checkPermission(perm);
+59:		if (originalSecurityManager != null)
+60:			originalSecurityManager.checkPermission(perm, context);
+65:		if (originalSecurityManager != null)
+66:			originalSecurityManager.checkCreateClassLoader();
+71:		if (originalSecurityManager != null)
+72:			originalSecurityManager.checkAccess(t);
+77:		if (originalSecurityManager != null)
+78:			originalSecurityManager.checkAccess(g);
+83:		if (originalSecurityManager != null)
+84:			originalSecurityManager.checkExec(cmd);
+89:		if (originalSecurityManager != null)
+90:			originalSecurityManager.checkLink(lib);
+95:		if (originalSecurityManager != null)
+96:			originalSecurityManager.checkRead(fd);
+101:		if (originalSecurityManager != null)
+102:			originalSecurityManager.checkRead(file);
+107:		if (originalSecurityManager != null)
+108:			originalSecurityManager.checkRead(file, context);
+113:		if (originalSecurityManager != null)
+114:			originalSecurityManager.checkWrite(fd);
+119:		if (originalSecurityManager != null)
+120:			originalSecurityManager.checkWrite(file);
+125:		if (originalSecurityManager != null)
+126:			originalSecurityManager.checkDelete(file);
+131:		if (originalSecurityManager != null)
+132:			originalSecurityManager.checkConnect(host, port);
+137:		if (originalSecurityManager != null)
+138:			originalSecurityManager.checkConnect(host, port, context);
+143:		if (originalSecurityManager != null)
+144:			originalSecurityManager.checkListen(port);
+149:		if (originalSecurityManager != null)
+150:			originalSecurityManager.checkAccept(host, port);
+155:		if (originalSecurityManager != null)
+156:			originalSecurityManager.checkMulticast(maddr);
+161:		if (originalSecurityManager != null)
+162:			originalSecurityManager.checkMulticast(maddr, ttl);
+167:		if (originalSecurityManager != null)
+168:			originalSecurityManager.checkPropertiesAccess();
+173:		if (originalSecurityManager != null)
+174:			originalSecurityManager.checkPropertyAccess(key);
+179:		return (originalSecurityManager == null) ? super
+180:				.checkTopLevelWindow(window) : originalSecurityManager
+186:		if (originalSecurityManager != null)
+187:			originalSecurityManager.checkPrintJobAccess();
+192:		if (originalSecurityManager != null)
+193:			originalSecurityManager.checkSystemClipboardAccess();
+198:		if (originalSecurityManager != null)
+199:			originalSecurityManager.checkAwtEventQueueAccess();
+204:		if (originalSecurityManager != null)
+205:			originalSecurityManager.checkPackageAccess(pkg);
+210:		if (originalSecurityManager != null)
+211:			originalSecurityManager.checkPackageDefinition(pkg);
+216:		if (originalSecurityManager != null)
+217:			originalSecurityManager.checkSetFactory();
+222:		if (originalSecurityManager != null)
+223:			originalSecurityManager.checkMemberAccess(clazz, which);
+228:		if (originalSecurityManager != null)
+229:			originalSecurityManager.checkSecurityAccess(target);
+234:		return (originalSecurityManager == null) ? super.getThreadGroup()
+235:				: originalSecurityManager.getThreadGroup();
+</t>
   </si>
   <si>
     <t>oxygen-libcore</t>
@@ -5486,7 +5771,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5601,12 +5886,6 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Droid Sans Fallback"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -5747,11 +6026,11 @@
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5856,23 +6135,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5884,7 +6159,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5896,13 +6171,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -5974,8 +6249,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -35461,7 +35736,7 @@
         <v>248</v>
       </c>
       <c r="E35" s="6"/>
-      <c r="G35" s="26" t="s">
+      <c r="G35" s="6" t="s">
         <v>249</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -35470,16 +35745,16 @@
       <c r="K35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="27" t="n">
+      <c r="A36" s="26" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="26" t="s">
         <v>252</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="28" t="s">
         <v>253</v>
       </c>
       <c r="E36" s="6"/>
@@ -35498,7 +35773,7 @@
       <c r="B37" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="29" t="s">
         <v>255</v>
       </c>
       <c r="D37" s="24" t="s">
@@ -35518,7 +35793,7 @@
       <c r="B38" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="29" t="s">
         <v>259</v>
       </c>
       <c r="D38" s="24" t="s">
@@ -35540,7 +35815,7 @@
       <c r="B39" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="29" t="s">
         <v>263</v>
       </c>
       <c r="D39" s="24" t="s">
@@ -35558,10 +35833,10 @@
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="30" t="s">
         <v>267</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="29" t="s">
         <v>268</v>
       </c>
       <c r="D40" s="24" t="s">
@@ -35582,7 +35857,7 @@
       <c r="B41" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="31" t="s">
         <v>273</v>
       </c>
       <c r="D41" s="24" t="s">
@@ -35597,71 +35872,90 @@
       <c r="B42" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="C42" s="33" t="s">
+      <c r="C42" s="32" t="s">
         <v>276</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>277</v>
       </c>
       <c r="E42" s="6"/>
+      <c r="G42" s="10" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="C43" s="30" t="s">
         <v>279</v>
       </c>
+      <c r="C43" s="29" t="s">
+        <v>280</v>
+      </c>
       <c r="D43" s="24" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E43" s="6"/>
+      <c r="G43" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="H43" s="0"/>
+      <c r="K43" s="1" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E44" s="6"/>
+      <c r="G44" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="E45" s="6"/>
+      <c r="G45" s="10" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="E46" s="6"/>
     </row>
@@ -35670,73 +35964,90 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="E47" s="6"/>
+      <c r="G47" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="K47" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="E48" s="6"/>
+        <v>303</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="E49" s="6"/>
+      <c r="G49" s="10" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="E50" s="6"/>
+      <c r="G50" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="27" t="n">
+      <c r="A51" s="26" t="n">
         <v>49</v>
       </c>
-      <c r="B51" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="C51" s="27" t="s">
-        <v>303</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>304</v>
+      <c r="B51" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>313</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -35750,12 +36061,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a couple of summaries of general notes
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="440" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="474" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="317">
   <si>
     <t>Index</t>
   </si>
@@ -4366,7 +4366,8 @@
 294:			System.setSecurityManager(oldSecurityManager);</t>
   </si>
   <si>
-    <t>The code basically does System.setSecurityManager(System.getSecurityManager()); Policy is maintained.</t>
+    <t>The code basically does System.setSecurityManager(System.getSecurityManager()); Policy is maintained. 
+Zack – based on the Grep, the SM is only changed in test cases.  Other sandbox interactions are to check if a sandbox is set.</t>
   </si>
   <si>
     <t>struts</t>
@@ -4806,7 +4807,8 @@
 146:      SESecurityManager.exitVM(-1);</t>
   </si>
   <si>
-    <t>This program sets a SecurityManager during normal execution.  It allows weakening if a SecurityManager is set before running which allows for changing the SecurityManager and it contains code to save the old SecurityManager and use it in general permission checks.  It seems that the SecurityManager can only be set once (the that does it is a singleton), however there is one file which seems to call it with a parameter.  However, I don't see a constuctor with a parameter so I think that is dead code, if that is not the case, the SecurityManager may be set twice on some executions.  However, it is only set once on a normal Execution.  Also, that constructor with a parameter is used to return a different type so I think this section is buggy at best (in file UtilitiesImpl.java)</t>
+    <t>This program sets a SecurityManager during normal execution.  It allows weakening if a SecurityManager is set before running which allows for changing the SecurityManager and it contains code to save the old SecurityManager and use it in general permission checks.  It seems that the SecurityManager can only be set once (the that does it is a singleton), however there is one file which seems to call it with a parameter.  However, I don't see a constuctor with a parameter so I think that is dead code, if that is not the case, the SecurityManager may be set twice on some executions.  However, it is only set once on a normal Execution.  Also, that constructor with a parameter is used to return a different type so I think this section is buggy at best (in file UtilitiesImpl.java)
+Overall – no weakening or nulling occurs</t>
   </si>
   <si>
     <t>Callback on VMStart.
@@ -5306,6 +5308,9 @@
     <t>https://github.com/JSansalone/NetBeansIDE</t>
   </si>
   <si>
+    <t>p</t>
+  </si>
+  <si>
     <t>FileManagerFtpHttpServer (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
   </si>
   <si>
@@ -5441,8 +5446,7 @@
 ./external/source/exploits/cve-2013-0422/B.java
 16:    System.setSecurityManager(null);
 ./external/source/exploits/cve-2012-5076_2/B.java
-16:    System.setSecurityManager(null);
-</t>
+16:    System.setSecurityManager(null);</t>
   </si>
   <si>
     <t>driveddoc</t>
@@ -5532,8 +5536,7 @@
     <t>./lib/gjman/java_hacks/ForbidSystemExit.java
 10:    final SecurityManager securityManager = new SecurityManager() {
 17:    System.setSecurityManager( securityManager ) ;
-21:    System.setSecurityManager( null ) ;
-</t>
+21:    System.setSecurityManager( null ) ;</t>
   </si>
   <si>
     <t>Related code:class ForbidSystemExit
@@ -5735,8 +5738,7 @@
 228:		if (originalSecurityManager != null)
 229:			originalSecurityManager.checkSecurityAccess(target);
 234:		return (originalSecurityManager == null) ? super.getThreadGroup()
-235:				: originalSecurityManager.getThreadGroup();
-</t>
+235:				: originalSecurityManager.getThreadGroup();</t>
   </si>
   <si>
     <t>oxygen-libcore</t>
@@ -6171,13 +6173,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -6245,12 +6247,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -35679,6 +35682,7 @@
       </c>
       <c r="H32" s="0"/>
       <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -35701,6 +35705,7 @@
         <v>241</v>
       </c>
       <c r="K33" s="0"/>
+      <c r="L33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
@@ -35721,6 +35726,7 @@
       </c>
       <c r="H34" s="0"/>
       <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -35743,6 +35749,7 @@
         <v>250</v>
       </c>
       <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="26" t="n">
@@ -35765,222 +35772,246 @@
         <v>250</v>
       </c>
       <c r="K36" s="0"/>
+      <c r="L36" s="0"/>
+      <c r="O36" s="1" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G37" s="0"/>
       <c r="H37" s="0"/>
       <c r="K37" s="0"/>
+      <c r="L37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E38" s="6"/>
       <c r="G38" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>250</v>
       </c>
       <c r="K38" s="0"/>
+      <c r="L38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E39" s="6"/>
       <c r="G39" s="10" t="s">
-        <v>265</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="H39" s="0"/>
       <c r="K39" s="1" t="s">
-        <v>266</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="L39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E40" s="6"/>
       <c r="G40" s="10" t="s">
-        <v>270</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="H40" s="0"/>
       <c r="K40" s="1" t="s">
-        <v>271</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="L40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E41" s="6"/>
+      <c r="G41" s="0"/>
+      <c r="H41" s="0"/>
+      <c r="K41" s="0"/>
+      <c r="L41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E42" s="6"/>
       <c r="G42" s="10" t="s">
-        <v>278</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="H42" s="0"/>
+      <c r="K42" s="0"/>
+      <c r="L42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E43" s="6"/>
       <c r="G43" s="10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H43" s="0"/>
       <c r="K43" s="1" t="s">
-        <v>283</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="L43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E44" s="6"/>
       <c r="G44" s="10" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="L44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E45" s="6"/>
       <c r="G45" s="10" t="s">
-        <v>291</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E46" s="6"/>
+      <c r="G46" s="0"/>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E47" s="6"/>
       <c r="G47" s="10" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35988,34 +36019,35 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>257</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="G48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E49" s="6"/>
       <c r="G49" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36023,13 +36055,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E50" s="6"/>
       <c r="G50" s="1" t="s">
@@ -36041,13 +36073,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -36061,12 +36093,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished 6 of the programs in the github dataset
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="322">
   <si>
     <t>Index</t>
   </si>
@@ -5236,6 +5236,12 @@
 22:      securityManager = new SecurityManager();</t>
   </si>
   <si>
+    <t>This application should be removed from the dataset.  It doesn't effect the system security manager in any way.  The program creates a user defined SecurityManager class wihich does not extend the java.lang.SecurityManager in any way.  The class is then used as an authentication manager.</t>
+  </si>
+  <si>
+    <t>In general notes</t>
+  </si>
+  <si>
     <t>DemoPermissions (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
   </si>
   <si>
@@ -5254,19 +5260,38 @@
 15:	private SecurityManager() {</t>
   </si>
   <si>
-    <t>Simply from grep result we know that it doesn't change SM anyways.</t>
+    <t>Tianyuan: Simply from grep result we know that it doesn't change SM anyways.
+Zack: This application can be removed from the data set.  It creates its own SecurityManager class and never uses the java.lang.SecurityManager class.</t>
   </si>
   <si>
     <t>AspectJ</t>
   </si>
   <si>
-    <t>93c58e39cf0512d0920c37a40026a6aa5f1ff26b</t>
+    <t>d0b8c7a1bfbc2b2f92b22bcf63598ab2442781b6</t>
   </si>
   <si>
     <t>https://github.com/eclipse/org.aspectj</t>
   </si>
   <si>
-    <t>./testing/src/org/aspectj/testing/harness/bridge/JavaRun.java
+    <t>./ajdoc/src/org/aspectj/tools/ajdoc/JavadocRunner.java
+41:		// final SecurityManager defaultSecurityManager = System.getSecurityManager();
+43:		// System.setSecurityManager( new SecurityManager() {
+49:		// System.setSecurityManager(defaultSecurityManager);
+56:		// if ( defaultSecurityManager != null )
+57:		// defaultSecurityManager.checkPermission( permission );
+61:		// if ( defaultSecurityManager != null )
+62:		// defaultSecurityManager.checkPermission( permission, context );
+93:		// System.setSecurityManager(defaultSecurityManager);
+./org.aspectj.ajdt.core/testsrc/org/aspectj/tools/ajc/AjcTestCase.java
+663://			SecurityManager sm = new SecurityManager();
+664://			System.setSecurityManager(sm);
+666://			// SecurityManager already set
+701://				SecurityManager sm = new SecurityManager();
+702://				System.setSecurityManager(null);
+705://				// SecurityManager already set
+./tests/ltw/NullSecurityManager.java
+2:public class NullSecurityManager extends SecurityManager {
+./testing/src/org/aspectj/testing/harness/bridge/JavaRun.java
 183:            RunSecurityManager.ME.setJavaRunThread(this);
 202:            if (thrown instanceof RunSecurityManager.ExitCalledException) {
 203:                int i = ((RunSecurityManager.ExitCalledException) thrown).exitCode;
@@ -5278,8 +5303,10 @@
 795:    public static class RunSecurityManager extends SecurityManager {
 796:        public static RunSecurityManager ME = new RunSecurityManager();
 798:        private RunSecurityManager(){}
-./tests/ltw/NullSecurityManager.java
-2:public class NullSecurityManager extends SecurityManager {</t>
+</t>
+  </si>
+  <si>
+    <t>This program only sets a SecurityManager in a test case.  Even in the test case, the SecurityManager only stops system.exit calls.  They also create a fully permissive SecurityManager but don't use it in one of the test packages.</t>
   </si>
   <si>
     <t>MCVersion-Control (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
@@ -5296,7 +5323,7 @@
 }</t>
   </si>
   <si>
-    <t>A trivial one</t>
+    <t>This application should be removed from the dataset.  It doesn't effect the system security manager in any way.  It only defines a user defined SecurityManager class.</t>
   </si>
   <si>
     <t>Netbeans (I think this one can be removed because we are already covering it in the qualitas corpus)</t>
@@ -5308,19 +5335,45 @@
     <t>https://github.com/JSansalone/NetBeansIDE</t>
   </si>
   <si>
+    <t>Already coved in qualitas</t>
+  </si>
+  <si>
     <t>p</t>
   </si>
   <si>
     <t>FileManagerFtpHttpServer (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
   </si>
   <si>
-    <t>02f775b196ed6eae8e0cd2a7760193c315846498</t>
+    <t>02f775b196ed6eae8e0cd2a7760193c315846498 (can't update repository- I can't authenticate anymore)</t>
   </si>
   <si>
     <t>https://github.com/Almaz-KG/FileManagerFtpHttpServer</t>
   </si>
   <si>
-    <t>404 not found</t>
+    <t>./FileManagerFtpHttpServer/src/filemanager/server/ftp/FtpServer.java
+12:import filemanager.server.manager.SecurityManager;
+16:	private SecurityManager manager;
+25:	public FtpServer(File configFile, SecurityManager manager, DataAccessObject dao) throws ServerException{ 
+108:	public SecurityManager getManager() {
+111:	public void setManager(SecurityManager manager) {
+./FileManagerFtpHttpServer/src/filemanager/server/ftp/FtpClientThread.java
+11:import filemanager.server.manager.SecurityManager;
+20:	private SecurityManager manager;
+28:	public FtpClientThread(Socket socket, SecurityManager manager, DataAccessObject dao, File log)
+165:	public void setManager(SecurityManager manager) {
+171:	public SecurityManager getManager(){
+./FileManagerFtpHttpServer/src/filemanager/server/manager/SecurityManager.java
+3:public interface SecurityManager {
+./FileManagerFtpHttpServer/src/filemanager/server/main/FileManagerServer.java
+10:import filemanager.server.manager.SecurityManager;
+20:	private static SecurityManager manager;
+./FileManagerFtpHttpServer/src/filemanager/server/http/HttpServer.java
+9:import filemanager.server.manager.SecurityManager;
+13:	private SecurityManager manager;
+20:	public HttpServer(File serverConfig, SecurityManager manager, DataAccessObject dao) 
+43:	public SecurityManager getManager() {
+46:	public void setManager(SecurityManager manager) {
+</t>
   </si>
   <si>
     <t>NGOMS</t>
@@ -5570,6 +5623,9 @@
     <t>https://github.com/hypernet/visor</t>
   </si>
   <si>
+    <t>404 not found</t>
+  </si>
+  <si>
     <t>System Rules</t>
   </si>
   <si>
@@ -5773,7 +5829,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5885,6 +5941,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="1"/>
@@ -5903,6 +5965,12 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="9">
@@ -6028,11 +6096,11 @@
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6133,35 +6201,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6173,13 +6253,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -6247,13 +6327,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -35676,105 +35756,178 @@
       <c r="D32" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="E32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G32" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="H32" s="0"/>
-      <c r="K32" s="0"/>
+      <c r="H32" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>238</v>
+      </c>
       <c r="L32" s="0"/>
+      <c r="O32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="D33" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="E33" s="6"/>
-      <c r="G33" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="K33" s="0"/>
       <c r="L33" s="0"/>
+      <c r="O33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>242</v>
+      <c r="B34" s="26" t="s">
+        <v>244</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="E34" s="6"/>
+        <v>246</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G34" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="H34" s="0"/>
-      <c r="K34" s="0"/>
+        <v>247</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K34" s="25" t="s">
+        <v>238</v>
+      </c>
       <c r="L34" s="0"/>
+      <c r="O34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="E35" s="6"/>
+        <v>251</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G35" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="K35" s="0"/>
+        <v>252</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K35" s="25" t="s">
+        <v>238</v>
+      </c>
       <c r="L35" s="0"/>
+      <c r="O35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="26" t="n">
+      <c r="A36" s="27" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="E36" s="6"/>
+      <c r="B36" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G36" s="0" t="s">
         <v>60</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="K36" s="0"/>
+        <v>257</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="L36" s="0"/>
       <c r="O36" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35782,20 +35935,35 @@
         <v>35</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>256</v>
+        <v>259</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>260</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="G37" s="0"/>
-      <c r="H37" s="0"/>
-      <c r="K37" s="0"/>
+        <v>60</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K37" s="25" t="s">
+        <v>238</v>
+      </c>
       <c r="L37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35803,22 +35971,35 @@
         <v>36</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="C38" s="29" t="s">
-        <v>260</v>
+        <v>263</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>264</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="E38" s="6"/>
+        <v>265</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G38" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="K38" s="0"/>
+        <v>266</v>
+      </c>
+      <c r="H38" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>238</v>
+      </c>
       <c r="L38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35826,21 +36007,21 @@
         <v>37</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>264</v>
+        <v>267</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>268</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E39" s="6"/>
       <c r="G39" s="10" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H39" s="0"/>
       <c r="K39" s="1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="L39" s="0"/>
     </row>
@@ -35848,22 +36029,22 @@
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>269</v>
+      <c r="B40" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>273</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E40" s="6"/>
       <c r="G40" s="10" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="H40" s="0"/>
       <c r="K40" s="1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="L40" s="0"/>
     </row>
@@ -35872,13 +36053,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="C41" s="31" t="s">
-        <v>274</v>
+        <v>277</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>278</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E41" s="6"/>
       <c r="G41" s="0"/>
@@ -35891,17 +36072,17 @@
         <v>40</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="C42" s="32" t="s">
-        <v>277</v>
+        <v>280</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>281</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E42" s="6"/>
       <c r="G42" s="10" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="H42" s="0"/>
       <c r="K42" s="0"/>
@@ -35912,21 +36093,21 @@
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>281</v>
+        <v>284</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>285</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E43" s="6"/>
       <c r="G43" s="10" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="H43" s="0"/>
       <c r="K43" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="L43" s="0"/>
     </row>
@@ -35935,17 +36116,17 @@
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E44" s="6"/>
       <c r="G44" s="10" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>108</v>
@@ -35957,17 +36138,17 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="E45" s="6"/>
       <c r="G45" s="10" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="K45" s="0"/>
       <c r="L45" s="0"/>
@@ -35977,13 +36158,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E46" s="6"/>
       <c r="G46" s="0"/>
@@ -35995,23 +36176,23 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="E47" s="6"/>
       <c r="G47" s="10" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36019,16 +36200,16 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
       <c r="G48" s="0"/>
     </row>
@@ -36037,17 +36218,17 @@
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="E49" s="6"/>
       <c r="G49" s="10" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36055,13 +36236,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="E50" s="6"/>
       <c r="G50" s="1" t="s">
@@ -36069,21 +36250,21 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="26" t="n">
+      <c r="A51" s="27" t="n">
         <v>49</v>
       </c>
-      <c r="B51" s="27" t="s">
-        <v>312</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="D51" s="28" t="s">
-        <v>314</v>
+      <c r="B51" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>318</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>319</v>
       </c>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="10"/>
       <c r="D52" s="24"/>
       <c r="E52" s="6"/>
@@ -36093,12 +36274,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing latest work on github dataset
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="323">
   <si>
     <t>Index</t>
   </si>
@@ -5408,7 +5408,11 @@
 ./src/test/java/org/refact4j/util/SecurityManagerDecorator.java
 7:public class SecurityManagerDecorator extends SecurityManager {
 9:    private SecurityManager securityManager;
-11:    public SecurityManagerDecorator(SecurityManager securityManager) {</t>
+11:    public SecurityManagerDecorator(SecurityManager securityManager) {
+</t>
+  </si>
+  <si>
+    <t>Creates SecurityManager in test case.  Never sets one during execution or any tests.</t>
   </si>
   <si>
     <t>Defines SM in the test code but never set it explicitly.</t>
@@ -6332,8 +6336,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36015,13 +36019,26 @@
       <c r="D39" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G39" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="H39" s="0"/>
-      <c r="K39" s="1" t="s">
+      <c r="H39" s="6" t="s">
         <v>271</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>272</v>
       </c>
       <c r="L39" s="0"/>
     </row>
@@ -36030,21 +36047,21 @@
         <v>38</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E40" s="6"/>
       <c r="G40" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H40" s="0"/>
-      <c r="K40" s="1" t="s">
-        <v>276</v>
+      <c r="K40" s="10" t="s">
+        <v>277</v>
       </c>
       <c r="L40" s="0"/>
     </row>
@@ -36053,13 +36070,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E41" s="6"/>
       <c r="G41" s="0"/>
@@ -36072,17 +36089,17 @@
         <v>40</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E42" s="6"/>
       <c r="G42" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H42" s="0"/>
       <c r="K42" s="0"/>
@@ -36093,21 +36110,21 @@
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E43" s="6"/>
       <c r="G43" s="10" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H43" s="0"/>
       <c r="K43" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L43" s="0"/>
     </row>
@@ -36116,17 +36133,17 @@
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E44" s="6"/>
       <c r="G44" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>108</v>
@@ -36138,17 +36155,17 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E45" s="6"/>
       <c r="G45" s="10" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K45" s="0"/>
       <c r="L45" s="0"/>
@@ -36158,13 +36175,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E46" s="6"/>
       <c r="G46" s="0"/>
@@ -36176,23 +36193,23 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E47" s="6"/>
       <c r="G47" s="10" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36200,16 +36217,16 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G48" s="0"/>
     </row>
@@ -36218,17 +36235,17 @@
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E49" s="6"/>
       <c r="G49" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36236,13 +36253,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E50" s="6"/>
       <c r="G50" s="1" t="s">
@@ -36254,13 +36271,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -36274,12 +36291,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing to merge changes
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="324">
   <si>
     <t>Index</t>
   </si>
@@ -5302,8 +5302,7 @@
 595:                System.setSecurityManager(RunSecurityManager.ME);
 795:    public static class RunSecurityManager extends SecurityManager {
 796:        public static RunSecurityManager ME = new RunSecurityManager();
-798:        private RunSecurityManager(){}
-</t>
+798:        private RunSecurityManager(){}</t>
   </si>
   <si>
     <t>This program only sets a SecurityManager in a test case.  Even in the test case, the SecurityManager only stops system.exit calls.  They also create a fully permissive SecurityManager but don't use it in one of the test packages.</t>
@@ -5372,8 +5371,7 @@
 13:	private SecurityManager manager;
 20:	public HttpServer(File serverConfig, SecurityManager manager, DataAccessObject dao) 
 43:	public SecurityManager getManager() {
-46:	public void setManager(SecurityManager manager) {
-</t>
+46:	public void setManager(SecurityManager manager) {</t>
   </si>
   <si>
     <t>NGOMS</t>
@@ -5408,8 +5406,7 @@
 ./src/test/java/org/refact4j/util/SecurityManagerDecorator.java
 7:public class SecurityManagerDecorator extends SecurityManager {
 9:    private SecurityManager securityManager;
-11:    public SecurityManagerDecorator(SecurityManager securityManager) {
-</t>
+11:    public SecurityManagerDecorator(SecurityManager securityManager) {</t>
   </si>
   <si>
     <t>Creates SecurityManager in test case.  Never sets one during execution or any tests.</t>
@@ -5431,6 +5428,9 @@
 6:        System.setSecurityManager(null);</t>
   </si>
   <si>
+    <t>Skipping this one for now.  Having trouble running the jnlp file.  Will come back later.</t>
+  </si>
+  <si>
     <t>It's setting SM to null in Jtimelag.java and set a frame visible.</t>
   </si>
   <si>
@@ -5443,7 +5443,7 @@
     <t>https://github.com/JetBrains/intellij-community</t>
   </si>
   <si>
-    <t>Metasploit-framework</t>
+    <t>Metasploit-framework (excluding this one)</t>
   </si>
   <si>
     <t>4eeab66ebed17b91b09d4bbc9d8a302fa25bcb3e</t>
@@ -5833,7 +5833,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5945,12 +5945,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Droid Sans Fallback"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="1"/>
@@ -5969,12 +5963,6 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri Light"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="9">
@@ -6100,11 +6088,11 @@
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6205,47 +6193,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" xfId="26" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="1" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6257,13 +6237,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -6336,8 +6316,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -35815,7 +35795,7 @@
       <c r="J33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K33" s="25" t="s">
+      <c r="K33" s="14" t="s">
         <v>238</v>
       </c>
       <c r="L33" s="0"/>
@@ -35825,7 +35805,7 @@
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="25" t="s">
         <v>244</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -35852,7 +35832,7 @@
       <c r="J34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K34" s="25" t="s">
+      <c r="K34" s="14" t="s">
         <v>238</v>
       </c>
       <c r="L34" s="0"/>
@@ -35889,23 +35869,23 @@
       <c r="J35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K35" s="25" t="s">
+      <c r="K35" s="14" t="s">
         <v>238</v>
       </c>
       <c r="L35" s="0"/>
       <c r="O35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="27" t="n">
+      <c r="A36" s="26" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="28" t="s">
         <v>256</v>
       </c>
       <c r="E36" s="6" t="s">
@@ -35941,7 +35921,7 @@
       <c r="B37" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="29" t="s">
         <v>260</v>
       </c>
       <c r="D37" s="24" t="s">
@@ -35956,7 +35936,7 @@
       <c r="G37" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="H37" s="31" t="s">
+      <c r="H37" s="30" t="s">
         <v>253</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -35965,7 +35945,7 @@
       <c r="J37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K37" s="25" t="s">
+      <c r="K37" s="14" t="s">
         <v>238</v>
       </c>
       <c r="L37" s="0"/>
@@ -35977,7 +35957,7 @@
       <c r="B38" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="29" t="s">
         <v>264</v>
       </c>
       <c r="D38" s="24" t="s">
@@ -35992,7 +35972,7 @@
       <c r="G38" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="H38" s="32" t="s">
+      <c r="H38" s="10" t="s">
         <v>253</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -36001,7 +35981,7 @@
       <c r="J38" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K38" s="25" t="s">
+      <c r="K38" s="14" t="s">
         <v>238</v>
       </c>
       <c r="L38" s="0"/>
@@ -36013,7 +35993,7 @@
       <c r="B39" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="29" t="s">
         <v>268</v>
       </c>
       <c r="D39" s="24" t="s">
@@ -36046,10 +36026,10 @@
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="29" t="s">
         <v>274</v>
       </c>
       <c r="D40" s="24" t="s">
@@ -36059,9 +36039,11 @@
       <c r="G40" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="H40" s="0"/>
+      <c r="H40" s="6" t="s">
+        <v>277</v>
+      </c>
       <c r="K40" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="L40" s="0"/>
     </row>
@@ -36070,13 +36052,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="C41" s="34" t="s">
         <v>279</v>
       </c>
+      <c r="C41" s="32" t="s">
+        <v>280</v>
+      </c>
       <c r="D41" s="24" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E41" s="6"/>
       <c r="G41" s="0"/>
@@ -36089,17 +36071,17 @@
         <v>40</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C42" s="35" t="s">
         <v>282</v>
       </c>
+      <c r="C42" s="33" t="s">
+        <v>283</v>
+      </c>
       <c r="D42" s="24" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E42" s="6"/>
       <c r="G42" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H42" s="0"/>
       <c r="K42" s="0"/>
@@ -36110,21 +36092,21 @@
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="C43" s="30" t="s">
         <v>286</v>
       </c>
+      <c r="C43" s="29" t="s">
+        <v>287</v>
+      </c>
       <c r="D43" s="24" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E43" s="6"/>
       <c r="G43" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H43" s="0"/>
       <c r="K43" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L43" s="0"/>
     </row>
@@ -36133,17 +36115,17 @@
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E44" s="6"/>
       <c r="G44" s="10" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>108</v>
@@ -36155,17 +36137,17 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E45" s="6"/>
       <c r="G45" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="K45" s="0"/>
       <c r="L45" s="0"/>
@@ -36175,13 +36157,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E46" s="6"/>
       <c r="G46" s="0"/>
@@ -36193,23 +36175,23 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E47" s="6"/>
       <c r="G47" s="10" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36217,16 +36199,16 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G48" s="0"/>
     </row>
@@ -36235,17 +36217,17 @@
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E49" s="6"/>
       <c r="G49" s="10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36253,13 +36235,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E50" s="6"/>
       <c r="G50" s="1" t="s">
@@ -36267,17 +36249,17 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="27" t="n">
+      <c r="A51" s="26" t="n">
         <v>49</v>
       </c>
-      <c r="B51" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="C51" s="27" t="s">
+      <c r="B51" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="C51" s="26" t="s">
         <v>320</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>321</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -36291,12 +36273,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing categorizations of Tianyuan's parts
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="331">
   <si>
     <t>Index</t>
   </si>
@@ -151,7 +151,8 @@
 154:            perms.restoreSecurityManager();</t>
   </si>
   <si>
-    <t>It looks like we may be able to see a SecurityManager change if we are using special compilers that need to execute Java while compiling or write an application to use vendor specific extensions.  The only setSecurityManager I found that was valid is in the ExecuteJava.java file which is not called normally.</t>
+    <t>It looks like we may be able to see a SecurityManager change if we are using special compilers that need to execute Java while compiling or write an application to use vendor specific extensions.  The only setSecurityManager I found that was valid is in the ExecuteJava.java file which is not called normally.
+Classification: Change SM but not in main application (weakening – allows setting and restoring SM)</t>
   </si>
   <si>
     <t>No output.  Probably don't have good code coverage although any classes loaded through another classloader than the default one would not be seen with the current Emma method I used.  
@@ -372,7 +373,8 @@
 1248:            securityManager = System.getSecurityManager();</t>
   </si>
   <si>
-    <t>The code contains a possibly valid null and/or weakening of the SecurityManager.  The method enforceSecurity in the file ApplicationSecurityEnforcer.java should be investigated further.  See the Piazza post for more information.</t>
+    <t>The code contains a possibly valid null and/or weakening of the SecurityManager.  The method enforceSecurity in the file ApplicationSecurityEnforcer.java should be investigated further.  See the Piazza post for more information.
+</t>
   </si>
   <si>
     <t>Slideshow sample output:
@@ -620,7 +622,8 @@
 122:			if (System.getSecurityManager() != null)</t>
   </si>
   <si>
-    <t>From the static analysis, SM is changed from the third-party libraries – ant, jboss and quartz. However, such behavior doesn't come into play because it's not detected by the dynamic analysis. The grep result also verifies this fact.</t>
+    <t>From the static analysis, SM is changed from the third-party libraries – ant, jboss and quartz. However, such behavior doesn't come into play because it's not detected by the dynamic analysis. The grep result also verifies this fact.
+Category: Doesn't interact with SM at all (possibly third party library but unlikely)</t>
   </si>
   <si>
     <t>Sets SM to null from the third-party libraries</t>
@@ -3263,7 +3266,8 @@
 105:      System.setSecurityManager(null);</t>
   </si>
   <si>
-    <t>no comments</t>
+    <t>no comments
+Category: Interact with SM only in test cases.</t>
   </si>
   <si>
     <t>only modifies SM in test cases</t>
@@ -3282,6 +3286,9 @@
 117:		if ( System.getSecurityManager() == null ) {</t>
   </si>
   <si>
+    <t>Category:  interacts with SM in main program – only checks if one is set</t>
+  </si>
+  <si>
     <t>hsqldb</t>
   </si>
   <si>
@@ -3289,6 +3296,10 @@
   </si>
   <si>
     <t>http://hsqldb.org/</t>
+  </si>
+  <si>
+    <t>New version doesn't contain any SecurityManager interactions – old version had SecurityManager lines commented out
+Category: Doesn't interact with SM at all – can remove from Database </t>
   </si>
   <si>
     <t>jboss</t>
@@ -3892,7 +3903,7 @@
 4756:            SecurityManager sm = System.getSecurityManager();</t>
   </si>
   <si>
-    <t>No SM is changed in general</t>
+    <t>Category:  interacts with SM in main program – checks if one is set</t>
   </si>
   <si>
     <t>According to the static results, SM is changed in a third-party code, which we don't really care about.</t>
@@ -3949,6 +3960,10 @@
 39:  public TestSecurityManager() {</t>
   </si>
   <si>
+    <t>no comments
+Category: Only interacts in test cases</t>
+  </si>
+  <si>
     <t>A third-party library – apache ant that could potentially changes SM, while this behavior isn't cached</t>
   </si>
   <si>
@@ -4000,6 +4015,10 @@
 363:            if (System.getSecurityManager() != null) {</t>
   </si>
   <si>
+    <t>no comments
+Category: Interacts in the main program but doesn't change anything</t>
+  </si>
+  <si>
     <t>nekohtml</t>
   </si>
   <si>
@@ -4029,7 +4048,8 @@
     <t>see attached file</t>
   </si>
   <si>
-    <t>Only one place detected. When the program is run, the GuiRunlevel.java runs the GUI and then installs the SM to advance the policy. SM is defined in TopSecurityManager.java</t>
+    <t>Only one place detected. When the program is run, the GuiRunlevel.java runs the GUI and then installs the SM to add policy checks. SM is defined in TopSecurityManager.java
+Category: sets and changes SM –  (strengthening)</t>
   </si>
   <si>
     <t>see left, there is also a place that sets TopSM to null, in Activatior.java line 105. However, this behavior is not detected</t>
@@ -4429,6 +4449,9 @@
 327:				SecurityManager sm = System.getSecurityManager();</t>
   </si>
   <si>
+    <t>Interacts with SM in main program – sets SM in test cases</t>
+  </si>
+  <si>
     <t>tapestry</t>
   </si>
   <si>
@@ -4471,7 +4494,8 @@
 76:        binder.bind(RequestSecurityManager.class, RequestSecurityManagerImpl.class);</t>
   </si>
   <si>
-    <t>By a manually going through the RequestSecurityManagerImpl.java, the so-called SM is actually used to manage the relationship between the security of a request and the security of a page. By secure, we mean whether a request uses HTTPS and whether a page demands the use of HTTPS – from the comments</t>
+    <t>By a manually going through the RequestSecurityManagerImpl.java, the so-called SM is actually used to manage the relationship between the security of a request and the security of a page. By secure, we mean whether a request uses HTTPS and whether a page demands the use of HTTPS – from the comments
+Category: No interaction at all – can remove from dataset</t>
   </si>
   <si>
     <t>tomcat</t>
@@ -4566,6 +4590,10 @@
 43:        if (System.getSecurityManager() == null) {
 ./java/javax/el/ExpressionFactory.java
 49:        (System.getSecurityManager() != null);</t>
+  </si>
+  <si>
+    <t>no comments
+Category: Interacts in main program</t>
   </si>
   <si>
     <t>Vuze (originally Azureus)</t>
@@ -5174,6 +5202,9 @@
 482:        SecurityManager security = System.getSecurityManager();
 ./src/org/apache/xpath/functions/ObjectFactory.java
 482:        SecurityManager security = System.getSecurityManager();</t>
+  </si>
+  <si>
+    <t>Interacts with SM in main program </t>
   </si>
   <si>
     <t>xerces</t>
@@ -6237,13 +6268,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -6316,8 +6347,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15864,7 +15895,9 @@
       <c r="G12" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="I12" s="0"/>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
@@ -16887,13 +16920,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>60</v>
@@ -16905,7 +16938,7 @@
         <v>60</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
@@ -17929,40 +17962,40 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>60</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
       <c r="L14" s="10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="P14" s="0"/>
       <c r="Q14" s="0"/>
@@ -18979,34 +19012,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="0"/>
@@ -20027,32 +20060,32 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="I16" s="0"/>
       <c r="J16" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
@@ -21073,13 +21106,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>60</v>
@@ -21088,10 +21121,10 @@
         <v>60</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
@@ -22115,13 +22148,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>60</v>
@@ -22130,10 +22163,10 @@
         <v>60</v>
       </c>
       <c r="G18" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="I18" s="0"/>
       <c r="J18" s="0"/>
@@ -23157,34 +23190,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
@@ -24205,25 +24238,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>37</v>
@@ -24232,7 +24265,7 @@
         <v>38</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
@@ -25253,34 +25286,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
@@ -26301,34 +26334,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
@@ -27349,25 +27382,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>60</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
@@ -28391,25 +28424,25 @@
         <v>23</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>190</v>
-      </c>
       <c r="F24" s="6" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
@@ -29433,25 +29466,25 @@
         <v>24</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>60</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
@@ -30475,13 +30508,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>60</v>
@@ -30490,10 +30523,10 @@
         <v>60</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>107</v>
+        <v>212</v>
       </c>
       <c r="I26" s="0"/>
       <c r="J26" s="0"/>
@@ -31517,34 +31550,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="L27" s="0"/>
       <c r="M27" s="0"/>
@@ -32565,34 +32598,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>3.6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="L28" s="0"/>
       <c r="M28" s="0"/>
@@ -33613,13 +33646,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>60</v>
@@ -33628,10 +33661,10 @@
         <v>60</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>107</v>
+        <v>235</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="I29" s="0"/>
       <c r="J29" s="0"/>
@@ -34655,13 +34688,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>60</v>
@@ -34670,10 +34703,10 @@
         <v>60</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>107</v>
+        <v>122</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="I30" s="0"/>
       <c r="J30" s="0"/>
@@ -35732,13 +35765,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>60</v>
@@ -35747,10 +35780,10 @@
         <v>60</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>60</v>
@@ -35759,7 +35792,7 @@
         <v>60</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="L32" s="0"/>
       <c r="O32" s="0"/>
@@ -35769,13 +35802,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>60</v>
@@ -35784,10 +35817,10 @@
         <v>60</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>60</v>
@@ -35796,7 +35829,7 @@
         <v>60</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="L33" s="0"/>
       <c r="O33" s="0"/>
@@ -35806,13 +35839,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>60</v>
@@ -35821,10 +35854,10 @@
         <v>60</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>60</v>
@@ -35833,7 +35866,7 @@
         <v>60</v>
       </c>
       <c r="K34" s="14" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="L34" s="0"/>
       <c r="O34" s="0"/>
@@ -35843,13 +35876,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>60</v>
@@ -35858,10 +35891,10 @@
         <v>60</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>60</v>
@@ -35870,7 +35903,7 @@
         <v>60</v>
       </c>
       <c r="K35" s="14" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="L35" s="0"/>
       <c r="O35" s="0"/>
@@ -35880,13 +35913,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>60</v>
@@ -35898,7 +35931,7 @@
         <v>60</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>60</v>
@@ -35911,7 +35944,7 @@
       </c>
       <c r="L36" s="0"/>
       <c r="O36" s="1" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35919,13 +35952,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>60</v>
@@ -35934,10 +35967,10 @@
         <v>60</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>60</v>
@@ -35946,7 +35979,7 @@
         <v>60</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="L37" s="0"/>
     </row>
@@ -35955,13 +35988,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>60</v>
@@ -35970,10 +36003,10 @@
         <v>60</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>60</v>
@@ -35982,7 +36015,7 @@
         <v>60</v>
       </c>
       <c r="K38" s="14" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="L38" s="0"/>
     </row>
@@ -35991,13 +36024,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>60</v>
@@ -36006,10 +36039,10 @@
         <v>60</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>60</v>
@@ -36018,7 +36051,7 @@
         <v>60</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="L39" s="0"/>
     </row>
@@ -36027,23 +36060,23 @@
         <v>38</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="E40" s="6"/>
       <c r="G40" s="10" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="L40" s="0"/>
     </row>
@@ -36052,13 +36085,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E41" s="6"/>
       <c r="G41" s="0"/>
@@ -36071,17 +36104,17 @@
         <v>40</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E42" s="6"/>
       <c r="G42" s="10" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="H42" s="0"/>
       <c r="K42" s="0"/>
@@ -36092,21 +36125,21 @@
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="E43" s="6"/>
       <c r="G43" s="10" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="H43" s="0"/>
       <c r="K43" s="1" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="L43" s="0"/>
     </row>
@@ -36115,17 +36148,17 @@
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="E44" s="6"/>
       <c r="G44" s="10" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>108</v>
@@ -36137,17 +36170,17 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="E45" s="6"/>
       <c r="G45" s="10" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="K45" s="0"/>
       <c r="L45" s="0"/>
@@ -36157,13 +36190,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="E46" s="6"/>
       <c r="G46" s="0"/>
@@ -36175,23 +36208,23 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="E47" s="6"/>
       <c r="G47" s="10" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36199,16 +36232,16 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="G48" s="0"/>
     </row>
@@ -36217,17 +36250,17 @@
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="E49" s="6"/>
       <c r="G49" s="10" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36235,17 +36268,17 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="E50" s="6"/>
       <c r="G50" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36253,13 +36286,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -36268,17 +36301,17 @@
       <c r="D52" s="24"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding oxygen libcore results
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="334">
   <si>
     <t>Index</t>
   </si>
@@ -373,8 +373,7 @@
 1248:            securityManager = System.getSecurityManager();</t>
   </si>
   <si>
-    <t>The code contains a possibly valid null and/or weakening of the SecurityManager.  The method enforceSecurity in the file ApplicationSecurityEnforcer.java should be investigated further.  See the Piazza post for more information.
-</t>
+    <t>The code contains a possibly valid null and/or weakening of the SecurityManager.  The method enforceSecurity in the file ApplicationSecurityEnforcer.java should be investigated further.  See the Piazza post for more information.</t>
   </si>
   <si>
     <t>Slideshow sample output:
@@ -3299,7 +3298,7 @@
   </si>
   <si>
     <t>New version doesn't contain any SecurityManager interactions – old version had SecurityManager lines commented out
-Category: Doesn't interact with SM at all – can remove from Database </t>
+Category: Doesn't interact with SM at all – can remove from Database</t>
   </si>
   <si>
     <t>jboss</t>
@@ -5204,7 +5203,7 @@
 482:        SecurityManager security = System.getSecurityManager();</t>
   </si>
   <si>
-    <t>Interacts with SM in main program </t>
+    <t>Interacts with SM in main program</t>
   </si>
   <si>
     <t>xerces</t>
@@ -5841,6 +5840,312 @@
     <t>https://github.com/ch33kybutt/oxygen_libcore</t>
   </si>
   <si>
+    <t>./luni/src/test/java/org/apache/harmony/sql/tests/java/sql/DriverManagerTest.java
+610:    class TestSecurityManager extends SecurityManager {
+617:                "setSecurityManager");
+619:        TestSecurityManager() {
+621:        } // end method TestSecurityManager()
+642:    } // end class TestSecurityManager
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/AllTests.java
+91:        suite.addTestSuite(SecurityManagerTest.class);
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/RuntimeTest.java
+244:        SecurityManager sm = new SecurityManager() {
+295:        SecurityManager sm = new SecurityManager() {
+348:        SecurityManager sm = new SecurityManager() {
+400:        SecurityManager sm = new SecurityManager() {
+455:        SecurityManager sm = new SecurityManager() {
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/ClassTest.java
+1782:    SecurityManager sm = new SecurityManager() {
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/MockSecurityManager.java
+8:class MockSecurityManager extends SecurityManager {
+30:        if (perm.equals(new RuntimePermission("createSecurityManager")) ||
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/MutableSecurityManager.java
+24:class MutableSecurityManager extends SecurityManager {
+26:    static final RuntimePermission SET_SECURITY_MANAGER = new RuntimePermission("setSecurityManager");
+36:    public MutableSecurityManager() {
+41:    public MutableSecurityManager(Permission... permissions) {
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/SystemTest.java
+464:     * @tests java.lang.System#getSecurityManager()
+469:        method = "getSecurityManager",
+472:    public void test_getSecurityManager() {
+473:        // Test for method java.lang.SecurityManager
+474:        // java.lang.System.getSecurityManager()
+475:        assertNull("Returned incorrect SecurityManager", System
+476:                .getSecurityManager());
+889:    private class MockSecurityManager extends SecurityManager {
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/SecurityManagerTest.java
+35: * Test case for java.lang.SecurityManager
+37:public class SecurityManagerTest extends TestCase {
+38:    MutableSecurityManager mutableSM = null;
+40:    MockSecurityManager mockSM = null;
+43:     * @tests java.lang.SecurityManager#checkPackageAccess(String)
+91:     * @tests java.lang.SecurityManager#checkPackageDefinition(String)
+139:     * @tests java.lang.SecurityManager#checkAccess(java.lang.Thread)
+150:        new SecurityManager().checkAccess(t);
+154:     * @tests {@link java.lang.SecurityManager#checkConnect(String, int, Object)}
+174:     * @tests {@link java.lang.SecurityManager#checkExec(String)}
+190:     * @tests {@link java.lang.SecurityManager#checkExit(int)}
+206:     * @tests {@link java.lang.SecurityManager#checkLink(String)}
+222:     * @tests {@link java.lang.SecurityManager#checkListen(int)}
+250:     * @tests {@link java.lang.SecurityManager#checkMulticast(java.net.InetAddress)}
+269:     * @tests {@link java.lang.SecurityManager#checkMulticast(java.net.InetAddress,byte)}
+290:     * @tests {@link java.lang.SecurityManager#checkPermission(Permission, Object)}
+311:     * @tests {@link java.lang.SecurityManager#checkPrintJobAccess()}
+327:     * @tests {@link java.lang.SecurityManager#checkRead(FileDescriptor)}
+343:     * @tests {@link java.lang.SecurityManager#checkRead(String,Object)}
+362:     * @tests {@link java.lang.SecurityManager#checkSetFactory()}
+378:     * @tests {@link java.lang.SecurityManager#getInCheck()}
+388:     * @tests {@link java.lang.SecurityManager#getSecurityContext()}
+404:     * @tests {@link java.lang.SecurityManager#classDepth(String)}
+412:     * @tests {@link java.lang.SecurityManager#classLoaderDepth()}
+419:     * @tests {@link java.lang.SecurityManager#currentClassLoader()}
+426:     * @tests {@link java.lang.SecurityManager#currentLoadedClass()}
+433:     * @tests {@link java.lang.SecurityManager#inClass(String)}
+438:        assertTrue(mockSM.inClass(MockSecurityManager.class.getName()));
+442:     * @tests {@link java.lang.SecurityManager#inClassLoader()}
+449:     * @tests {@link java.lang.SecurityManager#inClassLoader()}
+452:        assertEquals("MockSecurityManager should be the first in the classes stack",
+453:                mockSM.getClassContext()[0], MockSecurityManager.class);
+457:    class MockSecurityManager extends SecurityManager {
+502:        mutableSM = new MutableSecurityManager();
+503:        mockSM = new MockSecurityManager();
+./luni/src/test/java/org/apache/harmony/luni/tests/java/net/Inet6AddressTest.java
+32:import org.apache.harmony.luni.tests.java.net.InetAddressTest.MockSecurityManager;
+./luni/src/test/java/org/apache/harmony/luni/tests/java/net/InetAddressTest.java
+277:        class MockSecurityManager extends SecurityManager {
+279:                if (permission.getName().equals("setSecurityManager")){
+1052:    class MockSecurityManager extends SecurityManager {
+1054:            if (permission.getName().equals("setSecurityManager")){
+./luni/src/test/java/org/apache/harmony/luni/tests/java/io/BufferedReaderTest.java
+36:	String testString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+./luni/src/test/java/org/apache/harmony/luni/tests/java/io/RandomAccessFileTest.java
+44:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+./luni/src/test/java/org/apache/harmony/luni/tests/java/io/FileTest.java
+71:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_File\nTest_FileDescriptor\nTest_FileInputStream\nTest_FileNotFoundException\nTest_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+./luni/src/test/java/org/apache/harmony/nio/tests/java/nio/channels/MockSecurityManager.java
+5:class MockSecurityManager extends SecurityManager {
+14:    MockSecurityManager() {
+19:    MockSecurityManager(String host) {
+24:    MockSecurityManager(int port) {
+./luni/src/test/java/org/apache/harmony/archive/tests/java/util/jar/JarFileTest.java
+91:    SecurityManager sm = new SecurityManager() {
+./luni/src/test/java/org/apache/harmony/archive/tests/java/util/zip/ZipFileTest.java
+56:    SecurityManager sm = new SecurityManager() {
+./luni/src/test/java/org/apache/harmony/security/tests/java/security/ProviderTest.java
+697:    static class TestSecurityManager extends SecurityManager {
+701:        public TestSecurityManager(String permissionName) {
+./luni/src/test/java/org/apache/harmony/security/tests/java/security/Permissions2Test.java
+190:    class TestSecurityManager extends SecurityManager {
+./luni/src/test/java/org/apache/harmony/security/tests/java/security/IdentityScopeTest.java
+47:    public static class MySecurityManager extends SecurityManager {
+./luni/src/test/java/org/apache/harmony/security/tests/java/security/SignerTest.java
+54:    public static class MySecurityManager extends SecurityManager {
+./luni/src/test/java/tests/api/java/util/LocaleTest.java
+532:    SecurityManager sm = new SecurityManager() {
+./luni/src/test/java/tests/api/java/util/ResourceBundleTest.java
+43:    SecurityManager sm = new SecurityManager() {
+./luni/src/test/java/tests/api/java/util/concurrent/JSR166TestCase.java
+92:    private static final boolean useSecurityManager =
+93:        Boolean.getBoolean("jsr166.useSecurityManager");
+100:    //     if (useSecurityManager) {
+103:    //         System.setSecurityManager(new SecurityManager());
+404:        SecurityManager sm = System.getSecurityManager();
+410:                System.setSecurityManager(new SecurityManager());
+413:                System.setSecurityManager(null);
+473:             new RuntimePermission("setSecurityManager"),
+./luni/src/test/java/tests/api/java/util/concurrent/ExecutorsTest.java
+266:                        SecurityManager s = System.getSecurityManager();
+310:                        SecurityManager s = System.getSecurityManager();
+334:        SecurityManager sm = System.getSecurityManager();
+347:        SecurityManager sm = System.getSecurityManager();
+369:                if (System.getSecurityManager() == null)
+403:                if (System.getSecurityManager() == null)
+428://                     if (System.getSecurityManager() == null)
+445://                     if (System.getSecurityManager() == null)
+./luni/src/test/java/tests/api/java/io/PushbackInputStreamTest.java
+35:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+./luni/src/test/java/tests/api/java/io/ObjectOutputStreamTest.java
+43:import tests.support.Support_IOTestSecurityManager;
+724:        // Start testing without a SecurityManager.
+./luni/src/test/java/tests/api/java/io/FileOutputStreamTest.java
+60:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+./luni/src/test/java/tests/api/java/io/FilterOutputStreamTest.java
+41:    private final String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+./luni/src/test/java/tests/api/java/io/BufferedOutputStreamTest.java
+41:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+./luni/src/test/java/tests/api/java/io/FileInputStreamTest.java
+53:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_ja</t>
+  </si>
+  <si>
+    <t>Only does SecurityManager changes in test cases.  It checks if a SecurityManager is set to add permission checks if necessary.  No weakening or nulling.</t>
+  </si>
+  <si>
+    <t>./luni/src/test/java/org/apache/harmony/sql/tests/java/sql/DriverManagerTest.java
+610:    class TestSecurityManager extends SecurityManager {
+617:                "setSecurityManager");
+619:        TestSecurityManager() {
+621:        } // end method TestSecurityManager()
+642:    } // end class TestSecurityManager
+This is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/AllTests.java
+91:        suite.addTestSuite(SecurityManagerTest.class);
+this is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/RuntimeTest.java
+244:        SecurityManager sm = new SecurityManager() {
+295:        SecurityManager sm = new SecurityManager() {
+348:        SecurityManager sm = new SecurityManager() {
+400:        SecurityManager sm = new SecurityManager() {
+455:        SecurityManager sm = new SecurityManager() {
+This is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/ClassTest.java
+1782:    SecurityManager sm = new SecurityManager() {
+this is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/MockSecurityManager.java
+8:class MockSecurityManager extends SecurityManager {
+30:        if (perm.equals(new RuntimePermission("createSecurityManager")) ||
+this is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/MutableSecurityManager.java
+24:class MutableSecurityManager extends SecurityManager {
+26:    static final RuntimePermission SET_SECURITY_MANAGER = new RuntimePermission("setSecurityManager");
+36:    public MutableSecurityManager() {
+41:    public MutableSecurityManager(Permission... permissions) {
+This is a security manager that can change for test cases
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/SystemTest.java
+464:     * @tests java.lang.System#getSecurityManager()
+469:        method = "getSecurityManager",
+472:    public void test_getSecurityManager() {
+473:        // Test for method java.lang.SecurityManager
+474:        // java.lang.System.getSecurityManager()
+475:        assertNull("Returned incorrect SecurityManager", System
+476:                .getSecurityManager());
+889:    private class MockSecurityManager extends SecurityManager {
+This is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/lang/SecurityManagerTest.java
+35: * Test case for java.lang.SecurityManager
+37:public class SecurityManagerTest extends TestCase {
+38:    MutableSecurityManager mutableSM = null;
+40:    MockSecurityManager mockSM = null;
+43:     * @tests java.lang.SecurityManager#checkPackageAccess(String)
+91:     * @tests java.lang.SecurityManager#checkPackageDefinition(String)
+139:     * @tests java.lang.SecurityManager#checkAccess(java.lang.Thread)
+150:        new SecurityManager().checkAccess(t);
+154:     * @tests {@link java.lang.SecurityManager#checkConnect(String, int, Object)}
+174:     * @tests {@link java.lang.SecurityManager#checkExec(String)}
+190:     * @tests {@link java.lang.SecurityManager#checkExit(int)}
+206:     * @tests {@link java.lang.SecurityManager#checkLink(String)}
+222:     * @tests {@link java.lang.SecurityManager#checkListen(int)}
+250:     * @tests {@link java.lang.SecurityManager#checkMulticast(java.net.InetAddress)}
+269:     * @tests {@link java.lang.SecurityManager#checkMulticast(java.net.InetAddress,byte)}
+290:     * @tests {@link java.lang.SecurityManager#checkPermission(Permission, Object)}
+311:     * @tests {@link java.lang.SecurityManager#checkPrintJobAccess()}
+327:     * @tests {@link java.lang.SecurityManager#checkRead(FileDescriptor)}
+343:     * @tests {@link java.lang.SecurityManager#checkRead(String,Object)}
+362:     * @tests {@link java.lang.SecurityManager#checkSetFactory()}
+378:     * @tests {@link java.lang.SecurityManager#getInCheck()}
+388:     * @tests {@link java.lang.SecurityManager#getSecurityContext()}
+404:     * @tests {@link java.lang.SecurityManager#classDepth(String)}
+412:     * @tests {@link java.lang.SecurityManager#classLoaderDepth()}
+419:     * @tests {@link java.lang.SecurityManager#currentClassLoader()}
+426:     * @tests {@link java.lang.SecurityManager#currentLoadedClass()}
+433:     * @tests {@link java.lang.SecurityManager#inClass(String)}
+438:        assertTrue(mockSM.inClass(MockSecurityManager.class.getName()));
+442:     * @tests {@link java.lang.SecurityManager#inClassLoader()}
+449:     * @tests {@link java.lang.SecurityManager#inClassLoader()}
+452:        assertEquals("MockSecurityManager should be the first in the classes stack",
+453:                mockSM.getClassContext()[0], MockSecurityManager.class);
+457:    class MockSecurityManager extends SecurityManager {
+502:        mutableSM = new MutableSecurityManager();
+503:        mockSM = new MockSecurityManager();
+this is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/net/Inet6AddressTest.java
+32:import org.apache.harmony.luni.tests.java.net.InetAddressTest.MockSecurityManager;
+This is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/net/InetAddressTest.java
+277:        class MockSecurityManager extends SecurityManager {
+279:                if (permission.getName().equals("setSecurityManager")){
+1052:    class MockSecurityManager extends SecurityManager {
+1054:            if (permission.getName().equals("setSecurityManager")){
+This is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/io/BufferedReaderTest.java
+36:	String testString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+This is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/io/RandomAccessFileTest.java
+44:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+This is a test case
+./luni/src/test/java/org/apache/harmony/luni/tests/java/io/FileTest.java
+71:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_File\nTest_FileDescriptor\nTest_FileInputStream\nTest_FileNotFoundException\nTest_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+This is a test case
+./luni/src/test/java/org/apache/harmony/nio/tests/java/nio/channels/MockSecurityManager.java
+5:class MockSecurityManager extends SecurityManager {
+14:    MockSecurityManager() {
+19:    MockSecurityManager(String host) {
+24:    MockSecurityManager(int port) {
+This is a test case
+./luni/src/test/java/org/apache/harmony/archive/tests/java/util/jar/JarFileTest.java
+91:    SecurityManager sm = new SecurityManager() {
+This is a test case
+./luni/src/test/java/org/apache/harmony/archive/tests/java/util/zip/ZipFileTest.java
+56:    SecurityManager sm = new SecurityManager() {
+This is a test case
+./luni/src/test/java/org/apache/harmony/security/tests/java/security/ProviderTest.java
+697:    static class TestSecurityManager extends SecurityManager {
+701:        public TestSecurityManager(String permissionName) {
+This is a test case
+./luni/src/test/java/org/apache/harmony/security/tests/java/security/Permissions2Test.java
+190:    class TestSecurityManager extends SecurityManager {
+This is a test case
+./luni/src/test/java/org/apache/harmony/security/tests/java/security/IdentityScopeTest.java
+47:    public static class MySecurityManager extends SecurityManager {
+This is a test case
+./luni/src/test/java/org/apache/harmony/security/tests/java/security/SignerTest.java
+54:    public static class MySecurityManager extends SecurityManager {
+This is a test case
+./luni/src/test/java/tests/api/java/util/LocaleTest.java
+532:    SecurityManager sm = new SecurityManager() {
+This is a test case
+./luni/src/test/java/tests/api/java/util/ResourceBundleTest.java
+43:    SecurityManager sm = new SecurityManager() {
+This is a test case
+./luni/src/test/java/tests/api/java/util/concurrent/JSR166TestCase.java
+92:    private static final boolean useSecurityManager =
+93:        Boolean.getBoolean("jsr166.useSecurityManager");
+100:    //     if (useSecurityManager) {
+103:    //         System.setSecurityManager(new SecurityManager());
+404:        SecurityManager sm = System.getSecurityManager();
+410:                System.setSecurityManager(new SecurityManager());
+413:                System.setSecurityManager(null);
+473:             new RuntimePermission("setSecurityManager"),
+This is a test case
+./luni/src/test/java/tests/api/java/util/concurrent/ExecutorsTest.java
+266:                        SecurityManager s = System.getSecurityManager();
+310:                        SecurityManager s = System.getSecurityManager();
+334:        SecurityManager sm = System.getSecurityManager();
+347:        SecurityManager sm = System.getSecurityManager();
+369:                if (System.getSecurityManager() == null)
+403:                if (System.getSecurityManager() == null)
+428://                     if (System.getSecurityManager() == null)
+445://                     if (System.getSecurityManager() == null)
+This is a test case
+./luni/src/test/java/tests/api/java/io/PushbackInputStreamTest.java
+35:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+This is a test case
+./luni/src/test/java/tests/api/java/io/ObjectOutputStreamTest.java
+43:import tests.support.Support_IOTestSecurityManager;
+724:        // Start testing without a SecurityManager.
+This is a test case
+./luni/src/test/java/tests/api/java/io/FileOutputStreamTest.java
+60:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+This is a test case
+./luni/src/test/java/tests/api/java/io/FilterOutputStreamTest.java
+41:    private final String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+This is a test case
+./luni/src/test/java/tests/api/java/io/BufferedOutputStreamTest.java
+41:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\nTest_java_io_DataInputStream\nTest_java_io_File\nTest_java_io_FileDescriptor\nTest_java_io_FileInputStream\nTest_java_io_FileNotFoundException\nTest_java_io_FileOutputStream\nTest_java_io_FilterInputStream\nTest_java_io_FilterOutputStream\nTest_java_io_InputStream\nTest_java_io_IOException\nTest_java_io_OutputStream\nTest_java_io_PrintStream\nTest_java_io_RandomAccessFile\nTest_java_io_SyncFailedException\nTest_java_lang_AbstractMethodError\nTest_java_lang_ArithmeticException\nTest_java_lang_ArrayIndexOutOfBoundsException\nTest_java_lang_ArrayStoreException\nTest_java_lang_Boolean\nTest_java_lang_Byte\nTest_java_lang_Character\nTest_java_lang_Class\nTest_java_lang_ClassCastException\nTest_java_lang_ClassCircularityError\nTest_java_lang_ClassFormatError\nTest_java_lang_ClassLoader\nTest_java_lang_ClassNotFoundException\nTest_java_lang_CloneNotSupportedException\nTest_java_lang_Double\nTest_java_lang_Error\nTest_java_lang_Exception\nTest_java_lang_ExceptionInInitializerError\nTest_java_lang_Float\nTest_java_lang_IllegalAccessError\nTest_java_lang_IllegalAccessException\nTest_java_lang_IllegalArgumentException\nTest_java_lang_IllegalMonitorStateException\nTest_java_lang_IllegalThreadStateException\nTest_java_lang_IncompatibleClassChangeError\nTest_java_lang_IndexOutOfBoundsException\nTest_java_lang_InstantiationError\nTest_java_lang_InstantiationException\nTest_java_lang_Integer\nTest_java_lang_InternalError\nTest_java_lang_InterruptedException\nTest_java_lang_LinkageError\nTest_java_lang_Long\nTest_java_lang_Math\nTest_java_lang_NegativeArraySizeException\nTest_java_lang_NoClassDefFoundError\nTest_java_lang_NoSuchFieldError\nTest_java_lang_NoSuchMethodError\nTest_java_lang_NullPointerException\nTest_java_lang_Number\nTest_java_lang_NumberFormatException\nTest_java_lang_Object\nTest_java_lang_OutOfMemoryError\nTest_java_lang_RuntimeException\nTest_java_lang_SecurityManager\nTest_java_lang_Short\nTest_java_lang_StackOverflowError\nTest_java_lang_String\nTest_java_lang_StringBuffer\nTest_java_lang_StringIndexOutOfBoundsException\nTest_java_lang_System\nTest_java_lang_Thread\nTest_java_lang_ThreadDeath\nTest_java_lang_ThreadGroup\nTest_java_lang_Throwable\nTest_java_lang_UnknownError\nTest_java_lang_UnsatisfiedLinkError\nTest_java_lang_VerifyError\nTest_java_lang_VirtualMachineError\nTest_java_lang_vm_Image\nTest_java_lang_vm_MemorySegment\nTest_java_lang_vm_ROMStoreException\nTest_java_lang_vm_VM\nTest_java_lang_Void\nTest_java_net_BindException\nTest_java_net_ConnectException\nTest_java_net_DatagramPacket\nTest_java_net_DatagramSocket\nTest_java_net_DatagramSocketImpl\nTest_java_net_InetAddress\nTest_java_net_NoRouteToHostException\nTest_java_net_PlainDatagramSocketImpl\nTest_java_net_PlainSocketImpl\nTest_java_net_Socket\nTest_java_net_SocketException\nTest_java_net_SocketImpl\nTest_java_net_SocketInputStream\nTest_java_net_SocketOutputStream\nTest_java_net_UnknownHostException\nTest_java_util_ArrayEnumerator\nTest_java_util_Date\nTest_java_util_EventObject\nTest_java_util_HashEnumerator\nTest_java_util_Hashtable\nTest_java_util_Properties\nTest_java_util_ResourceBundle\nTest_java_util_tm\nTest_java_util_Vector\n";
+This is a test case
+./luni/src/test/java/tests/api/java/io/FileInputStreamTest.java
+53:    public String fileString = "Test_All_Tests\nTest_java_io_BufferedInputStream\nTest_java_io_BufferedOutputStream\nTest_java_io_ByteArrayInputStream\nTest_java_io_ByteArrayOutputStream\</t>
+  </si>
+  <si>
     <t>tomcat (this one can be removed because it is covered in qualitas)</t>
   </si>
   <si>
@@ -6268,13 +6573,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -6347,8 +6652,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36276,9 +36581,26 @@
       <c r="D50" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="E50" s="6"/>
-      <c r="G50" s="1" t="s">
-        <v>122</v>
+      <c r="E50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K50" s="10" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36286,13 +36608,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -36306,12 +36628,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added system rules analysis
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="336">
   <si>
     <t>Index</t>
   </si>
@@ -5831,6 +5831,178 @@
 235:				: originalSecurityManager.getThreadGroup();</t>
   </si>
   <si>
+    <t>This library provides methods to help with running Java test cases.  It provides two ways to effect the Security Manager in test cases.  One way which sets a SecurityManager before a test case and restores the original one after, and another way which sets a SecurityManager which stops System.exit and routes all other permission checks to the old manager (this allow tests to test if a System.exit works or not without killing the test program).  Overall, I would classify this program as only interacting with the SecurityManager in test cases.</t>
+  </si>
+  <si>
+    <t>./src/test/java/org/junit/contrib/java/lang/system/ProvideSecurityManagerTest.java
+3:import static java.lang.System.getSecurityManager;
+12:public class ProvideSecurityManagerTest {
+13:	private static final SecurityManager MANAGER = new SecurityManager() {
+22:			assertThat(getSecurityManager(), is(MANAGER));
+26:	public ProvideSecurityManager rule = new ProvideSecurityManager(MANAGER);
+34:	public void restoreOriginalSecurityManager() throws Throwable {
+35:		SecurityManager originalManager = getSecurityManager();
+37:		assertThat(getSecurityManager(), is(originalManager));
+this is a test case
+./src/test/java/org/junit/contrib/java/lang/system/internal/NoExitSecurityManagerTest.java
+22:public class NoExitSecurityManagerTest {
+31:	private final SecurityManager originalSecurityManager = mock(SecurityManager.class);
+32:	private final NoExitSecurityManager managerWithOriginal = new NoExitSecurityManager(
+33:			originalSecurityManager);
+34:	private final NoExitSecurityManager managerWithoutOriginal = new NoExitSecurityManager(
+46:		when(originalSecurityManager.getInCheck()).thenReturn(true);
+56:	public void provideSecurityContextOfOriginalSecurityManager() {
+58:		when(originalSecurityManager.getSecurityContext()).thenReturn(context);
+71:		verify(originalSecurityManager).checkPermission(permission);
+85:		verify(originalSecurityManager).checkPermission(permission, context);
+98:		verify(originalSecurityManager).checkCreateClassLoader();
+110:		verify(originalSecurityManager).checkAccess(thread);
+123:		verify(originalSecurityManager).checkAccess(threadGroup);
+135:		verify(originalSecurityManager).checkExec("arbitrary cmd");
+146:		verify(originalSecurityManager).checkLink("arbitrary lib");
+158:		verify(originalSecurityManager).checkRead(fileDescriptor);
+170:		verify(originalSecurityManager).checkRead("arbitrary file");
+182:		verify(originalSecurityManager).checkRead("arbitrary file", context);
+195:		verify(originalSecurityManager).checkWrite(fileDescriptor);
+207:		verify(originalSecurityManager).checkWrite("arbitrary file");
+218:		verify(originalSecurityManager).checkDelete("arbitrary file");
+230:		verify(originalSecurityManager).checkConnect("host", port);
+244:		verify(originalSecurityManager).checkConnect("host", port, context);
+258:		verify(originalSecurityManager).checkListen(port);
+271:		verify(originalSecurityManager).checkAccept("host", port);
+284:		verify(originalSecurityManager).checkMulticast(inetAddress);
+298:		verify(originalSecurityManager).checkMulticast(inetAddress, ttl);
+311:		verify(originalSecurityManager).checkPropertiesAccess();
+322:		verify(originalSecurityManager).checkPropertyAccess("arbitrary key");
+333:		when(originalSecurityManager.checkTopLevelWindow(window)).thenReturn(
+347:		verify(originalSecurityManager).checkPrintJobAccess();
+358:		verify(originalSecurityManager).checkSystemClipboardAccess();
+369:		verify(originalSecurityManager).checkAwtEventQueueAccess();
+380:		verify(originalSecurityManager).checkPackageAccess("arbitrary package");
+391:		verify(originalSecurityManager).checkPackageDefinition(
+403:		verify(originalSecurityManager).checkSetFactory();
+416:		verify(originalSecurityManager)
+430:		verify(originalSecurityManager).checkSecurityAccess("arbitrary target");
+439:	public void provideThreadGroupOfOriginalSecurityManager() {
+441:		when(originalSecurityManager.getThreadGroup()).thenReturn(threadGroup);
+This is a test case
+./src/test/java/org/junit/contrib/java/lang/system/ExpectedSystemExitTest.java
+3:import static java.lang.System.getSecurityManager;
+4:import static java.lang.System.setSecurityManager;
+113:	public void restoreOldSecurityManager() throws Throwable {
+114:		SecurityManager manager = new ArbitrarySecurityManager();
+115:		setSecurityManager(manager);
+117:		assertThat(getSecurityManager(), sameInstance(manager));
+121:	public void delegateToOldSecurityManager() throws Throwable {
+122:		SecurityManager manager = new ArbitrarySecurityManager();
+123:		setSecurityManager(manager);
+155:			assertEquals(ARBITRARY_CONTEXT, getSecurityManager()
+174:	private static class ArbitrarySecurityManager extends SecurityManager {
+This is a test case
+./src/main/java/org/junit/contrib/java/lang/system/ProvideSecurityManager.java
+3:import static java.lang.System.getSecurityManager;
+4:import static java.lang.System.setSecurityManager;
+9: * The {@code ProvideSecurityManager} rule provides an arbitrary security
+14: *     private final MySecurityManager securityManager
+15: *       = new MySecurityManager();
+18: *     public final ProvideSecurityManager provideSecurityManager
+19: *       = new ProvideSecurityManager(securityManager);
+23: *       assertEquals(securityManager, System.getSecurityManager());
+28:public class ProvideSecurityManager extends ExternalResource {
+29:	private final SecurityManager manager;
+30:	private SecurityManager originalManager;
+32:	public ProvideSecurityManager(SecurityManager manager) {
+38:		originalManager = getSecurityManager();
+39:		setSecurityManager(manager);
+44:		setSecurityManager(originalManager);
+This class provides SecurityManagers for running test cases.  It allows a security manager to be set before a test and restores the old one after the test.
+./src/main/java/org/junit/contrib/java/lang/system/internal/NoExitSecurityManager.java
+8: * A {@code NoExitSecurityManager} throws a {@link CheckExitCalled} exception
+12:public class NoExitSecurityManager extends SecurityManager {
+13:	private final SecurityManager originalSecurityManager;
+16:	public NoExitSecurityManager(SecurityManager originalSecurityManager) {
+17:		this.originalSecurityManager = originalSecurityManager;
+41:		return (originalSecurityManager != null)
+42:				&amp;&amp; originalSecurityManager.getInCheck();
+47:		return (originalSecurityManager == null) ? super.getSecurityContext()
+48:				: originalSecurityManager.getSecurityContext();
+53:		if (originalSecurityManager != null)
+54:			originalSecurityManager.checkPermission(perm);
+59:		if (originalSecurityManager != null)
+60:			originalSecurityManager.checkPermission(perm, context);
+65:		if (originalSecurityManager != null)
+66:			originalSecurityManager.checkCreateClassLoader();
+71:		if (originalSecurityManager != null)
+72:			originalSecurityManager.checkAccess(t);
+77:		if (originalSecurityManager != null)
+78:			originalSecurityManager.checkAccess(g);
+83:		if (originalSecurityManager != null)
+84:			originalSecurityManager.checkExec(cmd);
+89:		if (originalSecurityManager != null)
+90:			originalSecurityManager.checkLink(lib);
+95:		if (originalSecurityManager != null)
+96:			originalSecurityManager.checkRead(fd);
+101:		if (originalSecurityManager != null)
+102:			originalSecurityManager.checkRead(file);
+107:		if (originalSecurityManager != null)
+108:			originalSecurityManager.checkRead(file, context);
+113:		if (originalSecurityManager != null)
+114:			originalSecurityManager.checkWrite(fd);
+119:		if (originalSecurityManager != null)
+120:			originalSecurityManager.checkWrite(file);
+125:		if (originalSecurityManager != null)
+126:			originalSecurityManager.checkDelete(file);
+131:		if (originalSecurityManager != null)
+132:			originalSecurityManager.checkConnect(host, port);
+137:		if (originalSecurityManager != null)
+138:			originalSecurityManager.checkConnect(host, port, context);
+143:		if (originalSecurityManager != null)
+144:			originalSecurityManager.checkListen(port);
+149:		if (originalSecurityManager != null)
+150:			originalSecurityManager.checkAccept(host, port);
+155:		if (originalSecurityManager != null)
+156:			originalSecurityManager.checkMulticast(maddr);
+161:		if (originalSecurityManager != null)
+162:			originalSecurityManager.checkMulticast(maddr, ttl);
+167:		if (originalSecurityManager != null)
+168:			originalSecurityManager.checkPropertiesAccess();
+173:		if (originalSecurityManager != null)
+174:			originalSecurityManager.checkPropertyAccess(key);
+179:		return (originalSecurityManager == null) ? super
+180:				.checkTopLevelWindow(window) : originalSecurityManager
+186:		if (originalSecurityManager != null)
+187:			originalSecurityManager.checkPrintJobAccess();
+192:		if (originalSecurityManager != null)
+193:			originalSecurityManager.checkSystemClipboardAccess();
+198:		if (originalSecurityManager != null)
+199:			originalSecurityManager.checkAwtEventQueueAccess();
+204:		if (originalSecurityManager != null)
+205:			originalSecurityManager.checkPackageAccess(pkg);
+210:		if (originalSecurityManager != null)
+211:			originalSecurityManager.checkPackageDefinition(pkg);
+216:		if (originalSecurityManager != null)
+217:			originalSecurityManager.checkSetFactory();
+222:		if (originalSecurityManager != null)
+223:			originalSecurityManager.checkMemberAccess(clazz, which);
+228:		if (originalSecurityManager != null)
+229:			originalSecurityManager.checkSecurityAccess(target);
+234:		return (originalSecurityManager == null) ? super.getThreadGroup()
+235:				: originalSecurityManager.getThreadGroup();
+This class is used to stop system exits.  It delegates all other permission checks to the original security manager if one was set.
+./src/main/java/org/junit/contrib/java/lang/system/ExpectedSystemExit.java
+3:import static java.lang.System.getSecurityManager;
+11:import org.junit.contrib.java.lang.system.internal.NoExitSecurityManager;
+113:		ProvideSecurityManager noExitSecurityManagerRule = createNoExitSecurityManagerRule();
+115:		return noExitSecurityManagerRule.apply(statement, description);
+118:	private ProvideSecurityManager createNoExitSecurityManagerRule() {
+119:		NoExitSecurityManager noExitSecurityManager = new NoExitSecurityManager(
+120:				getSecurityManager());
+121:		return new ProvideSecurityManager(noExitSecurityManager);
+139:		NoExitSecurityManager securityManager = (NoExitSecurityManager) getSecurityManager();
+This class provides a way to catch expected system exits in test cases.
+</t>
+  </si>
+  <si>
     <t>oxygen-libcore</t>
   </si>
   <si>
@@ -6652,8 +6824,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36563,9 +36735,26 @@
       <c r="D49" s="24" t="s">
         <v>321</v>
       </c>
-      <c r="E49" s="6"/>
+      <c r="E49" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G49" s="10" t="s">
         <v>322</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36573,13 +36762,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>60</v>
@@ -36588,10 +36777,10 @@
         <v>60</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>60</v>
@@ -36600,7 +36789,7 @@
         <v>60</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36608,13 +36797,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -36628,12 +36817,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding the analysis for Gjman
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="339">
   <si>
     <t>Index</t>
   </si>
@@ -5626,6 +5626,9 @@
 21:    System.setSecurityManager( null ) ;</t>
   </si>
   <si>
+    <t>Contains a file used to set a SecurityManager that only prevents System.exit calls and contains another function to remove the SecurityManager after (setting it to null).  This file is not worried about security.  Only preventing an application from exiting prematurely. </t>
+  </si>
+  <si>
     <t>Related code:class ForbidSystemExit
 {
   public static class Exception extends SecurityException { }
@@ -5645,7 +5648,7 @@
 }</t>
   </si>
   <si>
-    <t>← don't think it's doing something harmful. In contrast, it fortfies the policy by preventing exiting.</t>
+    <t>← Tianyuan: I don't think it's doing something harmful. In contrast, it fortfies the policy by preventing exiting.</t>
   </si>
   <si>
     <t>visor</t>
@@ -5658,7 +5661,15 @@
 This repository seems to have been removed by the end of the summer</t>
   </si>
   <si>
-    <t>404 not found</t>
+    <t>./SecurityManager/src/io/hypernet/visor/security/SecurityManager.java
+7:public class SecurityManager extends java.lang.SecurityManager {
+14:	public SecurityManager() {</t>
+  </si>
+  <si>
+    <t>Contains a class that extends the SecurityManager but never sets a SecurityManager in the application.  I don't think the code was completed at the time this was downloaded and the SecurityManager section was isolated from the rest of the code.  The security manager seems to extend the basic security manager by override the networking check actions and the check property access.   I would classify as no weakening or nulling.</t>
+  </si>
+  <si>
+    <t>See general comments</t>
   </si>
   <si>
     <t>System Rules</t>
@@ -6000,8 +6011,7 @@
 120:				getSecurityManager());
 121:		return new ProvideSecurityManager(noExitSecurityManager);
 139:		NoExitSecurityManager securityManager = (NoExitSecurityManager) getSecurityManager();
-This class provides a way to catch expected system exits in test cases.
-</t>
+This class provides a way to catch expected system exits in test cases.</t>
   </si>
   <si>
     <t>oxygen-libcore</t>
@@ -6750,13 +6760,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -6829,8 +6839,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36551,12 +36561,15 @@
         <v>282</v>
       </c>
       <c r="E40" s="6"/>
+      <c r="F40" s="0"/>
       <c r="G40" s="10" t="s">
         <v>283</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>284</v>
       </c>
+      <c r="I40" s="0"/>
+      <c r="J40" s="0"/>
       <c r="K40" s="10" t="s">
         <v>285</v>
       </c>
@@ -36576,8 +36589,11 @@
         <v>288</v>
       </c>
       <c r="E41" s="6"/>
+      <c r="F41" s="0"/>
       <c r="G41" s="0"/>
       <c r="H41" s="0"/>
+      <c r="I41" s="0"/>
+      <c r="J41" s="0"/>
       <c r="K41" s="0"/>
       <c r="L41" s="0"/>
     </row>
@@ -36595,10 +36611,13 @@
         <v>291</v>
       </c>
       <c r="E42" s="6"/>
+      <c r="F42" s="0"/>
       <c r="G42" s="10" t="s">
         <v>292</v>
       </c>
       <c r="H42" s="0"/>
+      <c r="I42" s="0"/>
+      <c r="J42" s="0"/>
       <c r="K42" s="0"/>
       <c r="L42" s="0"/>
     </row>
@@ -36616,10 +36635,13 @@
         <v>295</v>
       </c>
       <c r="E43" s="6"/>
+      <c r="F43" s="0"/>
       <c r="G43" s="10" t="s">
         <v>296</v>
       </c>
       <c r="H43" s="0"/>
+      <c r="I43" s="0"/>
+      <c r="J43" s="0"/>
       <c r="K43" s="1" t="s">
         <v>297</v>
       </c>
@@ -36639,9 +36661,13 @@
         <v>300</v>
       </c>
       <c r="E44" s="6"/>
+      <c r="F44" s="0"/>
       <c r="G44" s="10" t="s">
         <v>301</v>
       </c>
+      <c r="H44" s="0"/>
+      <c r="I44" s="0"/>
+      <c r="J44" s="0"/>
       <c r="K44" s="1" t="s">
         <v>108</v>
       </c>
@@ -36661,9 +36687,13 @@
         <v>304</v>
       </c>
       <c r="E45" s="6"/>
+      <c r="F45" s="0"/>
       <c r="G45" s="10" t="s">
         <v>305</v>
       </c>
+      <c r="H45" s="0"/>
+      <c r="I45" s="0"/>
+      <c r="J45" s="0"/>
       <c r="K45" s="0"/>
       <c r="L45" s="0"/>
     </row>
@@ -36681,7 +36711,11 @@
         <v>308</v>
       </c>
       <c r="E46" s="6"/>
+      <c r="F46" s="0"/>
       <c r="G46" s="0"/>
+      <c r="H46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="J46" s="0"/>
       <c r="K46" s="0"/>
       <c r="L46" s="0"/>
     </row>
@@ -36698,15 +36732,29 @@
       <c r="D47" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="G47" s="10" t="s">
         <v>312</v>
       </c>
+      <c r="H47" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="K47" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="L47" s="1" t="s">
         <v>314</v>
+      </c>
+      <c r="L47" s="10" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36714,31 +36762,48 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="G48" s="0"/>
+        <v>60</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>60</v>
@@ -36747,10 +36812,10 @@
         <v>60</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>60</v>
@@ -36759,7 +36824,7 @@
         <v>60</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36767,13 +36832,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>60</v>
@@ -36782,10 +36847,10 @@
         <v>60</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>60</v>
@@ -36794,7 +36859,7 @@
         <v>60</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36802,13 +36867,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -36822,12 +36887,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished all but two of the git analysis
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="348">
   <si>
     <t>Index</t>
   </si>
@@ -5536,10 +5536,13 @@
 16:    System.setSecurityManager(null);</t>
   </si>
   <si>
+    <t>We decided to exclude this one since it is mainly written in ruby and the only Java sections are tests to see if the program is malicious.</t>
+  </si>
+  <si>
     <t>driveddoc</t>
   </si>
   <si>
-    <t>0b2a80d8c0f9ba2d3e8f38ff4716da7c900c1183</t>
+    <t>12993baabfd0dd0ca629e4bb8046097f290d1bb8</t>
   </si>
   <si>
     <t>https://github.com/aleksz/driveddoc</t>
@@ -5547,16 +5550,24 @@
   <si>
     <t>./src/test/java/com/gmail/at/zhuikov/aleksandr/driveddoc/RestrictedFileWritingRule.java
 12:		System.setSecurityManager(new SecurityManager() {
-28:		System.setSecurityManager(null); // or save and restore original</t>
+28:		System.setSecurityManager(null); // or save and restore original
+</t>
   </si>
   <si>
-    <t>Although it sets SM to null via after() method inRestrictedFileWritingRule.java, this method is called nowhere.</t>
+    <t>Sets a SecurityManager before a test case and removes it afterwards.  No weakening or nulling occurs.  The program also does not interact with the SecurityManager in the main file.</t>
+  </si>
+  <si>
+    <t>./src/test/java/com/gmail/at/zhuikov/aleksandr/driveddoc/RestrictedFileWritingRule.java
+12:		System.setSecurityManager(new SecurityManager() {
+28:		System.setSecurityManager(null); // or save and restore original
+Sets a SecurityManager for a test case and removes the SecurityManager after the test case
+</t>
   </si>
   <si>
     <t>TracEE</t>
   </si>
   <si>
-    <t>205ada0800e089131a35f5e885a627b3f79fba5b</t>
+    <t>c05cb9e8127a39017202e5bfa213d1879e6bdbc7</t>
   </si>
   <si>
     <t>https://github.com/holisticon/tracee</t>
@@ -5575,6 +5586,27 @@
 53:	private class TestSecurityManager extends SecurityManager {
 ./api/src/main/java/io/tracee/BackendProviderResolver.java
 139:			if (System.getSecurityManager() != null) {</t>
+  </si>
+  <si>
+    <t>Gets a class loader with do privileged if a SecurityManager is set.  No weakening or nulling occurs.</t>
+  </si>
+  <si>
+    <t>./api/src/test/java/io/tracee/BackendProviderResolverGetClassLoaderTest.java
+16:	public void shouldFetchContextClassloaderWithoutSecurityManager() {
+17:		System.setSecurityManager(null);
+23:	public void shouldReturnClassloaderOfClassWithoutSecurityManager() {
+24:		System.setSecurityManager(null);
+30:	public void shouldFetchContextClassloaderWithSecurityManager() {
+31:		System.setSecurityManager(new TestSecurityManager());
+37:	public void shouldReturnClassloaderOfClassWithSecurityManager() {
+38:		System.setSecurityManager(new TestSecurityManager());
+50:		System.setSecurityManager(null);
+53:	private class TestSecurityManager extends SecurityManager {
+Test cases - test if the program can get a class loader without a SM set and with an SM set
+./api/src/main/java/io/tracee/BackendProviderResolver.java
+139:			if (System.getSecurityManager() != null) {
+runs doPriveleged if a SM is set to get a class loader
+</t>
   </si>
   <si>
     <t>Spring-modules</t>
@@ -5602,13 +5634,210 @@
 86:	public void setSecurityManager(SecurityManager securityManager) {</t>
   </si>
   <si>
-    <t>Security-Manager (This is a SecuirtyManager - not a program that uses one)</t>
+    <t>This library allows setting and restoring a SecurityManager thus allowing weakening and nulling.  I decided not to test because with dynamic analysis because it wasn't straightforward how (project states it is currently being fixed from a non-working state; hasn't been changed in about 5 years; and interacts directly with spring-framework but doesn't say how to set it up together) and the application was easy to understand from the grep analysis.</t>
   </si>
   <si>
-    <t>f9dec14f40e0cbad54532b4dd578a9bd8bb6a11e</t>
+    <t>./projects/javaspaces/src/test/org/springmodules/javaspaces/SecurityTests.java
+9:import java.rmi.RMISecurityManager;
+22:	public void testRMISecurityManager() throws Exception {
+23:		SecurityManager securityManager = System.getSecurityManager();
+29:			System.setSecurityManager(new RMISecurityManager());
+30:			System.setSecurityManager(null);
+33:			System.setSecurityManager(securityManager);
+Tests if the current policy allows turning off and on the security manager.
+./projects/javaspaces/src/java/org/springmodules/jini/JiniSecuritySetter.java
+28:	private SecurityManager securityManager, oldSecurityManager;
+51:		System.setSecurityManager(oldSecurityManager);
+56:		oldSecurityManager = System.getSecurityManager();
+59:		System.setSecurityManager(securityManager);
+79:	public SecurityManager getSecurityManager() {
+86:	public void setSecurityManager(SecurityManager securityManager) {
+Allows all possible changes to the current SecurityManager.  This class is designed to set a specific security policy for the spring-modules application, and can then restore the old security policy afterwards.
+</t>
+  </si>
+  <si>
+    <t>Security-Manager (This is a SecurityManager - not a program that uses one)</t>
+  </si>
+  <si>
+    <t>96651247e313dd4662e52a6f8949632fdee2793e</t>
   </si>
   <si>
     <t>https://github.com/wildfly-security/security-manager</t>
+  </si>
+  <si>
+    <t>./src/main/java/org/wildfly/security/manager/StackInspector.java
+23:import static java.lang.System.getSecurityManager;
+25:import static org.wildfly.security.manager.WildFlySecurityManagerPermission.GET_STACK_INSPECTOR_PERMISSION;
+46:        if (WildFlySecurityManager.isChecking()) {
+47:            getSecurityManager().checkPermission(GET_STACK_INSPECTOR_PERMISSION);
+60:        return WildFlySecurityManager.getCallerClass(max(0, skipFrames) + 2);
+72:        final Class&lt;?&gt;[] stack = WildFlySecurityManager.getCallStack();
+85:        final Class&lt;?&gt;[] stack = WildFlySecurityManager.getCallStack();
+96:        final Class&lt;?&gt;[] stack = WildFlySecurityManager.getCallStack();
+107:        final Class&lt;?&gt;[] stack = WildFlySecurityManager.getCallStack();
+./src/main/java/org/wildfly/security/manager/WildFlySecurityManagerPermission.java
+41:public final class WildFlySecurityManagerPermission extends BasicPermission {
+50:        private final WildFlySecurityManagerPermission permission;
+53:            this.permission = new WildFlySecurityManagerPermission(this);
+56:        WildFlySecurityManagerPermission getPermission() {
+70:    static final WildFlySecurityManagerPermission DO_UNCHECKED_PERMISSION = Name.doUnchecked.getPermission();
+71:    static final WildFlySecurityManagerPermission GET_STACK_INSPECTOR_PERMISSION = Name.getStackInspector.getPermission();
+77:    WildFlySecurityManagerPermission(final Name name) {
+82:    public WildFlySecurityManagerPermission(final String name) {
+86:    public WildFlySecurityManagerPermission(final String name, final String actions) {
+94:        return new WildFlySecurityManagerPermissionCollection();
+98:        return p instanceof WildFlySecurityManagerPermission &amp;&amp; name == ((WildFlySecurityManagerPermission) p).name;
+102:        return obj instanceof WildFlySecurityManagerPermission &amp;&amp; name == ((WildFlySecurityManagerPermission) obj).name;
+./src/main/java/org/wildfly/security/manager/WildFlySecurityManagerPermissionCollection.java
+39: * A permission collection for {@link WildFlySecurityManagerPermission} instances.
+43:public final class WildFlySecurityManagerPermissionCollection extends PermissionCollection {
+55:        if (permission instanceof WildFlySecurityManagerPermission) {
+56:            setBit(((WildFlySecurityManagerPermission) permission).getKind().ordinal());
+58:            throw SecurityMessages.permission.wrongPermType(WildFlySecurityManagerPermission.class, permission);
+80:        return permission instanceof WildFlySecurityManagerPermission &amp;&amp; isSet(((WildFlySecurityManagerPermission) permission).getKind().ordinal());
+97:                return WildFlySecurityManagerPermission.values[Integer.numberOfTrailingZeros(bit)].getPermission();
+103:        return obj instanceof WildFlySecurityManagerPermissionCollection &amp;&amp; set.get() == ((WildFlySecurityManagerPermissionCollection) obj).set.get();
+./src/main/java/org/wildfly/security/manager/WildFlySecurityManager.java
+64:import static java.lang.System.getSecurityManager;
+69:import static org.wildfly.security.manager.WildFlySecurityManagerPermission.DO_UNCHECKED_PERMISSION;
+79:public final class WildFlySecurityManager extends SecurityManager {
+81:    private static final Permission SECURITY_MANAGER_PERMISSION = new RuntimePermission("setSecurityManager");
+102:    private static final WildFlySecurityManager INSTANCE;
+108:        INSTANCE = doPrivileged(new PrivilegedAction&lt;WildFlySecurityManager&gt;() {
+109:            public WildFlySecurityManager run() {
+110:                return new WildFlySecurityManager();
+117:            result = Reflection.getCallerClass(1) == WildFlySecurityManager.class || Reflection.getCallerClass(2) == WildFlySecurityManager.class;
+133:    public WildFlySecurityManager() throws SecurityException {
+138:        if (System.getSecurityManager() instanceof WildFlySecurityManager) return;
+139:        System.setSecurityManager(new WildFlySecurityManager());
+161:        final SecurityManager sm = getSecurityManager();
+162:        return sm instanceof WildFlySecurityManager ? doCheck() : sm != null;
+288:    private static boolean doCheck(final WildFlySecurityManager.Context ctx) {
+681:            final SecurityManager sm = getSecurityManager();
+711:            final SecurityManager sm = getSecurityManager();
+739:            final SecurityManager sm = getSecurityManager();
+766:            final SecurityManager sm = getSecurityManager();
+779:        if (getSecurityManager() instanceof WildFlySecurityManager) {
+799:        if (getSecurityManager() instanceof WildFlySecurityManager) {
+819:        if (getSecurityManager() instanceof WildFlySecurityManager) {
+839:        if (getSecurityManager() instanceof WildFlySecurityManager) {
+860:        final SecurityManager sm = getSecurityManager();
+864:        if (sm instanceof WildFlySecurityManager) {
+894:        final SecurityManager sm = getSecurityManager();
+898:        if (sm instanceof WildFlySecurityManager) {
+924:        final SecurityManager sm = getSecurityManager();
+928:        if (sm instanceof WildFlySecurityManager) {
+953:        final SecurityManager sm = getSecurityManager();
+957:        if (sm instanceof WildFlySecurityManager) {
+982:        final SecurityManager sm = System.getSecurityManager();
+986:        if (sm instanceof WildFlySecurityManager) {
+1012:        final SecurityManager sm = System.getSecurityManager();
+1019:        if (sm instanceof WildFlySecurityManager) {
+1052:        final SecurityManager sm = System.getSecurityManager();
+1059:        if (sm instanceof WildFlySecurityManager) {
+1095:        final SecurityManager sm = System.getSecurityManager();
+1099:        if (sm instanceof WildFlySecurityManager) {
+1124:        final SecurityManager sm = System.getSecurityManager();
+1128:        if (sm instanceof WildFlySecurityManager) {
+1154:        final SecurityManager sm = System.getSecurityManager();
+1158:        if (sm instanceof WildFlySecurityManager) {
+./src/main/java/org/wildfly/security/manager/package-info.java
+25: * the security manager, see {@link WildFlySecurityManager#install()}.
+./src/main/java/org/wildfly/security/manager/_private/SecurityMessages.java
+33:import org.wildfly.security.manager.WildFlySecurityManagerPermission;
+</t>
+  </si>
+  <si>
+    <t>This program is a SecurityManager, so it doesn't ever set a SecurityManager.  This extension allows turning the security checks off if the class already has the permission to do so (reimplementing how doPrivileged works in my opinion) and adds logs explaining why security checks fail. No nulling but allows weaken (although debatable).  Decided not to statically and dynamically test because it was easy to understand from the grep analysis.</t>
+  </si>
+  <si>
+    <t>./src/main/java/org/wildfly/security/manager/StackInspector.java
+23:import static java.lang.System.getSecurityManager;
+25:import static org.wildfly.security.manager.WildFlySecurityManagerPermission.GET_STACK_INSPECTOR_PERMISSION;
+46:        if (WildFlySecurityManager.isChecking()) {
+47:            getSecurityManager().checkPermission(GET_STACK_INSPECTOR_PERMISSION);
+60:        return WildFlySecurityManager.getCallerClass(max(0, skipFrames) + 2);
+72:        final Class&lt;?&gt;[] stack = WildFlySecurityManager.getCallStack();
+85:        final Class&lt;?&gt;[] stack = WildFlySecurityManager.getCallStack();
+96:        final Class&lt;?&gt;[] stack = WildFlySecurityManager.getCallStack();
+107:        final Class&lt;?&gt;[] stack = WildFlySecurityManager.getCallStack();
+uses the security manager to inspect the current call stack.
+./src/main/java/org/wildfly/security/manager/WildFlySecurityManagerPermission.java
+41:public final class WildFlySecurityManagerPermission extends BasicPermission {
+50:        private final WildFlySecurityManagerPermission permission;
+53:            this.permission = new WildFlySecurityManagerPermission(this);
+56:        WildFlySecurityManagerPermission getPermission() {
+70:    static final WildFlySecurityManagerPermission DO_UNCHECKED_PERMISSION = Name.doUnchecked.getPermission();
+71:    static final WildFlySecurityManagerPermission GET_STACK_INSPECTOR_PERMISSION = Name.getStackInspector.getPermission();
+77:    WildFlySecurityManagerPermission(final Name name) {
+82:    public WildFlySecurityManagerPermission(final String name) {
+86:    public WildFlySecurityManagerPermission(final String name, final String actions) {
+94:        return new WildFlySecurityManagerPermissionCollection();
+98:        return p instanceof WildFlySecurityManagerPermission &amp;&amp; name == ((WildFlySecurityManagerPermission) p).name;
+102:        return obj instanceof WildFlySecurityManagerPermission &amp;&amp; name == ((WildFlySecurityManagerPermission) obj).name;
+creates a new permission for their SecurityManager
+./src/main/java/org/wildfly/security/manager/WildFlySecurityManagerPermissionCollection.java
+39: * A permission collection for {@link WildFlySecurityManagerPermission} instances.
+43:public final class WildFlySecurityManagerPermissionCollection extends PermissionCollection {
+55:        if (permission instanceof WildFlySecurityManagerPermission) {
+56:            setBit(((WildFlySecurityManagerPermission) permission).getKind().ordinal());
+58:            throw SecurityMessages.permission.wrongPermType(WildFlySecurityManagerPermission.class, permission);
+80:        return permission instanceof WildFlySecurityManagerPermission &amp;&amp; isSet(((WildFlySecurityManagerPermission) permission).getKind().ordinal());
+97:                return WildFlySecurityManagerPermission.values[Integer.numberOfTrailingZeros(bit)].getPermission();
+103:        return obj instanceof WildFlySecurityManagerPermissionCollection &amp;&amp; set.get() == ((WildFlySecurityManagerPermissionCollection) obj).set.get();
+A permission collection of only wildflysecurtymanagerpermission instances
+./src/main/java/org/wildfly/security/manager/WildFlySecurityManager.java
+64:import static java.lang.System.getSecurityManager;
+69:import static org.wildfly.security.manager.WildFlySecurityManagerPermission.DO_UNCHECKED_PERMISSION;
+79:public final class WildFlySecurityManager extends SecurityManager {
+81:    private static final Permission SECURITY_MANAGER_PERMISSION = new RuntimePermission("setSecurityManager");
+102:    private static final WildFlySecurityManager INSTANCE;
+108:        INSTANCE = doPrivileged(new PrivilegedAction&lt;WildFlySecurityManager&gt;() {
+109:            public WildFlySecurityManager run() {
+110:                return new WildFlySecurityManager();
+117:            result = Reflection.getCallerClass(1) == WildFlySecurityManager.class || Reflection.getCallerClass(2) == WildFlySecurityManager.class;
+133:    public WildFlySecurityManager() throws SecurityException {
+138:        if (System.getSecurityManager() instanceof WildFlySecurityManager) return;
+139:        System.setSecurityManager(new WildFlySecurityManager());
+161:        final SecurityManager sm = getSecurityManager();
+162:        return sm instanceof WildFlySecurityManager ? doCheck() : sm != null;
+288:    private static boolean doCheck(final WildFlySecurityManager.Context ctx) {
+681:            final SecurityManager sm = getSecurityManager();
+711:            final SecurityManager sm = getSecurityManager();
+739:            final SecurityManager sm = getSecurityManager();
+766:            final SecurityManager sm = getSecurityManager();
+779:        if (getSecurityManager() instanceof WildFlySecurityManager) {
+799:        if (getSecurityManager() instanceof WildFlySecurityManager) {
+819:        if (getSecurityManager() instanceof WildFlySecurityManager) {
+839:        if (getSecurityManager() instanceof WildFlySecurityManager) {
+860:        final SecurityManager sm = getSecurityManager();
+864:        if (sm instanceof WildFlySecurityManager) {
+894:        final SecurityManager sm = getSecurityManager();
+898:        if (sm instanceof WildFlySecurityManager) {
+924:        final SecurityManager sm = getSecurityManager();
+928:        if (sm instanceof WildFlySecurityManager) {
+953:        final SecurityManager sm = getSecurityManager();
+957:        if (sm instanceof WildFlySecurityManager) {
+982:        final SecurityManager sm = System.getSecurityManager();
+986:        if (sm instanceof WildFlySecurityManager) {
+1012:        final SecurityManager sm = System.getSecurityManager();
+1019:        if (sm instanceof WildFlySecurityManager) {
+1052:        final SecurityManager sm = System.getSecurityManager();
+1059:        if (sm instanceof WildFlySecurityManager) {
+1095:        final SecurityManager sm = System.getSecurityManager();
+1099:        if (sm instanceof WildFlySecurityManager) {
+1124:        final SecurityManager sm = System.getSecurityManager();
+1128:        if (sm instanceof WildFlySecurityManager) {
+1154:        final SecurityManager sm = System.getSecurityManager();
+1158:        if (sm instanceof WildFlySecurityManager) {
+Allows callers to have a permission to turn off security checks and then will run privileged actions without the security check.  However, this seems like remimplementing how permissions and doPriveleged works.  So this is debateable weakening in my opinion.  Also logs which class caused the security check to fail.
+./src/main/java/org/wildfly/security/manager/package-info.java
+25: * the security manager, see {@link WildFlySecurityManager#install()}.
+in a comment.
+./src/main/java/org/wildfly/security/manager/_private/SecurityMessages.java
+33:import org.wildfly.security.manager.WildFlySecurityManagerPermission;
+this is a privelege import statement.
+</t>
   </si>
   <si>
     <t>Gjman</t>
@@ -5626,7 +5855,7 @@
 21:    System.setSecurityManager( null ) ;</t>
   </si>
   <si>
-    <t>Contains a file used to set a SecurityManager that only prevents System.exit calls and contains another function to remove the SecurityManager after (setting it to null).  This file is not worried about security.  Only preventing an application from exiting prematurely. </t>
+    <t>Contains a file used to set a SecurityManager that only prevents System.exit calls and contains another function to remove the SecurityManager after (setting it to null).  This file is not worried about security.  Only preventing an application from exiting prematurely.</t>
   </si>
   <si>
     <t>Related code:class ForbidSystemExit
@@ -6760,13 +6989,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -6839,8 +7068,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36610,15 +36839,27 @@
       <c r="D42" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="0"/>
+      <c r="E42" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="G42" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="H42" s="0"/>
-      <c r="I42" s="0"/>
-      <c r="J42" s="0"/>
-      <c r="K42" s="0"/>
+      <c r="H42" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="L42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36626,24 +36867,30 @@
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="0"/>
       <c r="G43" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="H43" s="0"/>
-      <c r="I43" s="0"/>
-      <c r="J43" s="0"/>
-      <c r="K43" s="1" t="s">
         <v>297</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K43" s="10" t="s">
+        <v>299</v>
       </c>
       <c r="L43" s="0"/>
     </row>
@@ -36652,24 +36899,34 @@
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="0"/>
+        <v>302</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="G44" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="H44" s="0"/>
-      <c r="I44" s="0"/>
-      <c r="J44" s="0"/>
-      <c r="K44" s="1" t="s">
-        <v>108</v>
+        <v>303</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>305</v>
       </c>
       <c r="L44" s="0"/>
     </row>
@@ -36678,23 +36935,35 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>304</v>
-      </c>
-      <c r="E45" s="6"/>
-      <c r="F45" s="0"/>
+        <v>308</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="G45" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="H45" s="0"/>
-      <c r="I45" s="0"/>
-      <c r="J45" s="0"/>
-      <c r="K45" s="0"/>
+        <v>309</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="L45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36702,21 +36971,35 @@
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="0"/>
-      <c r="G46" s="0"/>
-      <c r="H46" s="0"/>
-      <c r="I46" s="0"/>
-      <c r="J46" s="0"/>
-      <c r="K46" s="0"/>
+        <v>314</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="L46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36724,13 +37007,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>60</v>
@@ -36739,10 +37022,10 @@
         <v>60</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>60</v>
@@ -36751,10 +37034,10 @@
         <v>60</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36762,13 +37045,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>60</v>
@@ -36777,10 +37060,10 @@
         <v>60</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>60</v>
@@ -36789,7 +37072,7 @@
         <v>60</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36797,13 +37080,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>60</v>
@@ -36812,10 +37095,10 @@
         <v>60</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>60</v>
@@ -36824,7 +37107,7 @@
         <v>60</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36832,13 +37115,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>60</v>
@@ -36847,10 +37130,10 @@
         <v>60</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>60</v>
@@ -36859,7 +37142,7 @@
         <v>60</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36867,13 +37150,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -36887,12 +37170,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished all but one of the git analysis
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="352">
   <si>
     <t>Index</t>
   </si>
@@ -5454,14 +5454,38 @@
     <t>https://github.com/Babast/Timelag</t>
   </si>
   <si>
+    <t>Callback on VMStart.
+#################################################
+WARNING: The SecurityManager is being disabled!!!
+SecurityManager Changed:
+JTimelag.java, main, 6
+#################################################
+Agent OnUnload, agent exits.</t>
+  </si>
+  <si>
+    <t>Bug kind and pattern: SMSLB - DETECT_SECURITY_MANAGER_SET_LOCATION_BUG
+At JTimelag.java:[line 6]
+ In method jtimelag.JTimelag.main(String[]) 
+Value Set to null:
+Value aconst_null 
+Value aconst_null[1](1) 
+Value Variable is set at:</t>
+  </si>
+  <si>
     <t>./src/jtimelag/JTimelag.java
 6:        System.setSecurityManager(null);</t>
   </si>
   <si>
-    <t>Skipping this one for now.  Having trouble running the jnlp file.  Will come back later.</t>
+    <t>This application nulls the security manager at start up.  I think the application is being lazy with dealing with permissions.  Nulling occurs in this case.</t>
   </si>
   <si>
-    <t>It's setting SM to null in Jtimelag.java and set a frame visible.</t>
+    <t>Dynamically confirms the SecurityManager is set to null at the start of the application</t>
+  </si>
+  <si>
+    <t>Found the SecurityManager is set to null at the start of the application.</t>
+  </si>
+  <si>
+    <t>Sets the SM to to null in the first line of the application</t>
   </si>
   <si>
     <t>IntelliJ IDEA Community Edition</t>
@@ -7068,8 +7092,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36789,18 +36813,26 @@
       <c r="D40" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="0"/>
+      <c r="E40" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>284</v>
+      </c>
       <c r="G40" s="10" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="I40" s="0"/>
-      <c r="J40" s="0"/>
+        <v>286</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>288</v>
+      </c>
       <c r="K40" s="10" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="L40" s="0"/>
     </row>
@@ -36809,13 +36841,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="0"/>
@@ -36831,13 +36863,13 @@
         <v>40</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>60</v>
@@ -36846,10 +36878,10 @@
         <v>60</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="I42" s="0" t="s">
         <v>60</v>
@@ -36867,21 +36899,21 @@
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="0"/>
       <c r="G43" s="10" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="I43" s="0" t="s">
         <v>60</v>
@@ -36890,7 +36922,7 @@
         <v>60</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="L43" s="0"/>
     </row>
@@ -36899,13 +36931,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>60</v>
@@ -36914,10 +36946,10 @@
         <v>60</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="I44" s="0" t="s">
         <v>60</v>
@@ -36926,7 +36958,7 @@
         <v>60</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="L44" s="0"/>
     </row>
@@ -36935,13 +36967,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>60</v>
@@ -36950,10 +36982,10 @@
         <v>60</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="I45" s="0" t="s">
         <v>60</v>
@@ -36962,7 +36994,7 @@
         <v>60</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="L45" s="0"/>
     </row>
@@ -36971,13 +37003,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>60</v>
@@ -36986,10 +37018,10 @@
         <v>60</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="I46" s="0" t="s">
         <v>60</v>
@@ -36998,7 +37030,7 @@
         <v>60</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="L46" s="0"/>
     </row>
@@ -37007,13 +37039,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>60</v>
@@ -37022,10 +37054,10 @@
         <v>60</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>60</v>
@@ -37034,10 +37066,10 @@
         <v>60</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37045,13 +37077,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>60</v>
@@ -37060,10 +37092,10 @@
         <v>60</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>60</v>
@@ -37072,7 +37104,7 @@
         <v>60</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37080,13 +37112,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>60</v>
@@ -37095,10 +37127,10 @@
         <v>60</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>60</v>
@@ -37107,7 +37139,7 @@
         <v>60</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37115,13 +37147,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>60</v>
@@ -37130,10 +37162,10 @@
         <v>60</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>60</v>
@@ -37142,7 +37174,7 @@
         <v>60</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37150,13 +37182,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -37170,12 +37202,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added IntelliJ analysis - git application analysis complete
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="360">
   <si>
     <t>Index</t>
   </si>
@@ -5491,10 +5491,136 @@
     <t>IntelliJ IDEA Community Edition</t>
   </si>
   <si>
-    <t>0e8564a197eb4584a1df56670bb7ed2a47be8da2</t>
+    <t>4ec1634e99ab375bb44ecf2b22a62ee4f0e39a4d</t>
   </si>
   <si>
     <t>https://github.com/JetBrains/intellij-community</t>
+  </si>
+  <si>
+    <t>While I wasn't sure how to run the version I downloaded off github and compiled, I was able to run the latest intelliJ communty tools version 135.1289.  I received no output when I ran the program, which I expected from the grep output.</t>
+  </si>
+  <si>
+    <t>(static analysis is dieing half-way through (meaning won't run on 2 out of 4 jars) with index out of bounds error) no results from the 2 that ran</t>
+  </si>
+  <si>
+    <t>./plugins/InspectionGadgets/test/com/siyeh/igtest/security/SystemSetSecurityManagerInspection.java
+3:public class SystemSetSecurityManagerInspection
+7:       System.setSecurityManager(null);
+./plugins/InspectionGadgets/test/com/siyeh/igtest/security/CustomSecurityManager.java
+3:public class CustomSecurityManager extends SecurityManager{
+./plugins/InspectionGadgets/InspectionGadgetsAnalysis/src/com/siyeh/ig/security/CustomSecurityManagerInspection.java
+25:public class CustomSecurityManagerInspection extends BaseInspection {
+43:    return new CustomSecurityManagerVisitor();
+46:  private static class CustomSecurityManagerVisitor
+52:                                       "java.lang.SecurityManager")) {
+55:      if ("java.lang.SecurityManager".equals(aClass.getQualifiedName())) {
+./plugins/InspectionGadgets/InspectionGadgetsAnalysis/src/com/siyeh/ig/security/SystemSetSecurityManagerInspection.java
+28:public class SystemSetSecurityManagerInspection extends BaseInspection {
+33:    return "CallToSystemSetSecurityManager";
+52:    return new SystemSetSecurityManagerVisitor();
+55:  private static class SystemSetSecurityManagerVisitor
+62:      if (!isSetSecurityManager(expression)) {
+68:    private static boolean isSetSecurityManager(
+74:      if (!"setSecurityManager".equals(methodName)) {
+./java/java-tests/testSrc/com/intellij/psi/PsiNameHelperTest.java
+258:    doTest("java.lang.SecurityManager", "SecurityManager");
+./java/java-tests/testData/codeInsight/daemonCodeAnalyzer/advHighlighting/aClassLoader_hl.java
+205:     * @see       java.lang.SecurityManager#checkCreateClassLoader()
+209:	&lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; security = System.getSecurityManager();
+230:     * @see       java.lang.SecurityManager#checkCreateClassLoader()
+233:	&lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; security = System.getSecurityManager();
+318:	final &lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; sm = System.getSecurityManager();
+688:     * @see SecurityManager#checkPermission
+696:	&lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; sm = System.getSecurityManager();
+1017:     * @see SecurityManager#checkPermission
+1026:	&lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; sm = System.getSecurityManager();
+./java/java-tests/testData/codeInsight/daemonCodeAnalyzer/advHighlighting/aClassLoader.java
+205:     * @see       java.lang.SecurityManager#checkCreateClassLoader()
+209:	SecurityManager security = System.getSecurityManager();
+230:     * @see       java.lang.SecurityManager#checkCreateClassLoader()
+233:	SecurityManager security = System.getSecurityManager();
+318:	final SecurityManager sm = System.getSecurityManager();
+688:     * @see SecurityManager#checkPermission
+696:	SecurityManager sm = System.getSecurityManager();
+1017:     * @see SecurityManager#checkPermission
+1026:	SecurityManager sm = System.getSecurityManager();
+./platform/util/src/com/intellij/util/ReflectionUtil.java
+528:  private static class MySecurityManager extends SecurityManager {
+529:    private static final MySecurityManager INSTANCE = new MySecurityManager();
+546:      Class[] stack = MySecurityManager.INSTANCE.getStack();
+./platform/util/src/com/intellij/Patches.java
+150:   * AtomicIntegerFieldUpdater does not work when SecurityManager is installed
+./platform/platform-api/src/com/intellij/openapi/vfs/VirtualFileWrapper.java
+55:   *          java.lang.SecurityManager#checkRead(java.lang.String)}&lt;/code&gt;
+</t>
+  </si>
+  <si>
+    <t>Only sets a SecurityManager in test cases.  Interestingly, the code contains static analysis tools to check if  SecurityManager is set in the code.  It also contains a static analysis check to see if a custom SecurityManager is set.  Both of these are reported as a possible security error.  Further information on these checks can be found at: http://www.jetbrains.com/idea/documentation/inspections.jsp in the security section.  Otherwise, the code just states that SecurityExceptions may be thrown in certain areas if a SecurityManager is set.  No weakening or nulling.</t>
+  </si>
+  <si>
+    <t>No output so no analysis</t>
+  </si>
+  <si>
+    <t>./plugins/InspectionGadgets/test/com/siyeh/igtest/security/SystemSetSecurityManagerInspection.java
+3:public class SystemSetSecurityManagerInspection
+7:       System.setSecurityManager(null);
+This is a test case.
+./plugins/InspectionGadgets/test/com/siyeh/igtest/security/CustomSecurityManager.java
+3:public class CustomSecurityManager extends SecurityManager{
+This is an empty class
+./plugins/InspectionGadgets/InspectionGadgetsAnalysis/src/com/siyeh/ig/security/CustomSecurityManagerInspection.java
+25:public class CustomSecurityManagerInspection extends BaseInspection {
+43:    return new CustomSecurityManagerVisitor();
+46:  private static class CustomSecurityManagerVisitor
+52:                                       "java.lang.SecurityManager")) {
+55:      if ("java.lang.SecurityManager".equals(aClass.getQualifiedName())) {
+This class checks other classes to see if they are a custom security manager.  This one might be interesting with more review.
+./plugins/InspectionGadgets/InspectionGadgetsAnalysis/src/com/siyeh/ig/security/SystemSetSecurityManagerInspection.java
+28:public class SystemSetSecurityManagerInspection extends BaseInspection {
+33:    return "CallToSystemSetSecurityManager";
+52:    return new SystemSetSecurityManagerVisitor();
+55:  private static class SystemSetSecurityManagerVisitor
+62:      if (!isSetSecurityManager(expression)) {
+68:    private static boolean isSetSecurityManager(
+74:      if (!"setSecurityManager".equals(methodName)) {
+This checks to see if a class tries to set a SecurityManager.  I think these last two classes are designed to stop plugins from setting a SecurityManager but I'm not 100% sure at the moment.
+./java/java-tests/testSrc/com/intellij/psi/PsiNameHelperTest.java
+258:    doTest("java.lang.SecurityManager", "SecurityManager");
+This class is saving the extended import name of the SecurityManager class.  
+./java/java-tests/testData/codeInsight/daemonCodeAnalyzer/advHighlighting/aClassLoader_hl.java
+205:     * @see       java.lang.SecurityManager#checkCreateClassLoader()
+209:	&lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; security = System.getSecurityManager();
+230:     * @see       java.lang.SecurityManager#checkCreateClassLoader()
+233:	&lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; security = System.getSecurityManager();
+318:	final &lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; sm = System.getSecurityManager();
+688:     * @see SecurityManager#checkPermission
+696:	&lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; sm = System.getSecurityManager();
+1017:     * @see SecurityManager#checkPermission
+1026:	&lt;error descr="Cannot resolve symbol 'SecurityManager'"&gt;SecurityManager&lt;/error&gt; sm = System.getSecurityManager();
+contains comments that say methods may throw errors if a SecurityManager is present.  The class seems to be for running test cases.
+./java/java-tests/testData/codeInsight/daemonCodeAnalyzer/advHighlighting/aClassLoader.java
+205:     * @see       java.lang.SecurityManager#checkCreateClassLoader()
+209:	SecurityManager security = System.getSecurityManager();
+230:     * @see       java.lang.SecurityManager#checkCreateClassLoader()
+233:	SecurityManager security = System.getSecurityManager();
+318:	final SecurityManager sm = System.getSecurityManager();
+688:     * @see SecurityManager#checkPermission
+696:	SecurityManager sm = System.getSecurityManager();
+1017:     * @see SecurityManager#checkPermission
+1026:	SecurityManager sm = System.getSecurityManager();
+checks permissions if SecurityManager set.  Also calls doPrivileged if SecurityManager is set.
+./platform/util/src/com/intellij/util/ReflectionUtil.java
+528:  private static class MySecurityManager extends SecurityManager {
+529:    private static final MySecurityManager INSTANCE = new MySecurityManager();
+546:      Class[] stack = MySecurityManager.INSTANCE.getStack();
+Defines a securityManager class for returning the current call stack.
+./platform/util/src/com/intellij/Patches.java
+150:   * AtomicIntegerFieldUpdater does not work when SecurityManager is installed
+only a comment saying the code may not work if a SecurityManager is set.
+./platform/platform-api/src/com/intellij/openapi/vfs/VirtualFileWrapper.java
+55:   *          java.lang.SecurityManager#checkRead(java.lang.String)}&lt;/code&gt;
+test case comment saying it may not work if a SecurityManager is set.
+</t>
   </si>
   <si>
     <t>Metasploit-framework (excluding this one)</t>
@@ -5504,6 +5630,9 @@
   </si>
   <si>
     <t>https://github.com/rapid7/metasploit-framework</t>
+  </si>
+  <si>
+    <t>#################################################</t>
   </si>
   <si>
     <t>./external/source/exploits/cve-2012-5076/MyPayload.java
@@ -5574,8 +5703,7 @@
   <si>
     <t>./src/test/java/com/gmail/at/zhuikov/aleksandr/driveddoc/RestrictedFileWritingRule.java
 12:		System.setSecurityManager(new SecurityManager() {
-28:		System.setSecurityManager(null); // or save and restore original
-</t>
+28:		System.setSecurityManager(null); // or save and restore original</t>
   </si>
   <si>
     <t>Sets a SecurityManager before a test case and removes it afterwards.  No weakening or nulling occurs.  The program also does not interact with the SecurityManager in the main file.</t>
@@ -5584,8 +5712,7 @@
     <t>./src/test/java/com/gmail/at/zhuikov/aleksandr/driveddoc/RestrictedFileWritingRule.java
 12:		System.setSecurityManager(new SecurityManager() {
 28:		System.setSecurityManager(null); // or save and restore original
-Sets a SecurityManager for a test case and removes the SecurityManager after the test case
-</t>
+Sets a SecurityManager for a test case and removes the SecurityManager after the test case</t>
   </si>
   <si>
     <t>TracEE</t>
@@ -5595,6 +5722,9 @@
   </si>
   <si>
     <t>https://github.com/holisticon/tracee</t>
+  </si>
+  <si>
+    <t>Agent OnUnload, agent exits.</t>
   </si>
   <si>
     <t>./api/src/test/java/io/tracee/BackendProviderResolverGetClassLoaderTest.java
@@ -5629,8 +5759,7 @@
 Test cases - test if the program can get a class loader without a SM set and with an SM set
 ./api/src/main/java/io/tracee/BackendProviderResolver.java
 139:			if (System.getSecurityManager() != null) {
-runs doPriveleged if a SM is set to get a class loader
-</t>
+runs doPriveleged if a SM is set to get a class loader</t>
   </si>
   <si>
     <t>Spring-modules</t>
@@ -5676,8 +5805,7 @@
 59:		System.setSecurityManager(securityManager);
 79:	public SecurityManager getSecurityManager() {
 86:	public void setSecurityManager(SecurityManager securityManager) {
-Allows all possible changes to the current SecurityManager.  This class is designed to set a specific security policy for the spring-modules application, and can then restore the old security policy afterwards.
-</t>
+Allows all possible changes to the current SecurityManager.  This class is designed to set a specific security policy for the spring-modules application, and can then restore the old security policy afterwards.</t>
   </si>
   <si>
     <t>Security-Manager (This is a SecurityManager - not a program that uses one)</t>
@@ -5768,8 +5896,7 @@
 ./src/main/java/org/wildfly/security/manager/package-info.java
 25: * the security manager, see {@link WildFlySecurityManager#install()}.
 ./src/main/java/org/wildfly/security/manager/_private/SecurityMessages.java
-33:import org.wildfly.security.manager.WildFlySecurityManagerPermission;
-</t>
+33:import org.wildfly.security.manager.WildFlySecurityManagerPermission;</t>
   </si>
   <si>
     <t>This program is a SecurityManager, so it doesn't ever set a SecurityManager.  This extension allows turning the security checks off if the class already has the permission to do so (reimplementing how doPrivileged works in my opinion) and adds logs explaining why security checks fail. No nulling but allows weaken (although debatable).  Decided not to statically and dynamically test because it was easy to understand from the grep analysis.</t>
@@ -5860,8 +5987,7 @@
 in a comment.
 ./src/main/java/org/wildfly/security/manager/_private/SecurityMessages.java
 33:import org.wildfly.security.manager.WildFlySecurityManagerPermission;
-this is a privelege import statement.
-</t>
+this is a privelege import statement.</t>
   </si>
   <si>
     <t>Gjman</t>
@@ -7013,13 +7139,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -7092,8 +7218,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36849,13 +36975,27 @@
       <c r="D41" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
-      <c r="H41" s="0"/>
-      <c r="I41" s="0"/>
-      <c r="J41" s="0"/>
-      <c r="K41" s="0"/>
+      <c r="E41" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>298</v>
+      </c>
       <c r="L41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -36863,25 +37003,25 @@
         <v>40</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>60</v>
+        <v>302</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>60</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="I42" s="0" t="s">
         <v>60</v>
@@ -36899,21 +37039,23 @@
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="E43" s="6"/>
+        <v>307</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>302</v>
+      </c>
       <c r="F43" s="0"/>
       <c r="G43" s="10" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="I43" s="0" t="s">
         <v>60</v>
@@ -36922,7 +37064,7 @@
         <v>60</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="L43" s="0"/>
     </row>
@@ -36931,25 +37073,25 @@
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>60</v>
+        <v>314</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>60</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="I44" s="0" t="s">
         <v>60</v>
@@ -36958,7 +37100,7 @@
         <v>60</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="L44" s="0"/>
     </row>
@@ -36967,13 +37109,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>60</v>
@@ -36982,10 +37124,10 @@
         <v>60</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="I45" s="0" t="s">
         <v>60</v>
@@ -36994,7 +37136,7 @@
         <v>60</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="L45" s="0"/>
     </row>
@@ -37003,13 +37145,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>60</v>
@@ -37018,10 +37160,10 @@
         <v>60</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="I46" s="0" t="s">
         <v>60</v>
@@ -37030,7 +37172,7 @@
         <v>60</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="L46" s="0"/>
     </row>
@@ -37039,13 +37181,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>60</v>
@@ -37054,10 +37196,10 @@
         <v>60</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>60</v>
@@ -37066,10 +37208,10 @@
         <v>60</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37077,13 +37219,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>60</v>
@@ -37092,10 +37234,10 @@
         <v>60</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>60</v>
@@ -37104,7 +37246,7 @@
         <v>60</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37112,13 +37254,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>60</v>
@@ -37127,10 +37269,10 @@
         <v>60</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>60</v>
@@ -37139,7 +37281,7 @@
         <v>60</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37147,13 +37289,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>60</v>
@@ -37162,10 +37304,10 @@
         <v>60</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>60</v>
@@ -37174,7 +37316,7 @@
         <v>60</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37182,13 +37324,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="E51" s="6"/>
     </row>
@@ -37202,12 +37344,12 @@
     </row>
     <row r="54" customFormat="false" ht="79.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -37246,14 +37388,15 @@
     <hyperlink ref="D38" r:id="rId32" display="https://github.com/zoomis/NGOMS"/>
     <hyperlink ref="D40" r:id="rId33" display="https://github.com/Babast/Timelag"/>
     <hyperlink ref="D41" r:id="rId34" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="D43" r:id="rId35" display="https://github.com/aleksz/driveddoc"/>
-    <hyperlink ref="D44" r:id="rId36" display="https://github.com/holisticon/tracee"/>
-    <hyperlink ref="D45" r:id="rId37" display="https://github.com/astubbs/spring-modules"/>
-    <hyperlink ref="D46" r:id="rId38" display="https://github.com/wildfly-security/security-manager"/>
-    <hyperlink ref="D47" r:id="rId39" display="https://github.com/ngty/gjman"/>
-    <hyperlink ref="D49" r:id="rId40" display="https://github.com/stefanbirkner/system-rules"/>
-    <hyperlink ref="D50" r:id="rId41" display="https://github.com/ch33kybutt/oxygen_libcore"/>
-    <hyperlink ref="D51" r:id="rId42" display="https://github.com/apache/tomcat70"/>
+    <hyperlink ref="H41" r:id="rId35" display="http://www.jetbrains.com/idea/documentation/inspections.jsp"/>
+    <hyperlink ref="D43" r:id="rId36" display="https://github.com/aleksz/driveddoc"/>
+    <hyperlink ref="D44" r:id="rId37" display="https://github.com/holisticon/tracee"/>
+    <hyperlink ref="D45" r:id="rId38" display="https://github.com/astubbs/spring-modules"/>
+    <hyperlink ref="D46" r:id="rId39" display="https://github.com/wildfly-security/security-manager"/>
+    <hyperlink ref="D47" r:id="rId40" display="https://github.com/ngty/gjman"/>
+    <hyperlink ref="D49" r:id="rId41" display="https://github.com/stefanbirkner/system-rules"/>
+    <hyperlink ref="D50" r:id="rId42" display="https://github.com/ch33kybutt/oxygen_libcore"/>
+    <hyperlink ref="D51" r:id="rId43" display="https://github.com/apache/tomcat70"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
added way to set and restore SM in Ant
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -72,7 +72,19 @@
 “Callback on VMStart.
 #################################################
 #################################################
-Agent OnUnload, agent exits.”</t>
+Agent OnUnload, agent exits.”
+--------------------------------------------------------------------------------------
+When running a compilation that executes a Java class:
+Callback on VMStart.
+#################################################
+SecurityManager Changed:
+Permissions.java, setSecurityManager, 101
+WARNING: The SecurityManager is being disabled!!!
+SecurityManager Changed:
+Permissions.java, restoreSecurityManager, 171
+#################################################
+Agent OnUnload, agent exits.
+</t>
   </si>
   <si>
     <t>At Main.java:[line 856] 
@@ -151,12 +163,11 @@
 154:            perms.restoreSecurityManager();</t>
   </si>
   <si>
-    <t>It looks like we may be able to see a SecurityManager change if we are using special compilers that need to execute Java while compiling or write an application to use vendor specific extensions.  The only setSecurityManager I found that was valid is in the ExecuteJava.java file which is not called normally.
-Classification: Change SM but not in main application (weakening – allows setting and restoring SM)</t>
+    <t>Can cause the Ant to set and restore a SecurityManager if executing a Java class (not a jar) during the build process.  Ant will wrap the class's execution in a temporary SecurityManager.
+Classification: Change SMs  in main application (weakening – allows setting and restoring SM)</t>
   </si>
   <si>
-    <t>No output.  Probably don't have good code coverage although any classes loaded through another classloader than the default one would not be seen with the current Emma method I used.  
-Tests involed compiling Netbeans and Jruby.  No output for either.</t>
+    <t>Found that Ant will set a SecurityManager to execute a java class during compilation.  It will then restore the old SecurityManager after executing.</t>
   </si>
   <si>
     <t>At Main.java:[line 856] 
@@ -183,7 +194,7 @@
 Value Not null: org.apache.tools.ant.types.Permissions$MySM 
 Value new Value new[187](3) 14 
 Value Variable is set at:
-The method to set the SecurityManager when running unit tests although may be reachable from a different compiler in the main execution. - If a securityException is thrown, the exception is caught and returned as a specific exit code.
+The method to set the SecurityManager when running unit tests although may be reachable from a different compiler in the main execution. - If a securityException is thrown, the exception is caught and returned as a specific exit code. - Later it was determined that this is executable
 ---------------------------------------------------------------
  At Permissions.java:[line 171]
 In method org.apache.tools.ant.types.Permissions.restoreSecurityManager()
@@ -5551,8 +5562,7 @@
 ./platform/util/src/com/intellij/Patches.java
 150:   * AtomicIntegerFieldUpdater does not work when SecurityManager is installed
 ./platform/platform-api/src/com/intellij/openapi/vfs/VirtualFileWrapper.java
-55:   *          java.lang.SecurityManager#checkRead(java.lang.String)}&lt;/code&gt;
-</t>
+55:   *          java.lang.SecurityManager#checkRead(java.lang.String)}&lt;/code&gt;</t>
   </si>
   <si>
     <t>Only sets a SecurityManager in test cases.  Interestingly, the code contains static analysis tools to check if  SecurityManager is set in the code.  It also contains a static analysis check to see if a custom SecurityManager is set.  Both of these are reported as a possible security error.  Further information on these checks can be found at: http://www.jetbrains.com/idea/documentation/inspections.jsp in the security section.  Otherwise, the code just states that SecurityExceptions may be thrown in certain areas if a SecurityManager is set.  No weakening or nulling.</t>
@@ -5619,8 +5629,7 @@
 only a comment saying the code may not work if a SecurityManager is set.
 ./platform/platform-api/src/com/intellij/openapi/vfs/VirtualFileWrapper.java
 55:   *          java.lang.SecurityManager#checkRead(java.lang.String)}&lt;/code&gt;
-test case comment saying it may not work if a SecurityManager is set.
-</t>
+test case comment saying it may not work if a SecurityManager is set.</t>
   </si>
   <si>
     <t>Metasploit-framework (excluding this one)</t>
@@ -7139,13 +7148,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -7218,8 +7227,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -37388,7 +37397,7 @@
     <hyperlink ref="D38" r:id="rId32" display="https://github.com/zoomis/NGOMS"/>
     <hyperlink ref="D40" r:id="rId33" display="https://github.com/Babast/Timelag"/>
     <hyperlink ref="D41" r:id="rId34" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="H41" r:id="rId35" display="http://www.jetbrains.com/idea/documentation/inspections.jsp"/>
+    <hyperlink ref="H41" r:id="rId35" display="Only sets a SecurityManager in test cases.  Interestingly, the code contains static analysis tools to check if  SecurityManager is set in the code.  It also contains a static analysis check to see if a custom SecurityManager is set.  Both of these are reported as a possible security error.  Further information on these checks can be found at: http://www.jetbrains.com/idea/documentation/inspections.jsp in the security section.  Otherwise, the code just states that SecurityExceptions may be thrown in certain areas if a SecurityManager is set.  No weakening or nulling."/>
     <hyperlink ref="D43" r:id="rId36" display="https://github.com/aleksz/driveddoc"/>
     <hyperlink ref="D44" r:id="rId37" display="https://github.com/holisticon/tracee"/>
     <hyperlink ref="D45" r:id="rId38" display="https://github.com/astubbs/spring-modules"/>

</xml_diff>

<commit_message>
committing a couple of categorization labels in the general notes section
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -83,8 +83,7 @@
 SecurityManager Changed:
 Permissions.java, restoreSecurityManager, 171
 #################################################
-Agent OnUnload, agent exits.
-</t>
+Agent OnUnload, agent exits.</t>
   </si>
   <si>
     <t>At Main.java:[line 856] 
@@ -5346,7 +5345,8 @@
 798:        private RunSecurityManager(){}</t>
   </si>
   <si>
-    <t>This program only sets a SecurityManager in a test case.  Even in the test case, the SecurityManager only stops system.exit calls.  They also create a fully permissive SecurityManager but don't use it in one of the test packages.</t>
+    <t>This program only sets a SecurityManager in a test case.  Even in the test case, the SecurityManager only stops system.exit calls.  They also create a fully permissive SecurityManager but don't use it in one of the test packages.
+Classification: Only test cases</t>
   </si>
   <si>
     <t>MCVersion-Control (This program uses a user defined SecurityManager which I think does not extend the SecurityManager class)</t>
@@ -5450,7 +5450,8 @@
 11:    public SecurityManagerDecorator(SecurityManager securityManager) {</t>
   </si>
   <si>
-    <t>Creates SecurityManager in test case.  Never sets one during execution or any tests.</t>
+    <t>Creates SecurityManager in test case.  Never sets one during execution or any tests.
+Classification: Only interacts with SM in test cases</t>
   </si>
   <si>
     <t>Defines SM in the test code but never set it explicitly.</t>
@@ -5565,7 +5566,7 @@
 55:   *          java.lang.SecurityManager#checkRead(java.lang.String)}&lt;/code&gt;</t>
   </si>
   <si>
-    <t>Only sets a SecurityManager in test cases.  Interestingly, the code contains static analysis tools to check if  SecurityManager is set in the code.  It also contains a static analysis check to see if a custom SecurityManager is set.  Both of these are reported as a possible security error.  Further information on these checks can be found at: http://www.jetbrains.com/idea/documentation/inspections.jsp in the security section.  Otherwise, the code just states that SecurityExceptions may be thrown in certain areas if a SecurityManager is set.  No weakening or nulling.</t>
+    <t>Only sets a SecurityManager in test cases.  Interestingly, the code contains static analysis tools to check if  SecurityManager is set in the code.  It also contains a static analysis check to see if a custom SecurityManager is set.  Both of these are reported as a possible security error.  Further information on these checks can be found at: http://www.jetbrains.com/idea/documentation/inspections.jsp in the security section.  Otherwise, the code just states that SecurityExceptions may be thrown in certain areas if a SecurityManager is set.  No weakening or nulling. And interacts with</t>
   </si>
   <si>
     <t>No output so no analysis</t>
@@ -7148,13 +7149,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -7227,8 +7228,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
updated one of the versions
</commit_message>
<xml_diff>
--- a/projects list.xlsx
+++ b/projects list.xlsx
@@ -4248,7 +4248,7 @@
     <t>spring framework</t>
   </si>
   <si>
-    <t>(var),4.0.6 for current*</t>
+    <t> 4.0.6</t>
   </si>
   <si>
     <t>http://projects.spring.io/spring-framework/#quick-start</t>
@@ -7149,13 +7149,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -7228,8 +7228,8 @@
   </sheetPr>
   <dimension ref="1:55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -37398,7 +37398,7 @@
     <hyperlink ref="D38" r:id="rId32" display="https://github.com/zoomis/NGOMS"/>
     <hyperlink ref="D40" r:id="rId33" display="https://github.com/Babast/Timelag"/>
     <hyperlink ref="D41" r:id="rId34" display="https://github.com/JetBrains/intellij-community"/>
-    <hyperlink ref="H41" r:id="rId35" display="Only sets a SecurityManager in test cases.  Interestingly, the code contains static analysis tools to check if  SecurityManager is set in the code.  It also contains a static analysis check to see if a custom SecurityManager is set.  Both of these are reported as a possible security error.  Further information on these checks can be found at: http://www.jetbrains.com/idea/documentation/inspections.jsp in the security section.  Otherwise, the code just states that SecurityExceptions may be thrown in certain areas if a SecurityManager is set.  No weakening or nulling."/>
+    <hyperlink ref="H41" r:id="rId35" display="Only sets a SecurityManager in test cases.  Interestingly, the code contains static analysis tools to check if  SecurityManager is set in the code.  It also contains a static analysis check to see if a custom SecurityManager is set.  Both of these are reported as a possible security error.  Further information on these checks can be found at: http://www.jetbrains.com/idea/documentation/inspections.jsp in the security section.  Otherwise, the code just states that SecurityExceptions may be thrown in certain areas if a SecurityManager is set.  No weakening or nulling. And interacts with"/>
     <hyperlink ref="D43" r:id="rId36" display="https://github.com/aleksz/driveddoc"/>
     <hyperlink ref="D44" r:id="rId37" display="https://github.com/holisticon/tracee"/>
     <hyperlink ref="D45" r:id="rId38" display="https://github.com/astubbs/spring-modules"/>

</xml_diff>